<commit_message>
Update event handler for table collection onChanged event
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18816"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19106"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3756C24-477F-4801-8313-03F20D868E29}" xr6:coauthVersionLast="29" xr6:coauthVersionMax="29" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10778" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="214">
   <si>
     <t>Class</t>
   </si>
@@ -645,9 +646,6 @@
     <t>excel-events-tablecollection-changed</t>
   </si>
   <si>
-    <t>onDataChange</t>
-  </si>
-  <si>
     <t>tableId</t>
   </si>
   <si>
@@ -655,6 +653,15 @@
   </si>
   <si>
     <t>excel-events-table-changed</t>
+  </si>
+  <si>
+    <t>registerOnChangedHandler</t>
+  </si>
+  <si>
+    <t>onChanged</t>
+  </si>
+  <si>
+    <t>onChange</t>
   </si>
 </sst>
 </file>
@@ -1045,17 +1052,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1069,7 +1078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1083,7 +1092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1097,7 +1106,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1111,7 +1120,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1125,7 +1134,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1139,7 +1148,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1153,7 +1162,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1167,7 +1176,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1181,7 +1190,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1195,7 +1204,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1209,7 +1218,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1223,7 +1232,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1237,7 +1246,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1251,7 +1260,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1265,7 +1274,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1279,7 +1288,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1293,7 +1302,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1307,7 +1316,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1321,7 +1330,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1335,7 +1344,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1349,7 +1358,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1363,7 +1372,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -1377,7 +1386,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
@@ -1391,7 +1400,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1405,7 +1414,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -1419,7 +1428,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>57</v>
       </c>
@@ -1433,7 +1442,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
@@ -1447,7 +1456,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
@@ -1461,7 +1470,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>67</v>
       </c>
@@ -1475,7 +1484,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -1489,7 +1498,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>71</v>
       </c>
@@ -1503,7 +1512,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
@@ -1517,7 +1526,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>65</v>
       </c>
@@ -1531,7 +1540,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>77</v>
       </c>
@@ -1545,7 +1554,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -1559,7 +1568,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
@@ -1573,7 +1582,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>81</v>
       </c>
@@ -1587,7 +1596,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
@@ -1601,7 +1610,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>85</v>
       </c>
@@ -1615,7 +1624,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -1629,7 +1638,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>65</v>
       </c>
@@ -1643,7 +1652,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>89</v>
       </c>
@@ -1657,7 +1666,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>89</v>
       </c>
@@ -1671,7 +1680,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>92</v>
       </c>
@@ -1685,7 +1694,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>92</v>
       </c>
@@ -1699,7 +1708,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>65</v>
       </c>
@@ -1713,7 +1722,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
@@ -1727,7 +1736,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
@@ -1741,7 +1750,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
@@ -1755,7 +1764,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>98</v>
       </c>
@@ -1769,7 +1778,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>65</v>
       </c>
@@ -1783,7 +1792,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>100</v>
       </c>
@@ -1797,7 +1806,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>100</v>
       </c>
@@ -1811,7 +1820,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>103</v>
       </c>
@@ -1825,7 +1834,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
@@ -1839,7 +1848,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>63</v>
       </c>
@@ -1853,7 +1862,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -1867,7 +1876,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
@@ -1881,7 +1890,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>28</v>
       </c>
@@ -1895,7 +1904,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>107</v>
       </c>
@@ -1909,7 +1918,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>107</v>
       </c>
@@ -1923,7 +1932,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>107</v>
       </c>
@@ -1937,7 +1946,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>107</v>
       </c>
@@ -1951,7 +1960,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>115</v>
       </c>
@@ -1965,7 +1974,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>117</v>
       </c>
@@ -1979,7 +1988,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>117</v>
       </c>
@@ -1993,7 +2002,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>117</v>
       </c>
@@ -2007,7 +2016,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>117</v>
       </c>
@@ -2021,7 +2030,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>117</v>
       </c>
@@ -2035,7 +2044,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>54</v>
       </c>
@@ -2049,7 +2058,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>54</v>
       </c>
@@ -2063,7 +2072,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>131</v>
       </c>
@@ -2077,7 +2086,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>135</v>
       </c>
@@ -2091,7 +2100,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>139</v>
       </c>
@@ -2105,7 +2114,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>139</v>
       </c>
@@ -2119,7 +2128,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>143</v>
       </c>
@@ -2133,7 +2142,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>146</v>
       </c>
@@ -2147,7 +2156,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>146</v>
       </c>
@@ -2158,10 +2167,10 @@
         <v>149</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>150</v>
       </c>
@@ -2175,7 +2184,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>150</v>
       </c>
@@ -2189,7 +2198,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>154</v>
       </c>
@@ -2203,7 +2212,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>158</v>
       </c>
@@ -2217,7 +2226,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>161</v>
       </c>
@@ -2231,7 +2240,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>165</v>
       </c>
@@ -2245,7 +2254,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>169</v>
       </c>
@@ -2259,7 +2268,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>169</v>
       </c>
@@ -2273,7 +2282,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>165</v>
       </c>
@@ -2287,7 +2296,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>165</v>
       </c>
@@ -2301,7 +2310,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>165</v>
       </c>
@@ -2315,7 +2324,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>165</v>
       </c>
@@ -2329,7 +2338,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>178</v>
       </c>
@@ -2343,7 +2352,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>178</v>
       </c>
@@ -2357,7 +2366,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>182</v>
       </c>
@@ -2365,13 +2374,13 @@
         <v>113</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>184</v>
       </c>
@@ -2379,13 +2388,13 @@
         <v>5</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>186</v>
       </c>
@@ -2393,13 +2402,13 @@
         <v>187</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>184</v>
       </c>
@@ -2413,7 +2422,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>192</v>
       </c>
@@ -2427,7 +2436,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>193</v>
       </c>
@@ -2441,7 +2450,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>146</v>
       </c>
@@ -2455,7 +2464,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>146</v>
       </c>
@@ -2469,7 +2478,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>146</v>
       </c>
@@ -2483,7 +2492,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>146</v>
       </c>
@@ -2497,7 +2506,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>182</v>
       </c>
@@ -2511,7 +2520,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>182</v>
       </c>
@@ -2525,21 +2534,21 @@
         <v>203</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>182</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>5</v>
+        <v>212</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>207</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>182</v>
       </c>
@@ -2550,21 +2559,21 @@
         <v>207</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>182</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>207</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update event handler for table collection onChanged event (#136)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18816"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19106"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3756C24-477F-4801-8313-03F20D868E29}" xr6:coauthVersionLast="29" xr6:coauthVersionMax="29" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10778" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="214">
   <si>
     <t>Class</t>
   </si>
@@ -645,9 +646,6 @@
     <t>excel-events-tablecollection-changed</t>
   </si>
   <si>
-    <t>onDataChange</t>
-  </si>
-  <si>
     <t>tableId</t>
   </si>
   <si>
@@ -655,6 +653,15 @@
   </si>
   <si>
     <t>excel-events-table-changed</t>
+  </si>
+  <si>
+    <t>registerOnChangedHandler</t>
+  </si>
+  <si>
+    <t>onChanged</t>
+  </si>
+  <si>
+    <t>onChange</t>
   </si>
 </sst>
 </file>
@@ -1045,17 +1052,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1069,7 +1078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1083,7 +1092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1097,7 +1106,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1111,7 +1120,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1125,7 +1134,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1139,7 +1148,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1153,7 +1162,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1167,7 +1176,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1181,7 +1190,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1195,7 +1204,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1209,7 +1218,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1223,7 +1232,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1237,7 +1246,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1251,7 +1260,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1265,7 +1274,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1279,7 +1288,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1293,7 +1302,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1307,7 +1316,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1321,7 +1330,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1335,7 +1344,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1349,7 +1358,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1363,7 +1372,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -1377,7 +1386,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
@@ -1391,7 +1400,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1405,7 +1414,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -1419,7 +1428,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>57</v>
       </c>
@@ -1433,7 +1442,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
@@ -1447,7 +1456,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
@@ -1461,7 +1470,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>67</v>
       </c>
@@ -1475,7 +1484,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -1489,7 +1498,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>71</v>
       </c>
@@ -1503,7 +1512,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
@@ -1517,7 +1526,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>65</v>
       </c>
@@ -1531,7 +1540,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>77</v>
       </c>
@@ -1545,7 +1554,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -1559,7 +1568,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
@@ -1573,7 +1582,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>81</v>
       </c>
@@ -1587,7 +1596,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
@@ -1601,7 +1610,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>85</v>
       </c>
@@ -1615,7 +1624,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -1629,7 +1638,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>65</v>
       </c>
@@ -1643,7 +1652,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>89</v>
       </c>
@@ -1657,7 +1666,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>89</v>
       </c>
@@ -1671,7 +1680,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>92</v>
       </c>
@@ -1685,7 +1694,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>92</v>
       </c>
@@ -1699,7 +1708,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>65</v>
       </c>
@@ -1713,7 +1722,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
@@ -1727,7 +1736,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
@@ -1741,7 +1750,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
@@ -1755,7 +1764,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>98</v>
       </c>
@@ -1769,7 +1778,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>65</v>
       </c>
@@ -1783,7 +1792,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>100</v>
       </c>
@@ -1797,7 +1806,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>100</v>
       </c>
@@ -1811,7 +1820,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>103</v>
       </c>
@@ -1825,7 +1834,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
@@ -1839,7 +1848,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>63</v>
       </c>
@@ -1853,7 +1862,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -1867,7 +1876,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
@@ -1881,7 +1890,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>28</v>
       </c>
@@ -1895,7 +1904,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>107</v>
       </c>
@@ -1909,7 +1918,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>107</v>
       </c>
@@ -1923,7 +1932,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>107</v>
       </c>
@@ -1937,7 +1946,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>107</v>
       </c>
@@ -1951,7 +1960,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>115</v>
       </c>
@@ -1965,7 +1974,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>117</v>
       </c>
@@ -1979,7 +1988,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>117</v>
       </c>
@@ -1993,7 +2002,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>117</v>
       </c>
@@ -2007,7 +2016,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>117</v>
       </c>
@@ -2021,7 +2030,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>117</v>
       </c>
@@ -2035,7 +2044,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>54</v>
       </c>
@@ -2049,7 +2058,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>54</v>
       </c>
@@ -2063,7 +2072,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>131</v>
       </c>
@@ -2077,7 +2086,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>135</v>
       </c>
@@ -2091,7 +2100,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>139</v>
       </c>
@@ -2105,7 +2114,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>139</v>
       </c>
@@ -2119,7 +2128,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>143</v>
       </c>
@@ -2133,7 +2142,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>146</v>
       </c>
@@ -2147,7 +2156,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>146</v>
       </c>
@@ -2158,10 +2167,10 @@
         <v>149</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>150</v>
       </c>
@@ -2175,7 +2184,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>150</v>
       </c>
@@ -2189,7 +2198,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>154</v>
       </c>
@@ -2203,7 +2212,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>158</v>
       </c>
@@ -2217,7 +2226,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>161</v>
       </c>
@@ -2231,7 +2240,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>165</v>
       </c>
@@ -2245,7 +2254,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>169</v>
       </c>
@@ -2259,7 +2268,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>169</v>
       </c>
@@ -2273,7 +2282,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>165</v>
       </c>
@@ -2287,7 +2296,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>165</v>
       </c>
@@ -2301,7 +2310,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>165</v>
       </c>
@@ -2315,7 +2324,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>165</v>
       </c>
@@ -2329,7 +2338,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>178</v>
       </c>
@@ -2343,7 +2352,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>178</v>
       </c>
@@ -2357,7 +2366,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>182</v>
       </c>
@@ -2365,13 +2374,13 @@
         <v>113</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>184</v>
       </c>
@@ -2379,13 +2388,13 @@
         <v>5</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>186</v>
       </c>
@@ -2393,13 +2402,13 @@
         <v>187</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>184</v>
       </c>
@@ -2413,7 +2422,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>192</v>
       </c>
@@ -2427,7 +2436,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>193</v>
       </c>
@@ -2441,7 +2450,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>146</v>
       </c>
@@ -2455,7 +2464,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>146</v>
       </c>
@@ -2469,7 +2478,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>146</v>
       </c>
@@ -2483,7 +2492,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>146</v>
       </c>
@@ -2497,7 +2506,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>182</v>
       </c>
@@ -2511,7 +2520,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>182</v>
       </c>
@@ -2525,21 +2534,21 @@
         <v>203</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>182</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>5</v>
+        <v>212</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>207</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>182</v>
       </c>
@@ -2550,21 +2559,21 @@
         <v>207</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>182</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>207</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update code samples for onChanged events
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19106"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3756C24-477F-4801-8313-03F20D868E29}" xr6:coauthVersionLast="29" xr6:coauthVersionMax="29" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F1E29E-8B89-47B2-901E-6D0CCAA7E449}" xr6:coauthVersionLast="29" xr6:coauthVersionMax="29" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="213">
   <si>
     <t>Class</t>
   </si>
@@ -575,9 +575,6 @@
   </si>
   <si>
     <t>WorksheetAddedEvent</t>
-  </si>
-  <si>
-    <t>registerOnDataChangedHandler</t>
   </si>
   <si>
     <t>WorksheetDataChangedEvent</t>
@@ -1052,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2167,7 +2164,7 @@
         <v>149</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2374,7 +2371,7 @@
         <v>113</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>183</v>
@@ -2385,27 +2382,27 @@
         <v>184</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>5</v>
+        <v>211</v>
       </c>
       <c r="C95" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="C96" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2413,41 +2410,41 @@
         <v>184</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>5</v>
+        <v>211</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="C99" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2455,13 +2452,13 @@
         <v>146</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2469,13 +2466,13 @@
         <v>146</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2483,13 +2480,13 @@
         <v>146</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="D102" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2497,13 +2494,13 @@
         <v>146</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C103" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2511,13 +2508,13 @@
         <v>182</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C104" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2525,13 +2522,13 @@
         <v>182</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2539,13 +2536,13 @@
         <v>182</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2553,13 +2550,13 @@
         <v>182</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2567,13 +2564,13 @@
         <v>182</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update code samples for onChanged events (#138)
* Update code samples for onChanged events

* Update code samples for onChanged event
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19106"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3756C24-477F-4801-8313-03F20D868E29}" xr6:coauthVersionLast="29" xr6:coauthVersionMax="29" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F1E29E-8B89-47B2-901E-6D0CCAA7E449}" xr6:coauthVersionLast="29" xr6:coauthVersionMax="29" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="213">
   <si>
     <t>Class</t>
   </si>
@@ -575,9 +575,6 @@
   </si>
   <si>
     <t>WorksheetAddedEvent</t>
-  </si>
-  <si>
-    <t>registerOnDataChangedHandler</t>
   </si>
   <si>
     <t>WorksheetDataChangedEvent</t>
@@ -1052,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2167,7 +2164,7 @@
         <v>149</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2374,7 +2371,7 @@
         <v>113</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>183</v>
@@ -2385,27 +2382,27 @@
         <v>184</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>5</v>
+        <v>211</v>
       </c>
       <c r="C95" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="C96" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2413,41 +2410,41 @@
         <v>184</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>5</v>
+        <v>211</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="C99" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2455,13 +2452,13 @@
         <v>146</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2469,13 +2466,13 @@
         <v>146</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2483,13 +2480,13 @@
         <v>146</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="D102" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2497,13 +2494,13 @@
         <v>146</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C103" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2511,13 +2508,13 @@
         <v>182</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C104" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2525,13 +2522,13 @@
         <v>182</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2539,13 +2536,13 @@
         <v>182</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2553,13 +2550,13 @@
         <v>182</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2567,13 +2564,13 @@
         <v>182</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to test generation of snippets.yaml files (Excel and OneNote) for input into API Documenter.
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19106"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19206"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F1E29E-8B89-47B2-901E-6D0CCAA7E449}" xr6:coauthVersionLast="29" xr6:coauthVersionMax="29" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C23CA1-8D11-431C-A682-93729F7DC902}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="216">
   <si>
     <t>Class</t>
   </si>
@@ -659,6 +659,15 @@
   </si>
   <si>
     <t>onChange</t>
+  </si>
+  <si>
+    <t>Chart</t>
+  </si>
+  <si>
+    <t>excel-ref-snippets-js</t>
+  </si>
+  <si>
+    <t>deleteChart</t>
   </si>
 </sst>
 </file>
@@ -738,8 +747,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D108" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D108" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D109" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D109" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -1047,21 +1056,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D108"/>
+  <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1075,7 +1085,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1089,7 +1099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1103,7 +1113,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1117,7 +1127,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1131,7 +1141,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1145,7 +1155,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1159,7 +1169,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1173,7 +1183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1187,7 +1197,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1201,7 +1211,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1215,7 +1225,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1229,7 +1239,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1243,7 +1253,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1257,7 +1267,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1271,7 +1281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1285,7 +1295,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1299,7 +1309,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1313,7 +1323,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1327,7 +1337,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1341,7 +1351,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1355,7 +1365,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1369,7 +1379,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -1383,7 +1393,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
@@ -1397,7 +1407,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1411,7 +1421,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -1425,7 +1435,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>57</v>
       </c>
@@ -1439,7 +1449,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
@@ -1453,7 +1463,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
@@ -1467,7 +1477,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>67</v>
       </c>
@@ -1481,7 +1491,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -1495,7 +1505,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>71</v>
       </c>
@@ -1509,7 +1519,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
@@ -1523,7 +1533,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>65</v>
       </c>
@@ -1537,7 +1547,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>77</v>
       </c>
@@ -1551,7 +1561,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -1565,7 +1575,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
@@ -1579,7 +1589,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>81</v>
       </c>
@@ -1593,7 +1603,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
@@ -1607,7 +1617,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>85</v>
       </c>
@@ -1621,7 +1631,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -1635,7 +1645,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>65</v>
       </c>
@@ -1649,7 +1659,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>89</v>
       </c>
@@ -1663,7 +1673,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>89</v>
       </c>
@@ -1677,7 +1687,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>92</v>
       </c>
@@ -1691,7 +1701,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>92</v>
       </c>
@@ -1705,7 +1715,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>65</v>
       </c>
@@ -1719,7 +1729,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
@@ -1733,7 +1743,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
@@ -1747,7 +1757,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
@@ -1761,7 +1771,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>98</v>
       </c>
@@ -1775,7 +1785,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>65</v>
       </c>
@@ -1789,7 +1799,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>100</v>
       </c>
@@ -1803,7 +1813,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>100</v>
       </c>
@@ -1817,7 +1827,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>103</v>
       </c>
@@ -1831,7 +1841,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
@@ -1845,7 +1855,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>63</v>
       </c>
@@ -1859,7 +1869,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -1873,7 +1883,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
@@ -1887,7 +1897,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>28</v>
       </c>
@@ -1901,7 +1911,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>107</v>
       </c>
@@ -1915,7 +1925,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>107</v>
       </c>
@@ -1929,7 +1939,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>107</v>
       </c>
@@ -1943,7 +1953,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>107</v>
       </c>
@@ -1957,7 +1967,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>115</v>
       </c>
@@ -1971,7 +1981,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>117</v>
       </c>
@@ -1985,7 +1995,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>117</v>
       </c>
@@ -1999,7 +2009,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
         <v>117</v>
       </c>
@@ -2013,7 +2023,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
         <v>117</v>
       </c>
@@ -2027,7 +2037,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
         <v>117</v>
       </c>
@@ -2041,7 +2051,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
         <v>54</v>
       </c>
@@ -2055,7 +2065,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
         <v>54</v>
       </c>
@@ -2069,7 +2079,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>131</v>
       </c>
@@ -2083,7 +2093,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
         <v>135</v>
       </c>
@@ -2097,7 +2107,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
         <v>139</v>
       </c>
@@ -2111,7 +2121,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
         <v>139</v>
       </c>
@@ -2125,7 +2135,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
         <v>143</v>
       </c>
@@ -2139,7 +2149,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
         <v>146</v>
       </c>
@@ -2153,7 +2163,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
         <v>146</v>
       </c>
@@ -2167,7 +2177,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
         <v>150</v>
       </c>
@@ -2181,7 +2191,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
         <v>150</v>
       </c>
@@ -2195,7 +2205,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
         <v>154</v>
       </c>
@@ -2209,7 +2219,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
         <v>158</v>
       </c>
@@ -2223,7 +2233,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
         <v>161</v>
       </c>
@@ -2237,7 +2247,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
         <v>165</v>
       </c>
@@ -2251,7 +2261,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
         <v>169</v>
       </c>
@@ -2265,7 +2275,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
         <v>169</v>
       </c>
@@ -2279,7 +2289,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
         <v>165</v>
       </c>
@@ -2293,7 +2303,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
         <v>165</v>
       </c>
@@ -2307,7 +2317,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
         <v>165</v>
       </c>
@@ -2321,7 +2331,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
         <v>165</v>
       </c>
@@ -2335,7 +2345,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
         <v>178</v>
       </c>
@@ -2349,7 +2359,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
         <v>178</v>
       </c>
@@ -2363,7 +2373,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
         <v>182</v>
       </c>
@@ -2377,7 +2387,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
         <v>184</v>
       </c>
@@ -2391,7 +2401,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96" s="1" t="s">
         <v>185</v>
       </c>
@@ -2405,7 +2415,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97" s="1" t="s">
         <v>184</v>
       </c>
@@ -2419,7 +2429,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98" s="1" t="s">
         <v>191</v>
       </c>
@@ -2433,7 +2443,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99" s="1" t="s">
         <v>192</v>
       </c>
@@ -2447,7 +2457,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
         <v>146</v>
       </c>
@@ -2461,7 +2471,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
         <v>146</v>
       </c>
@@ -2475,7 +2485,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A102" s="1" t="s">
         <v>146</v>
       </c>
@@ -2489,7 +2499,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A103" s="1" t="s">
         <v>146</v>
       </c>
@@ -2503,7 +2513,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A104" s="1" t="s">
         <v>182</v>
       </c>
@@ -2517,7 +2527,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="s">
         <v>182</v>
       </c>
@@ -2531,7 +2541,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
         <v>182</v>
       </c>
@@ -2545,7 +2555,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="s">
         <v>182</v>
       </c>
@@ -2559,7 +2569,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A108" s="1" t="s">
         <v>182</v>
       </c>
@@ -2571,6 +2581,20 @@
       </c>
       <c r="D108" s="1" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A109" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generate a single snippets.yaml file (for API Documenter) (#152)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19106"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19206"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F1E29E-8B89-47B2-901E-6D0CCAA7E449}" xr6:coauthVersionLast="29" xr6:coauthVersionMax="29" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C23CA1-8D11-431C-A682-93729F7DC902}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="216">
   <si>
     <t>Class</t>
   </si>
@@ -659,6 +659,15 @@
   </si>
   <si>
     <t>onChange</t>
+  </si>
+  <si>
+    <t>Chart</t>
+  </si>
+  <si>
+    <t>excel-ref-snippets-js</t>
+  </si>
+  <si>
+    <t>deleteChart</t>
   </si>
 </sst>
 </file>
@@ -738,8 +747,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D108" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D108" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D109" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D109" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -1047,21 +1056,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D108"/>
+  <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1075,7 +1085,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1089,7 +1099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1103,7 +1113,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1117,7 +1127,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1131,7 +1141,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1145,7 +1155,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1159,7 +1169,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1173,7 +1183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1187,7 +1197,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1201,7 +1211,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1215,7 +1225,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1229,7 +1239,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1243,7 +1253,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1257,7 +1267,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1271,7 +1281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1285,7 +1295,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1299,7 +1309,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1313,7 +1323,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1327,7 +1337,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1341,7 +1351,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1355,7 +1365,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1369,7 +1379,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -1383,7 +1393,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
@@ -1397,7 +1407,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1411,7 +1421,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -1425,7 +1435,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>57</v>
       </c>
@@ -1439,7 +1449,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
@@ -1453,7 +1463,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
@@ -1467,7 +1477,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>67</v>
       </c>
@@ -1481,7 +1491,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -1495,7 +1505,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>71</v>
       </c>
@@ -1509,7 +1519,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
@@ -1523,7 +1533,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>65</v>
       </c>
@@ -1537,7 +1547,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>77</v>
       </c>
@@ -1551,7 +1561,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -1565,7 +1575,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
@@ -1579,7 +1589,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>81</v>
       </c>
@@ -1593,7 +1603,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
@@ -1607,7 +1617,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>85</v>
       </c>
@@ -1621,7 +1631,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -1635,7 +1645,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>65</v>
       </c>
@@ -1649,7 +1659,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>89</v>
       </c>
@@ -1663,7 +1673,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>89</v>
       </c>
@@ -1677,7 +1687,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>92</v>
       </c>
@@ -1691,7 +1701,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>92</v>
       </c>
@@ -1705,7 +1715,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>65</v>
       </c>
@@ -1719,7 +1729,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
@@ -1733,7 +1743,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
@@ -1747,7 +1757,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
@@ -1761,7 +1771,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>98</v>
       </c>
@@ -1775,7 +1785,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>65</v>
       </c>
@@ -1789,7 +1799,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>100</v>
       </c>
@@ -1803,7 +1813,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>100</v>
       </c>
@@ -1817,7 +1827,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>103</v>
       </c>
@@ -1831,7 +1841,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
@@ -1845,7 +1855,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>63</v>
       </c>
@@ -1859,7 +1869,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -1873,7 +1883,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
@@ -1887,7 +1897,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>28</v>
       </c>
@@ -1901,7 +1911,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>107</v>
       </c>
@@ -1915,7 +1925,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>107</v>
       </c>
@@ -1929,7 +1939,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>107</v>
       </c>
@@ -1943,7 +1953,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>107</v>
       </c>
@@ -1957,7 +1967,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>115</v>
       </c>
@@ -1971,7 +1981,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>117</v>
       </c>
@@ -1985,7 +1995,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>117</v>
       </c>
@@ -1999,7 +2009,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
         <v>117</v>
       </c>
@@ -2013,7 +2023,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
         <v>117</v>
       </c>
@@ -2027,7 +2037,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
         <v>117</v>
       </c>
@@ -2041,7 +2051,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
         <v>54</v>
       </c>
@@ -2055,7 +2065,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
         <v>54</v>
       </c>
@@ -2069,7 +2079,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>131</v>
       </c>
@@ -2083,7 +2093,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
         <v>135</v>
       </c>
@@ -2097,7 +2107,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
         <v>139</v>
       </c>
@@ -2111,7 +2121,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
         <v>139</v>
       </c>
@@ -2125,7 +2135,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
         <v>143</v>
       </c>
@@ -2139,7 +2149,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
         <v>146</v>
       </c>
@@ -2153,7 +2163,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
         <v>146</v>
       </c>
@@ -2167,7 +2177,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
         <v>150</v>
       </c>
@@ -2181,7 +2191,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
         <v>150</v>
       </c>
@@ -2195,7 +2205,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
         <v>154</v>
       </c>
@@ -2209,7 +2219,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
         <v>158</v>
       </c>
@@ -2223,7 +2233,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
         <v>161</v>
       </c>
@@ -2237,7 +2247,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
         <v>165</v>
       </c>
@@ -2251,7 +2261,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
         <v>169</v>
       </c>
@@ -2265,7 +2275,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
         <v>169</v>
       </c>
@@ -2279,7 +2289,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
         <v>165</v>
       </c>
@@ -2293,7 +2303,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
         <v>165</v>
       </c>
@@ -2307,7 +2317,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
         <v>165</v>
       </c>
@@ -2321,7 +2331,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
         <v>165</v>
       </c>
@@ -2335,7 +2345,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
         <v>178</v>
       </c>
@@ -2349,7 +2359,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
         <v>178</v>
       </c>
@@ -2363,7 +2373,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
         <v>182</v>
       </c>
@@ -2377,7 +2387,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
         <v>184</v>
       </c>
@@ -2391,7 +2401,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96" s="1" t="s">
         <v>185</v>
       </c>
@@ -2405,7 +2415,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97" s="1" t="s">
         <v>184</v>
       </c>
@@ -2419,7 +2429,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98" s="1" t="s">
         <v>191</v>
       </c>
@@ -2433,7 +2443,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99" s="1" t="s">
         <v>192</v>
       </c>
@@ -2447,7 +2457,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
         <v>146</v>
       </c>
@@ -2461,7 +2471,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
         <v>146</v>
       </c>
@@ -2475,7 +2485,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A102" s="1" t="s">
         <v>146</v>
       </c>
@@ -2489,7 +2499,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A103" s="1" t="s">
         <v>146</v>
       </c>
@@ -2503,7 +2513,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A104" s="1" t="s">
         <v>182</v>
       </c>
@@ -2517,7 +2527,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="s">
         <v>182</v>
       </c>
@@ -2531,7 +2541,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
         <v>182</v>
       </c>
@@ -2545,7 +2555,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="s">
         <v>182</v>
       </c>
@@ -2559,7 +2569,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A108" s="1" t="s">
         <v>182</v>
       </c>
@@ -2571,6 +2581,20 @@
       </c>
       <c r="D108" s="1" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A109" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove code snippets (and mapping file info) that I previously created for JS snippets to inject into API Reference docs.
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19206"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19229"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C23CA1-8D11-431C-A682-93729F7DC902}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A584B0-FD15-4851-BC3E-4A363B1F0021}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="213">
   <si>
     <t>Class</t>
   </si>
@@ -659,15 +659,6 @@
   </si>
   <si>
     <t>onChange</t>
-  </si>
-  <si>
-    <t>Chart</t>
-  </si>
-  <si>
-    <t>excel-ref-snippets-js</t>
-  </si>
-  <si>
-    <t>deleteChart</t>
   </si>
 </sst>
 </file>
@@ -747,8 +738,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D109" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D109" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D108" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D108" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -1056,11 +1047,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A109" sqref="A109"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2583,20 +2574,6 @@
         <v>212</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A109" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Remove code snippets (and mapping file info) for JS snippets (#154)
This PR removes data that I previously added to test our ability to auto-inject JS snippets into the API Reference docs in the same way that we do for TS snippets; Script Lab content/functionality isn't in any way affected by this PR.
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19206"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19229"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C23CA1-8D11-431C-A682-93729F7DC902}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A584B0-FD15-4851-BC3E-4A363B1F0021}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="213">
   <si>
     <t>Class</t>
   </si>
@@ -659,15 +659,6 @@
   </si>
   <si>
     <t>onChange</t>
-  </si>
-  <si>
-    <t>Chart</t>
-  </si>
-  <si>
-    <t>excel-ref-snippets-js</t>
-  </si>
-  <si>
-    <t>deleteChart</t>
   </si>
 </sst>
 </file>
@@ -747,8 +738,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D109" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D109" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D108" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D108" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -1056,11 +1047,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A109" sqref="A109"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2583,20 +2574,6 @@
         <v>212</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A109" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added new snippet to extractor metadata
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19209"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A584B0-FD15-4851-BC3E-4A363B1F0021}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D8A636-2DDB-44EC-9967-3D185B102250}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="215">
   <si>
     <t>Class</t>
   </si>
@@ -659,6 +659,12 @@
   </si>
   <si>
     <t>onChange</t>
+  </si>
+  <si>
+    <t>excel-range-areas</t>
+  </si>
+  <si>
+    <t>colorAllFormulaCells</t>
   </si>
 </sst>
 </file>
@@ -738,8 +744,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D108" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D108" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D109" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D109" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -1047,22 +1053,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D108"/>
+  <dimension ref="A1:D109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +1082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1104,7 +1110,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1118,7 +1124,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1132,7 +1138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1146,7 +1152,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1160,7 +1166,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1174,7 +1180,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1188,7 +1194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1202,7 +1208,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1216,7 +1222,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1230,7 +1236,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1244,7 +1250,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1258,7 +1264,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1272,7 +1278,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1286,7 +1292,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1300,7 +1306,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1314,7 +1320,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1328,7 +1334,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1342,7 +1348,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1356,7 +1362,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1370,7 +1376,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -1384,7 +1390,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
@@ -1398,7 +1404,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1412,7 +1418,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -1426,7 +1432,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>57</v>
       </c>
@@ -1440,7 +1446,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
@@ -1454,7 +1460,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
@@ -1468,7 +1474,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>67</v>
       </c>
@@ -1482,7 +1488,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -1496,7 +1502,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>71</v>
       </c>
@@ -1510,7 +1516,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
@@ -1524,7 +1530,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>65</v>
       </c>
@@ -1538,7 +1544,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>77</v>
       </c>
@@ -1552,7 +1558,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -1566,7 +1572,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
@@ -1580,7 +1586,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>81</v>
       </c>
@@ -1594,7 +1600,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
@@ -1608,7 +1614,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>85</v>
       </c>
@@ -1622,7 +1628,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -1636,7 +1642,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>65</v>
       </c>
@@ -1650,7 +1656,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>89</v>
       </c>
@@ -1664,7 +1670,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>89</v>
       </c>
@@ -1678,7 +1684,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>92</v>
       </c>
@@ -1692,7 +1698,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>92</v>
       </c>
@@ -1706,7 +1712,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>65</v>
       </c>
@@ -1720,7 +1726,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
@@ -1734,7 +1740,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
@@ -1748,7 +1754,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
@@ -1762,7 +1768,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>98</v>
       </c>
@@ -1776,7 +1782,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>65</v>
       </c>
@@ -1790,7 +1796,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>100</v>
       </c>
@@ -1804,7 +1810,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>100</v>
       </c>
@@ -1818,7 +1824,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>103</v>
       </c>
@@ -1832,7 +1838,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
@@ -1846,7 +1852,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>63</v>
       </c>
@@ -1860,7 +1866,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -1874,7 +1880,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
@@ -1888,7 +1894,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>28</v>
       </c>
@@ -1902,7 +1908,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>107</v>
       </c>
@@ -1916,7 +1922,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>107</v>
       </c>
@@ -1930,7 +1936,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>107</v>
       </c>
@@ -1944,7 +1950,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>107</v>
       </c>
@@ -1958,7 +1964,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>115</v>
       </c>
@@ -1972,7 +1978,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>117</v>
       </c>
@@ -1986,7 +1992,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>117</v>
       </c>
@@ -2000,7 +2006,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>117</v>
       </c>
@@ -2014,7 +2020,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>117</v>
       </c>
@@ -2028,7 +2034,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>117</v>
       </c>
@@ -2042,7 +2048,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>54</v>
       </c>
@@ -2056,7 +2062,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>54</v>
       </c>
@@ -2070,7 +2076,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>131</v>
       </c>
@@ -2084,7 +2090,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>135</v>
       </c>
@@ -2098,7 +2104,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>139</v>
       </c>
@@ -2112,7 +2118,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>139</v>
       </c>
@@ -2126,7 +2132,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>143</v>
       </c>
@@ -2140,7 +2146,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>146</v>
       </c>
@@ -2154,7 +2160,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>146</v>
       </c>
@@ -2168,7 +2174,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>150</v>
       </c>
@@ -2182,7 +2188,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>150</v>
       </c>
@@ -2196,7 +2202,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>154</v>
       </c>
@@ -2210,7 +2216,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>158</v>
       </c>
@@ -2224,7 +2230,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>161</v>
       </c>
@@ -2238,7 +2244,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>165</v>
       </c>
@@ -2252,7 +2258,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>169</v>
       </c>
@@ -2266,7 +2272,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>169</v>
       </c>
@@ -2280,7 +2286,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>165</v>
       </c>
@@ -2294,7 +2300,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>165</v>
       </c>
@@ -2308,7 +2314,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>165</v>
       </c>
@@ -2322,7 +2328,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>165</v>
       </c>
@@ -2336,7 +2342,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>178</v>
       </c>
@@ -2350,7 +2356,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>178</v>
       </c>
@@ -2364,7 +2370,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>182</v>
       </c>
@@ -2378,7 +2384,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>184</v>
       </c>
@@ -2392,7 +2398,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>185</v>
       </c>
@@ -2406,7 +2412,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>184</v>
       </c>
@@ -2420,7 +2426,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>191</v>
       </c>
@@ -2434,7 +2440,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>192</v>
       </c>
@@ -2448,7 +2454,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>146</v>
       </c>
@@ -2462,7 +2468,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>146</v>
       </c>
@@ -2476,7 +2482,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>146</v>
       </c>
@@ -2490,7 +2496,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>146</v>
       </c>
@@ -2504,7 +2510,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>182</v>
       </c>
@@ -2518,7 +2524,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>182</v>
       </c>
@@ -2532,7 +2538,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>182</v>
       </c>
@@ -2546,7 +2552,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>182</v>
       </c>
@@ -2560,7 +2566,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>182</v>
       </c>
@@ -2572,6 +2578,20 @@
       </c>
       <c r="D108" s="1" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add missing snippets (#157)
* add missing snippets

* added other functions
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19313"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D8A636-2DDB-44EC-9967-3D185B102250}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C757C6E3-8114-4FF4-B5C6-BA3DF82859BB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="22500" windowHeight="10788" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="232">
   <si>
     <t>Class</t>
   </si>
@@ -665,6 +665,57 @@
   </si>
   <si>
     <t>colorAllFormulaCells</t>
+  </si>
+  <si>
+    <t>Workbook</t>
+  </si>
+  <si>
+    <t>getActiveCell</t>
+  </si>
+  <si>
+    <t>excel-workbook-get-active-cell</t>
+  </si>
+  <si>
+    <t>copy</t>
+  </si>
+  <si>
+    <t>excel-worksheet-copy</t>
+  </si>
+  <si>
+    <t>protect</t>
+  </si>
+  <si>
+    <t>excel-protect-data-in-worksheet-and-workbook-structure</t>
+  </si>
+  <si>
+    <t>protectDataInWorksheet</t>
+  </si>
+  <si>
+    <t>protectWorkbookStructure</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>unprotect</t>
+  </si>
+  <si>
+    <t>unprotectDataInWorksheet</t>
+  </si>
+  <si>
+    <t>unprotectWorkbookStructure</t>
+  </si>
+  <si>
+    <t>passwordProtectDataInWorksheet</t>
+  </si>
+  <si>
+    <t>passwordUnprotectDataInWorksheet</t>
+  </si>
+  <si>
+    <t>passwordProtectWorkbookStructure</t>
+  </si>
+  <si>
+    <t>passwordUnprotectWorkbookStructure</t>
   </si>
 </sst>
 </file>
@@ -744,8 +795,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D109" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D109" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D119" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D119" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -1053,22 +1104,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F104" sqref="F104"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1082,7 +1133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1096,7 +1147,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1110,7 +1161,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1124,7 +1175,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1138,7 +1189,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1152,7 +1203,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1166,7 +1217,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1180,7 +1231,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1194,7 +1245,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1208,7 +1259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1222,7 +1273,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1236,7 +1287,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1250,7 +1301,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1264,7 +1315,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1278,7 +1329,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1292,7 +1343,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1306,7 +1357,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1320,7 +1371,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1334,7 +1385,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1348,7 +1399,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1362,7 +1413,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1376,7 +1427,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -1390,7 +1441,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
@@ -1404,7 +1455,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1418,7 +1469,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -1432,7 +1483,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>57</v>
       </c>
@@ -1446,7 +1497,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
@@ -1460,7 +1511,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
@@ -1474,7 +1525,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>67</v>
       </c>
@@ -1488,7 +1539,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -1502,7 +1553,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>71</v>
       </c>
@@ -1516,7 +1567,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
@@ -1530,7 +1581,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>65</v>
       </c>
@@ -1544,7 +1595,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>77</v>
       </c>
@@ -1558,7 +1609,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -1572,7 +1623,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
@@ -1586,7 +1637,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>81</v>
       </c>
@@ -1600,7 +1651,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
@@ -1614,7 +1665,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>85</v>
       </c>
@@ -1628,7 +1679,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -1642,7 +1693,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>65</v>
       </c>
@@ -1656,7 +1707,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>89</v>
       </c>
@@ -1670,7 +1721,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>89</v>
       </c>
@@ -1684,7 +1735,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>92</v>
       </c>
@@ -1698,7 +1749,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>92</v>
       </c>
@@ -1712,7 +1763,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>65</v>
       </c>
@@ -1726,7 +1777,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
@@ -1740,7 +1791,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
@@ -1754,7 +1805,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
@@ -1768,7 +1819,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>98</v>
       </c>
@@ -1782,7 +1833,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>65</v>
       </c>
@@ -1796,7 +1847,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>100</v>
       </c>
@@ -1810,7 +1861,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>100</v>
       </c>
@@ -1824,7 +1875,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>103</v>
       </c>
@@ -1838,7 +1889,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
@@ -1852,7 +1903,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>63</v>
       </c>
@@ -1866,7 +1917,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -1880,7 +1931,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
@@ -1894,7 +1945,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>28</v>
       </c>
@@ -1908,7 +1959,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>107</v>
       </c>
@@ -1922,7 +1973,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>107</v>
       </c>
@@ -1936,7 +1987,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>107</v>
       </c>
@@ -1950,7 +2001,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>107</v>
       </c>
@@ -1964,7 +2015,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>115</v>
       </c>
@@ -1978,7 +2029,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>117</v>
       </c>
@@ -1992,7 +2043,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>117</v>
       </c>
@@ -2006,7 +2057,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>117</v>
       </c>
@@ -2020,7 +2071,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>117</v>
       </c>
@@ -2034,7 +2085,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>117</v>
       </c>
@@ -2048,7 +2099,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>54</v>
       </c>
@@ -2062,7 +2113,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>54</v>
       </c>
@@ -2076,7 +2127,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>131</v>
       </c>
@@ -2090,7 +2141,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>135</v>
       </c>
@@ -2104,7 +2155,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>139</v>
       </c>
@@ -2118,7 +2169,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>139</v>
       </c>
@@ -2132,7 +2183,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>143</v>
       </c>
@@ -2146,7 +2197,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>146</v>
       </c>
@@ -2160,7 +2211,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>146</v>
       </c>
@@ -2174,7 +2225,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>150</v>
       </c>
@@ -2188,7 +2239,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>150</v>
       </c>
@@ -2202,7 +2253,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>154</v>
       </c>
@@ -2216,7 +2267,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>158</v>
       </c>
@@ -2230,7 +2281,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>161</v>
       </c>
@@ -2244,7 +2295,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>165</v>
       </c>
@@ -2258,7 +2309,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>169</v>
       </c>
@@ -2272,7 +2323,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>169</v>
       </c>
@@ -2286,7 +2337,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>165</v>
       </c>
@@ -2300,7 +2351,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>165</v>
       </c>
@@ -2314,7 +2365,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>165</v>
       </c>
@@ -2328,7 +2379,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>165</v>
       </c>
@@ -2342,7 +2393,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>178</v>
       </c>
@@ -2356,7 +2407,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>178</v>
       </c>
@@ -2370,7 +2421,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>182</v>
       </c>
@@ -2384,7 +2435,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>184</v>
       </c>
@@ -2398,7 +2449,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>185</v>
       </c>
@@ -2412,7 +2463,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>184</v>
       </c>
@@ -2426,7 +2477,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>191</v>
       </c>
@@ -2440,7 +2491,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>192</v>
       </c>
@@ -2454,7 +2505,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>146</v>
       </c>
@@ -2468,7 +2519,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>146</v>
       </c>
@@ -2482,7 +2533,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>146</v>
       </c>
@@ -2496,7 +2547,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>146</v>
       </c>
@@ -2510,7 +2561,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>182</v>
       </c>
@@ -2524,7 +2575,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>182</v>
       </c>
@@ -2538,7 +2589,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>182</v>
       </c>
@@ -2552,7 +2603,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>182</v>
       </c>
@@ -2566,7 +2617,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>182</v>
       </c>
@@ -2580,7 +2631,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>54</v>
       </c>
@@ -2592,6 +2643,146 @@
       </c>
       <c r="D109" s="1" t="s">
         <v>214</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update based on feedback
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20314"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C1D188-676E-4BDA-8B2F-E8B021B5B7FF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724B9D85-9BB0-4C5E-AA29-0B9DE048E945}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="22500" windowHeight="10788" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="22500" windowHeight="10788" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -1104,8 +1104,8 @@
   <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D119" sqref="D119"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1440,7 +1440,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
update name to showGridlines
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20316"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724B9D85-9BB0-4C5E-AA29-0B9DE048E945}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3499E99-1DC3-45E6-A880-9E74E426CE76}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="22500" windowHeight="10788" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="22500" windowHeight="10788" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="230">
   <si>
     <t>Class</t>
   </si>
@@ -416,9 +416,6 @@
   </si>
   <si>
     <t>ChartTrendlineCollection</t>
-  </si>
-  <si>
-    <t>gridlines</t>
   </si>
   <si>
     <t>excel-gridlines</t>
@@ -2129,13 +2126,13 @@
         <v>54</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -2143,13 +2140,13 @@
         <v>54</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -2160,164 +2157,164 @@
         <v>9</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="D78" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="D79" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="D86" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -2328,136 +2325,136 @@
         <v>86</v>
       </c>
       <c r="C87" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C95" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B96" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -2465,13 +2462,13 @@
         <v>57</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -2479,27 +2476,27 @@
         <v>54</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -2507,13 +2504,13 @@
         <v>57</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -2521,111 +2518,111 @@
         <v>57</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="D102" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C103" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C104" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -2636,24 +2633,24 @@
         <v>106</v>
       </c>
       <c r="C109" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="C110" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="D110" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -2661,125 +2658,125 @@
         <v>54</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="D111" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="D114" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="D116" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B118" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="D118" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Elizs update mapping (#179)
* update name to showGridlines

* updated mapping
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20316"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724B9D85-9BB0-4C5E-AA29-0B9DE048E945}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3499E99-1DC3-45E6-A880-9E74E426CE76}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="22500" windowHeight="10788" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="22500" windowHeight="10788" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="230">
   <si>
     <t>Class</t>
   </si>
@@ -416,9 +416,6 @@
   </si>
   <si>
     <t>ChartTrendlineCollection</t>
-  </si>
-  <si>
-    <t>gridlines</t>
   </si>
   <si>
     <t>excel-gridlines</t>
@@ -2129,13 +2126,13 @@
         <v>54</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -2143,13 +2140,13 @@
         <v>54</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -2160,164 +2157,164 @@
         <v>9</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="D78" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="D79" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="D86" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -2328,136 +2325,136 @@
         <v>86</v>
       </c>
       <c r="C87" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C95" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B96" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -2465,13 +2462,13 @@
         <v>57</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -2479,27 +2476,27 @@
         <v>54</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -2507,13 +2504,13 @@
         <v>57</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -2521,111 +2518,111 @@
         <v>57</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="D102" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C103" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C104" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -2636,24 +2633,24 @@
         <v>106</v>
       </c>
       <c r="C109" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="C110" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="D110" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -2661,125 +2658,125 @@
         <v>54</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="D111" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="D114" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="D116" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B118" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="D118" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unmap 1.9 snippet and fix pivot text
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20316"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20822"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3499E99-1DC3-45E6-A880-9E74E426CE76}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0D5419-DF3D-4B7D-99FD-3FDA7F92EDB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="22500" windowHeight="10788" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="228">
   <si>
     <t>Class</t>
   </si>
@@ -626,12 +626,6 @@
   </si>
   <si>
     <t>onChange</t>
-  </si>
-  <si>
-    <t>excel-range-areas</t>
-  </si>
-  <si>
-    <t>colorAllFormulaCells</t>
   </si>
   <si>
     <t>Workbook</t>
@@ -789,8 +783,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D119" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D119" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D118" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D118" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -1098,22 +1092,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O91" sqref="O91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1127,7 +1121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1141,7 +1135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1155,7 +1149,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1169,7 +1163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1183,7 +1177,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1197,7 +1191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1211,7 +1205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1225,7 +1219,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1239,7 +1233,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1253,7 +1247,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1267,7 +1261,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1281,7 +1275,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1295,7 +1289,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -1309,7 +1303,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1323,7 +1317,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
@@ -1337,7 +1331,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -1351,7 +1345,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1365,7 +1359,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1379,7 +1373,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1393,7 +1387,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -1407,7 +1401,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1421,7 +1415,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -1435,7 +1429,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
@@ -1449,7 +1443,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>50</v>
       </c>
@@ -1463,7 +1457,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -1477,7 +1471,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>54</v>
       </c>
@@ -1491,7 +1485,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>57</v>
       </c>
@@ -1505,7 +1499,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -1519,7 +1513,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
@@ -1533,7 +1527,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -1547,7 +1541,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>67</v>
       </c>
@@ -1561,7 +1555,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
@@ -1575,7 +1569,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
@@ -1589,7 +1583,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -1603,7 +1597,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -1617,7 +1611,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
@@ -1631,7 +1625,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>65</v>
       </c>
@@ -1645,7 +1639,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>81</v>
       </c>
@@ -1659,7 +1653,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>81</v>
       </c>
@@ -1673,7 +1667,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -1687,7 +1681,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>85</v>
       </c>
@@ -1701,7 +1695,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>85</v>
       </c>
@@ -1715,7 +1709,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -1729,7 +1723,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>89</v>
       </c>
@@ -1743,7 +1737,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>89</v>
       </c>
@@ -1757,7 +1751,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>85</v>
       </c>
@@ -1771,7 +1765,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>92</v>
       </c>
@@ -1785,7 +1779,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>65</v>
       </c>
@@ -1799,7 +1793,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>94</v>
       </c>
@@ -1813,7 +1807,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>94</v>
       </c>
@@ -1827,7 +1821,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>98</v>
       </c>
@@ -1841,7 +1835,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>98</v>
       </c>
@@ -1855,7 +1849,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>65</v>
       </c>
@@ -1869,7 +1863,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>100</v>
       </c>
@@ -1883,7 +1877,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>71</v>
       </c>
@@ -1897,7 +1891,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>103</v>
       </c>
@@ -1911,7 +1905,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -1925,7 +1919,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
@@ -1939,7 +1933,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -1953,7 +1947,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>63</v>
       </c>
@@ -1967,7 +1961,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>28</v>
       </c>
@@ -1981,7 +1975,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>107</v>
       </c>
@@ -1995,7 +1989,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>107</v>
       </c>
@@ -2009,7 +2003,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>107</v>
       </c>
@@ -2023,7 +2017,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>107</v>
       </c>
@@ -2037,7 +2031,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>115</v>
       </c>
@@ -2051,7 +2045,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>117</v>
       </c>
@@ -2065,7 +2059,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>117</v>
       </c>
@@ -2079,7 +2073,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>117</v>
       </c>
@@ -2093,7 +2087,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>117</v>
       </c>
@@ -2107,7 +2101,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>117</v>
       </c>
@@ -2121,7 +2115,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>54</v>
       </c>
@@ -2135,7 +2129,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>54</v>
       </c>
@@ -2149,7 +2143,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>131</v>
       </c>
@@ -2163,7 +2157,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>134</v>
       </c>
@@ -2177,7 +2171,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>138</v>
       </c>
@@ -2191,7 +2185,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>138</v>
       </c>
@@ -2205,7 +2199,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>144</v>
       </c>
@@ -2219,7 +2213,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>144</v>
       </c>
@@ -2233,7 +2227,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>144</v>
       </c>
@@ -2247,7 +2241,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>148</v>
       </c>
@@ -2261,7 +2255,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>148</v>
       </c>
@@ -2275,9 +2269,9 @@
         <v>157</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>158</v>
@@ -2289,7 +2283,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>155</v>
       </c>
@@ -2303,9 +2297,9 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>166</v>
@@ -2317,7 +2311,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>28</v>
       </c>
@@ -2331,7 +2325,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>165</v>
       </c>
@@ -2345,7 +2339,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>165</v>
       </c>
@@ -2359,7 +2353,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>161</v>
       </c>
@@ -2373,7 +2367,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>161</v>
       </c>
@@ -2387,12 +2381,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>161</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>169</v>
@@ -2401,7 +2395,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>161</v>
       </c>
@@ -2415,9 +2409,9 @@
         <v>170</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>113</v>
@@ -2429,9 +2423,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>200</v>
@@ -2443,9 +2437,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>177</v>
@@ -2457,7 +2451,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>57</v>
       </c>
@@ -2471,7 +2465,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>54</v>
       </c>
@@ -2485,9 +2479,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>182</v>
@@ -2499,7 +2493,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>57</v>
       </c>
@@ -2513,7 +2507,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>57</v>
       </c>
@@ -2527,7 +2521,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>144</v>
       </c>
@@ -2541,7 +2535,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>144</v>
       </c>
@@ -2555,7 +2549,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>144</v>
       </c>
@@ -2569,7 +2563,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>144</v>
       </c>
@@ -2583,9 +2577,9 @@
         <v>191</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>200</v>
@@ -2597,9 +2591,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>182</v>
@@ -2611,9 +2605,9 @@
         <v>201</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>196</v>
@@ -2625,23 +2619,23 @@
         <v>201</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>205</v>
@@ -2650,12 +2644,12 @@
         <v>206</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>54</v>
+        <v>220</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>207</v>
@@ -2664,119 +2658,105 @@
         <v>208</v>
       </c>
       <c r="D111" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C112" s="1" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B113" s="1" t="s">
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D113" s="1" t="s">
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D114" s="1" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D115" s="1" t="s">
+      <c r="C116" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D116" s="1" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D117" s="1" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unmap 1.9 snippet and fix pivot text (#194)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20316"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20822"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3499E99-1DC3-45E6-A880-9E74E426CE76}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0D5419-DF3D-4B7D-99FD-3FDA7F92EDB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="22500" windowHeight="10788" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="228">
   <si>
     <t>Class</t>
   </si>
@@ -626,12 +626,6 @@
   </si>
   <si>
     <t>onChange</t>
-  </si>
-  <si>
-    <t>excel-range-areas</t>
-  </si>
-  <si>
-    <t>colorAllFormulaCells</t>
   </si>
   <si>
     <t>Workbook</t>
@@ -789,8 +783,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D119" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D119" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D118" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D118" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -1098,22 +1092,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O91" sqref="O91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1127,7 +1121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1141,7 +1135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1155,7 +1149,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1169,7 +1163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1183,7 +1177,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1197,7 +1191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1211,7 +1205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1225,7 +1219,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1239,7 +1233,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1253,7 +1247,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1267,7 +1261,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1281,7 +1275,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1295,7 +1289,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -1309,7 +1303,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1323,7 +1317,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
@@ -1337,7 +1331,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -1351,7 +1345,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1365,7 +1359,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1379,7 +1373,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1393,7 +1387,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -1407,7 +1401,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1421,7 +1415,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -1435,7 +1429,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
@@ -1449,7 +1443,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>50</v>
       </c>
@@ -1463,7 +1457,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -1477,7 +1471,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>54</v>
       </c>
@@ -1491,7 +1485,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>57</v>
       </c>
@@ -1505,7 +1499,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -1519,7 +1513,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
@@ -1533,7 +1527,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -1547,7 +1541,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>67</v>
       </c>
@@ -1561,7 +1555,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
@@ -1575,7 +1569,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
@@ -1589,7 +1583,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -1603,7 +1597,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -1617,7 +1611,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
@@ -1631,7 +1625,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>65</v>
       </c>
@@ -1645,7 +1639,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>81</v>
       </c>
@@ -1659,7 +1653,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>81</v>
       </c>
@@ -1673,7 +1667,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -1687,7 +1681,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>85</v>
       </c>
@@ -1701,7 +1695,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>85</v>
       </c>
@@ -1715,7 +1709,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -1729,7 +1723,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>89</v>
       </c>
@@ -1743,7 +1737,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>89</v>
       </c>
@@ -1757,7 +1751,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>85</v>
       </c>
@@ -1771,7 +1765,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>92</v>
       </c>
@@ -1785,7 +1779,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>65</v>
       </c>
@@ -1799,7 +1793,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>94</v>
       </c>
@@ -1813,7 +1807,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>94</v>
       </c>
@@ -1827,7 +1821,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>98</v>
       </c>
@@ -1841,7 +1835,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>98</v>
       </c>
@@ -1855,7 +1849,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>65</v>
       </c>
@@ -1869,7 +1863,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>100</v>
       </c>
@@ -1883,7 +1877,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>71</v>
       </c>
@@ -1897,7 +1891,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>103</v>
       </c>
@@ -1911,7 +1905,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -1925,7 +1919,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
@@ -1939,7 +1933,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -1953,7 +1947,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>63</v>
       </c>
@@ -1967,7 +1961,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>28</v>
       </c>
@@ -1981,7 +1975,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>107</v>
       </c>
@@ -1995,7 +1989,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>107</v>
       </c>
@@ -2009,7 +2003,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>107</v>
       </c>
@@ -2023,7 +2017,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>107</v>
       </c>
@@ -2037,7 +2031,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>115</v>
       </c>
@@ -2051,7 +2045,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>117</v>
       </c>
@@ -2065,7 +2059,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>117</v>
       </c>
@@ -2079,7 +2073,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>117</v>
       </c>
@@ -2093,7 +2087,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>117</v>
       </c>
@@ -2107,7 +2101,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>117</v>
       </c>
@@ -2121,7 +2115,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>54</v>
       </c>
@@ -2135,7 +2129,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>54</v>
       </c>
@@ -2149,7 +2143,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>131</v>
       </c>
@@ -2163,7 +2157,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>134</v>
       </c>
@@ -2177,7 +2171,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>138</v>
       </c>
@@ -2191,7 +2185,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>138</v>
       </c>
@@ -2205,7 +2199,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>144</v>
       </c>
@@ -2219,7 +2213,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>144</v>
       </c>
@@ -2233,7 +2227,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>144</v>
       </c>
@@ -2247,7 +2241,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>148</v>
       </c>
@@ -2261,7 +2255,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>148</v>
       </c>
@@ -2275,9 +2269,9 @@
         <v>157</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>158</v>
@@ -2289,7 +2283,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>155</v>
       </c>
@@ -2303,9 +2297,9 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>166</v>
@@ -2317,7 +2311,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>28</v>
       </c>
@@ -2331,7 +2325,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>165</v>
       </c>
@@ -2345,7 +2339,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>165</v>
       </c>
@@ -2359,7 +2353,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>161</v>
       </c>
@@ -2373,7 +2367,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>161</v>
       </c>
@@ -2387,12 +2381,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>161</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>169</v>
@@ -2401,7 +2395,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>161</v>
       </c>
@@ -2415,9 +2409,9 @@
         <v>170</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>113</v>
@@ -2429,9 +2423,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>200</v>
@@ -2443,9 +2437,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>177</v>
@@ -2457,7 +2451,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>57</v>
       </c>
@@ -2471,7 +2465,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>54</v>
       </c>
@@ -2485,9 +2479,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>182</v>
@@ -2499,7 +2493,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>57</v>
       </c>
@@ -2513,7 +2507,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>57</v>
       </c>
@@ -2527,7 +2521,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>144</v>
       </c>
@@ -2541,7 +2535,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>144</v>
       </c>
@@ -2555,7 +2549,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>144</v>
       </c>
@@ -2569,7 +2563,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>144</v>
       </c>
@@ -2583,9 +2577,9 @@
         <v>191</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>200</v>
@@ -2597,9 +2591,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>182</v>
@@ -2611,9 +2605,9 @@
         <v>201</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>196</v>
@@ -2625,23 +2619,23 @@
         <v>201</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>205</v>
@@ -2650,12 +2644,12 @@
         <v>206</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>54</v>
+        <v>220</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>207</v>
@@ -2664,119 +2658,105 @@
         <v>208</v>
       </c>
       <c r="D111" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C112" s="1" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B113" s="1" t="s">
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D113" s="1" t="s">
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D114" s="1" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D115" s="1" t="s">
+      <c r="C116" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D116" s="1" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D117" s="1" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merge to prod (#198)
* Unmap 1.9 snippet and fix pivot text (#194)

* Correcting PivotTable capitalization (#195)

* Adding a showAs PivotTable sample (#196)

* Adding a showAs PivotTable sample

* Removing references to other snippets

* Update lodash version (#197)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20316"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20822"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3499E99-1DC3-45E6-A880-9E74E426CE76}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0D5419-DF3D-4B7D-99FD-3FDA7F92EDB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="22500" windowHeight="10788" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="228">
   <si>
     <t>Class</t>
   </si>
@@ -626,12 +626,6 @@
   </si>
   <si>
     <t>onChange</t>
-  </si>
-  <si>
-    <t>excel-range-areas</t>
-  </si>
-  <si>
-    <t>colorAllFormulaCells</t>
   </si>
   <si>
     <t>Workbook</t>
@@ -789,8 +783,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D119" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D119" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D118" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D118" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -1098,22 +1092,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O91" sqref="O91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1127,7 +1121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1141,7 +1135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1155,7 +1149,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1169,7 +1163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1183,7 +1177,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1197,7 +1191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1211,7 +1205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1225,7 +1219,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1239,7 +1233,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1253,7 +1247,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1267,7 +1261,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1281,7 +1275,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1295,7 +1289,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -1309,7 +1303,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1323,7 +1317,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
@@ -1337,7 +1331,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -1351,7 +1345,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1365,7 +1359,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1379,7 +1373,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1393,7 +1387,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -1407,7 +1401,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1421,7 +1415,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -1435,7 +1429,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
@@ -1449,7 +1443,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>50</v>
       </c>
@@ -1463,7 +1457,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -1477,7 +1471,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>54</v>
       </c>
@@ -1491,7 +1485,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>57</v>
       </c>
@@ -1505,7 +1499,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -1519,7 +1513,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
@@ -1533,7 +1527,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -1547,7 +1541,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>67</v>
       </c>
@@ -1561,7 +1555,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
@@ -1575,7 +1569,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
@@ -1589,7 +1583,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -1603,7 +1597,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -1617,7 +1611,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
@@ -1631,7 +1625,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>65</v>
       </c>
@@ -1645,7 +1639,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>81</v>
       </c>
@@ -1659,7 +1653,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>81</v>
       </c>
@@ -1673,7 +1667,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -1687,7 +1681,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>85</v>
       </c>
@@ -1701,7 +1695,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>85</v>
       </c>
@@ -1715,7 +1709,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -1729,7 +1723,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>89</v>
       </c>
@@ -1743,7 +1737,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>89</v>
       </c>
@@ -1757,7 +1751,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>85</v>
       </c>
@@ -1771,7 +1765,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>92</v>
       </c>
@@ -1785,7 +1779,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>65</v>
       </c>
@@ -1799,7 +1793,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>94</v>
       </c>
@@ -1813,7 +1807,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>94</v>
       </c>
@@ -1827,7 +1821,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>98</v>
       </c>
@@ -1841,7 +1835,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>98</v>
       </c>
@@ -1855,7 +1849,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>65</v>
       </c>
@@ -1869,7 +1863,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>100</v>
       </c>
@@ -1883,7 +1877,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>71</v>
       </c>
@@ -1897,7 +1891,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>103</v>
       </c>
@@ -1911,7 +1905,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -1925,7 +1919,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
@@ -1939,7 +1933,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -1953,7 +1947,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>63</v>
       </c>
@@ -1967,7 +1961,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>28</v>
       </c>
@@ -1981,7 +1975,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>107</v>
       </c>
@@ -1995,7 +1989,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>107</v>
       </c>
@@ -2009,7 +2003,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>107</v>
       </c>
@@ -2023,7 +2017,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>107</v>
       </c>
@@ -2037,7 +2031,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>115</v>
       </c>
@@ -2051,7 +2045,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>117</v>
       </c>
@@ -2065,7 +2059,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>117</v>
       </c>
@@ -2079,7 +2073,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>117</v>
       </c>
@@ -2093,7 +2087,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>117</v>
       </c>
@@ -2107,7 +2101,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>117</v>
       </c>
@@ -2121,7 +2115,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>54</v>
       </c>
@@ -2135,7 +2129,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>54</v>
       </c>
@@ -2149,7 +2143,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>131</v>
       </c>
@@ -2163,7 +2157,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>134</v>
       </c>
@@ -2177,7 +2171,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>138</v>
       </c>
@@ -2191,7 +2185,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>138</v>
       </c>
@@ -2205,7 +2199,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>144</v>
       </c>
@@ -2219,7 +2213,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>144</v>
       </c>
@@ -2233,7 +2227,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>144</v>
       </c>
@@ -2247,7 +2241,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>148</v>
       </c>
@@ -2261,7 +2255,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>148</v>
       </c>
@@ -2275,9 +2269,9 @@
         <v>157</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>158</v>
@@ -2289,7 +2283,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>155</v>
       </c>
@@ -2303,9 +2297,9 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>166</v>
@@ -2317,7 +2311,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>28</v>
       </c>
@@ -2331,7 +2325,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>165</v>
       </c>
@@ -2345,7 +2339,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>165</v>
       </c>
@@ -2359,7 +2353,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>161</v>
       </c>
@@ -2373,7 +2367,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>161</v>
       </c>
@@ -2387,12 +2381,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>161</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>169</v>
@@ -2401,7 +2395,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>161</v>
       </c>
@@ -2415,9 +2409,9 @@
         <v>170</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>113</v>
@@ -2429,9 +2423,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>200</v>
@@ -2443,9 +2437,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>177</v>
@@ -2457,7 +2451,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>57</v>
       </c>
@@ -2471,7 +2465,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>54</v>
       </c>
@@ -2485,9 +2479,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>182</v>
@@ -2499,7 +2493,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>57</v>
       </c>
@@ -2513,7 +2507,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>57</v>
       </c>
@@ -2527,7 +2521,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>144</v>
       </c>
@@ -2541,7 +2535,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>144</v>
       </c>
@@ -2555,7 +2549,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>144</v>
       </c>
@@ -2569,7 +2563,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>144</v>
       </c>
@@ -2583,9 +2577,9 @@
         <v>191</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>200</v>
@@ -2597,9 +2591,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>182</v>
@@ -2611,9 +2605,9 @@
         <v>201</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>196</v>
@@ -2625,23 +2619,23 @@
         <v>201</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>205</v>
@@ -2650,12 +2644,12 @@
         <v>206</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>54</v>
+        <v>220</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>207</v>
@@ -2664,119 +2658,105 @@
         <v>208</v>
       </c>
       <c r="D111" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C112" s="1" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B113" s="1" t="s">
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D113" s="1" t="s">
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D114" s="1" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D115" s="1" t="s">
+      <c r="C116" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D116" s="1" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D117" s="1" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mapping Excel 1.8 snippets to ref docs git push
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20822"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21005"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0D5419-DF3D-4B7D-99FD-3FDA7F92EDB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E29BEE-F499-4FDF-A9BD-532936C2497E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3000" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="263">
   <si>
     <t>Class</t>
   </si>
@@ -704,6 +704,111 @@
   </si>
   <si>
     <t>TableChangedEventArgs</t>
+  </si>
+  <si>
+    <t>addPositiveNumberRequirement</t>
+  </si>
+  <si>
+    <t>requireApprovedName</t>
+  </si>
+  <si>
+    <t>warnAboutCommentRedundancy</t>
+  </si>
+  <si>
+    <t>excel-data-validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataValidationRule </t>
+  </si>
+  <si>
+    <t>wholeNumber</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>errorAlert</t>
+  </si>
+  <si>
+    <t>DataValidation</t>
+  </si>
+  <si>
+    <t>PivotTableCollection</t>
+  </si>
+  <si>
+    <t>excel-pivottable-create-and-modify</t>
+  </si>
+  <si>
+    <t>createWithNames</t>
+  </si>
+  <si>
+    <t>PivotTable</t>
+  </si>
+  <si>
+    <t>deletePivot</t>
+  </si>
+  <si>
+    <t>toggleColumn</t>
+  </si>
+  <si>
+    <t>columnHierarchies</t>
+  </si>
+  <si>
+    <t>dataHierarchies</t>
+  </si>
+  <si>
+    <t>addValues</t>
+  </si>
+  <si>
+    <t>changeHierarchyNames</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>DataPivotHierarchy</t>
+  </si>
+  <si>
+    <t>layout</t>
+  </si>
+  <si>
+    <t>changeLayout</t>
+  </si>
+  <si>
+    <t>filterHierarchies</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>PivotLayout</t>
+  </si>
+  <si>
+    <t>getDataBodyRange</t>
+  </si>
+  <si>
+    <t>getCrateTotal</t>
+  </si>
+  <si>
+    <t>showPercentages</t>
+  </si>
+  <si>
+    <t>excel-pivottable-filters-and-summaries</t>
+  </si>
+  <si>
+    <t>excel-pivottable-calculations</t>
+  </si>
+  <si>
+    <t>showAs</t>
+  </si>
+  <si>
+    <t>ShowAsRule</t>
+  </si>
+  <si>
+    <t>baseItem</t>
+  </si>
+  <si>
+    <t>showDifferenceFrom</t>
   </si>
 </sst>
 </file>
@@ -783,8 +888,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D118" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D118" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D131" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D131" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -1092,11 +1197,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D118"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O91" sqref="O91"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2759,6 +2864,188 @@
         <v>218</v>
       </c>
     </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sorting the Excel excel file
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21005"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E29BEE-F499-4FDF-A9BD-532936C2497E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E127CD-5093-412C-BD88-B69B7E038B97}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3000" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -890,6 +890,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D131" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:D131" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D131">
+    <sortCondition ref="A3"/>
+  </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -1200,8 +1203,8 @@
   <dimension ref="A1:D131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B134" sqref="B134"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,394 +1245,394 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>152</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>153</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>162</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>163</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>221</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>158</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>159</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>26</v>
+      <c r="A9" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>147</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>150</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>31</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>189</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>190</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>34</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>192</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>190</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>193</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>190</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>194</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>190</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>40</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>134</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>43</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>45</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>138</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>142</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>43</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>138</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>142</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1637,21 +1640,21 @@
         <v>65</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>68</v>
@@ -1662,80 +1665,80 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>68</v>
@@ -1746,730 +1749,730 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>65</v>
+        <v>248</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>101</v>
+        <v>247</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>68</v>
+        <v>238</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>102</v>
+        <v>246</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>100</v>
+        <v>248</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>93</v>
+        <v>259</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>68</v>
+        <v>258</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>102</v>
+        <v>256</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>71</v>
+        <v>236</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>76</v>
+        <v>235</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>68</v>
+        <v>231</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>102</v>
+        <v>230</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>103</v>
+        <v>232</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>17</v>
+        <v>233</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>68</v>
+        <v>231</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>102</v>
+        <v>228</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>65</v>
+        <v>232</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>87</v>
+        <v>234</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>68</v>
+        <v>231</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>104</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>109</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>110</v>
+        <v>17</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>111</v>
+        <v>18</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>112</v>
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>111</v>
+        <v>10</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>112</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>114</v>
+        <v>9</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>111</v>
+        <v>12</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>112</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>107</v>
+        <v>253</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>116</v>
+        <v>254</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>111</v>
+        <v>257</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>112</v>
+        <v>255</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>107</v>
+        <v>240</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>118</v>
+        <v>14</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>111</v>
+        <v>238</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>119</v>
+        <v>241</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>115</v>
+        <v>240</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>120</v>
+        <v>243</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>121</v>
+        <v>238</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>122</v>
+        <v>242</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>117</v>
+        <v>240</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>123</v>
+        <v>244</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>124</v>
+        <v>238</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>123</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>117</v>
+        <v>240</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>125</v>
+        <v>249</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>124</v>
+        <v>257</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>125</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>117</v>
+        <v>240</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>126</v>
+        <v>251</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>124</v>
+        <v>257</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>126</v>
+        <v>252</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>117</v>
+        <v>237</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>127</v>
+        <v>9</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>124</v>
+        <v>238</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>128</v>
+        <v>239</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>117</v>
+        <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>129</v>
+        <v>76</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>124</v>
+        <v>68</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>130</v>
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>135</v>
+        <v>29</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>136</v>
+        <v>30</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>137</v>
+        <v>31</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>131</v>
+        <v>28</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>139</v>
+        <v>33</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>140</v>
+        <v>34</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>134</v>
+        <v>28</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>139</v>
+        <v>33</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>141</v>
+        <v>34</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>138</v>
+        <v>28</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>142</v>
+        <v>37</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>139</v>
+        <v>38</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>143</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>138</v>
+        <v>28</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>142</v>
+        <v>37</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>139</v>
+        <v>38</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>145</v>
+        <v>40</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>197</v>
+      <c r="A79" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>144</v>
+        <v>28</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>148</v>
+        <v>107</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>154</v>
+        <v>112</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>148</v>
+        <v>107</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>156</v>
+        <v>114</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>157</v>
+        <v>112</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>221</v>
+        <v>107</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>155</v>
+        <v>107</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>162</v>
+        <v>118</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>163</v>
+        <v>111</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>164</v>
+        <v>119</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>202</v>
+        <v>24</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>166</v>
+        <v>14</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>167</v>
+        <v>25</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>168</v>
+        <v>26</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>169</v>
+        <v>22</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>170</v>
+        <v>23</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>165</v>
+        <v>20</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>169</v>
+        <v>22</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>171</v>
+        <v>23</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>165</v>
+        <v>20</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>169</v>
+        <v>25</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>171</v>
+        <v>26</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>161</v>
+        <v>260</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>158</v>
+        <v>261</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>169</v>
+        <v>258</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>172</v>
+        <v>262</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2477,13 +2480,13 @@
         <v>161</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>14</v>
+        <v>158</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>169</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2491,13 +2494,13 @@
         <v>161</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>222</v>
+        <v>14</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>169</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2505,545 +2508,545 @@
         <v>161</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>174</v>
+        <v>222</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>169</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>223</v>
+        <v>161</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>113</v>
+        <v>174</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>224</v>
+        <v>165</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>200</v>
+        <v>44</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>224</v>
+        <v>165</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>177</v>
+        <v>9</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>57</v>
+        <v>224</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>179</v>
+        <v>200</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>54</v>
+        <v>224</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>182</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>57</v>
+        <v>227</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>57</v>
+        <v>226</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>144</v>
+        <v>223</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>189</v>
+        <v>113</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>144</v>
+        <v>89</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>192</v>
+        <v>93</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>190</v>
+        <v>68</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>191</v>
+        <v>91</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>144</v>
+        <v>89</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>193</v>
+        <v>76</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>190</v>
+        <v>68</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>191</v>
+        <v>91</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>144</v>
+        <v>202</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>54</v>
+        <v>219</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>220</v>
+        <v>54</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>207</v>
+        <v>58</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>208</v>
+        <v>59</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>209</v>
+        <v>60</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>220</v>
+        <v>54</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>212</v>
+        <v>61</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>208</v>
+        <v>59</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>213</v>
+        <v>62</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>219</v>
+        <v>54</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>207</v>
+        <v>133</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>208</v>
+        <v>132</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>210</v>
+        <v>133</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>219</v>
+        <v>54</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>212</v>
+        <v>135</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>208</v>
+        <v>136</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>214</v>
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>220</v>
+        <v>54</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>220</v>
+        <v>54</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>219</v>
+        <v>57</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>212</v>
+        <v>64</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>208</v>
+        <v>59</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>218</v>
+        <v>62</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>232</v>
+        <v>57</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>233</v>
+        <v>66</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>231</v>
+        <v>59</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>228</v>
+        <v>62</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>232</v>
+        <v>57</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>234</v>
+        <v>179</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>231</v>
+        <v>180</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>229</v>
+        <v>181</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>236</v>
+        <v>57</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>235</v>
+        <v>184</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>231</v>
+        <v>185</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>230</v>
+        <v>186</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>237</v>
+        <v>57</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>9</v>
+        <v>187</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>238</v>
+        <v>185</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>239</v>
+        <v>188</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>240</v>
+        <v>117</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>14</v>
+        <v>123</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>238</v>
+        <v>124</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>241</v>
+        <v>123</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>240</v>
+        <v>117</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>243</v>
+        <v>125</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>238</v>
+        <v>124</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>242</v>
+        <v>125</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>240</v>
+        <v>117</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>244</v>
+        <v>126</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>238</v>
+        <v>124</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>245</v>
+        <v>126</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>248</v>
+        <v>117</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>247</v>
+        <v>127</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>238</v>
+        <v>124</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>246</v>
+        <v>128</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>240</v>
+        <v>117</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>249</v>
+        <v>129</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>257</v>
+        <v>124</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>250</v>
+        <v>130</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>251</v>
+        <v>207</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>252</v>
+        <v>209</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>253</v>
+        <v>220</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>254</v>
+        <v>212</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>255</v>
+        <v>213</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>259</v>
+        <v>207</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>258</v>
+        <v>208</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>256</v>
+        <v>215</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>260</v>
+        <v>220</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>261</v>
+        <v>212</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>258</v>
+        <v>208</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>262</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mapping Excel 1.8 snippets to ref docs (#211)
* Mapping Excel 1.8 snippets to ref docs
git push

* Sorting the Excel excel file

* Removing preview comment

* Fix layout map
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20822"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21005"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0D5419-DF3D-4B7D-99FD-3FDA7F92EDB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402CA407-B759-43FA-9B08-5F156F2843ED}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3000" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="263">
   <si>
     <t>Class</t>
   </si>
@@ -704,6 +704,111 @@
   </si>
   <si>
     <t>TableChangedEventArgs</t>
+  </si>
+  <si>
+    <t>addPositiveNumberRequirement</t>
+  </si>
+  <si>
+    <t>requireApprovedName</t>
+  </si>
+  <si>
+    <t>warnAboutCommentRedundancy</t>
+  </si>
+  <si>
+    <t>excel-data-validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataValidationRule </t>
+  </si>
+  <si>
+    <t>wholeNumber</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>errorAlert</t>
+  </si>
+  <si>
+    <t>DataValidation</t>
+  </si>
+  <si>
+    <t>PivotTableCollection</t>
+  </si>
+  <si>
+    <t>excel-pivottable-create-and-modify</t>
+  </si>
+  <si>
+    <t>createWithNames</t>
+  </si>
+  <si>
+    <t>PivotTable</t>
+  </si>
+  <si>
+    <t>deletePivot</t>
+  </si>
+  <si>
+    <t>toggleColumn</t>
+  </si>
+  <si>
+    <t>columnHierarchies</t>
+  </si>
+  <si>
+    <t>dataHierarchies</t>
+  </si>
+  <si>
+    <t>addValues</t>
+  </si>
+  <si>
+    <t>changeHierarchyNames</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>DataPivotHierarchy</t>
+  </si>
+  <si>
+    <t>layout</t>
+  </si>
+  <si>
+    <t>changeLayout</t>
+  </si>
+  <si>
+    <t>filterHierarchies</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>PivotLayout</t>
+  </si>
+  <si>
+    <t>getDataBodyRange</t>
+  </si>
+  <si>
+    <t>getCrateTotal</t>
+  </si>
+  <si>
+    <t>showPercentages</t>
+  </si>
+  <si>
+    <t>excel-pivottable-filters-and-summaries</t>
+  </si>
+  <si>
+    <t>excel-pivottable-calculations</t>
+  </si>
+  <si>
+    <t>showAs</t>
+  </si>
+  <si>
+    <t>ShowAsRule</t>
+  </si>
+  <si>
+    <t>baseItem</t>
+  </si>
+  <si>
+    <t>showDifferenceFrom</t>
   </si>
 </sst>
 </file>
@@ -783,8 +888,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D118" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D118" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D131" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D131" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D131">
+    <sortCondition ref="A3"/>
+  </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
@@ -1092,11 +1200,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D118"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O91" sqref="O91"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,394 +1245,394 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>152</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>153</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>162</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>163</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>221</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>158</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>159</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>26</v>
+      <c r="A9" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>147</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>150</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>31</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>189</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>190</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>34</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>192</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>190</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>193</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>190</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>194</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>190</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>40</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>134</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>43</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>45</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>138</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>142</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>43</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>138</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>142</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1532,21 +1640,21 @@
         <v>65</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>68</v>
@@ -1557,80 +1665,80 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>68</v>
@@ -1641,730 +1749,730 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>65</v>
+        <v>248</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>101</v>
+        <v>247</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>68</v>
+        <v>238</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>102</v>
+        <v>246</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>100</v>
+        <v>248</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>93</v>
+        <v>259</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>68</v>
+        <v>258</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>102</v>
+        <v>256</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>71</v>
+        <v>236</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>76</v>
+        <v>235</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>68</v>
+        <v>231</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>102</v>
+        <v>230</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>103</v>
+        <v>232</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>17</v>
+        <v>233</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>68</v>
+        <v>231</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>102</v>
+        <v>228</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>65</v>
+        <v>232</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>87</v>
+        <v>234</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>68</v>
+        <v>231</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>104</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>109</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>110</v>
+        <v>17</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>111</v>
+        <v>18</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>112</v>
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>111</v>
+        <v>10</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>112</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>114</v>
+        <v>9</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>111</v>
+        <v>12</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>112</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>107</v>
+        <v>253</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>116</v>
+        <v>254</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>111</v>
+        <v>257</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>112</v>
+        <v>255</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>107</v>
+        <v>240</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>118</v>
+        <v>14</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>111</v>
+        <v>238</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>119</v>
+        <v>241</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>115</v>
+        <v>240</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>120</v>
+        <v>243</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>121</v>
+        <v>238</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>122</v>
+        <v>242</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>117</v>
+        <v>240</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>123</v>
+        <v>244</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>124</v>
+        <v>238</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>123</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>117</v>
+        <v>240</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>125</v>
+        <v>249</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>124</v>
+        <v>238</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>125</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>117</v>
+        <v>240</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>126</v>
+        <v>251</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>124</v>
+        <v>257</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>126</v>
+        <v>252</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>117</v>
+        <v>237</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>127</v>
+        <v>9</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>124</v>
+        <v>238</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>128</v>
+        <v>239</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>117</v>
+        <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>129</v>
+        <v>76</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>124</v>
+        <v>68</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>130</v>
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>135</v>
+        <v>29</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>136</v>
+        <v>30</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>137</v>
+        <v>31</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>131</v>
+        <v>28</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>139</v>
+        <v>33</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>140</v>
+        <v>34</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>134</v>
+        <v>28</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>139</v>
+        <v>33</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>141</v>
+        <v>34</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>138</v>
+        <v>28</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>142</v>
+        <v>37</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>139</v>
+        <v>38</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>143</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>138</v>
+        <v>28</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>142</v>
+        <v>37</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>139</v>
+        <v>38</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>145</v>
+        <v>40</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>197</v>
+      <c r="A79" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>144</v>
+        <v>28</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>148</v>
+        <v>107</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>154</v>
+        <v>112</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>148</v>
+        <v>107</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>156</v>
+        <v>114</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>157</v>
+        <v>112</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>221</v>
+        <v>107</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>155</v>
+        <v>107</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>162</v>
+        <v>118</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>163</v>
+        <v>111</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>164</v>
+        <v>119</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>202</v>
+        <v>24</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>166</v>
+        <v>14</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>167</v>
+        <v>25</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>168</v>
+        <v>26</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>169</v>
+        <v>22</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>170</v>
+        <v>23</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>165</v>
+        <v>20</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>169</v>
+        <v>22</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>171</v>
+        <v>23</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>165</v>
+        <v>20</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>169</v>
+        <v>25</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>171</v>
+        <v>26</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>161</v>
+        <v>260</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>158</v>
+        <v>261</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>169</v>
+        <v>258</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>172</v>
+        <v>262</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2372,13 +2480,13 @@
         <v>161</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>14</v>
+        <v>158</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>169</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2386,13 +2494,13 @@
         <v>161</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>222</v>
+        <v>14</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>169</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2400,363 +2508,545 @@
         <v>161</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>174</v>
+        <v>222</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>169</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>223</v>
+        <v>161</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>113</v>
+        <v>174</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>224</v>
+        <v>165</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>200</v>
+        <v>44</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>224</v>
+        <v>165</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>177</v>
+        <v>9</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>57</v>
+        <v>224</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>179</v>
+        <v>200</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>54</v>
+        <v>224</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>182</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>57</v>
+        <v>227</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>57</v>
+        <v>226</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>144</v>
+        <v>223</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>189</v>
+        <v>113</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>144</v>
+        <v>89</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>192</v>
+        <v>93</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>190</v>
+        <v>68</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>191</v>
+        <v>91</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>144</v>
+        <v>89</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>193</v>
+        <v>76</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>190</v>
+        <v>68</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>191</v>
+        <v>91</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>144</v>
+        <v>202</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>54</v>
+        <v>219</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>220</v>
+        <v>54</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>207</v>
+        <v>58</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>208</v>
+        <v>59</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>209</v>
+        <v>60</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>220</v>
+        <v>54</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>212</v>
+        <v>61</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>208</v>
+        <v>59</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>213</v>
+        <v>62</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>219</v>
+        <v>54</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>207</v>
+        <v>133</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>208</v>
+        <v>132</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>210</v>
+        <v>133</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>219</v>
+        <v>54</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>212</v>
+        <v>135</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>208</v>
+        <v>136</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>214</v>
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>220</v>
+        <v>54</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>220</v>
+        <v>54</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>219</v>
+        <v>57</v>
       </c>
       <c r="B118" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B129" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C129" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D118" s="1" t="s">
-        <v>218</v>
+      <c r="D129" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding event snippet and running npm start
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21005"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402CA407-B759-43FA-9B08-5F156F2843ED}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EDC635-DBFF-4447-970F-4A0914649426}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3000" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="267">
   <si>
     <t>Class</t>
   </si>
@@ -809,6 +809,18 @@
   </si>
   <si>
     <t>showDifferenceFrom</t>
+  </si>
+  <si>
+    <t>Runtime</t>
+  </si>
+  <si>
+    <t>enableEvents</t>
+  </si>
+  <si>
+    <t>excel-events-disable-events</t>
+  </si>
+  <si>
+    <t>toggleEvents</t>
   </si>
 </sst>
 </file>
@@ -888,8 +900,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D131" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D131" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D132" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D132" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D131">
     <sortCondition ref="A3"/>
   </sortState>
@@ -1200,11 +1212,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:D132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3049,6 +3061,20 @@
         <v>216</v>
       </c>
     </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding event snippet to mapping and running npm start (#213)
* Adding event snippet and running npm start

* Resorting
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21005"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402CA407-B759-43FA-9B08-5F156F2843ED}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B1A8CA-58FE-4737-BF44-BCFA97B8C782}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3000" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="267">
   <si>
     <t>Class</t>
   </si>
@@ -809,6 +809,18 @@
   </si>
   <si>
     <t>showDifferenceFrom</t>
+  </si>
+  <si>
+    <t>Runtime</t>
+  </si>
+  <si>
+    <t>enableEvents</t>
+  </si>
+  <si>
+    <t>excel-events-disable-events</t>
+  </si>
+  <si>
+    <t>toggleEvents</t>
   </si>
 </sst>
 </file>
@@ -888,10 +900,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D131" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D131" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D131">
-    <sortCondition ref="A3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D132" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D132" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D132">
+    <sortCondition ref="C109"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1200,11 +1212,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:D132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J111" sqref="J111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,114 +1243,114 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>148</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>148</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>156</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>68</v>
+        <v>153</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>97</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>94</v>
+        <v>221</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>76</v>
+        <v>158</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>159</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>97</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>157</v>
+      <c r="A6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>162</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>221</v>
+        <v>144</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>197</v>
+      <c r="B9" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1346,13 +1358,13 @@
         <v>144</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>192</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>147</v>
+        <v>190</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>149</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1360,13 +1372,13 @@
         <v>144</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>150</v>
+        <v>193</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>147</v>
+        <v>190</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>151</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1374,7 +1386,7 @@
         <v>144</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>190</v>
@@ -1385,576 +1397,576 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>192</v>
+        <v>87</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>190</v>
+        <v>139</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>191</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>193</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>190</v>
+        <v>139</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>191</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>194</v>
+        <v>142</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>190</v>
+        <v>139</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>191</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>139</v>
+        <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>140</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>138</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>142</v>
+        <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>139</v>
+        <v>42</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>143</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>138</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>142</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>139</v>
+        <v>42</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>145</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>97</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>65</v>
+        <v>236</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>96</v>
+        <v>235</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>68</v>
+        <v>231</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>97</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>65</v>
+        <v>232</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>101</v>
+        <v>233</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>68</v>
+        <v>231</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>102</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>65</v>
+        <v>232</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>87</v>
+        <v>234</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>68</v>
+        <v>231</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>104</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>65</v>
+        <v>202</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>106</v>
+        <v>166</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>104</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>63</v>
+        <v>263</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>105</v>
+        <v>264</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>68</v>
+        <v>265</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>104</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>108</v>
+        <v>21</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>103</v>
+        <v>20</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>102</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>85</v>
+        <v>224</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>87</v>
+        <v>200</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>68</v>
+        <v>198</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>84</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>85</v>
+        <v>224</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>68</v>
+        <v>198</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>84</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>85</v>
+        <v>223</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>68</v>
+        <v>198</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>84</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>85</v>
+        <v>227</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>88</v>
+        <v>182</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>68</v>
+        <v>195</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>91</v>
+        <v>201</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>73</v>
+        <v>227</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>78</v>
+        <v>196</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>68</v>
+        <v>195</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>75</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>92</v>
+        <v>226</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>68</v>
+        <v>195</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>91</v>
+        <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>68</v>
+        <v>185</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>102</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>46</v>
+        <v>187</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>42</v>
+        <v>185</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>43</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>47</v>
+        <v>200</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>42</v>
+        <v>180</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>43</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>41</v>
+        <v>225</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>48</v>
+        <v>182</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>42</v>
+        <v>180</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>45</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>14</v>
+        <v>179</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>42</v>
+        <v>180</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>49</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>9</v>
+        <v>133</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>50</v>
+        <v>248</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>56</v>
+        <v>259</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>52</v>
+        <v>258</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>53</v>
+        <v>256</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>77</v>
+        <v>260</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>82</v>
+        <v>261</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>68</v>
+        <v>258</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>80</v>
+        <v>262</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1973,954 +1985,954 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>259</v>
+        <v>14</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>229</v>
+        <v>250</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>81</v>
+        <v>237</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>86</v>
+        <v>9</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>68</v>
+        <v>238</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>84</v>
+        <v>239</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>81</v>
+        <v>253</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>72</v>
+        <v>254</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>68</v>
+        <v>257</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>84</v>
+        <v>255</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>13</v>
+        <v>240</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>14</v>
+        <v>251</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>15</v>
+        <v>257</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>16</v>
+        <v>252</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>13</v>
+        <v>219</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>17</v>
+        <v>207</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>18</v>
+        <v>208</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>19</v>
+        <v>210</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>9</v>
+        <v>212</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>10</v>
+        <v>208</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>11</v>
+        <v>214</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>9</v>
+        <v>207</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>12</v>
+        <v>208</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>11</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>253</v>
+        <v>219</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>254</v>
+        <v>212</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>255</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>243</v>
+        <v>212</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>242</v>
+        <v>213</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>244</v>
+        <v>207</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>245</v>
+        <v>215</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>249</v>
+        <v>212</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>240</v>
+        <v>94</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>251</v>
+        <v>93</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>257</v>
+        <v>68</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>252</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>237</v>
+        <v>94</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>238</v>
+        <v>68</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>239</v>
+        <v>97</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>169</v>
+        <v>68</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>170</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>121</v>
+        <v>68</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>107</v>
+        <v>63</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>107</v>
+        <v>63</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>26</v>
+        <v>109</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>260</v>
+        <v>85</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>261</v>
+        <v>17</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>258</v>
+        <v>68</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>262</v>
+        <v>84</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>161</v>
+        <v>85</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>158</v>
+        <v>88</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>169</v>
+        <v>68</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>172</v>
+        <v>91</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>161</v>
+        <v>73</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>169</v>
+        <v>68</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>173</v>
+        <v>75</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>161</v>
+        <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>222</v>
+        <v>95</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>169</v>
+        <v>68</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>175</v>
+        <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>161</v>
+        <v>100</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>174</v>
+        <v>93</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>169</v>
+        <v>68</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>170</v>
+        <v>102</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>165</v>
+        <v>77</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>169</v>
+        <v>68</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>171</v>
+        <v>80</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>165</v>
+        <v>81</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>169</v>
+        <v>68</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>171</v>
+        <v>84</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>224</v>
+        <v>81</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>200</v>
+        <v>72</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>198</v>
+        <v>68</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>199</v>
+        <v>84</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>224</v>
+        <v>71</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>177</v>
+        <v>76</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>198</v>
+        <v>68</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>178</v>
+        <v>75</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>227</v>
+        <v>71</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>182</v>
+        <v>76</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>195</v>
+        <v>68</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>201</v>
+        <v>102</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>227</v>
+        <v>89</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>196</v>
+        <v>93</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>195</v>
+        <v>68</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>201</v>
+        <v>91</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>226</v>
+        <v>89</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>200</v>
+        <v>76</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>195</v>
+        <v>68</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>199</v>
+        <v>91</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>223</v>
+        <v>28</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>113</v>
+        <v>32</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>198</v>
+        <v>33</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>176</v>
+        <v>34</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>89</v>
+        <v>28</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>89</v>
+        <v>28</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>202</v>
+        <v>107</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>166</v>
+        <v>113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>167</v>
+        <v>111</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>168</v>
+        <v>112</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>202</v>
+        <v>107</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>203</v>
+        <v>114</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>204</v>
+        <v>111</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>211</v>
+        <v>112</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>219</v>
+        <v>107</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>207</v>
+        <v>116</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>208</v>
+        <v>111</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>210</v>
+        <v>112</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>219</v>
+        <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>212</v>
+        <v>118</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>208</v>
+        <v>111</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>214</v>
+        <v>119</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>219</v>
+        <v>28</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>207</v>
+        <v>29</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>208</v>
+        <v>30</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>217</v>
+        <v>31</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>219</v>
+        <v>115</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>212</v>
+        <v>120</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>208</v>
+        <v>121</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>218</v>
+        <v>122</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>133</v>
+        <v>86</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>132</v>
+        <v>169</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>54</v>
+        <v>161</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>137</v>
+        <v>172</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>54</v>
+        <v>161</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>200</v>
+        <v>14</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>54</v>
+        <v>161</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>206</v>
+        <v>169</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>225</v>
+        <v>161</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>57</v>
+        <v>165</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>59</v>
+        <v>169</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>62</v>
+        <v>171</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>57</v>
+        <v>165</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>59</v>
+        <v>169</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>62</v>
+        <v>171</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>179</v>
+        <v>17</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>180</v>
+        <v>18</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>181</v>
+        <v>19</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>57</v>
+        <v>202</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>184</v>
+        <v>203</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2995,58 +3007,72 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>220</v>
+        <v>54</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>207</v>
+        <v>58</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>208</v>
+        <v>59</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>209</v>
+        <v>60</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>220</v>
+        <v>54</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>212</v>
+        <v>61</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>208</v>
+        <v>59</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>213</v>
+        <v>62</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>220</v>
+        <v>57</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>207</v>
+        <v>64</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>208</v>
+        <v>59</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>215</v>
+        <v>62</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>220</v>
+        <v>57</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>212</v>
+        <v>66</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>208</v>
+        <v>59</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>216</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove whitespace from metadata
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21101"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B1A8CA-58FE-4737-BF44-BCFA97B8C782}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5D8021-2F59-4F9E-A94E-172DA06B79A7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="22500" windowHeight="10788" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -718,9 +718,6 @@
     <t>excel-data-validation</t>
   </si>
   <si>
-    <t xml:space="preserve">DataValidationRule </t>
-  </si>
-  <si>
     <t>wholeNumber</t>
   </si>
   <si>
@@ -821,6 +818,9 @@
   </si>
   <si>
     <t>toggleEvents</t>
+  </si>
+  <si>
+    <t>DataValidationRule</t>
   </si>
 </sst>
 </file>
@@ -1215,19 +1215,19 @@
   <dimension ref="A1:D132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J111" sqref="J111"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>148</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>148</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>221</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>155</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>144</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>144</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>144</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>144</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>144</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>144</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>144</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>134</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>131</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>138</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>138</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
@@ -1605,12 +1605,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>231</v>
@@ -1619,12 +1619,12 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>231</v>
@@ -1633,12 +1633,12 @@
         <v>228</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>232</v>
+        <v>266</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>231</v>
@@ -1647,7 +1647,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>202</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -1675,21 +1675,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>20</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>224</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>224</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>223</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>227</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>227</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>226</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>57</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>57</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>54</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>225</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>57</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>54</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>28</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>28</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>13</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>8</v>
       </c>
@@ -1941,147 +1941,147 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B56" s="1" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D59" s="1" t="s">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="B61" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>219</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>219</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>219</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>219</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>220</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>220</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>220</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>220</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>94</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>94</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>67</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>98</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>98</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>65</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>65</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>65</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>65</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>65</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>65</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>65</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>65</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>65</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>63</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>63</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>63</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>103</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>85</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>85</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>85</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>85</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>73</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>100</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>77</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>81</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>81</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>71</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>71</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>89</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>89</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>28</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>28</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>28</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>107</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>107</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>107</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>107</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>28</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>115</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>24</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>20</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>28</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>161</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>161</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>161</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>161</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>165</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>165</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>13</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>202</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>54</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>117</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>117</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>117</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>117</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>117</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>54</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>54</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>57</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>57</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Remove whitespace from metadata (#227)
* Remove whitespace from metadata

* ran npm start
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21101"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B1A8CA-58FE-4737-BF44-BCFA97B8C782}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5D8021-2F59-4F9E-A94E-172DA06B79A7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="22500" windowHeight="10788" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -718,9 +718,6 @@
     <t>excel-data-validation</t>
   </si>
   <si>
-    <t xml:space="preserve">DataValidationRule </t>
-  </si>
-  <si>
     <t>wholeNumber</t>
   </si>
   <si>
@@ -821,6 +818,9 @@
   </si>
   <si>
     <t>toggleEvents</t>
+  </si>
+  <si>
+    <t>DataValidationRule</t>
   </si>
 </sst>
 </file>
@@ -1215,19 +1215,19 @@
   <dimension ref="A1:D132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J111" sqref="J111"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>148</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>148</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>221</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>155</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>144</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>144</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>144</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>144</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>144</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>144</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>144</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>134</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>131</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>138</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>138</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
@@ -1605,12 +1605,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>231</v>
@@ -1619,12 +1619,12 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>231</v>
@@ -1633,12 +1633,12 @@
         <v>228</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>232</v>
+        <v>266</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>231</v>
@@ -1647,7 +1647,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>202</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -1675,21 +1675,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>20</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>224</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>224</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>223</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>227</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>227</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>226</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>57</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>57</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>54</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>225</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>57</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>54</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>28</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>28</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>13</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>8</v>
       </c>
@@ -1941,147 +1941,147 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B56" s="1" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D59" s="1" t="s">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="B61" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>219</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>219</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>219</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>219</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>220</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>220</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>220</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>220</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>94</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>94</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>67</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>98</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>98</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>65</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>65</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>65</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>65</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>65</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>65</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>65</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>65</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>65</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>63</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>63</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>63</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>103</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>85</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>85</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>85</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>85</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>73</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>100</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>77</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>81</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>81</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>71</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>71</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>89</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>89</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>28</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>28</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>28</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>107</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>107</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>107</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>107</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>28</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>115</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>24</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>20</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>28</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>161</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>161</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>161</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>161</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>165</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>165</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>13</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>202</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>54</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>117</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>117</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>117</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>117</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>117</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>54</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>54</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>57</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>57</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Returning basics to their own folder
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21108"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BDE4C6-50AB-4DC3-92AC-436892837611}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07454BF-5768-4C5F-B4E9-DAFDE4707CD5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3600" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -817,7 +817,7 @@
     <t>excel-worksheet-gridlines</t>
   </si>
   <si>
-    <t>excel-guidance-multiple-property-set</t>
+    <t>excel-scenarios-multiple-property-set</t>
   </si>
 </sst>
 </file>
@@ -1212,8 +1212,8 @@
   <dimension ref="A1:D132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I29" sqref="I29"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Rework Chart Title Substring into more general Chart Title snippet
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21108"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07454BF-5768-4C5F-B4E9-DAFDE4707CD5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EF771F-9AFE-43AB-B74A-DC799C689C86}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3600" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="270">
   <si>
     <t>Class</t>
   </si>
@@ -52,12 +52,6 @@
     <t>add</t>
   </si>
   <si>
-    <t>excel-create-and-use-named-item-for-range</t>
-  </si>
-  <si>
-    <t>addName</t>
-  </si>
-  <si>
     <t>NamedItem</t>
   </si>
   <si>
@@ -463,9 +457,6 @@
     <t>setValues</t>
   </si>
   <si>
-    <t>setSeriesValue</t>
-  </si>
-  <si>
     <t>displayUnit</t>
   </si>
   <si>
@@ -818,6 +809,27 @@
   </si>
   <si>
     <t>excel-scenarios-multiple-property-set</t>
+  </si>
+  <si>
+    <t>ChartTitle</t>
+  </si>
+  <si>
+    <t>getSubstring</t>
+  </si>
+  <si>
+    <t>excel-chart-title-format</t>
+  </si>
+  <si>
+    <t>changeTitleSubstring</t>
+  </si>
+  <si>
+    <t>changeTitleOrientation</t>
+  </si>
+  <si>
+    <t>addSeries</t>
+  </si>
+  <si>
+    <t>addNameToHeader</t>
   </si>
 </sst>
 </file>
@@ -897,10 +909,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D132" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D132" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D132">
-    <sortCondition ref="C109"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D133" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D133" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D131">
+    <sortCondition ref="C108"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1209,11 +1221,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D132"/>
+  <dimension ref="A1:D133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,212 +1252,212 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>147</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1456,206 +1468,206 @@
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>11</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="D27" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1674,335 +1686,335 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>8</v>
+        <v>238</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>9</v>
+        <v>249</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>14</v>
+        <v>248</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>11</v>
+        <v>246</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>240</v>
+        <v>11</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C55" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>235</v>
@@ -2010,97 +2022,97 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>242</v>
+        <v>9</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>9</v>
+        <v>244</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>250</v>
-      </c>
       <c r="D60" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>244</v>
+        <v>199</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>245</v>
+        <v>201</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>208</v>
@@ -2108,251 +2120,251 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>214</v>
+        <v>89</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>206</v>
+        <v>88</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>261</v>
+        <v>63</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>210</v>
+        <v>92</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>99</v>
@@ -2360,587 +2372,587 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>103</v>
+        <v>9</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B95" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>65</v>
+        <v>259</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>88</v>
+        <v>30</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>262</v>
+        <v>106</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>115</v>
+        <v>26</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>116</v>
+        <v>28</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>29</v>
+        <v>116</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>117</v>
+        <v>11</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>118</v>
+        <v>22</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>119</v>
+        <v>23</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>24</v>
+        <v>260</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>25</v>
+        <v>162</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>27</v>
+        <v>154</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>83</v>
+        <v>151</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>154</v>
+        <v>11</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>13</v>
+        <v>213</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>216</v>
+        <v>166</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>169</v>
+        <v>39</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>161</v>
+        <v>10</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>263</v>
+        <v>15</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>166</v>
+        <v>16</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>12</v>
+        <v>194</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>16</v>
+        <v>195</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>17</v>
+        <v>196</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>18</v>
+        <v>202</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="C121" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C121" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="D121" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>51</v>
+        <v>112</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>200</v>
+        <v>118</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>201</v>
+        <v>119</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>205</v>
+        <v>118</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>120</v>
@@ -2948,27 +2960,27 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C124" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>123</v>
@@ -2976,13 +2988,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>124</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>125</v>
@@ -2990,27 +3002,27 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>114</v>
+        <v>49</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>126</v>
+        <v>53</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>127</v>
+        <v>55</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>57</v>
@@ -3018,58 +3030,72 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>63</v>
+        <v>129</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>59</v>
+        <v>131</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>51</v>
+        <v>263</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>131</v>
+        <v>264</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>132</v>
+        <v>265</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>133</v>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Name and description updates
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21113"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B493AF24-C5AC-4C4E-B91D-F07CE1F0CAAA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3259C7B-17E7-4C99-B405-58EAD2E65096}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3600" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -100,9 +100,6 @@
     <t>getUsedRangeOrNullObject</t>
   </si>
   <si>
-    <t>excel-range-test-for-used-range</t>
-  </si>
-  <si>
     <t>tryCreateChartFromEmptyTable</t>
   </si>
   <si>
@@ -827,6 +824,9 @@
   </si>
   <si>
     <t>excel-events-worksheet</t>
+  </si>
+  <si>
+    <t>excel-range-used-range</t>
   </si>
 </sst>
 </file>
@@ -1220,8 +1220,8 @@
   <dimension ref="A1:D133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K98" sqref="K98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,212 +1248,212 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" t="s">
         <v>144</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>145</v>
-      </c>
-      <c r="D2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" t="s">
         <v>148</v>
-      </c>
-      <c r="C3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" t="s">
         <v>150</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>151</v>
-      </c>
-      <c r="D4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" t="s">
         <v>154</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>155</v>
-      </c>
-      <c r="D5" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" t="s">
         <v>178</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>179</v>
-      </c>
-      <c r="D9" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" t="s">
         <v>179</v>
-      </c>
-      <c r="D10" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C11" t="s">
+        <v>178</v>
+      </c>
+      <c r="D11" t="s">
         <v>179</v>
-      </c>
-      <c r="D11" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C12" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" t="s">
         <v>179</v>
-      </c>
-      <c r="D12" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" t="s">
         <v>132</v>
-      </c>
-      <c r="D14" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" t="s">
         <v>131</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>135</v>
-      </c>
-      <c r="C15" t="s">
-        <v>132</v>
-      </c>
-      <c r="D15" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" t="s">
         <v>131</v>
       </c>
-      <c r="B16" t="s">
-        <v>135</v>
-      </c>
-      <c r="C16" t="s">
-        <v>132</v>
-      </c>
       <c r="D16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1467,203 +1467,203 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>36</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>36</v>
-      </c>
-      <c r="D19" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
         <v>35</v>
       </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
         <v>36</v>
-      </c>
-      <c r="D22" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
         <v>38</v>
-      </c>
-      <c r="C23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
         <v>45</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>46</v>
-      </c>
-      <c r="D25" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" t="s">
         <v>46</v>
-      </c>
-      <c r="D26" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" t="s">
         <v>46</v>
-      </c>
-      <c r="D27" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B31" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" t="s">
         <v>158</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>159</v>
-      </c>
-      <c r="D31" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1682,16 +1682,16 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>249</v>
+      </c>
+      <c r="B33" t="s">
         <v>250</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>251</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>252</v>
-      </c>
-      <c r="D33" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1702,7 +1702,7 @@
         <v>18</v>
       </c>
       <c r="C34" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D34" t="s">
         <v>19</v>
@@ -1716,7 +1716,7 @@
         <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D35" t="s">
         <v>19</v>
@@ -1724,170 +1724,170 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B36" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" t="s">
         <v>187</v>
-      </c>
-      <c r="D36" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B37" t="s">
+        <v>167</v>
+      </c>
+      <c r="C37" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37" t="s">
         <v>168</v>
-      </c>
-      <c r="C37" t="s">
-        <v>187</v>
-      </c>
-      <c r="D37" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C39" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C40" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B41" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C41" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B42" t="s">
+        <v>173</v>
+      </c>
+      <c r="C42" t="s">
+        <v>266</v>
+      </c>
+      <c r="D42" t="s">
         <v>174</v>
-      </c>
-      <c r="C42" t="s">
-        <v>267</v>
-      </c>
-      <c r="D42" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B43" t="s">
+        <v>175</v>
+      </c>
+      <c r="C43" t="s">
+        <v>266</v>
+      </c>
+      <c r="D43" t="s">
         <v>176</v>
-      </c>
-      <c r="C43" t="s">
-        <v>267</v>
-      </c>
-      <c r="D43" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C44" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D44" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B45" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" t="s">
+        <v>266</v>
+      </c>
+      <c r="D45" t="s">
         <v>172</v>
-      </c>
-      <c r="C45" t="s">
-        <v>267</v>
-      </c>
-      <c r="D45" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
+        <v>169</v>
+      </c>
+      <c r="C46" t="s">
+        <v>266</v>
+      </c>
+      <c r="D46" t="s">
         <v>170</v>
-      </c>
-      <c r="C46" t="s">
-        <v>267</v>
-      </c>
-      <c r="D46" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C47" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1895,13 +1895,13 @@
         <v>24</v>
       </c>
       <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" t="s">
+        <v>258</v>
+      </c>
+      <c r="D48" t="s">
         <v>32</v>
-      </c>
-      <c r="C48" t="s">
-        <v>259</v>
-      </c>
-      <c r="D48" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1909,13 +1909,13 @@
         <v>24</v>
       </c>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C49" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D49" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1934,702 +1934,702 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B51" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C51" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>246</v>
+      </c>
+      <c r="B52" t="s">
         <v>247</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
+        <v>244</v>
+      </c>
+      <c r="D52" t="s">
         <v>248</v>
-      </c>
-      <c r="C52" t="s">
-        <v>245</v>
-      </c>
-      <c r="D52" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C53" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B54" t="s">
         <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D54" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B55" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C55" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D55" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B56" t="s">
+        <v>230</v>
+      </c>
+      <c r="C56" t="s">
+        <v>224</v>
+      </c>
+      <c r="D56" t="s">
         <v>231</v>
-      </c>
-      <c r="C56" t="s">
-        <v>225</v>
-      </c>
-      <c r="D56" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B57" t="s">
+        <v>235</v>
+      </c>
+      <c r="C57" t="s">
+        <v>224</v>
+      </c>
+      <c r="D57" t="s">
         <v>236</v>
-      </c>
-      <c r="C57" t="s">
-        <v>225</v>
-      </c>
-      <c r="D57" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
       </c>
       <c r="C58" t="s">
+        <v>224</v>
+      </c>
+      <c r="D58" t="s">
         <v>225</v>
-      </c>
-      <c r="D58" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>239</v>
+      </c>
+      <c r="B59" t="s">
         <v>240</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>243</v>
+      </c>
+      <c r="D59" t="s">
         <v>241</v>
-      </c>
-      <c r="C59" t="s">
-        <v>244</v>
-      </c>
-      <c r="D59" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B60" t="s">
+        <v>237</v>
+      </c>
+      <c r="C60" t="s">
+        <v>243</v>
+      </c>
+      <c r="D60" t="s">
         <v>238</v>
-      </c>
-      <c r="C60" t="s">
-        <v>244</v>
-      </c>
-      <c r="D60" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B61" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C61" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D61" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B62" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C62" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D62" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C63" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D63" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B64" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C64" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D64" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B65" t="s">
+        <v>195</v>
+      </c>
+      <c r="C65" t="s">
+        <v>254</v>
+      </c>
+      <c r="D65" t="s">
         <v>196</v>
-      </c>
-      <c r="C65" t="s">
-        <v>255</v>
-      </c>
-      <c r="D65" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B66" t="s">
+        <v>199</v>
+      </c>
+      <c r="C66" t="s">
+        <v>254</v>
+      </c>
+      <c r="D66" t="s">
         <v>200</v>
-      </c>
-      <c r="C66" t="s">
-        <v>255</v>
-      </c>
-      <c r="D66" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B67" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C67" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D67" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B68" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C68" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C69" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D70" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>60</v>
+      </c>
+      <c r="B71" t="s">
+        <v>65</v>
+      </c>
+      <c r="C71" t="s">
         <v>61</v>
       </c>
-      <c r="B71" t="s">
-        <v>66</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>62</v>
-      </c>
-      <c r="D71" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>91</v>
+      </c>
+      <c r="B72" t="s">
         <v>92</v>
       </c>
-      <c r="B72" t="s">
-        <v>93</v>
-      </c>
       <c r="C72" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D72" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C73" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D73" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B74" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C74" t="s">
+        <v>61</v>
+      </c>
+      <c r="D74" t="s">
         <v>62</v>
-      </c>
-      <c r="D74" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B75" t="s">
+        <v>67</v>
+      </c>
+      <c r="C75" t="s">
+        <v>61</v>
+      </c>
+      <c r="D75" t="s">
         <v>68</v>
-      </c>
-      <c r="C75" t="s">
-        <v>62</v>
-      </c>
-      <c r="D75" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B76" t="s">
+        <v>72</v>
+      </c>
+      <c r="C76" t="s">
+        <v>61</v>
+      </c>
+      <c r="D76" t="s">
         <v>73</v>
-      </c>
-      <c r="C76" t="s">
-        <v>62</v>
-      </c>
-      <c r="D76" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B77" t="s">
+        <v>76</v>
+      </c>
+      <c r="C77" t="s">
+        <v>61</v>
+      </c>
+      <c r="D77" t="s">
         <v>77</v>
-      </c>
-      <c r="C77" t="s">
-        <v>62</v>
-      </c>
-      <c r="D77" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B78" t="s">
+        <v>83</v>
+      </c>
+      <c r="C78" t="s">
+        <v>61</v>
+      </c>
+      <c r="D78" t="s">
         <v>84</v>
-      </c>
-      <c r="C78" t="s">
-        <v>62</v>
-      </c>
-      <c r="D78" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B79" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79" t="s">
+        <v>61</v>
+      </c>
+      <c r="D79" t="s">
         <v>90</v>
-      </c>
-      <c r="C79" t="s">
-        <v>62</v>
-      </c>
-      <c r="D79" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B80" t="s">
+        <v>94</v>
+      </c>
+      <c r="C80" t="s">
+        <v>61</v>
+      </c>
+      <c r="D80" t="s">
         <v>95</v>
-      </c>
-      <c r="C80" t="s">
-        <v>62</v>
-      </c>
-      <c r="D80" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B81" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C81" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D81" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C82" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D82" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
       </c>
       <c r="C83" t="s">
+        <v>61</v>
+      </c>
+      <c r="D83" t="s">
         <v>62</v>
-      </c>
-      <c r="D83" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B84" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C84" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D84" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B85" t="s">
+        <v>101</v>
+      </c>
+      <c r="C85" t="s">
+        <v>61</v>
+      </c>
+      <c r="D85" t="s">
         <v>102</v>
-      </c>
-      <c r="C85" t="s">
-        <v>62</v>
-      </c>
-      <c r="D85" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B86" t="s">
         <v>14</v>
       </c>
       <c r="C86" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D86" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B87" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C87" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D87" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C88" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D88" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B89" t="s">
         <v>14</v>
       </c>
       <c r="C89" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D89" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B90" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C90" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D90" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B91" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C91" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D91" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C92" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D92" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C93" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D93" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B94" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C94" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D94" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B95" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C95" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D95" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B96" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C96" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D96" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B97" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C97" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D97" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B98" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C98" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D98" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B99" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C99" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D99" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B100" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C100" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D100" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2637,13 +2637,13 @@
         <v>24</v>
       </c>
       <c r="B101" t="s">
+        <v>27</v>
+      </c>
+      <c r="C101" t="s">
+        <v>255</v>
+      </c>
+      <c r="D101" t="s">
         <v>28</v>
-      </c>
-      <c r="C101" t="s">
-        <v>256</v>
-      </c>
-      <c r="D101" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2651,13 +2651,13 @@
         <v>24</v>
       </c>
       <c r="B102" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C102" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D102" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2665,69 +2665,69 @@
         <v>24</v>
       </c>
       <c r="B103" t="s">
+        <v>103</v>
+      </c>
+      <c r="C103" t="s">
         <v>104</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
         <v>105</v>
-      </c>
-      <c r="D103" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B104" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C104" t="s">
+        <v>104</v>
+      </c>
+      <c r="D104" t="s">
         <v>105</v>
-      </c>
-      <c r="D104" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B105" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C105" t="s">
+        <v>104</v>
+      </c>
+      <c r="D105" t="s">
         <v>105</v>
-      </c>
-      <c r="D105" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B106" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C106" t="s">
+        <v>104</v>
+      </c>
+      <c r="D106" t="s">
         <v>105</v>
-      </c>
-      <c r="D106" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B107" t="s">
+        <v>111</v>
+      </c>
+      <c r="C107" t="s">
+        <v>104</v>
+      </c>
+      <c r="D107" t="s">
         <v>112</v>
-      </c>
-      <c r="C107" t="s">
-        <v>105</v>
-      </c>
-      <c r="D107" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2738,24 +2738,24 @@
         <v>25</v>
       </c>
       <c r="C108" t="s">
+        <v>268</v>
+      </c>
+      <c r="D108" t="s">
         <v>26</v>
-      </c>
-      <c r="D108" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B109" t="s">
+        <v>113</v>
+      </c>
+      <c r="C109" t="s">
         <v>114</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>115</v>
-      </c>
-      <c r="D109" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2791,97 +2791,97 @@
         <v>24</v>
       </c>
       <c r="B112" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C112" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D112" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B113" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C113" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D113" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B114" t="s">
         <v>11</v>
       </c>
       <c r="C114" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D114" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B115" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C115" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D115" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B116" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C116" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D116" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B117" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C117" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D117" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B118" t="s">
         <v>9</v>
       </c>
       <c r="C118" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D118" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -2900,198 +2900,198 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>190</v>
+      </c>
+      <c r="B120" t="s">
         <v>191</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" t="s">
         <v>192</v>
       </c>
-      <c r="C120" t="s">
-        <v>193</v>
-      </c>
       <c r="D120" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B121" t="s">
+        <v>193</v>
+      </c>
+      <c r="C121" t="s">
         <v>194</v>
       </c>
-      <c r="C121" t="s">
-        <v>195</v>
-      </c>
       <c r="D121" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B122" t="s">
+        <v>116</v>
+      </c>
+      <c r="C122" t="s">
         <v>117</v>
       </c>
-      <c r="C122" t="s">
-        <v>118</v>
-      </c>
       <c r="D122" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B123" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C123" t="s">
+        <v>117</v>
+      </c>
+      <c r="D123" t="s">
         <v>118</v>
-      </c>
-      <c r="D123" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B124" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C124" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D124" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B125" t="s">
+        <v>120</v>
+      </c>
+      <c r="C125" t="s">
+        <v>117</v>
+      </c>
+      <c r="D125" t="s">
         <v>121</v>
-      </c>
-      <c r="C125" t="s">
-        <v>118</v>
-      </c>
-      <c r="D125" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B126" t="s">
+        <v>122</v>
+      </c>
+      <c r="C126" t="s">
+        <v>117</v>
+      </c>
+      <c r="D126" t="s">
         <v>123</v>
-      </c>
-      <c r="C126" t="s">
-        <v>118</v>
-      </c>
-      <c r="D126" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B127" t="s">
+        <v>51</v>
+      </c>
+      <c r="C127" t="s">
         <v>52</v>
       </c>
-      <c r="C127" t="s">
+      <c r="D127" t="s">
         <v>53</v>
-      </c>
-      <c r="D127" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B128" t="s">
+        <v>54</v>
+      </c>
+      <c r="C128" t="s">
+        <v>52</v>
+      </c>
+      <c r="D128" t="s">
         <v>55</v>
-      </c>
-      <c r="C128" t="s">
-        <v>53</v>
-      </c>
-      <c r="D128" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B129" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C129" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D129" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B130" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C130" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D130" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B131" t="s">
+        <v>127</v>
+      </c>
+      <c r="C131" t="s">
         <v>128</v>
       </c>
-      <c r="C131" t="s">
+      <c r="D131" t="s">
         <v>129</v>
-      </c>
-      <c r="D131" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>259</v>
+      </c>
+      <c r="B132" t="s">
         <v>260</v>
       </c>
-      <c r="B132" t="s">
+      <c r="C132" t="s">
         <v>261</v>
       </c>
-      <c r="C132" t="s">
+      <c r="D132" t="s">
         <v>262</v>
-      </c>
-      <c r="D132" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B133" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C133" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D133" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Snippet standization cleanup (#231)
* Adding parens around context

* Remove unnecessary mention of JavaScript API

* Name and description updates

* Update basic instructions

* Chart format fixes

* Fix spacing

* Event, worksheet, and pivot fixes

* Standardizing console versus UI.notify

* Rerunning npm start
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21113"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B493AF24-C5AC-4C4E-B91D-F07CE1F0CAAA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3259C7B-17E7-4C99-B405-58EAD2E65096}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3600" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -100,9 +100,6 @@
     <t>getUsedRangeOrNullObject</t>
   </si>
   <si>
-    <t>excel-range-test-for-used-range</t>
-  </si>
-  <si>
     <t>tryCreateChartFromEmptyTable</t>
   </si>
   <si>
@@ -827,6 +824,9 @@
   </si>
   <si>
     <t>excel-events-worksheet</t>
+  </si>
+  <si>
+    <t>excel-range-used-range</t>
   </si>
 </sst>
 </file>
@@ -1220,8 +1220,8 @@
   <dimension ref="A1:D133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K98" sqref="K98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,212 +1248,212 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" t="s">
         <v>144</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>145</v>
-      </c>
-      <c r="D2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" t="s">
         <v>148</v>
-      </c>
-      <c r="C3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" t="s">
         <v>150</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>151</v>
-      </c>
-      <c r="D4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" t="s">
         <v>154</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>155</v>
-      </c>
-      <c r="D5" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" t="s">
         <v>178</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>179</v>
-      </c>
-      <c r="D9" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" t="s">
         <v>179</v>
-      </c>
-      <c r="D10" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C11" t="s">
+        <v>178</v>
+      </c>
+      <c r="D11" t="s">
         <v>179</v>
-      </c>
-      <c r="D11" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C12" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" t="s">
         <v>179</v>
-      </c>
-      <c r="D12" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" t="s">
         <v>132</v>
-      </c>
-      <c r="D14" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" t="s">
         <v>131</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>135</v>
-      </c>
-      <c r="C15" t="s">
-        <v>132</v>
-      </c>
-      <c r="D15" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" t="s">
         <v>131</v>
       </c>
-      <c r="B16" t="s">
-        <v>135</v>
-      </c>
-      <c r="C16" t="s">
-        <v>132</v>
-      </c>
       <c r="D16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1467,203 +1467,203 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>36</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>36</v>
-      </c>
-      <c r="D19" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
         <v>35</v>
       </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
         <v>36</v>
-      </c>
-      <c r="D22" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
         <v>38</v>
-      </c>
-      <c r="C23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
         <v>45</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>46</v>
-      </c>
-      <c r="D25" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" t="s">
         <v>46</v>
-      </c>
-      <c r="D26" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" t="s">
         <v>46</v>
-      </c>
-      <c r="D27" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B31" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" t="s">
         <v>158</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>159</v>
-      </c>
-      <c r="D31" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1682,16 +1682,16 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>249</v>
+      </c>
+      <c r="B33" t="s">
         <v>250</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>251</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>252</v>
-      </c>
-      <c r="D33" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1702,7 +1702,7 @@
         <v>18</v>
       </c>
       <c r="C34" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D34" t="s">
         <v>19</v>
@@ -1716,7 +1716,7 @@
         <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D35" t="s">
         <v>19</v>
@@ -1724,170 +1724,170 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B36" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" t="s">
         <v>187</v>
-      </c>
-      <c r="D36" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B37" t="s">
+        <v>167</v>
+      </c>
+      <c r="C37" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37" t="s">
         <v>168</v>
-      </c>
-      <c r="C37" t="s">
-        <v>187</v>
-      </c>
-      <c r="D37" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C39" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C40" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B41" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C41" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B42" t="s">
+        <v>173</v>
+      </c>
+      <c r="C42" t="s">
+        <v>266</v>
+      </c>
+      <c r="D42" t="s">
         <v>174</v>
-      </c>
-      <c r="C42" t="s">
-        <v>267</v>
-      </c>
-      <c r="D42" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B43" t="s">
+        <v>175</v>
+      </c>
+      <c r="C43" t="s">
+        <v>266</v>
+      </c>
+      <c r="D43" t="s">
         <v>176</v>
-      </c>
-      <c r="C43" t="s">
-        <v>267</v>
-      </c>
-      <c r="D43" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C44" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D44" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B45" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" t="s">
+        <v>266</v>
+      </c>
+      <c r="D45" t="s">
         <v>172</v>
-      </c>
-      <c r="C45" t="s">
-        <v>267</v>
-      </c>
-      <c r="D45" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
+        <v>169</v>
+      </c>
+      <c r="C46" t="s">
+        <v>266</v>
+      </c>
+      <c r="D46" t="s">
         <v>170</v>
-      </c>
-      <c r="C46" t="s">
-        <v>267</v>
-      </c>
-      <c r="D46" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C47" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1895,13 +1895,13 @@
         <v>24</v>
       </c>
       <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" t="s">
+        <v>258</v>
+      </c>
+      <c r="D48" t="s">
         <v>32</v>
-      </c>
-      <c r="C48" t="s">
-        <v>259</v>
-      </c>
-      <c r="D48" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1909,13 +1909,13 @@
         <v>24</v>
       </c>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C49" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D49" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1934,702 +1934,702 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B51" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C51" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>246</v>
+      </c>
+      <c r="B52" t="s">
         <v>247</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
+        <v>244</v>
+      </c>
+      <c r="D52" t="s">
         <v>248</v>
-      </c>
-      <c r="C52" t="s">
-        <v>245</v>
-      </c>
-      <c r="D52" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C53" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B54" t="s">
         <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D54" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B55" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C55" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D55" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B56" t="s">
+        <v>230</v>
+      </c>
+      <c r="C56" t="s">
+        <v>224</v>
+      </c>
+      <c r="D56" t="s">
         <v>231</v>
-      </c>
-      <c r="C56" t="s">
-        <v>225</v>
-      </c>
-      <c r="D56" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B57" t="s">
+        <v>235</v>
+      </c>
+      <c r="C57" t="s">
+        <v>224</v>
+      </c>
+      <c r="D57" t="s">
         <v>236</v>
-      </c>
-      <c r="C57" t="s">
-        <v>225</v>
-      </c>
-      <c r="D57" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
       </c>
       <c r="C58" t="s">
+        <v>224</v>
+      </c>
+      <c r="D58" t="s">
         <v>225</v>
-      </c>
-      <c r="D58" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>239</v>
+      </c>
+      <c r="B59" t="s">
         <v>240</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>243</v>
+      </c>
+      <c r="D59" t="s">
         <v>241</v>
-      </c>
-      <c r="C59" t="s">
-        <v>244</v>
-      </c>
-      <c r="D59" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B60" t="s">
+        <v>237</v>
+      </c>
+      <c r="C60" t="s">
+        <v>243</v>
+      </c>
+      <c r="D60" t="s">
         <v>238</v>
-      </c>
-      <c r="C60" t="s">
-        <v>244</v>
-      </c>
-      <c r="D60" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B61" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C61" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D61" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B62" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C62" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D62" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C63" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D63" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B64" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C64" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D64" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B65" t="s">
+        <v>195</v>
+      </c>
+      <c r="C65" t="s">
+        <v>254</v>
+      </c>
+      <c r="D65" t="s">
         <v>196</v>
-      </c>
-      <c r="C65" t="s">
-        <v>255</v>
-      </c>
-      <c r="D65" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B66" t="s">
+        <v>199</v>
+      </c>
+      <c r="C66" t="s">
+        <v>254</v>
+      </c>
+      <c r="D66" t="s">
         <v>200</v>
-      </c>
-      <c r="C66" t="s">
-        <v>255</v>
-      </c>
-      <c r="D66" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B67" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C67" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D67" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B68" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C68" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C69" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D70" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>60</v>
+      </c>
+      <c r="B71" t="s">
+        <v>65</v>
+      </c>
+      <c r="C71" t="s">
         <v>61</v>
       </c>
-      <c r="B71" t="s">
-        <v>66</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>62</v>
-      </c>
-      <c r="D71" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>91</v>
+      </c>
+      <c r="B72" t="s">
         <v>92</v>
       </c>
-      <c r="B72" t="s">
-        <v>93</v>
-      </c>
       <c r="C72" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D72" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C73" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D73" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B74" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C74" t="s">
+        <v>61</v>
+      </c>
+      <c r="D74" t="s">
         <v>62</v>
-      </c>
-      <c r="D74" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B75" t="s">
+        <v>67</v>
+      </c>
+      <c r="C75" t="s">
+        <v>61</v>
+      </c>
+      <c r="D75" t="s">
         <v>68</v>
-      </c>
-      <c r="C75" t="s">
-        <v>62</v>
-      </c>
-      <c r="D75" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B76" t="s">
+        <v>72</v>
+      </c>
+      <c r="C76" t="s">
+        <v>61</v>
+      </c>
+      <c r="D76" t="s">
         <v>73</v>
-      </c>
-      <c r="C76" t="s">
-        <v>62</v>
-      </c>
-      <c r="D76" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B77" t="s">
+        <v>76</v>
+      </c>
+      <c r="C77" t="s">
+        <v>61</v>
+      </c>
+      <c r="D77" t="s">
         <v>77</v>
-      </c>
-      <c r="C77" t="s">
-        <v>62</v>
-      </c>
-      <c r="D77" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B78" t="s">
+        <v>83</v>
+      </c>
+      <c r="C78" t="s">
+        <v>61</v>
+      </c>
+      <c r="D78" t="s">
         <v>84</v>
-      </c>
-      <c r="C78" t="s">
-        <v>62</v>
-      </c>
-      <c r="D78" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B79" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79" t="s">
+        <v>61</v>
+      </c>
+      <c r="D79" t="s">
         <v>90</v>
-      </c>
-      <c r="C79" t="s">
-        <v>62</v>
-      </c>
-      <c r="D79" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B80" t="s">
+        <v>94</v>
+      </c>
+      <c r="C80" t="s">
+        <v>61</v>
+      </c>
+      <c r="D80" t="s">
         <v>95</v>
-      </c>
-      <c r="C80" t="s">
-        <v>62</v>
-      </c>
-      <c r="D80" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B81" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C81" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D81" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C82" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D82" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
       </c>
       <c r="C83" t="s">
+        <v>61</v>
+      </c>
+      <c r="D83" t="s">
         <v>62</v>
-      </c>
-      <c r="D83" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B84" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C84" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D84" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B85" t="s">
+        <v>101</v>
+      </c>
+      <c r="C85" t="s">
+        <v>61</v>
+      </c>
+      <c r="D85" t="s">
         <v>102</v>
-      </c>
-      <c r="C85" t="s">
-        <v>62</v>
-      </c>
-      <c r="D85" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B86" t="s">
         <v>14</v>
       </c>
       <c r="C86" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D86" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B87" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C87" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D87" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C88" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D88" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B89" t="s">
         <v>14</v>
       </c>
       <c r="C89" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D89" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B90" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C90" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D90" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B91" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C91" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D91" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C92" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D92" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C93" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D93" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B94" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C94" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D94" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B95" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C95" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D95" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B96" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C96" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D96" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B97" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C97" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D97" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B98" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C98" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D98" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B99" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C99" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D99" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B100" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C100" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D100" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2637,13 +2637,13 @@
         <v>24</v>
       </c>
       <c r="B101" t="s">
+        <v>27</v>
+      </c>
+      <c r="C101" t="s">
+        <v>255</v>
+      </c>
+      <c r="D101" t="s">
         <v>28</v>
-      </c>
-      <c r="C101" t="s">
-        <v>256</v>
-      </c>
-      <c r="D101" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2651,13 +2651,13 @@
         <v>24</v>
       </c>
       <c r="B102" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C102" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D102" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2665,69 +2665,69 @@
         <v>24</v>
       </c>
       <c r="B103" t="s">
+        <v>103</v>
+      </c>
+      <c r="C103" t="s">
         <v>104</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
         <v>105</v>
-      </c>
-      <c r="D103" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B104" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C104" t="s">
+        <v>104</v>
+      </c>
+      <c r="D104" t="s">
         <v>105</v>
-      </c>
-      <c r="D104" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B105" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C105" t="s">
+        <v>104</v>
+      </c>
+      <c r="D105" t="s">
         <v>105</v>
-      </c>
-      <c r="D105" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B106" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C106" t="s">
+        <v>104</v>
+      </c>
+      <c r="D106" t="s">
         <v>105</v>
-      </c>
-      <c r="D106" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B107" t="s">
+        <v>111</v>
+      </c>
+      <c r="C107" t="s">
+        <v>104</v>
+      </c>
+      <c r="D107" t="s">
         <v>112</v>
-      </c>
-      <c r="C107" t="s">
-        <v>105</v>
-      </c>
-      <c r="D107" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2738,24 +2738,24 @@
         <v>25</v>
       </c>
       <c r="C108" t="s">
+        <v>268</v>
+      </c>
+      <c r="D108" t="s">
         <v>26</v>
-      </c>
-      <c r="D108" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B109" t="s">
+        <v>113</v>
+      </c>
+      <c r="C109" t="s">
         <v>114</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>115</v>
-      </c>
-      <c r="D109" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2791,97 +2791,97 @@
         <v>24</v>
       </c>
       <c r="B112" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C112" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D112" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B113" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C113" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D113" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B114" t="s">
         <v>11</v>
       </c>
       <c r="C114" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D114" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B115" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C115" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D115" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B116" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C116" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D116" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B117" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C117" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D117" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B118" t="s">
         <v>9</v>
       </c>
       <c r="C118" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D118" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -2900,198 +2900,198 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>190</v>
+      </c>
+      <c r="B120" t="s">
         <v>191</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" t="s">
         <v>192</v>
       </c>
-      <c r="C120" t="s">
-        <v>193</v>
-      </c>
       <c r="D120" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B121" t="s">
+        <v>193</v>
+      </c>
+      <c r="C121" t="s">
         <v>194</v>
       </c>
-      <c r="C121" t="s">
-        <v>195</v>
-      </c>
       <c r="D121" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B122" t="s">
+        <v>116</v>
+      </c>
+      <c r="C122" t="s">
         <v>117</v>
       </c>
-      <c r="C122" t="s">
-        <v>118</v>
-      </c>
       <c r="D122" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B123" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C123" t="s">
+        <v>117</v>
+      </c>
+      <c r="D123" t="s">
         <v>118</v>
-      </c>
-      <c r="D123" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B124" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C124" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D124" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B125" t="s">
+        <v>120</v>
+      </c>
+      <c r="C125" t="s">
+        <v>117</v>
+      </c>
+      <c r="D125" t="s">
         <v>121</v>
-      </c>
-      <c r="C125" t="s">
-        <v>118</v>
-      </c>
-      <c r="D125" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B126" t="s">
+        <v>122</v>
+      </c>
+      <c r="C126" t="s">
+        <v>117</v>
+      </c>
+      <c r="D126" t="s">
         <v>123</v>
-      </c>
-      <c r="C126" t="s">
-        <v>118</v>
-      </c>
-      <c r="D126" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B127" t="s">
+        <v>51</v>
+      </c>
+      <c r="C127" t="s">
         <v>52</v>
       </c>
-      <c r="C127" t="s">
+      <c r="D127" t="s">
         <v>53</v>
-      </c>
-      <c r="D127" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B128" t="s">
+        <v>54</v>
+      </c>
+      <c r="C128" t="s">
+        <v>52</v>
+      </c>
+      <c r="D128" t="s">
         <v>55</v>
-      </c>
-      <c r="C128" t="s">
-        <v>53</v>
-      </c>
-      <c r="D128" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B129" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C129" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D129" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B130" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C130" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D130" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B131" t="s">
+        <v>127</v>
+      </c>
+      <c r="C131" t="s">
         <v>128</v>
       </c>
-      <c r="C131" t="s">
+      <c r="D131" t="s">
         <v>129</v>
-      </c>
-      <c r="D131" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>259</v>
+      </c>
+      <c r="B132" t="s">
         <v>260</v>
       </c>
-      <c r="B132" t="s">
+      <c r="C132" t="s">
         <v>261</v>
       </c>
-      <c r="C132" t="s">
+      <c r="D132" t="s">
         <v>262</v>
-      </c>
-      <c r="D132" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B133" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C133" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D133" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding preview snippets to the mapping file
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21421"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3259C7B-17E7-4C99-B405-58EAD2E65096}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0175534A-4A60-436B-8AF8-460ADBA18AB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="345">
   <si>
     <t>Class</t>
   </si>
@@ -827,6 +827,234 @@
   </si>
   <si>
     <t>excel-range-used-range</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>suspendScreenUpdatingUntilNextSync</t>
+  </si>
+  <si>
+    <t>refreshData</t>
+  </si>
+  <si>
+    <t>getSelectedRanges</t>
+  </si>
+  <si>
+    <t>colorSelectedRanges</t>
+  </si>
+  <si>
+    <t>colorSpecifiedRanges</t>
+  </si>
+  <si>
+    <t>getRanges</t>
+  </si>
+  <si>
+    <t>getSpecialCells</t>
+  </si>
+  <si>
+    <t>colorAllLogicalAndTextRanges</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>rotation</t>
+  </si>
+  <si>
+    <t>createTriangle</t>
+  </si>
+  <si>
+    <t>ShapeCollection</t>
+  </si>
+  <si>
+    <t>addGeometricShape</t>
+  </si>
+  <si>
+    <t>createSmileyFace</t>
+  </si>
+  <si>
+    <t>fill</t>
+  </si>
+  <si>
+    <t>removeAll</t>
+  </si>
+  <si>
+    <t>copyFrom</t>
+  </si>
+  <si>
+    <t>copyFormula</t>
+  </si>
+  <si>
+    <t>find</t>
+  </si>
+  <si>
+    <t>findText</t>
+  </si>
+  <si>
+    <t>findOrNullObject</t>
+  </si>
+  <si>
+    <t>findTextWithNullCheck</t>
+  </si>
+  <si>
+    <t>findAllOrNullObject</t>
+  </si>
+  <si>
+    <t>findCompleted</t>
+  </si>
+  <si>
+    <t>addImage</t>
+  </si>
+  <si>
+    <t>readImageFromFile</t>
+  </si>
+  <si>
+    <t>excel-performance-optimization</t>
+  </si>
+  <si>
+    <t>excel-range-areas</t>
+  </si>
+  <si>
+    <t>excel-shape-create-and-delete</t>
+  </si>
+  <si>
+    <t>excel-range-copyfrom</t>
+  </si>
+  <si>
+    <t>excel-range-find</t>
+  </si>
+  <si>
+    <t>excel-worksheet-find-all</t>
+  </si>
+  <si>
+    <t>excel-shape-images</t>
+  </si>
+  <si>
+    <t>flipImage</t>
+  </si>
+  <si>
+    <t>incrementRotation</t>
+  </si>
+  <si>
+    <t>getImageFormat</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>writeOutImageString</t>
+  </si>
+  <si>
+    <t>saveAsPicture</t>
+  </si>
+  <si>
+    <t>insertSheets</t>
+  </si>
+  <si>
+    <t>addFromBase64</t>
+  </si>
+  <si>
+    <t>excel-workbook-insert-external-worksheets</t>
+  </si>
+  <si>
+    <t>incrementLeft</t>
+  </si>
+  <si>
+    <t>incrementTop</t>
+  </si>
+  <si>
+    <t>excel-shape-move-and-order</t>
+  </si>
+  <si>
+    <t>moveLeft</t>
+  </si>
+  <si>
+    <t>moveDown</t>
+  </si>
+  <si>
+    <t>scaleUp</t>
+  </si>
+  <si>
+    <t>moveZOrderDown</t>
+  </si>
+  <si>
+    <t>setZOrder</t>
+  </si>
+  <si>
+    <t>scaleHeight</t>
+  </si>
+  <si>
+    <t>scaleWidth</t>
+  </si>
+  <si>
+    <t>PageBreakCollection</t>
+  </si>
+  <si>
+    <t>excel-worksheet-page-layout</t>
+  </si>
+  <si>
+    <t>setPageBreaks</t>
+  </si>
+  <si>
+    <t>centerHorizontally</t>
+  </si>
+  <si>
+    <t>centerVertically</t>
+  </si>
+  <si>
+    <t>PageLayout</t>
+  </si>
+  <si>
+    <t>center</t>
+  </si>
+  <si>
+    <t>setPrintTitleRows</t>
+  </si>
+  <si>
+    <t>setPrintTitleRow</t>
+  </si>
+  <si>
+    <t>setPrintArea</t>
+  </si>
+  <si>
+    <t>orientation</t>
+  </si>
+  <si>
+    <t>deleteName</t>
+  </si>
+  <si>
+    <t>excel-range-remove-duplicates</t>
+  </si>
+  <si>
+    <t>removeDuplicates</t>
+  </si>
+  <si>
+    <t>uniqueRemaining</t>
+  </si>
+  <si>
+    <t>RemoveDuplicateResult</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>excel-workbook-save-and-close</t>
+  </si>
+  <si>
+    <t>saveWithoutPrompt</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>closeWithSave</t>
+  </si>
+  <si>
+    <t>createHexagon</t>
+  </si>
+  <si>
+    <t>changeOrientation</t>
   </si>
 </sst>
 </file>
@@ -905,10 +1133,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D133" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D133" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D131">
-    <sortCondition ref="C108"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D165" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D165" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D165">
+    <sortCondition ref="C1:C165"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1215,13 +1443,33 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="875" row="6">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{BDE84F77-942B-41ED-8015-10BF1F914B90}">
+  <we:reference id="wa104380862" version="1.5.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa104380862" version="1.5.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D133"/>
+  <dimension ref="A1:D165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K98" sqref="K98"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F156" sqref="F156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,7 +1477,7 @@
     <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1402,86 +1650,86 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>259</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>260</v>
       </c>
       <c r="C13" t="s">
-        <v>131</v>
+        <v>261</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>259</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
-        <v>131</v>
+        <v>261</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
         <v>131</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>134</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
         <v>131</v>
       </c>
       <c r="D16" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>131</v>
       </c>
       <c r="D17" t="s">
-        <v>265</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1489,7 +1737,7 @@
         <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
         <v>35</v>
@@ -1503,13 +1751,13 @@
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
         <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1517,27 +1765,27 @@
         <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
         <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1545,49 +1793,49 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
         <v>35</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
         <v>45</v>
@@ -1601,7 +1849,7 @@
         <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
         <v>45</v>
@@ -1612,30 +1860,30 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>222</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>221</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>218</v>
+        <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>217</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="B29" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C29" t="s">
         <v>218</v>
       </c>
       <c r="D29" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1643,83 +1891,83 @@
         <v>253</v>
       </c>
       <c r="B30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C30" t="s">
         <v>218</v>
       </c>
       <c r="D30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>190</v>
+        <v>253</v>
       </c>
       <c r="B31" t="s">
-        <v>157</v>
+        <v>220</v>
       </c>
       <c r="C31" t="s">
-        <v>158</v>
+        <v>218</v>
       </c>
       <c r="D31" t="s">
-        <v>159</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>190</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>158</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>249</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>250</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>251</v>
+        <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>252</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>249</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>250</v>
       </c>
       <c r="C34" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="D34" t="s">
-        <v>19</v>
+        <v>252</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>211</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>188</v>
       </c>
       <c r="C35" t="s">
-        <v>266</v>
+        <v>186</v>
       </c>
       <c r="D35" t="s">
-        <v>19</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1727,41 +1975,41 @@
         <v>211</v>
       </c>
       <c r="B36" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="C36" t="s">
         <v>186</v>
       </c>
       <c r="D36" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B37" t="s">
-        <v>167</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
         <v>186</v>
       </c>
       <c r="D37" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B38" t="s">
-        <v>106</v>
+        <v>171</v>
       </c>
       <c r="C38" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D38" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1769,7 +2017,7 @@
         <v>214</v>
       </c>
       <c r="B39" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="C39" t="s">
         <v>183</v>
@@ -1780,44 +2028,44 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B40" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C40" t="s">
         <v>183</v>
       </c>
       <c r="D40" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>213</v>
+        <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>188</v>
+        <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>183</v>
+        <v>266</v>
       </c>
       <c r="D41" t="s">
-        <v>187</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
         <v>266</v>
       </c>
       <c r="D42" t="s">
-        <v>174</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1825,27 +2073,27 @@
         <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C43" t="s">
         <v>266</v>
       </c>
       <c r="D43" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D44" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1881,55 +2129,55 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
       <c r="C47" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="D47" t="s">
-        <v>125</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>258</v>
+        <v>12</v>
       </c>
       <c r="D48" t="s">
-        <v>32</v>
+        <v>265</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>258</v>
+        <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>269</v>
       </c>
       <c r="B50" t="s">
-        <v>11</v>
+        <v>270</v>
       </c>
       <c r="C50" t="s">
-        <v>12</v>
+        <v>296</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>271</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2074,184 +2322,184 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B61" t="s">
-        <v>195</v>
+        <v>272</v>
       </c>
       <c r="C61" t="s">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="D61" t="s">
-        <v>197</v>
+        <v>273</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>206</v>
+        <v>47</v>
       </c>
       <c r="B62" t="s">
-        <v>199</v>
+        <v>275</v>
       </c>
       <c r="C62" t="s">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="D62" t="s">
-        <v>201</v>
+        <v>274</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>206</v>
+        <v>24</v>
       </c>
       <c r="B63" t="s">
-        <v>195</v>
+        <v>276</v>
       </c>
       <c r="C63" t="s">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="D63" t="s">
-        <v>204</v>
+        <v>277</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>206</v>
+        <v>87</v>
       </c>
       <c r="B64" t="s">
-        <v>199</v>
+        <v>86</v>
       </c>
       <c r="C64" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D64" t="s">
-        <v>205</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>207</v>
+        <v>87</v>
       </c>
       <c r="B65" t="s">
-        <v>195</v>
+        <v>69</v>
       </c>
       <c r="C65" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D65" t="s">
-        <v>196</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>207</v>
+        <v>60</v>
       </c>
       <c r="B66" t="s">
-        <v>199</v>
+        <v>65</v>
       </c>
       <c r="C66" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D66" t="s">
-        <v>200</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>207</v>
+        <v>91</v>
       </c>
       <c r="B67" t="s">
-        <v>195</v>
+        <v>92</v>
       </c>
       <c r="C67" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D67" t="s">
-        <v>202</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>207</v>
+        <v>91</v>
       </c>
       <c r="B68" t="s">
-        <v>199</v>
+        <v>81</v>
       </c>
       <c r="C68" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D68" t="s">
-        <v>203</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="B69" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="C69" t="s">
         <v>61</v>
       </c>
       <c r="D69" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="B70" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C70" t="s">
         <v>61</v>
       </c>
       <c r="D70" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B71" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C71" t="s">
         <v>61</v>
       </c>
       <c r="D71" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="B72" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C72" t="s">
         <v>61</v>
       </c>
       <c r="D72" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="B73" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C73" t="s">
         <v>61</v>
       </c>
       <c r="D73" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2259,13 +2507,13 @@
         <v>58</v>
       </c>
       <c r="B74" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="C74" t="s">
         <v>61</v>
       </c>
       <c r="D74" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2273,13 +2521,13 @@
         <v>58</v>
       </c>
       <c r="B75" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="C75" t="s">
         <v>61</v>
       </c>
       <c r="D75" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2287,13 +2535,13 @@
         <v>58</v>
       </c>
       <c r="B76" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C76" t="s">
         <v>61</v>
       </c>
       <c r="D76" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2301,231 +2549,231 @@
         <v>58</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="C77" t="s">
         <v>61</v>
       </c>
       <c r="D77" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B78" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C78" t="s">
         <v>61</v>
       </c>
       <c r="D78" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B79" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C79" t="s">
         <v>61</v>
       </c>
       <c r="D79" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B80" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="C80" t="s">
         <v>61</v>
       </c>
       <c r="D80" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="B81" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="C81" t="s">
         <v>61</v>
       </c>
       <c r="D81" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C82" t="s">
         <v>61</v>
       </c>
       <c r="D82" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B83" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="C83" t="s">
         <v>61</v>
       </c>
       <c r="D83" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B84" t="s">
-        <v>98</v>
+        <v>14</v>
       </c>
       <c r="C84" t="s">
         <v>61</v>
       </c>
       <c r="D84" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B85" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C85" t="s">
         <v>61</v>
       </c>
       <c r="D85" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="B86" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="C86" t="s">
         <v>61</v>
       </c>
       <c r="D86" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C87" t="s">
         <v>61</v>
       </c>
       <c r="D87" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B88" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C88" t="s">
         <v>61</v>
       </c>
       <c r="D88" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B89" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C89" t="s">
         <v>61</v>
       </c>
       <c r="D89" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B90" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C90" t="s">
         <v>61</v>
       </c>
       <c r="D90" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B91" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C91" t="s">
         <v>61</v>
       </c>
       <c r="D91" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="B92" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="C92" t="s">
         <v>61</v>
       </c>
       <c r="D92" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="B93" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C93" t="s">
         <v>61</v>
@@ -2536,562 +2784,1010 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B94" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C94" t="s">
         <v>61</v>
       </c>
       <c r="D94" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B95" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C95" t="s">
         <v>61</v>
       </c>
       <c r="D95" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="B96" t="s">
-        <v>65</v>
+        <v>286</v>
       </c>
       <c r="C96" t="s">
-        <v>61</v>
+        <v>299</v>
       </c>
       <c r="D96" t="s">
-        <v>77</v>
+        <v>287</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="B97" t="s">
-        <v>69</v>
+        <v>288</v>
       </c>
       <c r="C97" t="s">
-        <v>61</v>
+        <v>300</v>
       </c>
       <c r="D97" t="s">
-        <v>68</v>
+        <v>289</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="B98" t="s">
-        <v>69</v>
+        <v>290</v>
       </c>
       <c r="C98" t="s">
-        <v>61</v>
+        <v>300</v>
       </c>
       <c r="D98" t="s">
-        <v>95</v>
+        <v>291</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="B99" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C99" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="D99" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="C100" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="D100" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="C101" t="s">
-        <v>255</v>
+        <v>104</v>
       </c>
       <c r="D101" t="s">
-        <v>28</v>
+        <v>105</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="C102" t="s">
-        <v>255</v>
+        <v>104</v>
       </c>
       <c r="D102" t="s">
-        <v>28</v>
+        <v>105</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="B103" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C103" t="s">
         <v>104</v>
       </c>
       <c r="D103" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B104" t="s">
-        <v>106</v>
+        <v>27</v>
       </c>
       <c r="C104" t="s">
-        <v>104</v>
+        <v>255</v>
       </c>
       <c r="D104" t="s">
-        <v>105</v>
+        <v>28</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B105" t="s">
-        <v>107</v>
+        <v>29</v>
       </c>
       <c r="C105" t="s">
-        <v>104</v>
+        <v>255</v>
       </c>
       <c r="D105" t="s">
-        <v>105</v>
+        <v>28</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B106" t="s">
-        <v>109</v>
+        <v>335</v>
       </c>
       <c r="C106" t="s">
-        <v>104</v>
+        <v>334</v>
       </c>
       <c r="D106" t="s">
-        <v>105</v>
+        <v>333</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>100</v>
+        <v>337</v>
       </c>
       <c r="B107" t="s">
-        <v>111</v>
+        <v>336</v>
       </c>
       <c r="C107" t="s">
-        <v>104</v>
+        <v>334</v>
       </c>
       <c r="D107" t="s">
-        <v>112</v>
+        <v>333</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="C108" t="s">
-        <v>268</v>
+        <v>114</v>
       </c>
       <c r="D108" t="s">
-        <v>26</v>
+        <v>115</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>108</v>
+        <v>24</v>
       </c>
       <c r="B109" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="C109" t="s">
-        <v>114</v>
+        <v>268</v>
       </c>
       <c r="D109" t="s">
-        <v>115</v>
+        <v>26</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B110" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C110" t="s">
-        <v>21</v>
+        <v>258</v>
       </c>
       <c r="D110" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B111" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C111" t="s">
-        <v>21</v>
+        <v>258</v>
       </c>
       <c r="D111" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B112" t="s">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="C112" t="s">
-        <v>256</v>
+        <v>21</v>
       </c>
       <c r="D112" t="s">
-        <v>160</v>
+        <v>22</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>152</v>
+        <v>17</v>
       </c>
       <c r="B113" t="s">
-        <v>149</v>
+        <v>23</v>
       </c>
       <c r="C113" t="s">
-        <v>256</v>
+        <v>21</v>
       </c>
       <c r="D113" t="s">
-        <v>162</v>
+        <v>22</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>152</v>
+        <v>278</v>
       </c>
       <c r="B114" t="s">
-        <v>11</v>
+        <v>279</v>
       </c>
       <c r="C114" t="s">
-        <v>256</v>
+        <v>298</v>
       </c>
       <c r="D114" t="s">
-        <v>163</v>
+        <v>280</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>152</v>
+        <v>281</v>
       </c>
       <c r="B115" t="s">
-        <v>209</v>
+        <v>282</v>
       </c>
       <c r="C115" t="s">
-        <v>256</v>
+        <v>298</v>
       </c>
       <c r="D115" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>152</v>
+        <v>278</v>
       </c>
       <c r="B116" t="s">
-        <v>164</v>
+        <v>284</v>
       </c>
       <c r="C116" t="s">
-        <v>256</v>
+        <v>298</v>
       </c>
       <c r="D116" t="s">
-        <v>160</v>
+        <v>283</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B117" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C117" t="s">
-        <v>256</v>
+        <v>298</v>
       </c>
       <c r="D117" t="s">
-        <v>161</v>
+        <v>285</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>156</v>
+        <v>281</v>
       </c>
       <c r="B118" t="s">
-        <v>9</v>
+        <v>294</v>
       </c>
       <c r="C118" t="s">
-        <v>256</v>
+        <v>302</v>
       </c>
       <c r="D118" t="s">
-        <v>161</v>
+        <v>295</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>10</v>
+        <v>278</v>
       </c>
       <c r="B119" t="s">
-        <v>14</v>
+        <v>304</v>
       </c>
       <c r="C119" t="s">
-        <v>15</v>
+        <v>302</v>
       </c>
       <c r="D119" t="s">
-        <v>16</v>
+        <v>303</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>190</v>
+        <v>306</v>
       </c>
       <c r="B120" t="s">
-        <v>191</v>
+        <v>86</v>
       </c>
       <c r="C120" t="s">
-        <v>192</v>
+        <v>302</v>
       </c>
       <c r="D120" t="s">
-        <v>198</v>
+        <v>305</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>47</v>
+        <v>306</v>
       </c>
       <c r="B121" t="s">
-        <v>193</v>
+        <v>308</v>
       </c>
       <c r="C121" t="s">
-        <v>194</v>
+        <v>302</v>
       </c>
       <c r="D121" t="s">
-        <v>198</v>
+        <v>307</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>110</v>
+        <v>278</v>
       </c>
       <c r="B122" t="s">
-        <v>116</v>
+        <v>312</v>
       </c>
       <c r="C122" t="s">
-        <v>117</v>
+        <v>314</v>
       </c>
       <c r="D122" t="s">
-        <v>116</v>
+        <v>315</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>110</v>
+        <v>278</v>
       </c>
       <c r="B123" t="s">
-        <v>118</v>
+        <v>313</v>
       </c>
       <c r="C123" t="s">
-        <v>117</v>
+        <v>314</v>
       </c>
       <c r="D123" t="s">
-        <v>118</v>
+        <v>316</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>110</v>
+        <v>278</v>
       </c>
       <c r="B124" t="s">
-        <v>119</v>
+        <v>320</v>
       </c>
       <c r="C124" t="s">
-        <v>117</v>
+        <v>314</v>
       </c>
       <c r="D124" t="s">
-        <v>119</v>
+        <v>317</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>110</v>
+        <v>278</v>
       </c>
       <c r="B125" t="s">
-        <v>120</v>
+        <v>319</v>
       </c>
       <c r="C125" t="s">
-        <v>117</v>
+        <v>314</v>
       </c>
       <c r="D125" t="s">
-        <v>121</v>
+        <v>318</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>110</v>
+        <v>278</v>
       </c>
       <c r="B126" t="s">
-        <v>122</v>
+        <v>321</v>
       </c>
       <c r="C126" t="s">
-        <v>117</v>
+        <v>314</v>
       </c>
       <c r="D126" t="s">
-        <v>123</v>
+        <v>317</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B127" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="C127" t="s">
-        <v>52</v>
+        <v>256</v>
       </c>
       <c r="D127" t="s">
-        <v>53</v>
+        <v>160</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="B128" t="s">
-        <v>54</v>
+        <v>149</v>
       </c>
       <c r="C128" t="s">
-        <v>52</v>
+        <v>256</v>
       </c>
       <c r="D128" t="s">
-        <v>55</v>
+        <v>162</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>50</v>
+        <v>152</v>
       </c>
       <c r="B129" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="C129" t="s">
-        <v>52</v>
+        <v>256</v>
       </c>
       <c r="D129" t="s">
-        <v>55</v>
+        <v>163</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>50</v>
+        <v>152</v>
       </c>
       <c r="B130" t="s">
-        <v>59</v>
+        <v>209</v>
       </c>
       <c r="C130" t="s">
-        <v>52</v>
+        <v>256</v>
       </c>
       <c r="D130" t="s">
-        <v>55</v>
+        <v>165</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="B131" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="C131" t="s">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="D131" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>259</v>
+        <v>156</v>
       </c>
       <c r="B132" t="s">
-        <v>260</v>
+        <v>37</v>
       </c>
       <c r="C132" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D132" t="s">
-        <v>262</v>
+        <v>161</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>259</v>
+        <v>156</v>
       </c>
       <c r="B133" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="C133" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D133" t="s">
-        <v>263</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>10</v>
+      </c>
+      <c r="B134" t="s">
+        <v>14</v>
+      </c>
+      <c r="C134" t="s">
+        <v>15</v>
+      </c>
+      <c r="D134" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>206</v>
+      </c>
+      <c r="B135" t="s">
+        <v>195</v>
+      </c>
+      <c r="C135" t="s">
+        <v>254</v>
+      </c>
+      <c r="D135" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>206</v>
+      </c>
+      <c r="B136" t="s">
+        <v>199</v>
+      </c>
+      <c r="C136" t="s">
+        <v>254</v>
+      </c>
+      <c r="D136" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>206</v>
+      </c>
+      <c r="B137" t="s">
+        <v>195</v>
+      </c>
+      <c r="C137" t="s">
+        <v>254</v>
+      </c>
+      <c r="D137" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>206</v>
+      </c>
+      <c r="B138" t="s">
+        <v>199</v>
+      </c>
+      <c r="C138" t="s">
+        <v>254</v>
+      </c>
+      <c r="D138" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>207</v>
+      </c>
+      <c r="B139" t="s">
+        <v>195</v>
+      </c>
+      <c r="C139" t="s">
+        <v>254</v>
+      </c>
+      <c r="D139" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>207</v>
+      </c>
+      <c r="B140" t="s">
+        <v>199</v>
+      </c>
+      <c r="C140" t="s">
+        <v>254</v>
+      </c>
+      <c r="D140" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>207</v>
+      </c>
+      <c r="B141" t="s">
+        <v>195</v>
+      </c>
+      <c r="C141" t="s">
+        <v>254</v>
+      </c>
+      <c r="D141" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>207</v>
+      </c>
+      <c r="B142" t="s">
+        <v>199</v>
+      </c>
+      <c r="C142" t="s">
+        <v>254</v>
+      </c>
+      <c r="D142" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>190</v>
+      </c>
+      <c r="B143" t="s">
+        <v>191</v>
+      </c>
+      <c r="C143" t="s">
+        <v>192</v>
+      </c>
+      <c r="D143" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>50</v>
+      </c>
+      <c r="B144" t="s">
+        <v>310</v>
+      </c>
+      <c r="C144" t="s">
+        <v>311</v>
+      </c>
+      <c r="D144" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>190</v>
+      </c>
+      <c r="B145" t="s">
+        <v>338</v>
+      </c>
+      <c r="C145" t="s">
+        <v>339</v>
+      </c>
+      <c r="D145" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>190</v>
+      </c>
+      <c r="B146" t="s">
+        <v>341</v>
+      </c>
+      <c r="C146" t="s">
+        <v>339</v>
+      </c>
+      <c r="D146" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>47</v>
+      </c>
+      <c r="B147" t="s">
+        <v>193</v>
+      </c>
+      <c r="C147" t="s">
+        <v>194</v>
+      </c>
+      <c r="D147" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>47</v>
+      </c>
+      <c r="B148" t="s">
+        <v>292</v>
+      </c>
+      <c r="C148" t="s">
+        <v>301</v>
+      </c>
+      <c r="D148" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>110</v>
+      </c>
+      <c r="B149" t="s">
+        <v>116</v>
+      </c>
+      <c r="C149" t="s">
+        <v>117</v>
+      </c>
+      <c r="D149" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>110</v>
+      </c>
+      <c r="B150" t="s">
+        <v>118</v>
+      </c>
+      <c r="C150" t="s">
+        <v>117</v>
+      </c>
+      <c r="D150" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>110</v>
+      </c>
+      <c r="B151" t="s">
+        <v>119</v>
+      </c>
+      <c r="C151" t="s">
+        <v>117</v>
+      </c>
+      <c r="D151" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>110</v>
+      </c>
+      <c r="B152" t="s">
+        <v>120</v>
+      </c>
+      <c r="C152" t="s">
+        <v>117</v>
+      </c>
+      <c r="D152" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>110</v>
+      </c>
+      <c r="B153" t="s">
+        <v>122</v>
+      </c>
+      <c r="C153" t="s">
+        <v>117</v>
+      </c>
+      <c r="D153" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>47</v>
+      </c>
+      <c r="B154" t="s">
+        <v>125</v>
+      </c>
+      <c r="C154" t="s">
+        <v>257</v>
+      </c>
+      <c r="D154" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>322</v>
+      </c>
+      <c r="B155" t="s">
+        <v>9</v>
+      </c>
+      <c r="C155" t="s">
+        <v>323</v>
+      </c>
+      <c r="D155" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>327</v>
+      </c>
+      <c r="B156" t="s">
+        <v>325</v>
+      </c>
+      <c r="C156" t="s">
+        <v>323</v>
+      </c>
+      <c r="D156" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>327</v>
+      </c>
+      <c r="B157" t="s">
+        <v>326</v>
+      </c>
+      <c r="C157" t="s">
+        <v>323</v>
+      </c>
+      <c r="D157" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>327</v>
+      </c>
+      <c r="B158" t="s">
+        <v>329</v>
+      </c>
+      <c r="C158" t="s">
+        <v>323</v>
+      </c>
+      <c r="D158" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>327</v>
+      </c>
+      <c r="B159" t="s">
+        <v>331</v>
+      </c>
+      <c r="C159" t="s">
+        <v>323</v>
+      </c>
+      <c r="D159" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>327</v>
+      </c>
+      <c r="B160" t="s">
+        <v>332</v>
+      </c>
+      <c r="C160" t="s">
+        <v>323</v>
+      </c>
+      <c r="D160" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>47</v>
+      </c>
+      <c r="B161" t="s">
+        <v>51</v>
+      </c>
+      <c r="C161" t="s">
+        <v>52</v>
+      </c>
+      <c r="D161" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>47</v>
+      </c>
+      <c r="B162" t="s">
+        <v>54</v>
+      </c>
+      <c r="C162" t="s">
+        <v>52</v>
+      </c>
+      <c r="D162" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>50</v>
+      </c>
+      <c r="B163" t="s">
+        <v>57</v>
+      </c>
+      <c r="C163" t="s">
+        <v>52</v>
+      </c>
+      <c r="D163" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>50</v>
+      </c>
+      <c r="B164" t="s">
+        <v>59</v>
+      </c>
+      <c r="C164" t="s">
+        <v>52</v>
+      </c>
+      <c r="D164" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>47</v>
+      </c>
+      <c r="B165" t="s">
+        <v>127</v>
+      </c>
+      <c r="C165" t="s">
+        <v>128</v>
+      </c>
+      <c r="D165" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding preview snippets to the mapping file (#265)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21421"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3259C7B-17E7-4C99-B405-58EAD2E65096}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0175534A-4A60-436B-8AF8-460ADBA18AB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="22500" windowHeight="10785" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="345">
   <si>
     <t>Class</t>
   </si>
@@ -827,6 +827,234 @@
   </si>
   <si>
     <t>excel-range-used-range</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>suspendScreenUpdatingUntilNextSync</t>
+  </si>
+  <si>
+    <t>refreshData</t>
+  </si>
+  <si>
+    <t>getSelectedRanges</t>
+  </si>
+  <si>
+    <t>colorSelectedRanges</t>
+  </si>
+  <si>
+    <t>colorSpecifiedRanges</t>
+  </si>
+  <si>
+    <t>getRanges</t>
+  </si>
+  <si>
+    <t>getSpecialCells</t>
+  </si>
+  <si>
+    <t>colorAllLogicalAndTextRanges</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>rotation</t>
+  </si>
+  <si>
+    <t>createTriangle</t>
+  </si>
+  <si>
+    <t>ShapeCollection</t>
+  </si>
+  <si>
+    <t>addGeometricShape</t>
+  </si>
+  <si>
+    <t>createSmileyFace</t>
+  </si>
+  <si>
+    <t>fill</t>
+  </si>
+  <si>
+    <t>removeAll</t>
+  </si>
+  <si>
+    <t>copyFrom</t>
+  </si>
+  <si>
+    <t>copyFormula</t>
+  </si>
+  <si>
+    <t>find</t>
+  </si>
+  <si>
+    <t>findText</t>
+  </si>
+  <si>
+    <t>findOrNullObject</t>
+  </si>
+  <si>
+    <t>findTextWithNullCheck</t>
+  </si>
+  <si>
+    <t>findAllOrNullObject</t>
+  </si>
+  <si>
+    <t>findCompleted</t>
+  </si>
+  <si>
+    <t>addImage</t>
+  </si>
+  <si>
+    <t>readImageFromFile</t>
+  </si>
+  <si>
+    <t>excel-performance-optimization</t>
+  </si>
+  <si>
+    <t>excel-range-areas</t>
+  </si>
+  <si>
+    <t>excel-shape-create-and-delete</t>
+  </si>
+  <si>
+    <t>excel-range-copyfrom</t>
+  </si>
+  <si>
+    <t>excel-range-find</t>
+  </si>
+  <si>
+    <t>excel-worksheet-find-all</t>
+  </si>
+  <si>
+    <t>excel-shape-images</t>
+  </si>
+  <si>
+    <t>flipImage</t>
+  </si>
+  <si>
+    <t>incrementRotation</t>
+  </si>
+  <si>
+    <t>getImageFormat</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>writeOutImageString</t>
+  </si>
+  <si>
+    <t>saveAsPicture</t>
+  </si>
+  <si>
+    <t>insertSheets</t>
+  </si>
+  <si>
+    <t>addFromBase64</t>
+  </si>
+  <si>
+    <t>excel-workbook-insert-external-worksheets</t>
+  </si>
+  <si>
+    <t>incrementLeft</t>
+  </si>
+  <si>
+    <t>incrementTop</t>
+  </si>
+  <si>
+    <t>excel-shape-move-and-order</t>
+  </si>
+  <si>
+    <t>moveLeft</t>
+  </si>
+  <si>
+    <t>moveDown</t>
+  </si>
+  <si>
+    <t>scaleUp</t>
+  </si>
+  <si>
+    <t>moveZOrderDown</t>
+  </si>
+  <si>
+    <t>setZOrder</t>
+  </si>
+  <si>
+    <t>scaleHeight</t>
+  </si>
+  <si>
+    <t>scaleWidth</t>
+  </si>
+  <si>
+    <t>PageBreakCollection</t>
+  </si>
+  <si>
+    <t>excel-worksheet-page-layout</t>
+  </si>
+  <si>
+    <t>setPageBreaks</t>
+  </si>
+  <si>
+    <t>centerHorizontally</t>
+  </si>
+  <si>
+    <t>centerVertically</t>
+  </si>
+  <si>
+    <t>PageLayout</t>
+  </si>
+  <si>
+    <t>center</t>
+  </si>
+  <si>
+    <t>setPrintTitleRows</t>
+  </si>
+  <si>
+    <t>setPrintTitleRow</t>
+  </si>
+  <si>
+    <t>setPrintArea</t>
+  </si>
+  <si>
+    <t>orientation</t>
+  </si>
+  <si>
+    <t>deleteName</t>
+  </si>
+  <si>
+    <t>excel-range-remove-duplicates</t>
+  </si>
+  <si>
+    <t>removeDuplicates</t>
+  </si>
+  <si>
+    <t>uniqueRemaining</t>
+  </si>
+  <si>
+    <t>RemoveDuplicateResult</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>excel-workbook-save-and-close</t>
+  </si>
+  <si>
+    <t>saveWithoutPrompt</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>closeWithSave</t>
+  </si>
+  <si>
+    <t>createHexagon</t>
+  </si>
+  <si>
+    <t>changeOrientation</t>
   </si>
 </sst>
 </file>
@@ -905,10 +1133,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D133" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D133" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D131">
-    <sortCondition ref="C108"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D165" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D165" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D165">
+    <sortCondition ref="C1:C165"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1215,13 +1443,33 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="875" row="6">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{BDE84F77-942B-41ED-8015-10BF1F914B90}">
+  <we:reference id="wa104380862" version="1.5.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa104380862" version="1.5.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D133"/>
+  <dimension ref="A1:D165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K98" sqref="K98"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F156" sqref="F156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,7 +1477,7 @@
     <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1402,86 +1650,86 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>259</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>260</v>
       </c>
       <c r="C13" t="s">
-        <v>131</v>
+        <v>261</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>259</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
-        <v>131</v>
+        <v>261</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
         <v>131</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>134</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
         <v>131</v>
       </c>
       <c r="D16" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>131</v>
       </c>
       <c r="D17" t="s">
-        <v>265</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1489,7 +1737,7 @@
         <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
         <v>35</v>
@@ -1503,13 +1751,13 @@
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
         <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1517,27 +1765,27 @@
         <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
         <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1545,49 +1793,49 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
         <v>35</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
         <v>45</v>
@@ -1601,7 +1849,7 @@
         <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
         <v>45</v>
@@ -1612,30 +1860,30 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>222</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>221</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>218</v>
+        <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>217</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="B29" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C29" t="s">
         <v>218</v>
       </c>
       <c r="D29" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1643,83 +1891,83 @@
         <v>253</v>
       </c>
       <c r="B30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C30" t="s">
         <v>218</v>
       </c>
       <c r="D30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>190</v>
+        <v>253</v>
       </c>
       <c r="B31" t="s">
-        <v>157</v>
+        <v>220</v>
       </c>
       <c r="C31" t="s">
-        <v>158</v>
+        <v>218</v>
       </c>
       <c r="D31" t="s">
-        <v>159</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>190</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>158</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>249</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>250</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>251</v>
+        <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>252</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>249</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>250</v>
       </c>
       <c r="C34" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="D34" t="s">
-        <v>19</v>
+        <v>252</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>211</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>188</v>
       </c>
       <c r="C35" t="s">
-        <v>266</v>
+        <v>186</v>
       </c>
       <c r="D35" t="s">
-        <v>19</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1727,41 +1975,41 @@
         <v>211</v>
       </c>
       <c r="B36" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="C36" t="s">
         <v>186</v>
       </c>
       <c r="D36" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B37" t="s">
-        <v>167</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
         <v>186</v>
       </c>
       <c r="D37" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B38" t="s">
-        <v>106</v>
+        <v>171</v>
       </c>
       <c r="C38" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D38" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1769,7 +2017,7 @@
         <v>214</v>
       </c>
       <c r="B39" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="C39" t="s">
         <v>183</v>
@@ -1780,44 +2028,44 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B40" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C40" t="s">
         <v>183</v>
       </c>
       <c r="D40" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>213</v>
+        <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>188</v>
+        <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>183</v>
+        <v>266</v>
       </c>
       <c r="D41" t="s">
-        <v>187</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
         <v>266</v>
       </c>
       <c r="D42" t="s">
-        <v>174</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1825,27 +2073,27 @@
         <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C43" t="s">
         <v>266</v>
       </c>
       <c r="D43" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D44" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1881,55 +2129,55 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
       <c r="C47" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="D47" t="s">
-        <v>125</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>258</v>
+        <v>12</v>
       </c>
       <c r="D48" t="s">
-        <v>32</v>
+        <v>265</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>258</v>
+        <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>269</v>
       </c>
       <c r="B50" t="s">
-        <v>11</v>
+        <v>270</v>
       </c>
       <c r="C50" t="s">
-        <v>12</v>
+        <v>296</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>271</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2074,184 +2322,184 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B61" t="s">
-        <v>195</v>
+        <v>272</v>
       </c>
       <c r="C61" t="s">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="D61" t="s">
-        <v>197</v>
+        <v>273</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>206</v>
+        <v>47</v>
       </c>
       <c r="B62" t="s">
-        <v>199</v>
+        <v>275</v>
       </c>
       <c r="C62" t="s">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="D62" t="s">
-        <v>201</v>
+        <v>274</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>206</v>
+        <v>24</v>
       </c>
       <c r="B63" t="s">
-        <v>195</v>
+        <v>276</v>
       </c>
       <c r="C63" t="s">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="D63" t="s">
-        <v>204</v>
+        <v>277</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>206</v>
+        <v>87</v>
       </c>
       <c r="B64" t="s">
-        <v>199</v>
+        <v>86</v>
       </c>
       <c r="C64" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D64" t="s">
-        <v>205</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>207</v>
+        <v>87</v>
       </c>
       <c r="B65" t="s">
-        <v>195</v>
+        <v>69</v>
       </c>
       <c r="C65" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D65" t="s">
-        <v>196</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>207</v>
+        <v>60</v>
       </c>
       <c r="B66" t="s">
-        <v>199</v>
+        <v>65</v>
       </c>
       <c r="C66" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D66" t="s">
-        <v>200</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>207</v>
+        <v>91</v>
       </c>
       <c r="B67" t="s">
-        <v>195</v>
+        <v>92</v>
       </c>
       <c r="C67" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D67" t="s">
-        <v>202</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>207</v>
+        <v>91</v>
       </c>
       <c r="B68" t="s">
-        <v>199</v>
+        <v>81</v>
       </c>
       <c r="C68" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D68" t="s">
-        <v>203</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="B69" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="C69" t="s">
         <v>61</v>
       </c>
       <c r="D69" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="B70" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C70" t="s">
         <v>61</v>
       </c>
       <c r="D70" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B71" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C71" t="s">
         <v>61</v>
       </c>
       <c r="D71" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="B72" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C72" t="s">
         <v>61</v>
       </c>
       <c r="D72" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="B73" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C73" t="s">
         <v>61</v>
       </c>
       <c r="D73" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2259,13 +2507,13 @@
         <v>58</v>
       </c>
       <c r="B74" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="C74" t="s">
         <v>61</v>
       </c>
       <c r="D74" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2273,13 +2521,13 @@
         <v>58</v>
       </c>
       <c r="B75" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="C75" t="s">
         <v>61</v>
       </c>
       <c r="D75" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2287,13 +2535,13 @@
         <v>58</v>
       </c>
       <c r="B76" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C76" t="s">
         <v>61</v>
       </c>
       <c r="D76" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2301,231 +2549,231 @@
         <v>58</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="C77" t="s">
         <v>61</v>
       </c>
       <c r="D77" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B78" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C78" t="s">
         <v>61</v>
       </c>
       <c r="D78" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B79" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C79" t="s">
         <v>61</v>
       </c>
       <c r="D79" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B80" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="C80" t="s">
         <v>61</v>
       </c>
       <c r="D80" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="B81" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="C81" t="s">
         <v>61</v>
       </c>
       <c r="D81" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C82" t="s">
         <v>61</v>
       </c>
       <c r="D82" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B83" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="C83" t="s">
         <v>61</v>
       </c>
       <c r="D83" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B84" t="s">
-        <v>98</v>
+        <v>14</v>
       </c>
       <c r="C84" t="s">
         <v>61</v>
       </c>
       <c r="D84" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B85" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C85" t="s">
         <v>61</v>
       </c>
       <c r="D85" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="B86" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="C86" t="s">
         <v>61</v>
       </c>
       <c r="D86" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C87" t="s">
         <v>61</v>
       </c>
       <c r="D87" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B88" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C88" t="s">
         <v>61</v>
       </c>
       <c r="D88" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B89" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C89" t="s">
         <v>61</v>
       </c>
       <c r="D89" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B90" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C90" t="s">
         <v>61</v>
       </c>
       <c r="D90" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B91" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C91" t="s">
         <v>61</v>
       </c>
       <c r="D91" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="B92" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="C92" t="s">
         <v>61</v>
       </c>
       <c r="D92" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="B93" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C93" t="s">
         <v>61</v>
@@ -2536,562 +2784,1010 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B94" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C94" t="s">
         <v>61</v>
       </c>
       <c r="D94" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B95" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C95" t="s">
         <v>61</v>
       </c>
       <c r="D95" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="B96" t="s">
-        <v>65</v>
+        <v>286</v>
       </c>
       <c r="C96" t="s">
-        <v>61</v>
+        <v>299</v>
       </c>
       <c r="D96" t="s">
-        <v>77</v>
+        <v>287</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="B97" t="s">
-        <v>69</v>
+        <v>288</v>
       </c>
       <c r="C97" t="s">
-        <v>61</v>
+        <v>300</v>
       </c>
       <c r="D97" t="s">
-        <v>68</v>
+        <v>289</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="B98" t="s">
-        <v>69</v>
+        <v>290</v>
       </c>
       <c r="C98" t="s">
-        <v>61</v>
+        <v>300</v>
       </c>
       <c r="D98" t="s">
-        <v>95</v>
+        <v>291</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="B99" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C99" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="D99" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="C100" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="D100" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="C101" t="s">
-        <v>255</v>
+        <v>104</v>
       </c>
       <c r="D101" t="s">
-        <v>28</v>
+        <v>105</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="C102" t="s">
-        <v>255</v>
+        <v>104</v>
       </c>
       <c r="D102" t="s">
-        <v>28</v>
+        <v>105</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="B103" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C103" t="s">
         <v>104</v>
       </c>
       <c r="D103" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B104" t="s">
-        <v>106</v>
+        <v>27</v>
       </c>
       <c r="C104" t="s">
-        <v>104</v>
+        <v>255</v>
       </c>
       <c r="D104" t="s">
-        <v>105</v>
+        <v>28</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B105" t="s">
-        <v>107</v>
+        <v>29</v>
       </c>
       <c r="C105" t="s">
-        <v>104</v>
+        <v>255</v>
       </c>
       <c r="D105" t="s">
-        <v>105</v>
+        <v>28</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B106" t="s">
-        <v>109</v>
+        <v>335</v>
       </c>
       <c r="C106" t="s">
-        <v>104</v>
+        <v>334</v>
       </c>
       <c r="D106" t="s">
-        <v>105</v>
+        <v>333</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>100</v>
+        <v>337</v>
       </c>
       <c r="B107" t="s">
-        <v>111</v>
+        <v>336</v>
       </c>
       <c r="C107" t="s">
-        <v>104</v>
+        <v>334</v>
       </c>
       <c r="D107" t="s">
-        <v>112</v>
+        <v>333</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="C108" t="s">
-        <v>268</v>
+        <v>114</v>
       </c>
       <c r="D108" t="s">
-        <v>26</v>
+        <v>115</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>108</v>
+        <v>24</v>
       </c>
       <c r="B109" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="C109" t="s">
-        <v>114</v>
+        <v>268</v>
       </c>
       <c r="D109" t="s">
-        <v>115</v>
+        <v>26</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B110" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C110" t="s">
-        <v>21</v>
+        <v>258</v>
       </c>
       <c r="D110" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B111" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C111" t="s">
-        <v>21</v>
+        <v>258</v>
       </c>
       <c r="D111" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B112" t="s">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="C112" t="s">
-        <v>256</v>
+        <v>21</v>
       </c>
       <c r="D112" t="s">
-        <v>160</v>
+        <v>22</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>152</v>
+        <v>17</v>
       </c>
       <c r="B113" t="s">
-        <v>149</v>
+        <v>23</v>
       </c>
       <c r="C113" t="s">
-        <v>256</v>
+        <v>21</v>
       </c>
       <c r="D113" t="s">
-        <v>162</v>
+        <v>22</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>152</v>
+        <v>278</v>
       </c>
       <c r="B114" t="s">
-        <v>11</v>
+        <v>279</v>
       </c>
       <c r="C114" t="s">
-        <v>256</v>
+        <v>298</v>
       </c>
       <c r="D114" t="s">
-        <v>163</v>
+        <v>280</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>152</v>
+        <v>281</v>
       </c>
       <c r="B115" t="s">
-        <v>209</v>
+        <v>282</v>
       </c>
       <c r="C115" t="s">
-        <v>256</v>
+        <v>298</v>
       </c>
       <c r="D115" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>152</v>
+        <v>278</v>
       </c>
       <c r="B116" t="s">
-        <v>164</v>
+        <v>284</v>
       </c>
       <c r="C116" t="s">
-        <v>256</v>
+        <v>298</v>
       </c>
       <c r="D116" t="s">
-        <v>160</v>
+        <v>283</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B117" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C117" t="s">
-        <v>256</v>
+        <v>298</v>
       </c>
       <c r="D117" t="s">
-        <v>161</v>
+        <v>285</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>156</v>
+        <v>281</v>
       </c>
       <c r="B118" t="s">
-        <v>9</v>
+        <v>294</v>
       </c>
       <c r="C118" t="s">
-        <v>256</v>
+        <v>302</v>
       </c>
       <c r="D118" t="s">
-        <v>161</v>
+        <v>295</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>10</v>
+        <v>278</v>
       </c>
       <c r="B119" t="s">
-        <v>14</v>
+        <v>304</v>
       </c>
       <c r="C119" t="s">
-        <v>15</v>
+        <v>302</v>
       </c>
       <c r="D119" t="s">
-        <v>16</v>
+        <v>303</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>190</v>
+        <v>306</v>
       </c>
       <c r="B120" t="s">
-        <v>191</v>
+        <v>86</v>
       </c>
       <c r="C120" t="s">
-        <v>192</v>
+        <v>302</v>
       </c>
       <c r="D120" t="s">
-        <v>198</v>
+        <v>305</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>47</v>
+        <v>306</v>
       </c>
       <c r="B121" t="s">
-        <v>193</v>
+        <v>308</v>
       </c>
       <c r="C121" t="s">
-        <v>194</v>
+        <v>302</v>
       </c>
       <c r="D121" t="s">
-        <v>198</v>
+        <v>307</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>110</v>
+        <v>278</v>
       </c>
       <c r="B122" t="s">
-        <v>116</v>
+        <v>312</v>
       </c>
       <c r="C122" t="s">
-        <v>117</v>
+        <v>314</v>
       </c>
       <c r="D122" t="s">
-        <v>116</v>
+        <v>315</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>110</v>
+        <v>278</v>
       </c>
       <c r="B123" t="s">
-        <v>118</v>
+        <v>313</v>
       </c>
       <c r="C123" t="s">
-        <v>117</v>
+        <v>314</v>
       </c>
       <c r="D123" t="s">
-        <v>118</v>
+        <v>316</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>110</v>
+        <v>278</v>
       </c>
       <c r="B124" t="s">
-        <v>119</v>
+        <v>320</v>
       </c>
       <c r="C124" t="s">
-        <v>117</v>
+        <v>314</v>
       </c>
       <c r="D124" t="s">
-        <v>119</v>
+        <v>317</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>110</v>
+        <v>278</v>
       </c>
       <c r="B125" t="s">
-        <v>120</v>
+        <v>319</v>
       </c>
       <c r="C125" t="s">
-        <v>117</v>
+        <v>314</v>
       </c>
       <c r="D125" t="s">
-        <v>121</v>
+        <v>318</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>110</v>
+        <v>278</v>
       </c>
       <c r="B126" t="s">
-        <v>122</v>
+        <v>321</v>
       </c>
       <c r="C126" t="s">
-        <v>117</v>
+        <v>314</v>
       </c>
       <c r="D126" t="s">
-        <v>123</v>
+        <v>317</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B127" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="C127" t="s">
-        <v>52</v>
+        <v>256</v>
       </c>
       <c r="D127" t="s">
-        <v>53</v>
+        <v>160</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="B128" t="s">
-        <v>54</v>
+        <v>149</v>
       </c>
       <c r="C128" t="s">
-        <v>52</v>
+        <v>256</v>
       </c>
       <c r="D128" t="s">
-        <v>55</v>
+        <v>162</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>50</v>
+        <v>152</v>
       </c>
       <c r="B129" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="C129" t="s">
-        <v>52</v>
+        <v>256</v>
       </c>
       <c r="D129" t="s">
-        <v>55</v>
+        <v>163</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>50</v>
+        <v>152</v>
       </c>
       <c r="B130" t="s">
-        <v>59</v>
+        <v>209</v>
       </c>
       <c r="C130" t="s">
-        <v>52</v>
+        <v>256</v>
       </c>
       <c r="D130" t="s">
-        <v>55</v>
+        <v>165</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="B131" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="C131" t="s">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="D131" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>259</v>
+        <v>156</v>
       </c>
       <c r="B132" t="s">
-        <v>260</v>
+        <v>37</v>
       </c>
       <c r="C132" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D132" t="s">
-        <v>262</v>
+        <v>161</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>259</v>
+        <v>156</v>
       </c>
       <c r="B133" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="C133" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D133" t="s">
-        <v>263</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>10</v>
+      </c>
+      <c r="B134" t="s">
+        <v>14</v>
+      </c>
+      <c r="C134" t="s">
+        <v>15</v>
+      </c>
+      <c r="D134" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>206</v>
+      </c>
+      <c r="B135" t="s">
+        <v>195</v>
+      </c>
+      <c r="C135" t="s">
+        <v>254</v>
+      </c>
+      <c r="D135" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>206</v>
+      </c>
+      <c r="B136" t="s">
+        <v>199</v>
+      </c>
+      <c r="C136" t="s">
+        <v>254</v>
+      </c>
+      <c r="D136" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>206</v>
+      </c>
+      <c r="B137" t="s">
+        <v>195</v>
+      </c>
+      <c r="C137" t="s">
+        <v>254</v>
+      </c>
+      <c r="D137" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>206</v>
+      </c>
+      <c r="B138" t="s">
+        <v>199</v>
+      </c>
+      <c r="C138" t="s">
+        <v>254</v>
+      </c>
+      <c r="D138" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>207</v>
+      </c>
+      <c r="B139" t="s">
+        <v>195</v>
+      </c>
+      <c r="C139" t="s">
+        <v>254</v>
+      </c>
+      <c r="D139" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>207</v>
+      </c>
+      <c r="B140" t="s">
+        <v>199</v>
+      </c>
+      <c r="C140" t="s">
+        <v>254</v>
+      </c>
+      <c r="D140" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>207</v>
+      </c>
+      <c r="B141" t="s">
+        <v>195</v>
+      </c>
+      <c r="C141" t="s">
+        <v>254</v>
+      </c>
+      <c r="D141" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>207</v>
+      </c>
+      <c r="B142" t="s">
+        <v>199</v>
+      </c>
+      <c r="C142" t="s">
+        <v>254</v>
+      </c>
+      <c r="D142" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>190</v>
+      </c>
+      <c r="B143" t="s">
+        <v>191</v>
+      </c>
+      <c r="C143" t="s">
+        <v>192</v>
+      </c>
+      <c r="D143" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>50</v>
+      </c>
+      <c r="B144" t="s">
+        <v>310</v>
+      </c>
+      <c r="C144" t="s">
+        <v>311</v>
+      </c>
+      <c r="D144" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>190</v>
+      </c>
+      <c r="B145" t="s">
+        <v>338</v>
+      </c>
+      <c r="C145" t="s">
+        <v>339</v>
+      </c>
+      <c r="D145" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>190</v>
+      </c>
+      <c r="B146" t="s">
+        <v>341</v>
+      </c>
+      <c r="C146" t="s">
+        <v>339</v>
+      </c>
+      <c r="D146" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>47</v>
+      </c>
+      <c r="B147" t="s">
+        <v>193</v>
+      </c>
+      <c r="C147" t="s">
+        <v>194</v>
+      </c>
+      <c r="D147" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>47</v>
+      </c>
+      <c r="B148" t="s">
+        <v>292</v>
+      </c>
+      <c r="C148" t="s">
+        <v>301</v>
+      </c>
+      <c r="D148" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>110</v>
+      </c>
+      <c r="B149" t="s">
+        <v>116</v>
+      </c>
+      <c r="C149" t="s">
+        <v>117</v>
+      </c>
+      <c r="D149" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>110</v>
+      </c>
+      <c r="B150" t="s">
+        <v>118</v>
+      </c>
+      <c r="C150" t="s">
+        <v>117</v>
+      </c>
+      <c r="D150" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>110</v>
+      </c>
+      <c r="B151" t="s">
+        <v>119</v>
+      </c>
+      <c r="C151" t="s">
+        <v>117</v>
+      </c>
+      <c r="D151" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>110</v>
+      </c>
+      <c r="B152" t="s">
+        <v>120</v>
+      </c>
+      <c r="C152" t="s">
+        <v>117</v>
+      </c>
+      <c r="D152" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>110</v>
+      </c>
+      <c r="B153" t="s">
+        <v>122</v>
+      </c>
+      <c r="C153" t="s">
+        <v>117</v>
+      </c>
+      <c r="D153" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>47</v>
+      </c>
+      <c r="B154" t="s">
+        <v>125</v>
+      </c>
+      <c r="C154" t="s">
+        <v>257</v>
+      </c>
+      <c r="D154" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>322</v>
+      </c>
+      <c r="B155" t="s">
+        <v>9</v>
+      </c>
+      <c r="C155" t="s">
+        <v>323</v>
+      </c>
+      <c r="D155" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>327</v>
+      </c>
+      <c r="B156" t="s">
+        <v>325</v>
+      </c>
+      <c r="C156" t="s">
+        <v>323</v>
+      </c>
+      <c r="D156" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>327</v>
+      </c>
+      <c r="B157" t="s">
+        <v>326</v>
+      </c>
+      <c r="C157" t="s">
+        <v>323</v>
+      </c>
+      <c r="D157" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>327</v>
+      </c>
+      <c r="B158" t="s">
+        <v>329</v>
+      </c>
+      <c r="C158" t="s">
+        <v>323</v>
+      </c>
+      <c r="D158" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>327</v>
+      </c>
+      <c r="B159" t="s">
+        <v>331</v>
+      </c>
+      <c r="C159" t="s">
+        <v>323</v>
+      </c>
+      <c r="D159" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>327</v>
+      </c>
+      <c r="B160" t="s">
+        <v>332</v>
+      </c>
+      <c r="C160" t="s">
+        <v>323</v>
+      </c>
+      <c r="D160" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>47</v>
+      </c>
+      <c r="B161" t="s">
+        <v>51</v>
+      </c>
+      <c r="C161" t="s">
+        <v>52</v>
+      </c>
+      <c r="D161" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>47</v>
+      </c>
+      <c r="B162" t="s">
+        <v>54</v>
+      </c>
+      <c r="C162" t="s">
+        <v>52</v>
+      </c>
+      <c r="D162" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>50</v>
+      </c>
+      <c r="B163" t="s">
+        <v>57</v>
+      </c>
+      <c r="C163" t="s">
+        <v>52</v>
+      </c>
+      <c r="D163" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>50</v>
+      </c>
+      <c r="B164" t="s">
+        <v>59</v>
+      </c>
+      <c r="C164" t="s">
+        <v>52</v>
+      </c>
+      <c r="D164" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>47</v>
+      </c>
+      <c r="B165" t="s">
+        <v>127</v>
+      </c>
+      <c r="C165" t="s">
+        <v>128</v>
+      </c>
+      <c r="D165" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing mislabeled snippet mappings
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21421"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0175534A-4A60-436B-8AF8-460ADBA18AB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B13E8A5-864C-43B7-BD89-0E538008A445}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -1033,9 +1033,6 @@
     <t>uniqueRemaining</t>
   </si>
   <si>
-    <t>RemoveDuplicateResult</t>
-  </si>
-  <si>
     <t>save</t>
   </si>
   <si>
@@ -1055,6 +1052,9 @@
   </si>
   <si>
     <t>changeOrientation</t>
+  </si>
+  <si>
+    <t>RemoveDuplicatesResult</t>
   </si>
 </sst>
 </file>
@@ -1468,8 +1468,8 @@
   <dimension ref="A1:D165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F156" sqref="F156"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2966,7 +2966,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="B107" t="s">
         <v>336</v>
@@ -3087,7 +3087,7 @@
         <v>298</v>
       </c>
       <c r="D115" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3162,7 +3162,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>306</v>
+        <v>278</v>
       </c>
       <c r="B121" t="s">
         <v>308</v>
@@ -3501,13 +3501,13 @@
         <v>190</v>
       </c>
       <c r="B145" t="s">
+        <v>337</v>
+      </c>
+      <c r="C145" t="s">
         <v>338</v>
       </c>
-      <c r="C145" t="s">
+      <c r="D145" t="s">
         <v>339</v>
-      </c>
-      <c r="D145" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3515,13 +3515,13 @@
         <v>190</v>
       </c>
       <c r="B146" t="s">
+        <v>340</v>
+      </c>
+      <c r="C146" t="s">
+        <v>338</v>
+      </c>
+      <c r="D146" t="s">
         <v>341</v>
-      </c>
-      <c r="C146" t="s">
-        <v>339</v>
-      </c>
-      <c r="D146" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -3717,7 +3717,7 @@
         <v>323</v>
       </c>
       <c r="D160" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Snippet for textboxes and shapes
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21421"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B13E8A5-864C-43B7-BD89-0E538008A445}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC56AB44-34AF-4C53-B0E7-E284589FD2A5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="350">
   <si>
     <t>Class</t>
   </si>
@@ -1055,6 +1055,21 @@
   </si>
   <si>
     <t>RemoveDuplicatesResult</t>
+  </si>
+  <si>
+    <t>addTextBox</t>
+  </si>
+  <si>
+    <t>excel-shape-textboxes</t>
+  </si>
+  <si>
+    <t>createTextbox</t>
+  </si>
+  <si>
+    <t>deleteText</t>
+  </si>
+  <si>
+    <t>TextFrame</t>
   </si>
 </sst>
 </file>
@@ -1133,8 +1148,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D165" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D165" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D167" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D167" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D165">
     <sortCondition ref="C1:C165"/>
   </sortState>
@@ -1465,11 +1480,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D165"/>
+  <dimension ref="A1:D167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B167" sqref="B167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3790,6 +3805,34 @@
         <v>129</v>
       </c>
     </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>281</v>
+      </c>
+      <c r="B166" t="s">
+        <v>345</v>
+      </c>
+      <c r="C166" t="s">
+        <v>346</v>
+      </c>
+      <c r="D166" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>349</v>
+      </c>
+      <c r="B167" t="s">
+        <v>348</v>
+      </c>
+      <c r="C167" t="s">
+        <v>346</v>
+      </c>
+      <c r="D167" t="s">
+        <v>348</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[excel] (Shapes) Textbox and shape text snippet (#266)
* Fixing mislabeled snippet mappings

* Snippet for textboxes and shapes
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21421"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0175534A-4A60-436B-8AF8-460ADBA18AB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC56AB44-34AF-4C53-B0E7-E284589FD2A5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="350">
   <si>
     <t>Class</t>
   </si>
@@ -1033,9 +1033,6 @@
     <t>uniqueRemaining</t>
   </si>
   <si>
-    <t>RemoveDuplicateResult</t>
-  </si>
-  <si>
     <t>save</t>
   </si>
   <si>
@@ -1055,6 +1052,24 @@
   </si>
   <si>
     <t>changeOrientation</t>
+  </si>
+  <si>
+    <t>RemoveDuplicatesResult</t>
+  </si>
+  <si>
+    <t>addTextBox</t>
+  </si>
+  <si>
+    <t>excel-shape-textboxes</t>
+  </si>
+  <si>
+    <t>createTextbox</t>
+  </si>
+  <si>
+    <t>deleteText</t>
+  </si>
+  <si>
+    <t>TextFrame</t>
   </si>
 </sst>
 </file>
@@ -1133,8 +1148,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D165" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D165" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D167" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D167" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D165">
     <sortCondition ref="C1:C165"/>
   </sortState>
@@ -1465,11 +1480,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D165"/>
+  <dimension ref="A1:D167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F156" sqref="F156"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B167" sqref="B167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2966,7 +2981,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="B107" t="s">
         <v>336</v>
@@ -3087,7 +3102,7 @@
         <v>298</v>
       </c>
       <c r="D115" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3162,7 +3177,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>306</v>
+        <v>278</v>
       </c>
       <c r="B121" t="s">
         <v>308</v>
@@ -3501,13 +3516,13 @@
         <v>190</v>
       </c>
       <c r="B145" t="s">
+        <v>337</v>
+      </c>
+      <c r="C145" t="s">
         <v>338</v>
       </c>
-      <c r="C145" t="s">
+      <c r="D145" t="s">
         <v>339</v>
-      </c>
-      <c r="D145" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3515,13 +3530,13 @@
         <v>190</v>
       </c>
       <c r="B146" t="s">
+        <v>340</v>
+      </c>
+      <c r="C146" t="s">
+        <v>338</v>
+      </c>
+      <c r="D146" t="s">
         <v>341</v>
-      </c>
-      <c r="C146" t="s">
-        <v>339</v>
-      </c>
-      <c r="D146" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -3717,7 +3732,7 @@
         <v>323</v>
       </c>
       <c r="D160" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -3788,6 +3803,34 @@
       </c>
       <c r="D165" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>281</v>
+      </c>
+      <c r="B166" t="s">
+        <v>345</v>
+      </c>
+      <c r="C166" t="s">
+        <v>346</v>
+      </c>
+      <c r="D166" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>349</v>
+      </c>
+      <c r="B167" t="s">
+        <v>348</v>
+      </c>
+      <c r="C167" t="s">
+        <v>346</v>
+      </c>
+      <c r="D167" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Snippet for line-type shapes
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC56AB44-34AF-4C53-B0E7-E284589FD2A5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9071016E-A6BB-4426-A179-68463637A56B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="354">
   <si>
     <t>Class</t>
   </si>
@@ -1070,6 +1070,18 @@
   </si>
   <si>
     <t>TextFrame</t>
+  </si>
+  <si>
+    <t>addLine</t>
+  </si>
+  <si>
+    <t>excel-shape-lines</t>
+  </si>
+  <si>
+    <t>addStraightLine</t>
+  </si>
+  <si>
+    <t>arrowLine</t>
   </si>
 </sst>
 </file>
@@ -1148,8 +1160,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D167" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D167" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D169" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D169" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D165">
     <sortCondition ref="C1:C165"/>
   </sortState>
@@ -1460,7 +1472,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="875" row="6">
+  <wetp:taskpane dockstate="right" visibility="0" width="921" row="6">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1480,11 +1492,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D167"/>
+  <dimension ref="A1:D169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B167" sqref="B167"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A170" sqref="A170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3833,6 +3845,34 @@
         <v>348</v>
       </c>
     </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>281</v>
+      </c>
+      <c r="B168" t="s">
+        <v>350</v>
+      </c>
+      <c r="C168" t="s">
+        <v>351</v>
+      </c>
+      <c r="D168" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>278</v>
+      </c>
+      <c r="B169" t="s">
+        <v>134</v>
+      </c>
+      <c r="C169" t="s">
+        <v>351</v>
+      </c>
+      <c r="D169" t="s">
+        <v>353</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[excel] (Shapes) Snippet for line-type shapes (#267)
* Snippet for line-type shapes
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC56AB44-34AF-4C53-B0E7-E284589FD2A5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9071016E-A6BB-4426-A179-68463637A56B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="354">
   <si>
     <t>Class</t>
   </si>
@@ -1070,6 +1070,18 @@
   </si>
   <si>
     <t>TextFrame</t>
+  </si>
+  <si>
+    <t>addLine</t>
+  </si>
+  <si>
+    <t>excel-shape-lines</t>
+  </si>
+  <si>
+    <t>addStraightLine</t>
+  </si>
+  <si>
+    <t>arrowLine</t>
   </si>
 </sst>
 </file>
@@ -1148,8 +1160,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D167" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D167" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D169" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D169" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D165">
     <sortCondition ref="C1:C165"/>
   </sortState>
@@ -1460,7 +1472,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="875" row="6">
+  <wetp:taskpane dockstate="right" visibility="0" width="921" row="6">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1480,11 +1492,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D167"/>
+  <dimension ref="A1:D169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B167" sqref="B167"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A170" sqref="A170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3833,6 +3845,34 @@
         <v>348</v>
       </c>
     </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>281</v>
+      </c>
+      <c r="B168" t="s">
+        <v>350</v>
+      </c>
+      <c r="C168" t="s">
+        <v>351</v>
+      </c>
+      <c r="D168" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>278</v>
+      </c>
+      <c r="B169" t="s">
+        <v>134</v>
+      </c>
+      <c r="C169" t="s">
+        <v>351</v>
+      </c>
+      <c r="D169" t="s">
+        <v>353</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating shape snippets with latest API updates
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9071016E-A6BB-4426-A179-68463637A56B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FC99EB-D698-4CEE-A950-2D5FAED19149}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="361">
   <si>
     <t>Class</t>
   </si>
@@ -1082,6 +1082,27 @@
   </si>
   <si>
     <t>arrowLine</t>
+  </si>
+  <si>
+    <t>connectStraightLine</t>
+  </si>
+  <si>
+    <t>disconnectStraightLine</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>connectBeginShape</t>
+  </si>
+  <si>
+    <t>connectEndShape</t>
+  </si>
+  <si>
+    <t>disconnectBeginShape</t>
+  </si>
+  <si>
+    <t>disconnectEndShape</t>
   </si>
 </sst>
 </file>
@@ -1123,9 +1144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1160,8 +1182,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D169" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D169" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D173" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D173" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D165">
     <sortCondition ref="C1:C165"/>
   </sortState>
@@ -1492,11 +1514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D169"/>
+  <dimension ref="A1:D173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A170" sqref="A170"/>
+      <selection pane="bottomLeft" activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3873,6 +3895,62 @@
         <v>353</v>
       </c>
     </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C170" t="s">
+        <v>351</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C171" t="s">
+        <v>351</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C172" t="s">
+        <v>351</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C173" t="s">
+        <v>351</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating shape snippets with latest API updates (#271)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9071016E-A6BB-4426-A179-68463637A56B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FC99EB-D698-4CEE-A950-2D5FAED19149}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="361">
   <si>
     <t>Class</t>
   </si>
@@ -1082,6 +1082,27 @@
   </si>
   <si>
     <t>arrowLine</t>
+  </si>
+  <si>
+    <t>connectStraightLine</t>
+  </si>
+  <si>
+    <t>disconnectStraightLine</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>connectBeginShape</t>
+  </si>
+  <si>
+    <t>connectEndShape</t>
+  </si>
+  <si>
+    <t>disconnectBeginShape</t>
+  </si>
+  <si>
+    <t>disconnectEndShape</t>
   </si>
 </sst>
 </file>
@@ -1123,9 +1144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1160,8 +1182,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D169" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D169" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D173" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D173" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D165">
     <sortCondition ref="C1:C165"/>
   </sortState>
@@ -1492,11 +1514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D169"/>
+  <dimension ref="A1:D173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A170" sqref="A170"/>
+      <selection pane="bottomLeft" activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3873,6 +3895,62 @@
         <v>353</v>
       </c>
     </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C170" t="s">
+        <v>351</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C171" t="s">
+        <v>351</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C172" t="s">
+        <v>351</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C173" t="s">
+        <v>351</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Shape group snippet (#273)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FC99EB-D698-4CEE-A950-2D5FAED19149}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5385B40-3769-4072-9B94-20092A06181F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="5797" yWindow="3548" windowWidth="14401" windowHeight="7597" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="368">
   <si>
     <t>Class</t>
   </si>
@@ -1103,6 +1103,27 @@
   </si>
   <si>
     <t>disconnectEndShape</t>
+  </si>
+  <si>
+    <t>ShapeGroup</t>
+  </si>
+  <si>
+    <t>ungroup</t>
+  </si>
+  <si>
+    <t>excel-shape-groups</t>
+  </si>
+  <si>
+    <t>ungroupShapes</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>addGroup</t>
+  </si>
+  <si>
+    <t>groupShapes</t>
   </si>
 </sst>
 </file>
@@ -1182,8 +1203,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D173" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D173" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D176" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D176" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D165">
     <sortCondition ref="C1:C165"/>
   </sortState>
@@ -1514,11 +1535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D173"/>
+  <dimension ref="A1:D176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B173" sqref="B173"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D176" sqref="D176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3896,59 +3917,101 @@
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="2" t="s">
+      <c r="A170" t="s">
         <v>356</v>
       </c>
-      <c r="B170" s="2" t="s">
+      <c r="B170" t="s">
         <v>357</v>
       </c>
       <c r="C170" t="s">
         <v>351</v>
       </c>
-      <c r="D170" s="2" t="s">
+      <c r="D170" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="2" t="s">
+      <c r="A171" t="s">
         <v>356</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="B171" t="s">
         <v>358</v>
       </c>
       <c r="C171" t="s">
         <v>351</v>
       </c>
-      <c r="D171" s="2" t="s">
+      <c r="D171" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="2" t="s">
+      <c r="A172" t="s">
         <v>356</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="B172" t="s">
         <v>359</v>
       </c>
       <c r="C172" t="s">
         <v>351</v>
       </c>
-      <c r="D172" s="2" t="s">
+      <c r="D172" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="2" t="s">
+      <c r="A173" t="s">
         <v>356</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="B173" t="s">
         <v>360</v>
       </c>
       <c r="C173" t="s">
         <v>351</v>
       </c>
-      <c r="D173" s="2" t="s">
+      <c r="D173" t="s">
         <v>355</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C174" t="s">
+        <v>363</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Showcasing a better scenario for scaling shapes
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21514"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2A4B5C-6B60-45A6-948E-63D61636A1AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8996EFD9-04A2-46C9-BC66-2F9C12614000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -982,9 +982,6 @@
     <t>scaleHeight</t>
   </si>
   <si>
-    <t>scaleWidth</t>
-  </si>
-  <si>
     <t>PageBreakCollection</t>
   </si>
   <si>
@@ -1163,6 +1160,9 @@
   </si>
   <si>
     <t>deleteCommentReply</t>
+  </si>
+  <si>
+    <t>lockAspectRatio</t>
   </si>
 </sst>
 </file>
@@ -1204,10 +1204,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1578,19 +1577,19 @@
   <dimension ref="A1:D183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D160" sqref="D160"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1604,7 +1603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>269</v>
       </c>
@@ -1618,7 +1617,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1632,7 +1631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -1646,7 +1645,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -1660,7 +1659,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -1674,7 +1673,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>140</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>146</v>
       </c>
@@ -1702,7 +1701,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>208</v>
       </c>
@@ -1716,7 +1715,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>136</v>
       </c>
@@ -1730,7 +1729,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -1744,7 +1743,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>136</v>
       </c>
@@ -1758,7 +1757,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -1772,7 +1771,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>136</v>
       </c>
@@ -1786,7 +1785,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>136</v>
       </c>
@@ -1800,7 +1799,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>136</v>
       </c>
@@ -1814,7 +1813,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>259</v>
       </c>
@@ -1828,7 +1827,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>259</v>
       </c>
@@ -1842,7 +1841,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -1856,7 +1855,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>124</v>
       </c>
@@ -1870,7 +1869,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>130</v>
       </c>
@@ -1884,7 +1883,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>130</v>
       </c>
@@ -1898,7 +1897,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -1912,105 +1911,105 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>373</v>
+      </c>
+      <c r="B24" t="s">
+        <v>376</v>
+      </c>
+      <c r="C24" t="s">
+        <v>367</v>
+      </c>
+      <c r="D24" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>373</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>367</v>
+      </c>
+      <c r="D25" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>373</v>
+      </c>
+      <c r="B26" t="s">
         <v>374</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C26" t="s">
+        <v>367</v>
+      </c>
+      <c r="D26" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>368</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>367</v>
+      </c>
+      <c r="D27" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>377</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="B28" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="C28" t="s">
+        <v>367</v>
+      </c>
+      <c r="D28" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>377</v>
+      </c>
+      <c r="B29" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="C29" t="s">
+        <v>367</v>
+      </c>
+      <c r="D29" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="B27" s="2" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>370</v>
+      </c>
+      <c r="B30" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" s="2" t="s">
+      <c r="C30" t="s">
+        <v>367</v>
+      </c>
+      <c r="D30" t="s">
         <v>371</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -2024,7 +2023,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>91</v>
       </c>
@@ -2038,7 +2037,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -2052,7 +2051,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -2066,7 +2065,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -2080,7 +2079,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -2094,7 +2093,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -2108,7 +2107,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -2122,7 +2121,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -2136,7 +2135,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -2150,7 +2149,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -2164,7 +2163,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -2178,7 +2177,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -2192,7 +2191,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>56</v>
       </c>
@@ -2206,7 +2205,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -2220,7 +2219,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -2234,7 +2233,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -2248,7 +2247,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>78</v>
       </c>
@@ -2262,7 +2261,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>78</v>
       </c>
@@ -2276,7 +2275,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>66</v>
       </c>
@@ -2290,7 +2289,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>85</v>
       </c>
@@ -2304,7 +2303,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>93</v>
       </c>
@@ -2318,7 +2317,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>34</v>
       </c>
@@ -2332,7 +2331,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>34</v>
       </c>
@@ -2346,7 +2345,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>34</v>
       </c>
@@ -2360,7 +2359,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -2374,7 +2373,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>30</v>
       </c>
@@ -2388,7 +2387,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -2402,7 +2401,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>30</v>
       </c>
@@ -2416,7 +2415,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -2430,7 +2429,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -2444,7 +2443,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -2458,7 +2457,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -2472,7 +2471,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>234</v>
       </c>
@@ -2486,7 +2485,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>234</v>
       </c>
@@ -2500,7 +2499,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>222</v>
       </c>
@@ -2514,7 +2513,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>253</v>
       </c>
@@ -2528,7 +2527,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>253</v>
       </c>
@@ -2542,7 +2541,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -2556,7 +2555,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>74</v>
       </c>
@@ -2570,7 +2569,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>306</v>
       </c>
@@ -2584,63 +2583,63 @@
         <v>305</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>354</v>
+      </c>
+      <c r="B72" t="s">
         <v>355</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
+        <v>349</v>
+      </c>
+      <c r="D72" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>354</v>
+      </c>
+      <c r="B73" t="s">
         <v>356</v>
       </c>
-      <c r="C72" t="s">
-        <v>350</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="C73" t="s">
+        <v>349</v>
+      </c>
+      <c r="D73" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>354</v>
+      </c>
+      <c r="B74" t="s">
+        <v>357</v>
+      </c>
+      <c r="C74" t="s">
+        <v>349</v>
+      </c>
+      <c r="D74" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
-        <v>355</v>
-      </c>
-      <c r="B73" t="s">
-        <v>357</v>
-      </c>
-      <c r="C73" t="s">
-        <v>350</v>
-      </c>
-      <c r="D73" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>354</v>
+      </c>
+      <c r="B75" t="s">
+        <v>358</v>
+      </c>
+      <c r="C75" t="s">
+        <v>349</v>
+      </c>
+      <c r="D75" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
-        <v>355</v>
-      </c>
-      <c r="B74" t="s">
-        <v>358</v>
-      </c>
-      <c r="C74" t="s">
-        <v>350</v>
-      </c>
-      <c r="D74" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>355</v>
-      </c>
-      <c r="B75" t="s">
-        <v>359</v>
-      </c>
-      <c r="C75" t="s">
-        <v>350</v>
-      </c>
-      <c r="D75" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -2654,7 +2653,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -2668,7 +2667,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -2682,91 +2681,91 @@
         <v>265</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B79" t="s">
         <v>9</v>
       </c>
       <c r="C79" t="s">
+        <v>321</v>
+      </c>
+      <c r="D79" t="s">
         <v>322</v>
       </c>
-      <c r="D79" t="s">
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>325</v>
+      </c>
+      <c r="B80" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
+      <c r="C80" t="s">
+        <v>321</v>
+      </c>
+      <c r="D80" t="s">
         <v>326</v>
       </c>
-      <c r="B80" t="s">
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>325</v>
+      </c>
+      <c r="B81" t="s">
         <v>324</v>
       </c>
-      <c r="C80" t="s">
-        <v>322</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="C81" t="s">
+        <v>321</v>
+      </c>
+      <c r="D81" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>325</v>
+      </c>
+      <c r="B82" t="s">
+        <v>330</v>
+      </c>
+      <c r="C82" t="s">
+        <v>321</v>
+      </c>
+      <c r="D82" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>325</v>
+      </c>
+      <c r="B83" t="s">
+        <v>329</v>
+      </c>
+      <c r="C83" t="s">
+        <v>321</v>
+      </c>
+      <c r="D83" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>325</v>
+      </c>
+      <c r="B84" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>326</v>
-      </c>
-      <c r="B81" t="s">
-        <v>325</v>
-      </c>
-      <c r="C81" t="s">
-        <v>322</v>
-      </c>
-      <c r="D81" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
-        <v>326</v>
-      </c>
-      <c r="B82" t="s">
-        <v>331</v>
-      </c>
-      <c r="C82" t="s">
-        <v>322</v>
-      </c>
-      <c r="D82" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A83" t="s">
-        <v>326</v>
-      </c>
-      <c r="B83" t="s">
-        <v>330</v>
-      </c>
-      <c r="C83" t="s">
-        <v>322</v>
-      </c>
-      <c r="D83" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A84" t="s">
-        <v>326</v>
-      </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
+        <v>321</v>
+      </c>
+      <c r="D84" t="s">
         <v>328</v>
       </c>
-      <c r="C84" t="s">
-        <v>322</v>
-      </c>
-      <c r="D84" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>239</v>
       </c>
@@ -2780,7 +2779,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>226</v>
       </c>
@@ -2794,7 +2793,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>226</v>
       </c>
@@ -2808,7 +2807,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>226</v>
       </c>
@@ -2822,7 +2821,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>226</v>
       </c>
@@ -2836,7 +2835,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>226</v>
       </c>
@@ -2850,7 +2849,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>223</v>
       </c>
@@ -2864,7 +2863,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>64</v>
       </c>
@@ -2878,7 +2877,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>64</v>
       </c>
@@ -2892,7 +2891,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>24</v>
       </c>
@@ -2906,7 +2905,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>24</v>
       </c>
@@ -2920,7 +2919,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>24</v>
       </c>
@@ -2934,7 +2933,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>24</v>
       </c>
@@ -2948,7 +2947,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>24</v>
       </c>
@@ -2962,7 +2961,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>24</v>
       </c>
@@ -2976,7 +2975,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>24</v>
       </c>
@@ -2990,7 +2989,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>24</v>
       </c>
@@ -3004,21 +3003,21 @@
         <v>105</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>24</v>
       </c>
       <c r="B102" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C102" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D102" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>24</v>
       </c>
@@ -3032,7 +3031,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>24</v>
       </c>
@@ -3046,7 +3045,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>24</v>
       </c>
@@ -3060,7 +3059,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>108</v>
       </c>
@@ -3074,7 +3073,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>100</v>
       </c>
@@ -3088,7 +3087,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>100</v>
       </c>
@@ -3102,7 +3101,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>100</v>
       </c>
@@ -3116,7 +3115,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>100</v>
       </c>
@@ -3130,21 +3129,21 @@
         <v>105</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B111" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C111" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D111" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>249</v>
       </c>
@@ -3158,7 +3157,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>20</v>
       </c>
@@ -3172,7 +3171,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>17</v>
       </c>
@@ -3186,7 +3185,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>17</v>
       </c>
@@ -3200,7 +3199,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>17</v>
       </c>
@@ -3214,7 +3213,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>278</v>
       </c>
@@ -3228,7 +3227,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>278</v>
       </c>
@@ -3242,12 +3241,12 @@
         <v>283</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>278</v>
       </c>
       <c r="B119" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C119" t="s">
         <v>302</v>
@@ -3256,21 +3255,21 @@
         <v>307</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>278</v>
       </c>
       <c r="B120" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C120" t="s">
+        <v>361</v>
+      </c>
+      <c r="D120" t="s">
         <v>362</v>
       </c>
-      <c r="D120" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>278</v>
       </c>
@@ -3284,7 +3283,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>278</v>
       </c>
@@ -3298,7 +3297,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>278</v>
       </c>
@@ -3312,7 +3311,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>278</v>
       </c>
@@ -3320,13 +3319,13 @@
         <v>134</v>
       </c>
       <c r="C124" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D124" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>278</v>
       </c>
@@ -3340,7 +3339,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>278</v>
       </c>
@@ -3354,12 +3353,12 @@
         <v>316</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>278</v>
       </c>
       <c r="B127" t="s">
-        <v>320</v>
+        <v>380</v>
       </c>
       <c r="C127" t="s">
         <v>313</v>
@@ -3368,7 +3367,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>278</v>
       </c>
@@ -3382,7 +3381,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>281</v>
       </c>
@@ -3393,24 +3392,24 @@
         <v>298</v>
       </c>
       <c r="D129" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>281</v>
       </c>
       <c r="B130" t="s">
+        <v>364</v>
+      </c>
+      <c r="C130" t="s">
+        <v>361</v>
+      </c>
+      <c r="D130" t="s">
         <v>365</v>
       </c>
-      <c r="C130" t="s">
-        <v>362</v>
-      </c>
-      <c r="D130" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>281</v>
       </c>
@@ -3424,49 +3423,49 @@
         <v>295</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>281</v>
       </c>
       <c r="B132" t="s">
+        <v>348</v>
+      </c>
+      <c r="C132" t="s">
         <v>349</v>
       </c>
-      <c r="C132" t="s">
+      <c r="D132" t="s">
         <v>350</v>
       </c>
-      <c r="D132" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>281</v>
       </c>
       <c r="B133" t="s">
+        <v>343</v>
+      </c>
+      <c r="C133" t="s">
         <v>344</v>
       </c>
-      <c r="C133" t="s">
+      <c r="D133" t="s">
         <v>345</v>
       </c>
-      <c r="D133" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>359</v>
+      </c>
+      <c r="B134" t="s">
         <v>360</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
         <v>361</v>
       </c>
-      <c r="C134" t="s">
+      <c r="D134" t="s">
         <v>362</v>
       </c>
-      <c r="D134" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>246</v>
       </c>
@@ -3480,7 +3479,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>152</v>
       </c>
@@ -3494,7 +3493,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>152</v>
       </c>
@@ -3508,7 +3507,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>152</v>
       </c>
@@ -3522,7 +3521,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>152</v>
       </c>
@@ -3536,7 +3535,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>156</v>
       </c>
@@ -3550,7 +3549,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>156</v>
       </c>
@@ -3564,7 +3563,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>211</v>
       </c>
@@ -3578,7 +3577,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>211</v>
       </c>
@@ -3592,7 +3591,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>214</v>
       </c>
@@ -3606,7 +3605,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>214</v>
       </c>
@@ -3620,7 +3619,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>213</v>
       </c>
@@ -3634,7 +3633,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>210</v>
       </c>
@@ -3648,7 +3647,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>82</v>
       </c>
@@ -3662,7 +3661,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>82</v>
       </c>
@@ -3676,35 +3675,35 @@
         <v>84</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B150" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C150" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D150" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.45">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>190</v>
       </c>
       <c r="B151" t="s">
+        <v>338</v>
+      </c>
+      <c r="C151" t="s">
+        <v>336</v>
+      </c>
+      <c r="D151" t="s">
         <v>339</v>
       </c>
-      <c r="C151" t="s">
-        <v>337</v>
-      </c>
-      <c r="D151" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>190</v>
       </c>
@@ -3718,7 +3717,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>190</v>
       </c>
@@ -3732,7 +3731,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>190</v>
       </c>
@@ -3746,21 +3745,21 @@
         <v>159</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>190</v>
       </c>
       <c r="B155" t="s">
+        <v>335</v>
+      </c>
+      <c r="C155" t="s">
         <v>336</v>
       </c>
-      <c r="C155" t="s">
+      <c r="D155" t="s">
         <v>337</v>
       </c>
-      <c r="D155" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>206</v>
       </c>
@@ -3774,7 +3773,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>206</v>
       </c>
@@ -3788,7 +3787,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>206</v>
       </c>
@@ -3802,7 +3801,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>206</v>
       </c>
@@ -3816,7 +3815,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>47</v>
       </c>
@@ -3830,7 +3829,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>47</v>
       </c>
@@ -3844,7 +3843,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>47</v>
       </c>
@@ -3858,7 +3857,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>47</v>
       </c>
@@ -3872,7 +3871,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>47</v>
       </c>
@@ -3886,7 +3885,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>47</v>
       </c>
@@ -3900,7 +3899,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>47</v>
       </c>
@@ -3914,7 +3913,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>47</v>
       </c>
@@ -3928,7 +3927,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>212</v>
       </c>
@@ -3942,7 +3941,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>50</v>
       </c>
@@ -3956,7 +3955,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>50</v>
       </c>
@@ -3970,7 +3969,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>50</v>
       </c>
@@ -3984,7 +3983,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>50</v>
       </c>
@@ -3998,7 +3997,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>50</v>
       </c>
@@ -4012,7 +4011,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>50</v>
       </c>
@@ -4026,7 +4025,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>110</v>
       </c>
@@ -4040,7 +4039,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>110</v>
       </c>
@@ -4054,7 +4053,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>110</v>
       </c>
@@ -4068,7 +4067,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>110</v>
       </c>
@@ -4082,7 +4081,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>110</v>
       </c>
@@ -4096,7 +4095,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>207</v>
       </c>
@@ -4110,7 +4109,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>207</v>
       </c>
@@ -4124,7 +4123,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>207</v>
       </c>
@@ -4138,7 +4137,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>207</v>
       </c>

</xml_diff>

<commit_message>
Showcasing a better scenario for scaling shapes (#276)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21514"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2A4B5C-6B60-45A6-948E-63D61636A1AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8996EFD9-04A2-46C9-BC66-2F9C12614000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -982,9 +982,6 @@
     <t>scaleHeight</t>
   </si>
   <si>
-    <t>scaleWidth</t>
-  </si>
-  <si>
     <t>PageBreakCollection</t>
   </si>
   <si>
@@ -1163,6 +1160,9 @@
   </si>
   <si>
     <t>deleteCommentReply</t>
+  </si>
+  <si>
+    <t>lockAspectRatio</t>
   </si>
 </sst>
 </file>
@@ -1204,10 +1204,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1578,19 +1577,19 @@
   <dimension ref="A1:D183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D160" sqref="D160"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1604,7 +1603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>269</v>
       </c>
@@ -1618,7 +1617,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1632,7 +1631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -1646,7 +1645,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -1660,7 +1659,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -1674,7 +1673,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>140</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>146</v>
       </c>
@@ -1702,7 +1701,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>208</v>
       </c>
@@ -1716,7 +1715,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>136</v>
       </c>
@@ -1730,7 +1729,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -1744,7 +1743,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>136</v>
       </c>
@@ -1758,7 +1757,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -1772,7 +1771,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>136</v>
       </c>
@@ -1786,7 +1785,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>136</v>
       </c>
@@ -1800,7 +1799,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>136</v>
       </c>
@@ -1814,7 +1813,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>259</v>
       </c>
@@ -1828,7 +1827,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>259</v>
       </c>
@@ -1842,7 +1841,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -1856,7 +1855,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>124</v>
       </c>
@@ -1870,7 +1869,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>130</v>
       </c>
@@ -1884,7 +1883,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>130</v>
       </c>
@@ -1898,7 +1897,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -1912,105 +1911,105 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>373</v>
+      </c>
+      <c r="B24" t="s">
+        <v>376</v>
+      </c>
+      <c r="C24" t="s">
+        <v>367</v>
+      </c>
+      <c r="D24" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>373</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>367</v>
+      </c>
+      <c r="D25" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>373</v>
+      </c>
+      <c r="B26" t="s">
         <v>374</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C26" t="s">
+        <v>367</v>
+      </c>
+      <c r="D26" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>368</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>367</v>
+      </c>
+      <c r="D27" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>377</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="B28" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="C28" t="s">
+        <v>367</v>
+      </c>
+      <c r="D28" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>377</v>
+      </c>
+      <c r="B29" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="C29" t="s">
+        <v>367</v>
+      </c>
+      <c r="D29" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="B27" s="2" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>370</v>
+      </c>
+      <c r="B30" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" s="2" t="s">
+      <c r="C30" t="s">
+        <v>367</v>
+      </c>
+      <c r="D30" t="s">
         <v>371</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -2024,7 +2023,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>91</v>
       </c>
@@ -2038,7 +2037,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -2052,7 +2051,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -2066,7 +2065,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -2080,7 +2079,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -2094,7 +2093,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -2108,7 +2107,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -2122,7 +2121,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -2136,7 +2135,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -2150,7 +2149,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -2164,7 +2163,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -2178,7 +2177,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -2192,7 +2191,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>56</v>
       </c>
@@ -2206,7 +2205,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -2220,7 +2219,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -2234,7 +2233,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -2248,7 +2247,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>78</v>
       </c>
@@ -2262,7 +2261,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>78</v>
       </c>
@@ -2276,7 +2275,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>66</v>
       </c>
@@ -2290,7 +2289,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>85</v>
       </c>
@@ -2304,7 +2303,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>93</v>
       </c>
@@ -2318,7 +2317,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>34</v>
       </c>
@@ -2332,7 +2331,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>34</v>
       </c>
@@ -2346,7 +2345,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>34</v>
       </c>
@@ -2360,7 +2359,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -2374,7 +2373,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>30</v>
       </c>
@@ -2388,7 +2387,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -2402,7 +2401,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>30</v>
       </c>
@@ -2416,7 +2415,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -2430,7 +2429,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -2444,7 +2443,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -2458,7 +2457,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -2472,7 +2471,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>234</v>
       </c>
@@ -2486,7 +2485,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>234</v>
       </c>
@@ -2500,7 +2499,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>222</v>
       </c>
@@ -2514,7 +2513,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>253</v>
       </c>
@@ -2528,7 +2527,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>253</v>
       </c>
@@ -2542,7 +2541,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -2556,7 +2555,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>74</v>
       </c>
@@ -2570,7 +2569,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>306</v>
       </c>
@@ -2584,63 +2583,63 @@
         <v>305</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>354</v>
+      </c>
+      <c r="B72" t="s">
         <v>355</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
+        <v>349</v>
+      </c>
+      <c r="D72" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>354</v>
+      </c>
+      <c r="B73" t="s">
         <v>356</v>
       </c>
-      <c r="C72" t="s">
-        <v>350</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="C73" t="s">
+        <v>349</v>
+      </c>
+      <c r="D73" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>354</v>
+      </c>
+      <c r="B74" t="s">
+        <v>357</v>
+      </c>
+      <c r="C74" t="s">
+        <v>349</v>
+      </c>
+      <c r="D74" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
-        <v>355</v>
-      </c>
-      <c r="B73" t="s">
-        <v>357</v>
-      </c>
-      <c r="C73" t="s">
-        <v>350</v>
-      </c>
-      <c r="D73" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>354</v>
+      </c>
+      <c r="B75" t="s">
+        <v>358</v>
+      </c>
+      <c r="C75" t="s">
+        <v>349</v>
+      </c>
+      <c r="D75" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
-        <v>355</v>
-      </c>
-      <c r="B74" t="s">
-        <v>358</v>
-      </c>
-      <c r="C74" t="s">
-        <v>350</v>
-      </c>
-      <c r="D74" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>355</v>
-      </c>
-      <c r="B75" t="s">
-        <v>359</v>
-      </c>
-      <c r="C75" t="s">
-        <v>350</v>
-      </c>
-      <c r="D75" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -2654,7 +2653,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -2668,7 +2667,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -2682,91 +2681,91 @@
         <v>265</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B79" t="s">
         <v>9</v>
       </c>
       <c r="C79" t="s">
+        <v>321</v>
+      </c>
+      <c r="D79" t="s">
         <v>322</v>
       </c>
-      <c r="D79" t="s">
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>325</v>
+      </c>
+      <c r="B80" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
+      <c r="C80" t="s">
+        <v>321</v>
+      </c>
+      <c r="D80" t="s">
         <v>326</v>
       </c>
-      <c r="B80" t="s">
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>325</v>
+      </c>
+      <c r="B81" t="s">
         <v>324</v>
       </c>
-      <c r="C80" t="s">
-        <v>322</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="C81" t="s">
+        <v>321</v>
+      </c>
+      <c r="D81" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>325</v>
+      </c>
+      <c r="B82" t="s">
+        <v>330</v>
+      </c>
+      <c r="C82" t="s">
+        <v>321</v>
+      </c>
+      <c r="D82" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>325</v>
+      </c>
+      <c r="B83" t="s">
+        <v>329</v>
+      </c>
+      <c r="C83" t="s">
+        <v>321</v>
+      </c>
+      <c r="D83" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>325</v>
+      </c>
+      <c r="B84" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>326</v>
-      </c>
-      <c r="B81" t="s">
-        <v>325</v>
-      </c>
-      <c r="C81" t="s">
-        <v>322</v>
-      </c>
-      <c r="D81" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
-        <v>326</v>
-      </c>
-      <c r="B82" t="s">
-        <v>331</v>
-      </c>
-      <c r="C82" t="s">
-        <v>322</v>
-      </c>
-      <c r="D82" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A83" t="s">
-        <v>326</v>
-      </c>
-      <c r="B83" t="s">
-        <v>330</v>
-      </c>
-      <c r="C83" t="s">
-        <v>322</v>
-      </c>
-      <c r="D83" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A84" t="s">
-        <v>326</v>
-      </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
+        <v>321</v>
+      </c>
+      <c r="D84" t="s">
         <v>328</v>
       </c>
-      <c r="C84" t="s">
-        <v>322</v>
-      </c>
-      <c r="D84" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>239</v>
       </c>
@@ -2780,7 +2779,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>226</v>
       </c>
@@ -2794,7 +2793,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>226</v>
       </c>
@@ -2808,7 +2807,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>226</v>
       </c>
@@ -2822,7 +2821,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>226</v>
       </c>
@@ -2836,7 +2835,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>226</v>
       </c>
@@ -2850,7 +2849,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>223</v>
       </c>
@@ -2864,7 +2863,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>64</v>
       </c>
@@ -2878,7 +2877,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>64</v>
       </c>
@@ -2892,7 +2891,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>24</v>
       </c>
@@ -2906,7 +2905,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>24</v>
       </c>
@@ -2920,7 +2919,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>24</v>
       </c>
@@ -2934,7 +2933,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>24</v>
       </c>
@@ -2948,7 +2947,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>24</v>
       </c>
@@ -2962,7 +2961,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>24</v>
       </c>
@@ -2976,7 +2975,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>24</v>
       </c>
@@ -2990,7 +2989,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>24</v>
       </c>
@@ -3004,21 +3003,21 @@
         <v>105</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>24</v>
       </c>
       <c r="B102" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C102" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D102" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>24</v>
       </c>
@@ -3032,7 +3031,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>24</v>
       </c>
@@ -3046,7 +3045,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>24</v>
       </c>
@@ -3060,7 +3059,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>108</v>
       </c>
@@ -3074,7 +3073,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>100</v>
       </c>
@@ -3088,7 +3087,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>100</v>
       </c>
@@ -3102,7 +3101,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>100</v>
       </c>
@@ -3116,7 +3115,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>100</v>
       </c>
@@ -3130,21 +3129,21 @@
         <v>105</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B111" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C111" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D111" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>249</v>
       </c>
@@ -3158,7 +3157,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>20</v>
       </c>
@@ -3172,7 +3171,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>17</v>
       </c>
@@ -3186,7 +3185,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>17</v>
       </c>
@@ -3200,7 +3199,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>17</v>
       </c>
@@ -3214,7 +3213,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>278</v>
       </c>
@@ -3228,7 +3227,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>278</v>
       </c>
@@ -3242,12 +3241,12 @@
         <v>283</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>278</v>
       </c>
       <c r="B119" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C119" t="s">
         <v>302</v>
@@ -3256,21 +3255,21 @@
         <v>307</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>278</v>
       </c>
       <c r="B120" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C120" t="s">
+        <v>361</v>
+      </c>
+      <c r="D120" t="s">
         <v>362</v>
       </c>
-      <c r="D120" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>278</v>
       </c>
@@ -3284,7 +3283,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>278</v>
       </c>
@@ -3298,7 +3297,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>278</v>
       </c>
@@ -3312,7 +3311,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>278</v>
       </c>
@@ -3320,13 +3319,13 @@
         <v>134</v>
       </c>
       <c r="C124" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D124" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>278</v>
       </c>
@@ -3340,7 +3339,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>278</v>
       </c>
@@ -3354,12 +3353,12 @@
         <v>316</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>278</v>
       </c>
       <c r="B127" t="s">
-        <v>320</v>
+        <v>380</v>
       </c>
       <c r="C127" t="s">
         <v>313</v>
@@ -3368,7 +3367,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>278</v>
       </c>
@@ -3382,7 +3381,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>281</v>
       </c>
@@ -3393,24 +3392,24 @@
         <v>298</v>
       </c>
       <c r="D129" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>281</v>
       </c>
       <c r="B130" t="s">
+        <v>364</v>
+      </c>
+      <c r="C130" t="s">
+        <v>361</v>
+      </c>
+      <c r="D130" t="s">
         <v>365</v>
       </c>
-      <c r="C130" t="s">
-        <v>362</v>
-      </c>
-      <c r="D130" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>281</v>
       </c>
@@ -3424,49 +3423,49 @@
         <v>295</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>281</v>
       </c>
       <c r="B132" t="s">
+        <v>348</v>
+      </c>
+      <c r="C132" t="s">
         <v>349</v>
       </c>
-      <c r="C132" t="s">
+      <c r="D132" t="s">
         <v>350</v>
       </c>
-      <c r="D132" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>281</v>
       </c>
       <c r="B133" t="s">
+        <v>343</v>
+      </c>
+      <c r="C133" t="s">
         <v>344</v>
       </c>
-      <c r="C133" t="s">
+      <c r="D133" t="s">
         <v>345</v>
       </c>
-      <c r="D133" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>359</v>
+      </c>
+      <c r="B134" t="s">
         <v>360</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
         <v>361</v>
       </c>
-      <c r="C134" t="s">
+      <c r="D134" t="s">
         <v>362</v>
       </c>
-      <c r="D134" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>246</v>
       </c>
@@ -3480,7 +3479,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>152</v>
       </c>
@@ -3494,7 +3493,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>152</v>
       </c>
@@ -3508,7 +3507,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>152</v>
       </c>
@@ -3522,7 +3521,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>152</v>
       </c>
@@ -3536,7 +3535,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>156</v>
       </c>
@@ -3550,7 +3549,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>156</v>
       </c>
@@ -3564,7 +3563,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>211</v>
       </c>
@@ -3578,7 +3577,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>211</v>
       </c>
@@ -3592,7 +3591,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>214</v>
       </c>
@@ -3606,7 +3605,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>214</v>
       </c>
@@ -3620,7 +3619,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>213</v>
       </c>
@@ -3634,7 +3633,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>210</v>
       </c>
@@ -3648,7 +3647,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>82</v>
       </c>
@@ -3662,7 +3661,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>82</v>
       </c>
@@ -3676,35 +3675,35 @@
         <v>84</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B150" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C150" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D150" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.45">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>190</v>
       </c>
       <c r="B151" t="s">
+        <v>338</v>
+      </c>
+      <c r="C151" t="s">
+        <v>336</v>
+      </c>
+      <c r="D151" t="s">
         <v>339</v>
       </c>
-      <c r="C151" t="s">
-        <v>337</v>
-      </c>
-      <c r="D151" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>190</v>
       </c>
@@ -3718,7 +3717,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>190</v>
       </c>
@@ -3732,7 +3731,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>190</v>
       </c>
@@ -3746,21 +3745,21 @@
         <v>159</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>190</v>
       </c>
       <c r="B155" t="s">
+        <v>335</v>
+      </c>
+      <c r="C155" t="s">
         <v>336</v>
       </c>
-      <c r="C155" t="s">
+      <c r="D155" t="s">
         <v>337</v>
       </c>
-      <c r="D155" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>206</v>
       </c>
@@ -3774,7 +3773,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>206</v>
       </c>
@@ -3788,7 +3787,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>206</v>
       </c>
@@ -3802,7 +3801,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>206</v>
       </c>
@@ -3816,7 +3815,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>47</v>
       </c>
@@ -3830,7 +3829,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>47</v>
       </c>
@@ -3844,7 +3843,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>47</v>
       </c>
@@ -3858,7 +3857,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>47</v>
       </c>
@@ -3872,7 +3871,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>47</v>
       </c>
@@ -3886,7 +3885,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>47</v>
       </c>
@@ -3900,7 +3899,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>47</v>
       </c>
@@ -3914,7 +3913,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>47</v>
       </c>
@@ -3928,7 +3927,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>212</v>
       </c>
@@ -3942,7 +3941,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>50</v>
       </c>
@@ -3956,7 +3955,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>50</v>
       </c>
@@ -3970,7 +3969,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>50</v>
       </c>
@@ -3984,7 +3983,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>50</v>
       </c>
@@ -3998,7 +3997,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>50</v>
       </c>
@@ -4012,7 +4011,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>50</v>
       </c>
@@ -4026,7 +4025,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>110</v>
       </c>
@@ -4040,7 +4039,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>110</v>
       </c>
@@ -4054,7 +4053,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>110</v>
       </c>
@@ -4068,7 +4067,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>110</v>
       </c>
@@ -4082,7 +4081,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>110</v>
       </c>
@@ -4096,7 +4095,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>207</v>
       </c>
@@ -4110,7 +4109,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>207</v>
       </c>
@@ -4124,7 +4123,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>207</v>
       </c>
@@ -4138,7 +4137,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>207</v>
       </c>

</xml_diff>

<commit_message>
Data change event details snippet
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8996EFD9-04A2-46C9-BC66-2F9C12614000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C6FED1-05D3-4662-AC25-6A9916C9CE33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="384">
   <si>
     <t>Class</t>
   </si>
@@ -1163,6 +1163,15 @@
   </si>
   <si>
     <t>lockAspectRatio</t>
+  </si>
+  <si>
+    <t>onTableChanged</t>
+  </si>
+  <si>
+    <t>excel-data-change-event-details</t>
+  </si>
+  <si>
+    <t>details</t>
   </si>
 </sst>
 </file>
@@ -1204,9 +1213,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1241,8 +1251,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D183" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D183" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D184" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D184" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D183">
     <sortCondition ref="A2:A183"/>
     <sortCondition ref="B2:B183"/>
@@ -1574,11 +1584,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D183"/>
+  <dimension ref="A1:D184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C126" sqref="C126"/>
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D184" sqref="D184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4151,6 +4161,20 @@
         <v>203</v>
       </c>
     </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[excel] (Events) Data change event details snippet (#287)
* Data change event details snippet

* Fixing console log statement spacing
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8996EFD9-04A2-46C9-BC66-2F9C12614000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C6FED1-05D3-4662-AC25-6A9916C9CE33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="384">
   <si>
     <t>Class</t>
   </si>
@@ -1163,6 +1163,15 @@
   </si>
   <si>
     <t>lockAspectRatio</t>
+  </si>
+  <si>
+    <t>onTableChanged</t>
+  </si>
+  <si>
+    <t>excel-data-change-event-details</t>
+  </si>
+  <si>
+    <t>details</t>
   </si>
 </sst>
 </file>
@@ -1204,9 +1213,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1241,8 +1251,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D183" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D183" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D184" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D184" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D183">
     <sortCondition ref="A2:A183"/>
     <sortCondition ref="B2:B183"/>
@@ -1574,11 +1584,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D183"/>
+  <dimension ref="A1:D184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C126" sqref="C126"/>
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D184" sqref="D184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4151,6 +4161,20 @@
         <v>203</v>
       </c>
     </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding a sample for a worksheet autofilter
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21603"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C6FED1-05D3-4662-AC25-6A9916C9CE33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526A2DAE-C8EA-481C-B570-4B7C84C4490E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="389">
   <si>
     <t>Class</t>
   </si>
@@ -1172,6 +1172,21 @@
   </si>
   <si>
     <t>details</t>
+  </si>
+  <si>
+    <t>autofilter</t>
+  </si>
+  <si>
+    <t>addAutoFilter</t>
+  </si>
+  <si>
+    <t>excel-worksheet-auto-filter</t>
+  </si>
+  <si>
+    <t>AutoFilter</t>
+  </si>
+  <si>
+    <t>apply</t>
   </si>
 </sst>
 </file>
@@ -1251,8 +1266,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D184" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D184" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D186" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D186" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D183">
     <sortCondition ref="A2:A183"/>
     <sortCondition ref="B2:B183"/>
@@ -1584,11 +1599,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D184"/>
+  <dimension ref="A1:D186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D184" sqref="D184"/>
+      <selection pane="bottomLeft" activeCell="O178" sqref="O178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4162,17 +4177,45 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="2" t="s">
+      <c r="A184" t="s">
         <v>214</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B184" t="s">
         <v>383</v>
       </c>
-      <c r="C184" s="2" t="s">
+      <c r="C184" t="s">
         <v>382</v>
       </c>
-      <c r="D184" s="2" t="s">
+      <c r="D184" t="s">
         <v>381</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[excel] (Worksheet) Adding a sample for a worksheet autofilter (#290)
* Adding a sample for a worksheet autofilter

* Simplifying setup code
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21603"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C6FED1-05D3-4662-AC25-6A9916C9CE33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526A2DAE-C8EA-481C-B570-4B7C84C4490E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="389">
   <si>
     <t>Class</t>
   </si>
@@ -1172,6 +1172,21 @@
   </si>
   <si>
     <t>details</t>
+  </si>
+  <si>
+    <t>autofilter</t>
+  </si>
+  <si>
+    <t>addAutoFilter</t>
+  </si>
+  <si>
+    <t>excel-worksheet-auto-filter</t>
+  </si>
+  <si>
+    <t>AutoFilter</t>
+  </si>
+  <si>
+    <t>apply</t>
   </si>
 </sst>
 </file>
@@ -1251,8 +1266,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D184" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D184" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D186" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D186" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D183">
     <sortCondition ref="A2:A183"/>
     <sortCondition ref="B2:B183"/>
@@ -1584,11 +1599,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D184"/>
+  <dimension ref="A1:D186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D184" sqref="D184"/>
+      <selection pane="bottomLeft" activeCell="O178" sqref="O178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4162,17 +4177,45 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="2" t="s">
+      <c r="A184" t="s">
         <v>214</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B184" t="s">
         <v>383</v>
       </c>
-      <c r="C184" s="2" t="s">
+      <c r="C184" t="s">
         <v>382</v>
       </c>
-      <c r="D184" s="2" t="s">
+      <c r="D184" t="s">
         <v>381</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merging to prod (#291)
* Fixed Errors in README.md (#278)

- Hedging
- Remove pronouns for clarity
- Removed excess use of that
- Removed contractions to make more formal

* [excel] (Worksheet) Adding a sample for a worksheet autofilter (#290)

* Adding a sample for a worksheet autofilter

* Simplifying setup code
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21603"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C6FED1-05D3-4662-AC25-6A9916C9CE33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526A2DAE-C8EA-481C-B570-4B7C84C4490E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="389">
   <si>
     <t>Class</t>
   </si>
@@ -1172,6 +1172,21 @@
   </si>
   <si>
     <t>details</t>
+  </si>
+  <si>
+    <t>autofilter</t>
+  </si>
+  <si>
+    <t>addAutoFilter</t>
+  </si>
+  <si>
+    <t>excel-worksheet-auto-filter</t>
+  </si>
+  <si>
+    <t>AutoFilter</t>
+  </si>
+  <si>
+    <t>apply</t>
   </si>
 </sst>
 </file>
@@ -1251,8 +1266,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D184" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D184" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D186" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D186" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D183">
     <sortCondition ref="A2:A183"/>
     <sortCondition ref="B2:B183"/>
@@ -1584,11 +1599,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D184"/>
+  <dimension ref="A1:D186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D184" sqref="D184"/>
+      <selection pane="bottomLeft" activeCell="O178" sqref="O178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4162,17 +4177,45 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="2" t="s">
+      <c r="A184" t="s">
         <v>214</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B184" t="s">
         <v>383</v>
       </c>
-      <c r="C184" s="2" t="s">
+      <c r="C184" t="s">
         <v>382</v>
       </c>
-      <c r="D184" s="2" t="s">
+      <c r="D184" t="s">
         <v>381</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix snippet mapping (#293)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21603"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21611"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526A2DAE-C8EA-481C-B570-4B7C84C4490E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E0597E-7224-4B4C-BDB2-4BD305FD028F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -1174,9 +1174,6 @@
     <t>details</t>
   </si>
   <si>
-    <t>autofilter</t>
-  </si>
-  <si>
     <t>addAutoFilter</t>
   </si>
   <si>
@@ -1187,6 +1184,9 @@
   </si>
   <si>
     <t>apply</t>
+  </si>
+  <si>
+    <t>autoFilter</t>
   </si>
 </sst>
 </file>
@@ -1603,7 +1603,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O178" sqref="O178"/>
+      <selection pane="bottomLeft" activeCell="B185" sqref="B185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4195,27 +4195,27 @@
         <v>47</v>
       </c>
       <c r="B185" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D185" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="C185" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="D185" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B186" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="B186" s="2" t="s">
-        <v>388</v>
-      </c>
       <c r="C186" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[excel] (PivotTable, Slicer) Adding a slicer snippet (#296)
* Adding slicer snippet

* Update with feedback
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21622"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E0597E-7224-4B4C-BDB2-4BD305FD028F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F59E074-53C6-400D-A0ED-0EAFB7EB43A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="401">
   <si>
     <t>Class</t>
   </si>
@@ -1187,6 +1187,42 @@
   </si>
   <si>
     <t>autoFilter</t>
+  </si>
+  <si>
+    <t>SlicerCollection</t>
+  </si>
+  <si>
+    <t>addSlicer</t>
+  </si>
+  <si>
+    <t>excel-pivottable-slicer</t>
+  </si>
+  <si>
+    <t>slicers</t>
+  </si>
+  <si>
+    <t>formatSlicer</t>
+  </si>
+  <si>
+    <t>applyStyle</t>
+  </si>
+  <si>
+    <t>Slicer</t>
+  </si>
+  <si>
+    <t>addFilters</t>
+  </si>
+  <si>
+    <t>selectItems</t>
+  </si>
+  <si>
+    <t>clearFilters</t>
+  </si>
+  <si>
+    <t>removeFilters</t>
+  </si>
+  <si>
+    <t>removeSlicer</t>
   </si>
 </sst>
 </file>
@@ -1266,11 +1302,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D186" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D186" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D183">
-    <sortCondition ref="A2:A183"/>
-    <sortCondition ref="B2:B183"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D193" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D193" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D193">
+    <sortCondition ref="A1:A193"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1599,11 +1634,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D186"/>
+  <dimension ref="A1:D193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B185" sqref="B185"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G144" sqref="G144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,31 +1678,31 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
+      <c r="A3" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1675,7 +1710,7 @@
         <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>61</v>
@@ -1686,16 +1721,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>145</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1703,69 +1738,69 @@
         <v>140</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C7" t="s">
         <v>144</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C8" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D8" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>208</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>149</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>150</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>185</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>136</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1773,13 +1808,13 @@
         <v>136</v>
       </c>
       <c r="B12" t="s">
-        <v>182</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>178</v>
+        <v>139</v>
       </c>
       <c r="D12" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1787,7 +1822,7 @@
         <v>136</v>
       </c>
       <c r="B13" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C13" t="s">
         <v>178</v>
@@ -1801,7 +1836,7 @@
         <v>136</v>
       </c>
       <c r="B14" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C14" t="s">
         <v>178</v>
@@ -1815,7 +1850,7 @@
         <v>136</v>
       </c>
       <c r="B15" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C15" t="s">
         <v>178</v>
@@ -1829,27 +1864,27 @@
         <v>136</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
+        <v>177</v>
       </c>
       <c r="C16" t="s">
-        <v>139</v>
+        <v>178</v>
       </c>
       <c r="D16" t="s">
-        <v>264</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>259</v>
+        <v>136</v>
       </c>
       <c r="B17" t="s">
-        <v>260</v>
+        <v>142</v>
       </c>
       <c r="C17" t="s">
-        <v>261</v>
+        <v>139</v>
       </c>
       <c r="D17" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1857,55 +1892,55 @@
         <v>259</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>260</v>
       </c>
       <c r="C18" t="s">
         <v>261</v>
       </c>
       <c r="D18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>259</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>131</v>
+        <v>261</v>
       </c>
       <c r="D19" t="s">
-        <v>133</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
         <v>131</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>134</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
         <v>131</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1919,35 +1954,35 @@
         <v>131</v>
       </c>
       <c r="D22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>134</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>373</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>376</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>367</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>375</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1955,13 +1990,13 @@
         <v>373</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>376</v>
       </c>
       <c r="C25" t="s">
         <v>367</v>
       </c>
       <c r="D25" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1969,41 +2004,41 @@
         <v>373</v>
       </c>
       <c r="B26" t="s">
-        <v>374</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
         <v>367</v>
       </c>
       <c r="D26" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>374</v>
       </c>
       <c r="C27" t="s">
         <v>367</v>
       </c>
       <c r="D27" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="B28" t="s">
-        <v>376</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
         <v>367</v>
       </c>
       <c r="D28" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2011,41 +2046,41 @@
         <v>377</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>376</v>
       </c>
       <c r="C29" t="s">
         <v>367</v>
       </c>
       <c r="D29" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
         <v>367</v>
       </c>
       <c r="D30" t="s">
-        <v>371</v>
+        <v>379</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>370</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>367</v>
       </c>
       <c r="D31" t="s">
-        <v>90</v>
+        <v>371</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2053,7 +2088,7 @@
         <v>91</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C32" t="s">
         <v>61</v>
@@ -2064,10 +2099,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
         <v>61</v>
@@ -2081,13 +2116,13 @@
         <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="C34" t="s">
         <v>61</v>
       </c>
       <c r="D34" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2095,13 +2130,13 @@
         <v>58</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
         <v>61</v>
       </c>
       <c r="D35" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2109,13 +2144,13 @@
         <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="C36" t="s">
         <v>61</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2123,13 +2158,13 @@
         <v>58</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
         <v>61</v>
       </c>
       <c r="D37" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2137,13 +2172,13 @@
         <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2151,13 +2186,13 @@
         <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
         <v>61</v>
       </c>
       <c r="D39" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2165,13 +2200,13 @@
         <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C40" t="s">
         <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2179,27 +2214,27 @@
         <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C41" t="s">
         <v>61</v>
       </c>
       <c r="D41" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="C42" t="s">
         <v>61</v>
       </c>
       <c r="D42" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2207,13 +2242,13 @@
         <v>56</v>
       </c>
       <c r="B43" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="C43" t="s">
         <v>61</v>
       </c>
       <c r="D43" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2221,32 +2256,32 @@
         <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C44" t="s">
         <v>61</v>
       </c>
       <c r="D44" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="C45" t="s">
         <v>61</v>
       </c>
       <c r="D45" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="B46" t="s">
         <v>14</v>
@@ -2255,7 +2290,7 @@
         <v>61</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2263,7 +2298,7 @@
         <v>78</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="C47" t="s">
         <v>61</v>
@@ -2283,7 +2318,7 @@
         <v>61</v>
       </c>
       <c r="D48" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2291,69 +2326,69 @@
         <v>78</v>
       </c>
       <c r="B49" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C49" t="s">
         <v>61</v>
       </c>
       <c r="D49" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C50" t="s">
         <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="B51" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="C51" t="s">
         <v>61</v>
       </c>
       <c r="D51" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B52" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C52" t="s">
         <v>61</v>
       </c>
       <c r="D52" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="B53" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C53" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D53" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2361,13 +2396,13 @@
         <v>34</v>
       </c>
       <c r="B54" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="C54" t="s">
         <v>35</v>
       </c>
       <c r="D54" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2375,7 +2410,7 @@
         <v>34</v>
       </c>
       <c r="B55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C55" t="s">
         <v>35</v>
@@ -2389,27 +2424,27 @@
         <v>34</v>
       </c>
       <c r="B56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C56" t="s">
         <v>35</v>
       </c>
       <c r="D56" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="C57" t="s">
         <v>35</v>
       </c>
       <c r="D57" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2417,13 +2452,13 @@
         <v>30</v>
       </c>
       <c r="B58" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D58" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2431,27 +2466,27 @@
         <v>30</v>
       </c>
       <c r="B59" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C59" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D59" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B60" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C60" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D60" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2459,13 +2494,13 @@
         <v>43</v>
       </c>
       <c r="B61" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C61" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D61" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2473,41 +2508,41 @@
         <v>43</v>
       </c>
       <c r="B62" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="C62" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D62" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="B63" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="C63" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D63" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>234</v>
+        <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>233</v>
+        <v>75</v>
       </c>
       <c r="C64" t="s">
-        <v>224</v>
+        <v>61</v>
       </c>
       <c r="D64" t="s">
-        <v>232</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2515,41 +2550,41 @@
         <v>234</v>
       </c>
       <c r="B65" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="C65" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="D65" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="B66" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="C66" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="D66" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="B67" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C67" t="s">
         <v>218</v>
       </c>
       <c r="D67" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2557,27 +2592,27 @@
         <v>253</v>
       </c>
       <c r="B68" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C68" t="s">
         <v>218</v>
       </c>
       <c r="D68" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>74</v>
+        <v>253</v>
       </c>
       <c r="B69" t="s">
-        <v>65</v>
+        <v>219</v>
       </c>
       <c r="C69" t="s">
-        <v>61</v>
+        <v>218</v>
       </c>
       <c r="D69" t="s">
-        <v>77</v>
+        <v>215</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2585,7 +2620,7 @@
         <v>74</v>
       </c>
       <c r="B70" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C70" t="s">
         <v>61</v>
@@ -2596,30 +2631,30 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>306</v>
+        <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C71" t="s">
-        <v>302</v>
+        <v>61</v>
       </c>
       <c r="D71" t="s">
-        <v>305</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
       <c r="B72" t="s">
-        <v>355</v>
+        <v>86</v>
       </c>
       <c r="C72" t="s">
-        <v>349</v>
+        <v>302</v>
       </c>
       <c r="D72" t="s">
-        <v>352</v>
+        <v>305</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2627,7 +2662,7 @@
         <v>354</v>
       </c>
       <c r="B73" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C73" t="s">
         <v>349</v>
@@ -2641,13 +2676,13 @@
         <v>354</v>
       </c>
       <c r="B74" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C74" t="s">
         <v>349</v>
       </c>
       <c r="D74" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2655,7 +2690,7 @@
         <v>354</v>
       </c>
       <c r="B75" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C75" t="s">
         <v>349</v>
@@ -2666,16 +2701,16 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>10</v>
+        <v>354</v>
       </c>
       <c r="B76" t="s">
-        <v>11</v>
+        <v>358</v>
       </c>
       <c r="C76" t="s">
-        <v>12</v>
+        <v>349</v>
       </c>
       <c r="D76" t="s">
-        <v>13</v>
+        <v>353</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2683,55 +2718,55 @@
         <v>10</v>
       </c>
       <c r="B77" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C77" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D77" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B78" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C78" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D78" t="s">
-        <v>265</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>320</v>
+        <v>8</v>
       </c>
       <c r="B79" t="s">
         <v>9</v>
       </c>
       <c r="C79" t="s">
-        <v>321</v>
+        <v>12</v>
       </c>
       <c r="D79" t="s">
-        <v>322</v>
+        <v>265</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B80" t="s">
-        <v>323</v>
+        <v>9</v>
       </c>
       <c r="C80" t="s">
         <v>321</v>
       </c>
       <c r="D80" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2739,7 +2774,7 @@
         <v>325</v>
       </c>
       <c r="B81" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C81" t="s">
         <v>321</v>
@@ -2753,13 +2788,13 @@
         <v>325</v>
       </c>
       <c r="B82" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C82" t="s">
         <v>321</v>
       </c>
       <c r="D82" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2767,13 +2802,13 @@
         <v>325</v>
       </c>
       <c r="B83" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C83" t="s">
         <v>321</v>
       </c>
       <c r="D83" t="s">
-        <v>329</v>
+        <v>341</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2781,41 +2816,41 @@
         <v>325</v>
       </c>
       <c r="B84" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C84" t="s">
         <v>321</v>
       </c>
       <c r="D84" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>239</v>
+        <v>325</v>
       </c>
       <c r="B85" t="s">
-        <v>240</v>
+        <v>327</v>
       </c>
       <c r="C85" t="s">
-        <v>243</v>
+        <v>321</v>
       </c>
       <c r="D85" t="s">
-        <v>241</v>
+        <v>328</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="B86" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="C86" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="D86" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2823,13 +2858,13 @@
         <v>226</v>
       </c>
       <c r="B87" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C87" t="s">
         <v>224</v>
       </c>
       <c r="D87" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2837,13 +2872,13 @@
         <v>226</v>
       </c>
       <c r="B88" t="s">
-        <v>11</v>
+        <v>230</v>
       </c>
       <c r="C88" t="s">
         <v>224</v>
       </c>
       <c r="D88" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2851,13 +2886,13 @@
         <v>226</v>
       </c>
       <c r="B89" t="s">
-        <v>237</v>
+        <v>11</v>
       </c>
       <c r="C89" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="D89" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2865,41 +2900,41 @@
         <v>226</v>
       </c>
       <c r="B90" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C90" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="D90" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B91" t="s">
-        <v>9</v>
+        <v>235</v>
       </c>
       <c r="C91" t="s">
         <v>224</v>
       </c>
       <c r="D91" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>64</v>
+        <v>223</v>
       </c>
       <c r="B92" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="C92" t="s">
-        <v>61</v>
+        <v>224</v>
       </c>
       <c r="D92" t="s">
-        <v>68</v>
+        <v>225</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2913,21 +2948,21 @@
         <v>61</v>
       </c>
       <c r="D93" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B94" t="s">
-        <v>286</v>
+        <v>69</v>
       </c>
       <c r="C94" t="s">
-        <v>299</v>
+        <v>61</v>
       </c>
       <c r="D94" t="s">
-        <v>287</v>
+        <v>95</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2935,13 +2970,13 @@
         <v>24</v>
       </c>
       <c r="B95" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C95" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D95" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2949,13 +2984,13 @@
         <v>24</v>
       </c>
       <c r="B96" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C96" t="s">
         <v>300</v>
       </c>
       <c r="D96" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2963,13 +2998,13 @@
         <v>24</v>
       </c>
       <c r="B97" t="s">
-        <v>27</v>
+        <v>290</v>
       </c>
       <c r="C97" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="D97" t="s">
-        <v>28</v>
+        <v>291</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2977,13 +3012,13 @@
         <v>24</v>
       </c>
       <c r="B98" t="s">
-        <v>276</v>
+        <v>27</v>
       </c>
       <c r="C98" t="s">
-        <v>297</v>
+        <v>255</v>
       </c>
       <c r="D98" t="s">
-        <v>277</v>
+        <v>28</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2991,13 +3026,13 @@
         <v>24</v>
       </c>
       <c r="B99" t="s">
-        <v>29</v>
+        <v>276</v>
       </c>
       <c r="C99" t="s">
-        <v>255</v>
+        <v>297</v>
       </c>
       <c r="D99" t="s">
-        <v>28</v>
+        <v>277</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -3005,13 +3040,13 @@
         <v>24</v>
       </c>
       <c r="B100" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C100" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="D100" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3019,13 +3054,13 @@
         <v>24</v>
       </c>
       <c r="B101" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="C101" t="s">
-        <v>104</v>
+        <v>268</v>
       </c>
       <c r="D101" t="s">
-        <v>105</v>
+        <v>26</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -3033,13 +3068,13 @@
         <v>24</v>
       </c>
       <c r="B102" t="s">
-        <v>333</v>
+        <v>103</v>
       </c>
       <c r="C102" t="s">
-        <v>332</v>
+        <v>104</v>
       </c>
       <c r="D102" t="s">
-        <v>331</v>
+        <v>105</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3047,13 +3082,13 @@
         <v>24</v>
       </c>
       <c r="B103" t="s">
-        <v>31</v>
+        <v>333</v>
       </c>
       <c r="C103" t="s">
-        <v>258</v>
+        <v>332</v>
       </c>
       <c r="D103" t="s">
-        <v>32</v>
+        <v>331</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -3067,7 +3102,7 @@
         <v>258</v>
       </c>
       <c r="D104" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3075,41 +3110,41 @@
         <v>24</v>
       </c>
       <c r="B105" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="C105" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D105" t="s">
-        <v>160</v>
+        <v>33</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>108</v>
+        <v>24</v>
       </c>
       <c r="B106" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="C106" t="s">
-        <v>114</v>
+        <v>256</v>
       </c>
       <c r="D106" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B107" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C107" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="D107" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -3117,13 +3152,13 @@
         <v>100</v>
       </c>
       <c r="B108" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C108" t="s">
         <v>104</v>
       </c>
       <c r="D108" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3131,13 +3166,13 @@
         <v>100</v>
       </c>
       <c r="B109" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C109" t="s">
         <v>104</v>
       </c>
       <c r="D109" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -3145,7 +3180,7 @@
         <v>100</v>
       </c>
       <c r="B110" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C110" t="s">
         <v>104</v>
@@ -3156,58 +3191,58 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>342</v>
+        <v>100</v>
       </c>
       <c r="B111" t="s">
-        <v>334</v>
+        <v>109</v>
       </c>
       <c r="C111" t="s">
-        <v>332</v>
+        <v>104</v>
       </c>
       <c r="D111" t="s">
-        <v>331</v>
+        <v>105</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>249</v>
+        <v>342</v>
       </c>
       <c r="B112" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="C112" t="s">
-        <v>251</v>
+        <v>332</v>
       </c>
       <c r="D112" t="s">
-        <v>252</v>
+        <v>331</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
       <c r="B113" t="s">
-        <v>11</v>
+        <v>250</v>
       </c>
       <c r="C113" t="s">
-        <v>21</v>
+        <v>251</v>
       </c>
       <c r="D113" t="s">
-        <v>22</v>
+        <v>252</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B114" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C114" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="D114" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3215,13 +3250,13 @@
         <v>17</v>
       </c>
       <c r="B115" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C115" t="s">
-        <v>21</v>
+        <v>266</v>
       </c>
       <c r="D115" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3229,27 +3264,27 @@
         <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C116" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="D116" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="B117" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C117" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
       <c r="D117" t="s">
-        <v>285</v>
+        <v>19</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3257,13 +3292,13 @@
         <v>278</v>
       </c>
       <c r="B118" t="s">
-        <v>284</v>
+        <v>11</v>
       </c>
       <c r="C118" t="s">
         <v>298</v>
       </c>
       <c r="D118" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3271,13 +3306,13 @@
         <v>278</v>
       </c>
       <c r="B119" t="s">
-        <v>366</v>
+        <v>284</v>
       </c>
       <c r="C119" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D119" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3285,13 +3320,13 @@
         <v>278</v>
       </c>
       <c r="B120" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C120" t="s">
-        <v>361</v>
+        <v>302</v>
       </c>
       <c r="D120" t="s">
-        <v>362</v>
+        <v>307</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3299,13 +3334,13 @@
         <v>278</v>
       </c>
       <c r="B121" t="s">
-        <v>311</v>
+        <v>363</v>
       </c>
       <c r="C121" t="s">
-        <v>313</v>
+        <v>361</v>
       </c>
       <c r="D121" t="s">
-        <v>314</v>
+        <v>362</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3313,13 +3348,13 @@
         <v>278</v>
       </c>
       <c r="B122" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="C122" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="D122" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3327,13 +3362,13 @@
         <v>278</v>
       </c>
       <c r="B123" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="C123" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D123" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3341,13 +3376,13 @@
         <v>278</v>
       </c>
       <c r="B124" t="s">
-        <v>134</v>
+        <v>312</v>
       </c>
       <c r="C124" t="s">
-        <v>349</v>
+        <v>313</v>
       </c>
       <c r="D124" t="s">
-        <v>351</v>
+        <v>315</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3355,13 +3390,13 @@
         <v>278</v>
       </c>
       <c r="B125" t="s">
-        <v>279</v>
+        <v>134</v>
       </c>
       <c r="C125" t="s">
-        <v>298</v>
+        <v>349</v>
       </c>
       <c r="D125" t="s">
-        <v>280</v>
+        <v>351</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3369,13 +3404,13 @@
         <v>278</v>
       </c>
       <c r="B126" t="s">
-        <v>319</v>
+        <v>279</v>
       </c>
       <c r="C126" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="D126" t="s">
-        <v>316</v>
+        <v>280</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3383,7 +3418,7 @@
         <v>278</v>
       </c>
       <c r="B127" t="s">
-        <v>380</v>
+        <v>319</v>
       </c>
       <c r="C127" t="s">
         <v>313</v>
@@ -3397,27 +3432,27 @@
         <v>278</v>
       </c>
       <c r="B128" t="s">
-        <v>318</v>
+        <v>380</v>
       </c>
       <c r="C128" t="s">
         <v>313</v>
       </c>
       <c r="D128" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B129" t="s">
-        <v>282</v>
+        <v>318</v>
       </c>
       <c r="C129" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="D129" t="s">
-        <v>340</v>
+        <v>317</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3425,13 +3460,13 @@
         <v>281</v>
       </c>
       <c r="B130" t="s">
-        <v>364</v>
+        <v>282</v>
       </c>
       <c r="C130" t="s">
-        <v>361</v>
+        <v>298</v>
       </c>
       <c r="D130" t="s">
-        <v>365</v>
+        <v>340</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3439,13 +3474,13 @@
         <v>281</v>
       </c>
       <c r="B131" t="s">
-        <v>294</v>
+        <v>364</v>
       </c>
       <c r="C131" t="s">
-        <v>302</v>
+        <v>361</v>
       </c>
       <c r="D131" t="s">
-        <v>295</v>
+        <v>365</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3453,13 +3488,13 @@
         <v>281</v>
       </c>
       <c r="B132" t="s">
-        <v>348</v>
+        <v>294</v>
       </c>
       <c r="C132" t="s">
-        <v>349</v>
+        <v>302</v>
       </c>
       <c r="D132" t="s">
-        <v>350</v>
+        <v>295</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3467,388 +3502,388 @@
         <v>281</v>
       </c>
       <c r="B133" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="C133" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="D133" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>359</v>
+        <v>281</v>
       </c>
       <c r="B134" t="s">
-        <v>360</v>
+        <v>343</v>
       </c>
       <c r="C134" t="s">
-        <v>361</v>
+        <v>344</v>
       </c>
       <c r="D134" t="s">
-        <v>362</v>
+        <v>345</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>246</v>
+        <v>359</v>
       </c>
       <c r="B135" t="s">
-        <v>247</v>
+        <v>360</v>
       </c>
       <c r="C135" t="s">
-        <v>244</v>
+        <v>361</v>
       </c>
       <c r="D135" t="s">
-        <v>248</v>
+        <v>362</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>152</v>
+        <v>246</v>
       </c>
       <c r="B136" t="s">
+        <v>247</v>
+      </c>
+      <c r="C136" t="s">
+        <v>244</v>
+      </c>
+      <c r="D136" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B140" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C136" t="s">
-        <v>256</v>
-      </c>
-      <c r="D136" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>152</v>
-      </c>
-      <c r="B137" t="s">
-        <v>149</v>
-      </c>
-      <c r="C137" t="s">
-        <v>256</v>
-      </c>
-      <c r="D137" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>152</v>
-      </c>
-      <c r="B138" t="s">
-        <v>164</v>
-      </c>
-      <c r="C138" t="s">
-        <v>256</v>
-      </c>
-      <c r="D138" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>152</v>
-      </c>
-      <c r="B139" t="s">
-        <v>209</v>
-      </c>
-      <c r="C139" t="s">
-        <v>256</v>
-      </c>
-      <c r="D139" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>156</v>
-      </c>
-      <c r="B140" t="s">
+      <c r="C140" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C140" t="s">
-        <v>256</v>
-      </c>
-      <c r="D140" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>156</v>
-      </c>
-      <c r="B141" t="s">
+      <c r="C141" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C141" t="s">
-        <v>256</v>
-      </c>
-      <c r="D141" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>211</v>
-      </c>
-      <c r="B142" t="s">
-        <v>188</v>
-      </c>
-      <c r="C142" t="s">
-        <v>186</v>
-      </c>
-      <c r="D142" t="s">
-        <v>187</v>
+      <c r="C142" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>211</v>
+        <v>152</v>
       </c>
       <c r="B143" t="s">
-        <v>167</v>
+        <v>11</v>
       </c>
       <c r="C143" t="s">
-        <v>186</v>
+        <v>256</v>
       </c>
       <c r="D143" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="B144" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="C144" t="s">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="D144" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="B145" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C145" t="s">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="D145" t="s">
-        <v>189</v>
+        <v>160</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>213</v>
+        <v>152</v>
       </c>
       <c r="B146" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="C146" t="s">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="D146" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>210</v>
+        <v>156</v>
       </c>
       <c r="B147" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="C147" t="s">
-        <v>186</v>
+        <v>256</v>
       </c>
       <c r="D147" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="B148" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="C148" t="s">
-        <v>61</v>
+        <v>256</v>
       </c>
       <c r="D148" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>82</v>
+        <v>211</v>
       </c>
       <c r="B149" t="s">
-        <v>69</v>
+        <v>188</v>
       </c>
       <c r="C149" t="s">
-        <v>61</v>
+        <v>186</v>
       </c>
       <c r="D149" t="s">
-        <v>84</v>
+        <v>187</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>347</v>
+        <v>211</v>
       </c>
       <c r="B150" t="s">
-        <v>346</v>
+        <v>167</v>
       </c>
       <c r="C150" t="s">
-        <v>344</v>
+        <v>186</v>
       </c>
       <c r="D150" t="s">
-        <v>346</v>
+        <v>168</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="B151" t="s">
-        <v>338</v>
+        <v>184</v>
       </c>
       <c r="C151" t="s">
-        <v>336</v>
+        <v>183</v>
       </c>
       <c r="D151" t="s">
-        <v>339</v>
+        <v>189</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="B152" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="C152" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D152" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="B153" t="s">
-        <v>272</v>
+        <v>383</v>
       </c>
       <c r="C153" t="s">
-        <v>297</v>
+        <v>382</v>
       </c>
       <c r="D153" t="s">
-        <v>273</v>
+        <v>381</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="B154" t="s">
-        <v>157</v>
+        <v>188</v>
       </c>
       <c r="C154" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="D154" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B155" t="s">
-        <v>335</v>
+        <v>106</v>
       </c>
       <c r="C155" t="s">
-        <v>336</v>
+        <v>186</v>
       </c>
       <c r="D155" t="s">
-        <v>337</v>
+        <v>166</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>206</v>
+        <v>82</v>
       </c>
       <c r="B156" t="s">
-        <v>195</v>
+        <v>86</v>
       </c>
       <c r="C156" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D156" t="s">
-        <v>197</v>
+        <v>84</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>206</v>
+        <v>82</v>
       </c>
       <c r="B157" t="s">
-        <v>195</v>
+        <v>69</v>
       </c>
       <c r="C157" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D157" t="s">
-        <v>204</v>
+        <v>84</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>206</v>
+        <v>347</v>
       </c>
       <c r="B158" t="s">
-        <v>199</v>
+        <v>346</v>
       </c>
       <c r="C158" t="s">
-        <v>254</v>
+        <v>344</v>
       </c>
       <c r="D158" t="s">
-        <v>201</v>
+        <v>346</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B159" t="s">
-        <v>199</v>
+        <v>338</v>
       </c>
       <c r="C159" t="s">
-        <v>254</v>
+        <v>336</v>
       </c>
       <c r="D159" t="s">
-        <v>205</v>
+        <v>339</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="B160" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C160" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D160" t="s">
         <v>198</v>
@@ -3856,136 +3891,136 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="B161" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="C161" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D161" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="B162" t="s">
-        <v>54</v>
+        <v>157</v>
       </c>
       <c r="C162" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="D162" t="s">
-        <v>55</v>
+        <v>159</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="B163" t="s">
-        <v>51</v>
+        <v>335</v>
       </c>
       <c r="C163" t="s">
-        <v>52</v>
+        <v>336</v>
       </c>
       <c r="D163" t="s">
-        <v>53</v>
+        <v>337</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B164" t="s">
-        <v>275</v>
+        <v>195</v>
       </c>
       <c r="C164" t="s">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="D164" t="s">
-        <v>274</v>
+        <v>197</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B165" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C165" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="D165" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B166" t="s">
-        <v>125</v>
+        <v>199</v>
       </c>
       <c r="C166" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D166" t="s">
-        <v>125</v>
+        <v>201</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B167" t="s">
-        <v>127</v>
+        <v>199</v>
       </c>
       <c r="C167" t="s">
-        <v>128</v>
+        <v>254</v>
       </c>
       <c r="D167" t="s">
-        <v>129</v>
+        <v>205</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>212</v>
+        <v>47</v>
       </c>
       <c r="B168" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="C168" t="s">
-        <v>266</v>
+        <v>194</v>
       </c>
       <c r="D168" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B169" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="C169" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D169" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B170" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C170" t="s">
         <v>52</v>
@@ -3996,226 +4031,324 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B171" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C171" t="s">
         <v>52</v>
       </c>
       <c r="D171" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B172" t="s">
-        <v>175</v>
+        <v>275</v>
       </c>
       <c r="C172" t="s">
-        <v>266</v>
+        <v>297</v>
       </c>
       <c r="D172" t="s">
-        <v>176</v>
+        <v>274</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B173" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="C173" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D173" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B174" t="s">
-        <v>173</v>
+        <v>125</v>
       </c>
       <c r="C174" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="D174" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>110</v>
+        <v>47</v>
       </c>
       <c r="B175" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="C175" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="D175" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>110</v>
-      </c>
-      <c r="B176" t="s">
-        <v>118</v>
-      </c>
-      <c r="C176" t="s">
-        <v>117</v>
-      </c>
-      <c r="D176" t="s">
-        <v>118</v>
+      <c r="A176" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>110</v>
-      </c>
-      <c r="B177" t="s">
-        <v>119</v>
-      </c>
-      <c r="C177" t="s">
-        <v>117</v>
-      </c>
-      <c r="D177" t="s">
-        <v>119</v>
+      <c r="A177" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D177" s="2" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>110</v>
+        <v>212</v>
       </c>
       <c r="B178" t="s">
-        <v>120</v>
+        <v>171</v>
       </c>
       <c r="C178" t="s">
-        <v>117</v>
+        <v>266</v>
       </c>
       <c r="D178" t="s">
-        <v>121</v>
+        <v>172</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B179" t="s">
-        <v>122</v>
+        <v>309</v>
       </c>
       <c r="C179" t="s">
-        <v>117</v>
+        <v>310</v>
       </c>
       <c r="D179" t="s">
-        <v>123</v>
+        <v>308</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>207</v>
+        <v>50</v>
       </c>
       <c r="B180" t="s">
-        <v>195</v>
+        <v>57</v>
       </c>
       <c r="C180" t="s">
-        <v>254</v>
+        <v>52</v>
       </c>
       <c r="D180" t="s">
-        <v>196</v>
+        <v>55</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>207</v>
+        <v>50</v>
       </c>
       <c r="B181" t="s">
-        <v>195</v>
+        <v>59</v>
       </c>
       <c r="C181" t="s">
-        <v>254</v>
+        <v>52</v>
       </c>
       <c r="D181" t="s">
-        <v>202</v>
+        <v>55</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>207</v>
+        <v>50</v>
       </c>
       <c r="B182" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="C182" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="D182" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>207</v>
+        <v>50</v>
       </c>
       <c r="B183" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="C183" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="D183" t="s">
-        <v>203</v>
+        <v>170</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>214</v>
+        <v>50</v>
       </c>
       <c r="B184" t="s">
-        <v>383</v>
+        <v>173</v>
       </c>
       <c r="C184" t="s">
-        <v>382</v>
+        <v>266</v>
       </c>
       <c r="D184" t="s">
-        <v>381</v>
+        <v>174</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B185" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="C185" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="D185" s="2" t="s">
-        <v>384</v>
+      <c r="A185" t="s">
+        <v>110</v>
+      </c>
+      <c r="B185" t="s">
+        <v>116</v>
+      </c>
+      <c r="C185" t="s">
+        <v>117</v>
+      </c>
+      <c r="D185" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="C186" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="D186" s="2" t="s">
-        <v>384</v>
+      <c r="A186" t="s">
+        <v>110</v>
+      </c>
+      <c r="B186" t="s">
+        <v>118</v>
+      </c>
+      <c r="C186" t="s">
+        <v>117</v>
+      </c>
+      <c r="D186" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>110</v>
+      </c>
+      <c r="B187" t="s">
+        <v>119</v>
+      </c>
+      <c r="C187" t="s">
+        <v>117</v>
+      </c>
+      <c r="D187" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>110</v>
+      </c>
+      <c r="B188" t="s">
+        <v>120</v>
+      </c>
+      <c r="C188" t="s">
+        <v>117</v>
+      </c>
+      <c r="D188" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>110</v>
+      </c>
+      <c r="B189" t="s">
+        <v>122</v>
+      </c>
+      <c r="C189" t="s">
+        <v>117</v>
+      </c>
+      <c r="D189" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>207</v>
+      </c>
+      <c r="B190" t="s">
+        <v>195</v>
+      </c>
+      <c r="C190" t="s">
+        <v>254</v>
+      </c>
+      <c r="D190" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>207</v>
+      </c>
+      <c r="B191" t="s">
+        <v>195</v>
+      </c>
+      <c r="C191" t="s">
+        <v>254</v>
+      </c>
+      <c r="D191" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>207</v>
+      </c>
+      <c r="B192" t="s">
+        <v>199</v>
+      </c>
+      <c r="C192" t="s">
+        <v>254</v>
+      </c>
+      <c r="D192" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>207</v>
+      </c>
+      <c r="B193" t="s">
+        <v>199</v>
+      </c>
+      <c r="C193" t="s">
+        <v>254</v>
+      </c>
+      <c r="D193" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pulling Excel 1.9 snippets into release
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21622"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F59E074-53C6-400D-A0ED-0EAFB7EB43A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C867E7-84CE-4D73-9FF0-25CF61442C27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-36015" yWindow="0" windowWidth="33750" windowHeight="21000" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="403">
   <si>
     <t>Class</t>
   </si>
@@ -1223,6 +1223,12 @@
   </si>
   <si>
     <t>removeSlicer</t>
+  </si>
+  <si>
+    <t>RangeAreas</t>
+  </si>
+  <si>
+    <t>colorAllFormulaRanges</t>
   </si>
 </sst>
 </file>
@@ -1302,10 +1308,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D193" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D193" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D193">
-    <sortCondition ref="A1:A193"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D194" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D194" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D195">
+    <sortCondition ref="A1:A195"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1614,7 +1620,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="6">
+  <wetp:taskpane dockstate="right" visibility="0" width="700" row="7">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1634,11 +1640,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D193"/>
+  <dimension ref="A1:D194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G144" sqref="G144"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A195" sqref="A195:XFD195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3134,31 +3140,31 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>108</v>
-      </c>
-      <c r="B107" t="s">
-        <v>113</v>
-      </c>
-      <c r="C107" t="s">
-        <v>114</v>
-      </c>
-      <c r="D107" t="s">
-        <v>115</v>
+      <c r="A107" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C108" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="D108" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3166,13 +3172,13 @@
         <v>100</v>
       </c>
       <c r="B109" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C109" t="s">
         <v>104</v>
       </c>
       <c r="D109" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -3180,13 +3186,13 @@
         <v>100</v>
       </c>
       <c r="B110" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C110" t="s">
         <v>104</v>
       </c>
       <c r="D110" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -3194,7 +3200,7 @@
         <v>100</v>
       </c>
       <c r="B111" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C111" t="s">
         <v>104</v>
@@ -3205,58 +3211,58 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>342</v>
+        <v>100</v>
       </c>
       <c r="B112" t="s">
-        <v>334</v>
+        <v>109</v>
       </c>
       <c r="C112" t="s">
-        <v>332</v>
+        <v>104</v>
       </c>
       <c r="D112" t="s">
-        <v>331</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>249</v>
+        <v>342</v>
       </c>
       <c r="B113" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="C113" t="s">
-        <v>251</v>
+        <v>332</v>
       </c>
       <c r="D113" t="s">
-        <v>252</v>
+        <v>331</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
       <c r="B114" t="s">
-        <v>11</v>
+        <v>250</v>
       </c>
       <c r="C114" t="s">
-        <v>21</v>
+        <v>251</v>
       </c>
       <c r="D114" t="s">
-        <v>22</v>
+        <v>252</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B115" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C115" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="D115" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3264,13 +3270,13 @@
         <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C116" t="s">
-        <v>21</v>
+        <v>266</v>
       </c>
       <c r="D116" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3278,27 +3284,27 @@
         <v>17</v>
       </c>
       <c r="B117" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C117" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="D117" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="B118" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C118" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
       <c r="D118" t="s">
-        <v>285</v>
+        <v>19</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3306,13 +3312,13 @@
         <v>278</v>
       </c>
       <c r="B119" t="s">
-        <v>284</v>
+        <v>11</v>
       </c>
       <c r="C119" t="s">
         <v>298</v>
       </c>
       <c r="D119" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3320,13 +3326,13 @@
         <v>278</v>
       </c>
       <c r="B120" t="s">
-        <v>366</v>
+        <v>284</v>
       </c>
       <c r="C120" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D120" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3334,13 +3340,13 @@
         <v>278</v>
       </c>
       <c r="B121" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C121" t="s">
-        <v>361</v>
+        <v>302</v>
       </c>
       <c r="D121" t="s">
-        <v>362</v>
+        <v>307</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3348,13 +3354,13 @@
         <v>278</v>
       </c>
       <c r="B122" t="s">
-        <v>311</v>
+        <v>363</v>
       </c>
       <c r="C122" t="s">
-        <v>313</v>
+        <v>361</v>
       </c>
       <c r="D122" t="s">
-        <v>314</v>
+        <v>362</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3362,13 +3368,13 @@
         <v>278</v>
       </c>
       <c r="B123" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="C123" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="D123" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3376,13 +3382,13 @@
         <v>278</v>
       </c>
       <c r="B124" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="C124" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D124" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3390,13 +3396,13 @@
         <v>278</v>
       </c>
       <c r="B125" t="s">
-        <v>134</v>
+        <v>312</v>
       </c>
       <c r="C125" t="s">
-        <v>349</v>
+        <v>313</v>
       </c>
       <c r="D125" t="s">
-        <v>351</v>
+        <v>315</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3404,13 +3410,13 @@
         <v>278</v>
       </c>
       <c r="B126" t="s">
-        <v>279</v>
+        <v>134</v>
       </c>
       <c r="C126" t="s">
-        <v>298</v>
+        <v>349</v>
       </c>
       <c r="D126" t="s">
-        <v>280</v>
+        <v>351</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3418,13 +3424,13 @@
         <v>278</v>
       </c>
       <c r="B127" t="s">
-        <v>319</v>
+        <v>279</v>
       </c>
       <c r="C127" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="D127" t="s">
-        <v>316</v>
+        <v>280</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3432,7 +3438,7 @@
         <v>278</v>
       </c>
       <c r="B128" t="s">
-        <v>380</v>
+        <v>319</v>
       </c>
       <c r="C128" t="s">
         <v>313</v>
@@ -3446,27 +3452,27 @@
         <v>278</v>
       </c>
       <c r="B129" t="s">
-        <v>318</v>
+        <v>380</v>
       </c>
       <c r="C129" t="s">
         <v>313</v>
       </c>
       <c r="D129" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B130" t="s">
-        <v>282</v>
+        <v>318</v>
       </c>
       <c r="C130" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="D130" t="s">
-        <v>340</v>
+        <v>317</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3474,13 +3480,13 @@
         <v>281</v>
       </c>
       <c r="B131" t="s">
-        <v>364</v>
+        <v>282</v>
       </c>
       <c r="C131" t="s">
-        <v>361</v>
+        <v>298</v>
       </c>
       <c r="D131" t="s">
-        <v>365</v>
+        <v>340</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3488,13 +3494,13 @@
         <v>281</v>
       </c>
       <c r="B132" t="s">
-        <v>294</v>
+        <v>364</v>
       </c>
       <c r="C132" t="s">
-        <v>302</v>
+        <v>361</v>
       </c>
       <c r="D132" t="s">
-        <v>295</v>
+        <v>365</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3502,13 +3508,13 @@
         <v>281</v>
       </c>
       <c r="B133" t="s">
-        <v>348</v>
+        <v>294</v>
       </c>
       <c r="C133" t="s">
-        <v>349</v>
+        <v>302</v>
       </c>
       <c r="D133" t="s">
-        <v>350</v>
+        <v>295</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3516,55 +3522,55 @@
         <v>281</v>
       </c>
       <c r="B134" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="C134" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="D134" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>359</v>
+        <v>281</v>
       </c>
       <c r="B135" t="s">
-        <v>360</v>
+        <v>343</v>
       </c>
       <c r="C135" t="s">
-        <v>361</v>
+        <v>344</v>
       </c>
       <c r="D135" t="s">
-        <v>362</v>
+        <v>345</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>359</v>
+      </c>
+      <c r="B136" t="s">
+        <v>360</v>
+      </c>
+      <c r="C136" t="s">
+        <v>361</v>
+      </c>
+      <c r="D136" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>246</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B137" t="s">
         <v>247</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C137" t="s">
         <v>244</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D137" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3572,13 +3578,13 @@
         <v>395</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>397</v>
+        <v>79</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>391</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3586,13 +3592,13 @@
         <v>395</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>391</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3600,27 +3606,27 @@
         <v>395</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>11</v>
+        <v>398</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>391</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>391</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3628,27 +3634,27 @@
         <v>389</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>391</v>
       </c>
       <c r="D142" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D143" s="2" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>152</v>
-      </c>
-      <c r="B143" t="s">
-        <v>11</v>
-      </c>
-      <c r="C143" t="s">
-        <v>256</v>
-      </c>
-      <c r="D143" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -3656,13 +3662,13 @@
         <v>152</v>
       </c>
       <c r="B144" t="s">
-        <v>149</v>
+        <v>11</v>
       </c>
       <c r="C144" t="s">
         <v>256</v>
       </c>
       <c r="D144" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3670,13 +3676,13 @@
         <v>152</v>
       </c>
       <c r="B145" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="C145" t="s">
         <v>256</v>
       </c>
       <c r="D145" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3684,27 +3690,27 @@
         <v>152</v>
       </c>
       <c r="B146" t="s">
-        <v>209</v>
+        <v>164</v>
       </c>
       <c r="C146" t="s">
         <v>256</v>
       </c>
       <c r="D146" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B147" t="s">
-        <v>9</v>
+        <v>209</v>
       </c>
       <c r="C147" t="s">
         <v>256</v>
       </c>
       <c r="D147" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -3712,7 +3718,7 @@
         <v>156</v>
       </c>
       <c r="B148" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C148" t="s">
         <v>256</v>
@@ -3723,16 +3729,16 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>211</v>
+        <v>156</v>
       </c>
       <c r="B149" t="s">
-        <v>188</v>
+        <v>37</v>
       </c>
       <c r="C149" t="s">
-        <v>186</v>
+        <v>256</v>
       </c>
       <c r="D149" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -3740,27 +3746,27 @@
         <v>211</v>
       </c>
       <c r="B150" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="C150" t="s">
         <v>186</v>
       </c>
       <c r="D150" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B151" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="C151" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D151" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -3768,7 +3774,7 @@
         <v>214</v>
       </c>
       <c r="B152" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="C152" t="s">
         <v>183</v>
@@ -3782,55 +3788,55 @@
         <v>214</v>
       </c>
       <c r="B153" t="s">
-        <v>383</v>
+        <v>171</v>
       </c>
       <c r="C153" t="s">
-        <v>382</v>
+        <v>183</v>
       </c>
       <c r="D153" t="s">
-        <v>381</v>
+        <v>189</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B154" t="s">
-        <v>188</v>
+        <v>383</v>
       </c>
       <c r="C154" t="s">
-        <v>183</v>
+        <v>382</v>
       </c>
       <c r="D154" t="s">
-        <v>187</v>
+        <v>381</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B155" t="s">
-        <v>106</v>
+        <v>188</v>
       </c>
       <c r="C155" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D155" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>82</v>
+        <v>210</v>
       </c>
       <c r="B156" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C156" t="s">
-        <v>61</v>
+        <v>186</v>
       </c>
       <c r="D156" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -3838,7 +3844,7 @@
         <v>82</v>
       </c>
       <c r="B157" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C157" t="s">
         <v>61</v>
@@ -3849,30 +3855,30 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>347</v>
+        <v>82</v>
       </c>
       <c r="B158" t="s">
-        <v>346</v>
+        <v>69</v>
       </c>
       <c r="C158" t="s">
-        <v>344</v>
+        <v>61</v>
       </c>
       <c r="D158" t="s">
-        <v>346</v>
+        <v>84</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>190</v>
+        <v>347</v>
       </c>
       <c r="B159" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="C159" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="D159" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -3880,13 +3886,13 @@
         <v>190</v>
       </c>
       <c r="B160" t="s">
-        <v>191</v>
+        <v>338</v>
       </c>
       <c r="C160" t="s">
-        <v>192</v>
+        <v>336</v>
       </c>
       <c r="D160" t="s">
-        <v>198</v>
+        <v>339</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -3894,13 +3900,13 @@
         <v>190</v>
       </c>
       <c r="B161" t="s">
-        <v>272</v>
+        <v>191</v>
       </c>
       <c r="C161" t="s">
-        <v>297</v>
+        <v>192</v>
       </c>
       <c r="D161" t="s">
-        <v>273</v>
+        <v>198</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -3908,13 +3914,13 @@
         <v>190</v>
       </c>
       <c r="B162" t="s">
-        <v>157</v>
+        <v>272</v>
       </c>
       <c r="C162" t="s">
-        <v>158</v>
+        <v>297</v>
       </c>
       <c r="D162" t="s">
-        <v>159</v>
+        <v>273</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -3922,27 +3928,27 @@
         <v>190</v>
       </c>
       <c r="B163" t="s">
-        <v>335</v>
+        <v>157</v>
       </c>
       <c r="C163" t="s">
-        <v>336</v>
+        <v>158</v>
       </c>
       <c r="D163" t="s">
-        <v>337</v>
+        <v>159</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B164" t="s">
-        <v>195</v>
+        <v>335</v>
       </c>
       <c r="C164" t="s">
-        <v>254</v>
+        <v>336</v>
       </c>
       <c r="D164" t="s">
-        <v>197</v>
+        <v>337</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -3956,7 +3962,7 @@
         <v>254</v>
       </c>
       <c r="D165" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -3964,13 +3970,13 @@
         <v>206</v>
       </c>
       <c r="B166" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C166" t="s">
         <v>254</v>
       </c>
       <c r="D166" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -3984,21 +3990,21 @@
         <v>254</v>
       </c>
       <c r="D167" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B168" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C168" t="s">
-        <v>194</v>
+        <v>254</v>
       </c>
       <c r="D168" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4006,13 +4012,13 @@
         <v>47</v>
       </c>
       <c r="B169" t="s">
-        <v>292</v>
+        <v>193</v>
       </c>
       <c r="C169" t="s">
-        <v>301</v>
+        <v>194</v>
       </c>
       <c r="D169" t="s">
-        <v>293</v>
+        <v>198</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4020,13 +4026,13 @@
         <v>47</v>
       </c>
       <c r="B170" t="s">
-        <v>54</v>
+        <v>292</v>
       </c>
       <c r="C170" t="s">
-        <v>52</v>
+        <v>301</v>
       </c>
       <c r="D170" t="s">
-        <v>55</v>
+        <v>293</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4034,13 +4040,13 @@
         <v>47</v>
       </c>
       <c r="B171" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C171" t="s">
         <v>52</v>
       </c>
       <c r="D171" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4048,13 +4054,13 @@
         <v>47</v>
       </c>
       <c r="B172" t="s">
-        <v>275</v>
+        <v>51</v>
       </c>
       <c r="C172" t="s">
-        <v>297</v>
+        <v>52</v>
       </c>
       <c r="D172" t="s">
-        <v>274</v>
+        <v>53</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4062,13 +4068,13 @@
         <v>47</v>
       </c>
       <c r="B173" t="s">
-        <v>188</v>
+        <v>275</v>
       </c>
       <c r="C173" t="s">
-        <v>267</v>
+        <v>297</v>
       </c>
       <c r="D173" t="s">
-        <v>187</v>
+        <v>274</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4076,13 +4082,13 @@
         <v>47</v>
       </c>
       <c r="B174" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
       <c r="C174" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="D174" t="s">
-        <v>125</v>
+        <v>187</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4090,27 +4096,27 @@
         <v>47</v>
       </c>
       <c r="B175" t="s">
+        <v>125</v>
+      </c>
+      <c r="C175" t="s">
+        <v>257</v>
+      </c>
+      <c r="D175" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>47</v>
+      </c>
+      <c r="B176" t="s">
         <v>127</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C176" t="s">
         <v>128</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D176" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="D176" s="2" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4118,41 +4124,41 @@
         <v>47</v>
       </c>
       <c r="B177" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D177" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B178" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="C177" s="2" t="s">
+      <c r="C178" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="D177" s="2" t="s">
+      <c r="D178" s="2" t="s">
         <v>390</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>212</v>
-      </c>
-      <c r="B178" t="s">
-        <v>171</v>
-      </c>
-      <c r="C178" t="s">
-        <v>266</v>
-      </c>
-      <c r="D178" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>50</v>
+        <v>212</v>
       </c>
       <c r="B179" t="s">
-        <v>309</v>
+        <v>171</v>
       </c>
       <c r="C179" t="s">
-        <v>310</v>
+        <v>266</v>
       </c>
       <c r="D179" t="s">
-        <v>308</v>
+        <v>172</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4160,13 +4166,13 @@
         <v>50</v>
       </c>
       <c r="B180" t="s">
-        <v>57</v>
+        <v>309</v>
       </c>
       <c r="C180" t="s">
-        <v>52</v>
+        <v>310</v>
       </c>
       <c r="D180" t="s">
-        <v>55</v>
+        <v>308</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4174,7 +4180,7 @@
         <v>50</v>
       </c>
       <c r="B181" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C181" t="s">
         <v>52</v>
@@ -4188,13 +4194,13 @@
         <v>50</v>
       </c>
       <c r="B182" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="C182" t="s">
-        <v>266</v>
+        <v>52</v>
       </c>
       <c r="D182" t="s">
-        <v>176</v>
+        <v>55</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4202,13 +4208,13 @@
         <v>50</v>
       </c>
       <c r="B183" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C183" t="s">
         <v>266</v>
       </c>
       <c r="D183" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4216,27 +4222,27 @@
         <v>50</v>
       </c>
       <c r="B184" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C184" t="s">
         <v>266</v>
       </c>
       <c r="D184" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B185" t="s">
-        <v>116</v>
+        <v>173</v>
       </c>
       <c r="C185" t="s">
-        <v>117</v>
+        <v>266</v>
       </c>
       <c r="D185" t="s">
-        <v>116</v>
+        <v>174</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4244,13 +4250,13 @@
         <v>110</v>
       </c>
       <c r="B186" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C186" t="s">
         <v>117</v>
       </c>
       <c r="D186" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4258,13 +4264,13 @@
         <v>110</v>
       </c>
       <c r="B187" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C187" t="s">
         <v>117</v>
       </c>
       <c r="D187" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4272,13 +4278,13 @@
         <v>110</v>
       </c>
       <c r="B188" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C188" t="s">
         <v>117</v>
       </c>
       <c r="D188" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4286,27 +4292,27 @@
         <v>110</v>
       </c>
       <c r="B189" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C189" t="s">
         <v>117</v>
       </c>
       <c r="D189" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>207</v>
+        <v>110</v>
       </c>
       <c r="B190" t="s">
-        <v>195</v>
+        <v>122</v>
       </c>
       <c r="C190" t="s">
-        <v>254</v>
+        <v>117</v>
       </c>
       <c r="D190" t="s">
-        <v>196</v>
+        <v>123</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -4320,7 +4326,7 @@
         <v>254</v>
       </c>
       <c r="D191" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4328,13 +4334,13 @@
         <v>207</v>
       </c>
       <c r="B192" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C192" t="s">
         <v>254</v>
       </c>
       <c r="D192" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -4348,6 +4354,20 @@
         <v>254</v>
       </c>
       <c r="D193" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>207</v>
+      </c>
+      <c r="B194" t="s">
+        <v>199</v>
+      </c>
+      <c r="C194" t="s">
+        <v>254</v>
+      </c>
+      <c r="D194" t="s">
         <v>203</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[excel] (ExcelApi 1.9) Moving 1.9 snipets out of preview (#300)
* Merging to prod (#291)

* Fixed Errors in README.md (#278)

- Hedging
- Remove pronouns for clarity
- Removed excess use of that
- Removed contractions to make more formal

* [excel] (Worksheet) Adding a sample for a worksheet autofilter (#290)

* Adding a sample for a worksheet autofilter

* Simplifying setup code

* Pulling Excel 1.9 snippets into release
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21622"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F59E074-53C6-400D-A0ED-0EAFB7EB43A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C867E7-84CE-4D73-9FF0-25CF61442C27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-36015" yWindow="0" windowWidth="33750" windowHeight="21000" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="403">
   <si>
     <t>Class</t>
   </si>
@@ -1223,6 +1223,12 @@
   </si>
   <si>
     <t>removeSlicer</t>
+  </si>
+  <si>
+    <t>RangeAreas</t>
+  </si>
+  <si>
+    <t>colorAllFormulaRanges</t>
   </si>
 </sst>
 </file>
@@ -1302,10 +1308,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D193" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D193" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D193">
-    <sortCondition ref="A1:A193"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D194" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D194" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D195">
+    <sortCondition ref="A1:A195"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1614,7 +1620,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="6">
+  <wetp:taskpane dockstate="right" visibility="0" width="700" row="7">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1634,11 +1640,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D193"/>
+  <dimension ref="A1:D194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G144" sqref="G144"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A195" sqref="A195:XFD195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3134,31 +3140,31 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>108</v>
-      </c>
-      <c r="B107" t="s">
-        <v>113</v>
-      </c>
-      <c r="C107" t="s">
-        <v>114</v>
-      </c>
-      <c r="D107" t="s">
-        <v>115</v>
+      <c r="A107" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C108" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="D108" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3166,13 +3172,13 @@
         <v>100</v>
       </c>
       <c r="B109" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C109" t="s">
         <v>104</v>
       </c>
       <c r="D109" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -3180,13 +3186,13 @@
         <v>100</v>
       </c>
       <c r="B110" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C110" t="s">
         <v>104</v>
       </c>
       <c r="D110" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -3194,7 +3200,7 @@
         <v>100</v>
       </c>
       <c r="B111" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C111" t="s">
         <v>104</v>
@@ -3205,58 +3211,58 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>342</v>
+        <v>100</v>
       </c>
       <c r="B112" t="s">
-        <v>334</v>
+        <v>109</v>
       </c>
       <c r="C112" t="s">
-        <v>332</v>
+        <v>104</v>
       </c>
       <c r="D112" t="s">
-        <v>331</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>249</v>
+        <v>342</v>
       </c>
       <c r="B113" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="C113" t="s">
-        <v>251</v>
+        <v>332</v>
       </c>
       <c r="D113" t="s">
-        <v>252</v>
+        <v>331</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
       <c r="B114" t="s">
-        <v>11</v>
+        <v>250</v>
       </c>
       <c r="C114" t="s">
-        <v>21</v>
+        <v>251</v>
       </c>
       <c r="D114" t="s">
-        <v>22</v>
+        <v>252</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B115" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C115" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="D115" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3264,13 +3270,13 @@
         <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C116" t="s">
-        <v>21</v>
+        <v>266</v>
       </c>
       <c r="D116" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3278,27 +3284,27 @@
         <v>17</v>
       </c>
       <c r="B117" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C117" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="D117" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="B118" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C118" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
       <c r="D118" t="s">
-        <v>285</v>
+        <v>19</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3306,13 +3312,13 @@
         <v>278</v>
       </c>
       <c r="B119" t="s">
-        <v>284</v>
+        <v>11</v>
       </c>
       <c r="C119" t="s">
         <v>298</v>
       </c>
       <c r="D119" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3320,13 +3326,13 @@
         <v>278</v>
       </c>
       <c r="B120" t="s">
-        <v>366</v>
+        <v>284</v>
       </c>
       <c r="C120" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D120" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3334,13 +3340,13 @@
         <v>278</v>
       </c>
       <c r="B121" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C121" t="s">
-        <v>361</v>
+        <v>302</v>
       </c>
       <c r="D121" t="s">
-        <v>362</v>
+        <v>307</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3348,13 +3354,13 @@
         <v>278</v>
       </c>
       <c r="B122" t="s">
-        <v>311</v>
+        <v>363</v>
       </c>
       <c r="C122" t="s">
-        <v>313</v>
+        <v>361</v>
       </c>
       <c r="D122" t="s">
-        <v>314</v>
+        <v>362</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3362,13 +3368,13 @@
         <v>278</v>
       </c>
       <c r="B123" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="C123" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="D123" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3376,13 +3382,13 @@
         <v>278</v>
       </c>
       <c r="B124" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="C124" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D124" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3390,13 +3396,13 @@
         <v>278</v>
       </c>
       <c r="B125" t="s">
-        <v>134</v>
+        <v>312</v>
       </c>
       <c r="C125" t="s">
-        <v>349</v>
+        <v>313</v>
       </c>
       <c r="D125" t="s">
-        <v>351</v>
+        <v>315</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3404,13 +3410,13 @@
         <v>278</v>
       </c>
       <c r="B126" t="s">
-        <v>279</v>
+        <v>134</v>
       </c>
       <c r="C126" t="s">
-        <v>298</v>
+        <v>349</v>
       </c>
       <c r="D126" t="s">
-        <v>280</v>
+        <v>351</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3418,13 +3424,13 @@
         <v>278</v>
       </c>
       <c r="B127" t="s">
-        <v>319</v>
+        <v>279</v>
       </c>
       <c r="C127" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="D127" t="s">
-        <v>316</v>
+        <v>280</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3432,7 +3438,7 @@
         <v>278</v>
       </c>
       <c r="B128" t="s">
-        <v>380</v>
+        <v>319</v>
       </c>
       <c r="C128" t="s">
         <v>313</v>
@@ -3446,27 +3452,27 @@
         <v>278</v>
       </c>
       <c r="B129" t="s">
-        <v>318</v>
+        <v>380</v>
       </c>
       <c r="C129" t="s">
         <v>313</v>
       </c>
       <c r="D129" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B130" t="s">
-        <v>282</v>
+        <v>318</v>
       </c>
       <c r="C130" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="D130" t="s">
-        <v>340</v>
+        <v>317</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3474,13 +3480,13 @@
         <v>281</v>
       </c>
       <c r="B131" t="s">
-        <v>364</v>
+        <v>282</v>
       </c>
       <c r="C131" t="s">
-        <v>361</v>
+        <v>298</v>
       </c>
       <c r="D131" t="s">
-        <v>365</v>
+        <v>340</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3488,13 +3494,13 @@
         <v>281</v>
       </c>
       <c r="B132" t="s">
-        <v>294</v>
+        <v>364</v>
       </c>
       <c r="C132" t="s">
-        <v>302</v>
+        <v>361</v>
       </c>
       <c r="D132" t="s">
-        <v>295</v>
+        <v>365</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3502,13 +3508,13 @@
         <v>281</v>
       </c>
       <c r="B133" t="s">
-        <v>348</v>
+        <v>294</v>
       </c>
       <c r="C133" t="s">
-        <v>349</v>
+        <v>302</v>
       </c>
       <c r="D133" t="s">
-        <v>350</v>
+        <v>295</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3516,55 +3522,55 @@
         <v>281</v>
       </c>
       <c r="B134" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="C134" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="D134" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>359</v>
+        <v>281</v>
       </c>
       <c r="B135" t="s">
-        <v>360</v>
+        <v>343</v>
       </c>
       <c r="C135" t="s">
-        <v>361</v>
+        <v>344</v>
       </c>
       <c r="D135" t="s">
-        <v>362</v>
+        <v>345</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>359</v>
+      </c>
+      <c r="B136" t="s">
+        <v>360</v>
+      </c>
+      <c r="C136" t="s">
+        <v>361</v>
+      </c>
+      <c r="D136" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>246</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B137" t="s">
         <v>247</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C137" t="s">
         <v>244</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D137" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3572,13 +3578,13 @@
         <v>395</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>397</v>
+        <v>79</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>391</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3586,13 +3592,13 @@
         <v>395</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>391</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3600,27 +3606,27 @@
         <v>395</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>11</v>
+        <v>398</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>391</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>391</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3628,27 +3634,27 @@
         <v>389</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>391</v>
       </c>
       <c r="D142" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D143" s="2" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>152</v>
-      </c>
-      <c r="B143" t="s">
-        <v>11</v>
-      </c>
-      <c r="C143" t="s">
-        <v>256</v>
-      </c>
-      <c r="D143" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -3656,13 +3662,13 @@
         <v>152</v>
       </c>
       <c r="B144" t="s">
-        <v>149</v>
+        <v>11</v>
       </c>
       <c r="C144" t="s">
         <v>256</v>
       </c>
       <c r="D144" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3670,13 +3676,13 @@
         <v>152</v>
       </c>
       <c r="B145" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="C145" t="s">
         <v>256</v>
       </c>
       <c r="D145" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3684,27 +3690,27 @@
         <v>152</v>
       </c>
       <c r="B146" t="s">
-        <v>209</v>
+        <v>164</v>
       </c>
       <c r="C146" t="s">
         <v>256</v>
       </c>
       <c r="D146" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B147" t="s">
-        <v>9</v>
+        <v>209</v>
       </c>
       <c r="C147" t="s">
         <v>256</v>
       </c>
       <c r="D147" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -3712,7 +3718,7 @@
         <v>156</v>
       </c>
       <c r="B148" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C148" t="s">
         <v>256</v>
@@ -3723,16 +3729,16 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>211</v>
+        <v>156</v>
       </c>
       <c r="B149" t="s">
-        <v>188</v>
+        <v>37</v>
       </c>
       <c r="C149" t="s">
-        <v>186</v>
+        <v>256</v>
       </c>
       <c r="D149" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -3740,27 +3746,27 @@
         <v>211</v>
       </c>
       <c r="B150" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="C150" t="s">
         <v>186</v>
       </c>
       <c r="D150" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B151" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="C151" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D151" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -3768,7 +3774,7 @@
         <v>214</v>
       </c>
       <c r="B152" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="C152" t="s">
         <v>183</v>
@@ -3782,55 +3788,55 @@
         <v>214</v>
       </c>
       <c r="B153" t="s">
-        <v>383</v>
+        <v>171</v>
       </c>
       <c r="C153" t="s">
-        <v>382</v>
+        <v>183</v>
       </c>
       <c r="D153" t="s">
-        <v>381</v>
+        <v>189</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B154" t="s">
-        <v>188</v>
+        <v>383</v>
       </c>
       <c r="C154" t="s">
-        <v>183</v>
+        <v>382</v>
       </c>
       <c r="D154" t="s">
-        <v>187</v>
+        <v>381</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B155" t="s">
-        <v>106</v>
+        <v>188</v>
       </c>
       <c r="C155" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D155" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>82</v>
+        <v>210</v>
       </c>
       <c r="B156" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C156" t="s">
-        <v>61</v>
+        <v>186</v>
       </c>
       <c r="D156" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -3838,7 +3844,7 @@
         <v>82</v>
       </c>
       <c r="B157" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C157" t="s">
         <v>61</v>
@@ -3849,30 +3855,30 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>347</v>
+        <v>82</v>
       </c>
       <c r="B158" t="s">
-        <v>346</v>
+        <v>69</v>
       </c>
       <c r="C158" t="s">
-        <v>344</v>
+        <v>61</v>
       </c>
       <c r="D158" t="s">
-        <v>346</v>
+        <v>84</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>190</v>
+        <v>347</v>
       </c>
       <c r="B159" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="C159" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="D159" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -3880,13 +3886,13 @@
         <v>190</v>
       </c>
       <c r="B160" t="s">
-        <v>191</v>
+        <v>338</v>
       </c>
       <c r="C160" t="s">
-        <v>192</v>
+        <v>336</v>
       </c>
       <c r="D160" t="s">
-        <v>198</v>
+        <v>339</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -3894,13 +3900,13 @@
         <v>190</v>
       </c>
       <c r="B161" t="s">
-        <v>272</v>
+        <v>191</v>
       </c>
       <c r="C161" t="s">
-        <v>297</v>
+        <v>192</v>
       </c>
       <c r="D161" t="s">
-        <v>273</v>
+        <v>198</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -3908,13 +3914,13 @@
         <v>190</v>
       </c>
       <c r="B162" t="s">
-        <v>157</v>
+        <v>272</v>
       </c>
       <c r="C162" t="s">
-        <v>158</v>
+        <v>297</v>
       </c>
       <c r="D162" t="s">
-        <v>159</v>
+        <v>273</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -3922,27 +3928,27 @@
         <v>190</v>
       </c>
       <c r="B163" t="s">
-        <v>335</v>
+        <v>157</v>
       </c>
       <c r="C163" t="s">
-        <v>336</v>
+        <v>158</v>
       </c>
       <c r="D163" t="s">
-        <v>337</v>
+        <v>159</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B164" t="s">
-        <v>195</v>
+        <v>335</v>
       </c>
       <c r="C164" t="s">
-        <v>254</v>
+        <v>336</v>
       </c>
       <c r="D164" t="s">
-        <v>197</v>
+        <v>337</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -3956,7 +3962,7 @@
         <v>254</v>
       </c>
       <c r="D165" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -3964,13 +3970,13 @@
         <v>206</v>
       </c>
       <c r="B166" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C166" t="s">
         <v>254</v>
       </c>
       <c r="D166" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -3984,21 +3990,21 @@
         <v>254</v>
       </c>
       <c r="D167" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B168" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C168" t="s">
-        <v>194</v>
+        <v>254</v>
       </c>
       <c r="D168" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4006,13 +4012,13 @@
         <v>47</v>
       </c>
       <c r="B169" t="s">
-        <v>292</v>
+        <v>193</v>
       </c>
       <c r="C169" t="s">
-        <v>301</v>
+        <v>194</v>
       </c>
       <c r="D169" t="s">
-        <v>293</v>
+        <v>198</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4020,13 +4026,13 @@
         <v>47</v>
       </c>
       <c r="B170" t="s">
-        <v>54</v>
+        <v>292</v>
       </c>
       <c r="C170" t="s">
-        <v>52</v>
+        <v>301</v>
       </c>
       <c r="D170" t="s">
-        <v>55</v>
+        <v>293</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4034,13 +4040,13 @@
         <v>47</v>
       </c>
       <c r="B171" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C171" t="s">
         <v>52</v>
       </c>
       <c r="D171" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4048,13 +4054,13 @@
         <v>47</v>
       </c>
       <c r="B172" t="s">
-        <v>275</v>
+        <v>51</v>
       </c>
       <c r="C172" t="s">
-        <v>297</v>
+        <v>52</v>
       </c>
       <c r="D172" t="s">
-        <v>274</v>
+        <v>53</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4062,13 +4068,13 @@
         <v>47</v>
       </c>
       <c r="B173" t="s">
-        <v>188</v>
+        <v>275</v>
       </c>
       <c r="C173" t="s">
-        <v>267</v>
+        <v>297</v>
       </c>
       <c r="D173" t="s">
-        <v>187</v>
+        <v>274</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4076,13 +4082,13 @@
         <v>47</v>
       </c>
       <c r="B174" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
       <c r="C174" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="D174" t="s">
-        <v>125</v>
+        <v>187</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4090,27 +4096,27 @@
         <v>47</v>
       </c>
       <c r="B175" t="s">
+        <v>125</v>
+      </c>
+      <c r="C175" t="s">
+        <v>257</v>
+      </c>
+      <c r="D175" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>47</v>
+      </c>
+      <c r="B176" t="s">
         <v>127</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C176" t="s">
         <v>128</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D176" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="D176" s="2" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4118,41 +4124,41 @@
         <v>47</v>
       </c>
       <c r="B177" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D177" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B178" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="C177" s="2" t="s">
+      <c r="C178" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="D177" s="2" t="s">
+      <c r="D178" s="2" t="s">
         <v>390</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>212</v>
-      </c>
-      <c r="B178" t="s">
-        <v>171</v>
-      </c>
-      <c r="C178" t="s">
-        <v>266</v>
-      </c>
-      <c r="D178" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>50</v>
+        <v>212</v>
       </c>
       <c r="B179" t="s">
-        <v>309</v>
+        <v>171</v>
       </c>
       <c r="C179" t="s">
-        <v>310</v>
+        <v>266</v>
       </c>
       <c r="D179" t="s">
-        <v>308</v>
+        <v>172</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4160,13 +4166,13 @@
         <v>50</v>
       </c>
       <c r="B180" t="s">
-        <v>57</v>
+        <v>309</v>
       </c>
       <c r="C180" t="s">
-        <v>52</v>
+        <v>310</v>
       </c>
       <c r="D180" t="s">
-        <v>55</v>
+        <v>308</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4174,7 +4180,7 @@
         <v>50</v>
       </c>
       <c r="B181" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C181" t="s">
         <v>52</v>
@@ -4188,13 +4194,13 @@
         <v>50</v>
       </c>
       <c r="B182" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="C182" t="s">
-        <v>266</v>
+        <v>52</v>
       </c>
       <c r="D182" t="s">
-        <v>176</v>
+        <v>55</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4202,13 +4208,13 @@
         <v>50</v>
       </c>
       <c r="B183" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C183" t="s">
         <v>266</v>
       </c>
       <c r="D183" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4216,27 +4222,27 @@
         <v>50</v>
       </c>
       <c r="B184" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C184" t="s">
         <v>266</v>
       </c>
       <c r="D184" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B185" t="s">
-        <v>116</v>
+        <v>173</v>
       </c>
       <c r="C185" t="s">
-        <v>117</v>
+        <v>266</v>
       </c>
       <c r="D185" t="s">
-        <v>116</v>
+        <v>174</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4244,13 +4250,13 @@
         <v>110</v>
       </c>
       <c r="B186" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C186" t="s">
         <v>117</v>
       </c>
       <c r="D186" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4258,13 +4264,13 @@
         <v>110</v>
       </c>
       <c r="B187" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C187" t="s">
         <v>117</v>
       </c>
       <c r="D187" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4272,13 +4278,13 @@
         <v>110</v>
       </c>
       <c r="B188" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C188" t="s">
         <v>117</v>
       </c>
       <c r="D188" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4286,27 +4292,27 @@
         <v>110</v>
       </c>
       <c r="B189" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C189" t="s">
         <v>117</v>
       </c>
       <c r="D189" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>207</v>
+        <v>110</v>
       </c>
       <c r="B190" t="s">
-        <v>195</v>
+        <v>122</v>
       </c>
       <c r="C190" t="s">
-        <v>254</v>
+        <v>117</v>
       </c>
       <c r="D190" t="s">
-        <v>196</v>
+        <v>123</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -4320,7 +4326,7 @@
         <v>254</v>
       </c>
       <c r="D191" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4328,13 +4334,13 @@
         <v>207</v>
       </c>
       <c r="B192" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C192" t="s">
         <v>254</v>
       </c>
       <c r="D192" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -4348,6 +4354,20 @@
         <v>254</v>
       </c>
       <c r="D193" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>207</v>
+      </c>
+      <c r="B194" t="s">
+        <v>199</v>
+      </c>
+      <c r="C194" t="s">
+        <v>254</v>
+      </c>
+      <c r="D194" t="s">
         <v>203</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mapping snippets for structs that must be set together
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21814"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86714E1-80FA-4F75-91D3-3D1E120A7029}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1B50C3-5FAB-4A63-8138-9AD50D51D3E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="406">
   <si>
     <t>Class</t>
   </si>
@@ -1229,6 +1229,15 @@
   </si>
   <si>
     <t>colorAllFormulaRanges</t>
+  </si>
+  <si>
+    <t>prompt</t>
+  </si>
+  <si>
+    <t>zoom</t>
+  </si>
+  <si>
+    <t>setZoom</t>
   </si>
 </sst>
 </file>
@@ -1308,10 +1317,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D194" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D194" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D193">
-    <sortCondition ref="A1:A193"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D197" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D197" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D197">
+    <sortCondition ref="A1:A197"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1640,11 +1649,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D194"/>
+  <dimension ref="A1:D197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D194" sqref="D194"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B182" sqref="B182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2584,21 +2593,21 @@
         <v>222</v>
       </c>
       <c r="B67" t="s">
-        <v>221</v>
+        <v>403</v>
       </c>
       <c r="C67" t="s">
         <v>218</v>
       </c>
       <c r="D67" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="B68" t="s">
-        <v>220</v>
+        <v>69</v>
       </c>
       <c r="C68" t="s">
         <v>218</v>
@@ -2609,86 +2618,86 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="B69" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C69" t="s">
         <v>218</v>
       </c>
       <c r="D69" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>253</v>
       </c>
       <c r="B70" t="s">
-        <v>65</v>
+        <v>220</v>
       </c>
       <c r="C70" t="s">
-        <v>61</v>
+        <v>218</v>
       </c>
       <c r="D70" t="s">
-        <v>77</v>
+        <v>216</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>74</v>
+        <v>253</v>
       </c>
       <c r="B71" t="s">
-        <v>79</v>
+        <v>219</v>
       </c>
       <c r="C71" t="s">
-        <v>61</v>
+        <v>218</v>
       </c>
       <c r="D71" t="s">
-        <v>77</v>
+        <v>215</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>306</v>
+        <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C72" t="s">
-        <v>302</v>
+        <v>61</v>
       </c>
       <c r="D72" t="s">
-        <v>305</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>354</v>
+        <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>355</v>
+        <v>79</v>
       </c>
       <c r="C73" t="s">
-        <v>349</v>
+        <v>61</v>
       </c>
       <c r="D73" t="s">
-        <v>352</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
       <c r="B74" t="s">
-        <v>356</v>
+        <v>86</v>
       </c>
       <c r="C74" t="s">
-        <v>349</v>
+        <v>302</v>
       </c>
       <c r="D74" t="s">
-        <v>352</v>
+        <v>305</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2696,13 +2705,13 @@
         <v>354</v>
       </c>
       <c r="B75" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C75" t="s">
         <v>349</v>
       </c>
       <c r="D75" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2710,97 +2719,97 @@
         <v>354</v>
       </c>
       <c r="B76" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C76" t="s">
         <v>349</v>
       </c>
       <c r="D76" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>10</v>
+        <v>354</v>
       </c>
       <c r="B77" t="s">
-        <v>11</v>
+        <v>357</v>
       </c>
       <c r="C77" t="s">
-        <v>12</v>
+        <v>349</v>
       </c>
       <c r="D77" t="s">
-        <v>13</v>
+        <v>353</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>10</v>
+        <v>354</v>
       </c>
       <c r="B78" t="s">
-        <v>14</v>
+        <v>358</v>
       </c>
       <c r="C78" t="s">
-        <v>15</v>
+        <v>349</v>
       </c>
       <c r="D78" t="s">
-        <v>16</v>
+        <v>353</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B79" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C79" t="s">
         <v>12</v>
       </c>
       <c r="D79" t="s">
-        <v>265</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>320</v>
+        <v>10</v>
       </c>
       <c r="B80" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C80" t="s">
-        <v>321</v>
+        <v>15</v>
       </c>
       <c r="D80" t="s">
-        <v>322</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>325</v>
+        <v>8</v>
       </c>
       <c r="B81" t="s">
-        <v>323</v>
+        <v>9</v>
       </c>
       <c r="C81" t="s">
-        <v>321</v>
+        <v>12</v>
       </c>
       <c r="D81" t="s">
-        <v>326</v>
+        <v>265</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B82" t="s">
-        <v>324</v>
+        <v>9</v>
       </c>
       <c r="C82" t="s">
         <v>321</v>
       </c>
       <c r="D82" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2808,13 +2817,13 @@
         <v>325</v>
       </c>
       <c r="B83" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="C83" t="s">
         <v>321</v>
       </c>
       <c r="D83" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2822,13 +2831,13 @@
         <v>325</v>
       </c>
       <c r="B84" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C84" t="s">
         <v>321</v>
       </c>
       <c r="D84" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2836,69 +2845,69 @@
         <v>325</v>
       </c>
       <c r="B85" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="C85" t="s">
         <v>321</v>
       </c>
       <c r="D85" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>239</v>
+        <v>325</v>
       </c>
       <c r="B86" t="s">
-        <v>240</v>
+        <v>329</v>
       </c>
       <c r="C86" t="s">
-        <v>243</v>
+        <v>321</v>
       </c>
       <c r="D86" t="s">
-        <v>241</v>
+        <v>329</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>226</v>
+        <v>325</v>
       </c>
       <c r="B87" t="s">
-        <v>229</v>
+        <v>327</v>
       </c>
       <c r="C87" t="s">
-        <v>224</v>
+        <v>321</v>
       </c>
       <c r="D87" t="s">
-        <v>228</v>
+        <v>328</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>226</v>
-      </c>
-      <c r="B88" t="s">
-        <v>230</v>
+      <c r="A88" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>404</v>
       </c>
       <c r="C88" t="s">
-        <v>224</v>
-      </c>
-      <c r="D88" t="s">
-        <v>231</v>
+        <v>321</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="B89" t="s">
-        <v>11</v>
+        <v>240</v>
       </c>
       <c r="C89" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="D89" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2906,13 +2915,13 @@
         <v>226</v>
       </c>
       <c r="B90" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C90" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="D90" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2920,97 +2929,97 @@
         <v>226</v>
       </c>
       <c r="B91" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C91" t="s">
         <v>224</v>
       </c>
       <c r="D91" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B92" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C92" t="s">
         <v>224</v>
       </c>
       <c r="D92" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>64</v>
+        <v>226</v>
       </c>
       <c r="B93" t="s">
-        <v>69</v>
+        <v>237</v>
       </c>
       <c r="C93" t="s">
-        <v>61</v>
+        <v>243</v>
       </c>
       <c r="D93" t="s">
-        <v>68</v>
+        <v>238</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>64</v>
+        <v>226</v>
       </c>
       <c r="B94" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="C94" t="s">
-        <v>61</v>
+        <v>224</v>
       </c>
       <c r="D94" t="s">
-        <v>95</v>
+        <v>236</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>24</v>
+        <v>223</v>
       </c>
       <c r="B95" t="s">
-        <v>286</v>
+        <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>299</v>
+        <v>224</v>
       </c>
       <c r="D95" t="s">
-        <v>287</v>
+        <v>225</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B96" t="s">
-        <v>288</v>
+        <v>69</v>
       </c>
       <c r="C96" t="s">
-        <v>300</v>
+        <v>61</v>
       </c>
       <c r="D96" t="s">
-        <v>289</v>
+        <v>68</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B97" t="s">
-        <v>290</v>
+        <v>69</v>
       </c>
       <c r="C97" t="s">
-        <v>300</v>
+        <v>61</v>
       </c>
       <c r="D97" t="s">
-        <v>291</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3018,13 +3027,13 @@
         <v>24</v>
       </c>
       <c r="B98" t="s">
-        <v>27</v>
+        <v>286</v>
       </c>
       <c r="C98" t="s">
-        <v>255</v>
+        <v>299</v>
       </c>
       <c r="D98" t="s">
-        <v>28</v>
+        <v>287</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3032,13 +3041,13 @@
         <v>24</v>
       </c>
       <c r="B99" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="C99" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D99" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -3046,13 +3055,13 @@
         <v>24</v>
       </c>
       <c r="B100" t="s">
-        <v>29</v>
+        <v>290</v>
       </c>
       <c r="C100" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="D100" t="s">
-        <v>28</v>
+        <v>291</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3060,13 +3069,13 @@
         <v>24</v>
       </c>
       <c r="B101" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C101" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="D101" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -3074,13 +3083,13 @@
         <v>24</v>
       </c>
       <c r="B102" t="s">
-        <v>103</v>
+        <v>276</v>
       </c>
       <c r="C102" t="s">
-        <v>104</v>
+        <v>297</v>
       </c>
       <c r="D102" t="s">
-        <v>105</v>
+        <v>277</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3088,13 +3097,13 @@
         <v>24</v>
       </c>
       <c r="B103" t="s">
-        <v>333</v>
+        <v>29</v>
       </c>
       <c r="C103" t="s">
-        <v>332</v>
+        <v>255</v>
       </c>
       <c r="D103" t="s">
-        <v>331</v>
+        <v>28</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -3102,13 +3111,13 @@
         <v>24</v>
       </c>
       <c r="B104" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C104" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="D104" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3116,13 +3125,13 @@
         <v>24</v>
       </c>
       <c r="B105" t="s">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="C105" t="s">
-        <v>258</v>
+        <v>104</v>
       </c>
       <c r="D105" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -3130,223 +3139,223 @@
         <v>24</v>
       </c>
       <c r="B106" t="s">
-        <v>79</v>
+        <v>333</v>
       </c>
       <c r="C106" t="s">
-        <v>256</v>
+        <v>332</v>
       </c>
       <c r="D106" t="s">
-        <v>160</v>
+        <v>331</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>108</v>
+        <v>24</v>
       </c>
       <c r="B107" t="s">
-        <v>113</v>
+        <v>31</v>
       </c>
       <c r="C107" t="s">
-        <v>114</v>
+        <v>258</v>
       </c>
       <c r="D107" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B108" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="C108" t="s">
-        <v>104</v>
+        <v>258</v>
       </c>
       <c r="D108" t="s">
-        <v>105</v>
+        <v>33</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B109" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="C109" t="s">
-        <v>104</v>
+        <v>256</v>
       </c>
       <c r="D109" t="s">
-        <v>112</v>
+        <v>160</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>100</v>
-      </c>
-      <c r="B110" t="s">
-        <v>107</v>
+      <c r="A110" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="C110" t="s">
-        <v>104</v>
-      </c>
-      <c r="D110" t="s">
-        <v>105</v>
+        <v>297</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B111" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C111" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="D111" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>342</v>
+        <v>100</v>
       </c>
       <c r="B112" t="s">
-        <v>334</v>
+        <v>106</v>
       </c>
       <c r="C112" t="s">
-        <v>332</v>
+        <v>104</v>
       </c>
       <c r="D112" t="s">
-        <v>331</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>249</v>
+        <v>100</v>
       </c>
       <c r="B113" t="s">
-        <v>250</v>
+        <v>111</v>
       </c>
       <c r="C113" t="s">
-        <v>251</v>
+        <v>104</v>
       </c>
       <c r="D113" t="s">
-        <v>252</v>
+        <v>112</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="B114" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="C114" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="D114" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="B115" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="C115" t="s">
-        <v>266</v>
+        <v>104</v>
       </c>
       <c r="D115" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>17</v>
+        <v>342</v>
       </c>
       <c r="B116" t="s">
-        <v>23</v>
+        <v>334</v>
       </c>
       <c r="C116" t="s">
-        <v>21</v>
+        <v>332</v>
       </c>
       <c r="D116" t="s">
-        <v>22</v>
+        <v>331</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>17</v>
+        <v>249</v>
       </c>
       <c r="B117" t="s">
-        <v>18</v>
+        <v>250</v>
       </c>
       <c r="C117" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="D117" t="s">
-        <v>19</v>
+        <v>252</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>278</v>
+        <v>20</v>
       </c>
       <c r="B118" t="s">
         <v>11</v>
       </c>
       <c r="C118" t="s">
-        <v>298</v>
+        <v>21</v>
       </c>
       <c r="D118" t="s">
-        <v>285</v>
+        <v>22</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="B119" t="s">
-        <v>284</v>
+        <v>9</v>
       </c>
       <c r="C119" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
       <c r="D119" t="s">
-        <v>283</v>
+        <v>19</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="B120" t="s">
-        <v>366</v>
+        <v>23</v>
       </c>
       <c r="C120" t="s">
-        <v>302</v>
+        <v>21</v>
       </c>
       <c r="D120" t="s">
-        <v>307</v>
+        <v>22</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="B121" t="s">
-        <v>363</v>
+        <v>18</v>
       </c>
       <c r="C121" t="s">
-        <v>361</v>
+        <v>266</v>
       </c>
       <c r="D121" t="s">
-        <v>362</v>
+        <v>19</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3354,13 +3363,13 @@
         <v>278</v>
       </c>
       <c r="B122" t="s">
-        <v>311</v>
+        <v>11</v>
       </c>
       <c r="C122" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="D122" t="s">
-        <v>314</v>
+        <v>285</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3368,13 +3377,13 @@
         <v>278</v>
       </c>
       <c r="B123" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="C123" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D123" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3382,13 +3391,13 @@
         <v>278</v>
       </c>
       <c r="B124" t="s">
-        <v>312</v>
+        <v>366</v>
       </c>
       <c r="C124" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D124" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3396,13 +3405,13 @@
         <v>278</v>
       </c>
       <c r="B125" t="s">
-        <v>134</v>
+        <v>363</v>
       </c>
       <c r="C125" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="D125" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3410,13 +3419,13 @@
         <v>278</v>
       </c>
       <c r="B126" t="s">
-        <v>279</v>
+        <v>311</v>
       </c>
       <c r="C126" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="D126" t="s">
-        <v>280</v>
+        <v>314</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3424,13 +3433,13 @@
         <v>278</v>
       </c>
       <c r="B127" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="C127" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D127" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3438,13 +3447,13 @@
         <v>278</v>
       </c>
       <c r="B128" t="s">
-        <v>380</v>
+        <v>312</v>
       </c>
       <c r="C128" t="s">
         <v>313</v>
       </c>
       <c r="D128" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3452,69 +3461,69 @@
         <v>278</v>
       </c>
       <c r="B129" t="s">
-        <v>318</v>
+        <v>134</v>
       </c>
       <c r="C129" t="s">
-        <v>313</v>
+        <v>349</v>
       </c>
       <c r="D129" t="s">
-        <v>317</v>
+        <v>351</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B130" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C130" t="s">
         <v>298</v>
       </c>
       <c r="D130" t="s">
-        <v>340</v>
+        <v>280</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B131" t="s">
-        <v>364</v>
+        <v>319</v>
       </c>
       <c r="C131" t="s">
-        <v>361</v>
+        <v>313</v>
       </c>
       <c r="D131" t="s">
-        <v>365</v>
+        <v>316</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B132" t="s">
-        <v>294</v>
+        <v>380</v>
       </c>
       <c r="C132" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="D132" t="s">
-        <v>295</v>
+        <v>316</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B133" t="s">
-        <v>348</v>
+        <v>318</v>
       </c>
       <c r="C133" t="s">
-        <v>349</v>
+        <v>313</v>
       </c>
       <c r="D133" t="s">
-        <v>350</v>
+        <v>317</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3522,405 +3531,405 @@
         <v>281</v>
       </c>
       <c r="B134" t="s">
-        <v>343</v>
+        <v>282</v>
       </c>
       <c r="C134" t="s">
-        <v>344</v>
+        <v>298</v>
       </c>
       <c r="D134" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>359</v>
+        <v>281</v>
       </c>
       <c r="B135" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="C135" t="s">
         <v>361</v>
       </c>
       <c r="D135" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>281</v>
+      </c>
+      <c r="B136" t="s">
+        <v>294</v>
+      </c>
+      <c r="C136" t="s">
+        <v>302</v>
+      </c>
+      <c r="D136" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>281</v>
+      </c>
+      <c r="B137" t="s">
+        <v>348</v>
+      </c>
+      <c r="C137" t="s">
+        <v>349</v>
+      </c>
+      <c r="D137" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>281</v>
+      </c>
+      <c r="B138" t="s">
+        <v>343</v>
+      </c>
+      <c r="C138" t="s">
+        <v>344</v>
+      </c>
+      <c r="D138" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>359</v>
+      </c>
+      <c r="B139" t="s">
+        <v>360</v>
+      </c>
+      <c r="C139" t="s">
+        <v>361</v>
+      </c>
+      <c r="D139" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>246</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B140" t="s">
         <v>247</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C140" t="s">
         <v>244</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D140" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>391</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>37</v>
+        <v>397</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>391</v>
       </c>
       <c r="D142" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D146" s="2" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>152</v>
-      </c>
-      <c r="B143" t="s">
-        <v>11</v>
-      </c>
-      <c r="C143" t="s">
-        <v>256</v>
-      </c>
-      <c r="D143" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>152</v>
-      </c>
-      <c r="B144" t="s">
-        <v>149</v>
-      </c>
-      <c r="C144" t="s">
-        <v>256</v>
-      </c>
-      <c r="D144" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>152</v>
-      </c>
-      <c r="B145" t="s">
-        <v>164</v>
-      </c>
-      <c r="C145" t="s">
-        <v>256</v>
-      </c>
-      <c r="D145" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>152</v>
-      </c>
-      <c r="B146" t="s">
-        <v>209</v>
-      </c>
-      <c r="C146" t="s">
-        <v>256</v>
-      </c>
-      <c r="D146" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B147" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C147" t="s">
         <v>256</v>
       </c>
       <c r="D147" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B148" t="s">
-        <v>37</v>
+        <v>149</v>
       </c>
       <c r="C148" t="s">
         <v>256</v>
       </c>
       <c r="D148" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>211</v>
+        <v>152</v>
       </c>
       <c r="B149" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="C149" t="s">
-        <v>186</v>
+        <v>256</v>
       </c>
       <c r="D149" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>211</v>
+        <v>152</v>
       </c>
       <c r="B150" t="s">
-        <v>167</v>
+        <v>209</v>
       </c>
       <c r="C150" t="s">
-        <v>186</v>
+        <v>256</v>
       </c>
       <c r="D150" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>214</v>
+        <v>156</v>
       </c>
       <c r="B151" t="s">
-        <v>184</v>
+        <v>9</v>
       </c>
       <c r="C151" t="s">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="D151" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>214</v>
+        <v>156</v>
       </c>
       <c r="B152" t="s">
-        <v>171</v>
+        <v>37</v>
       </c>
       <c r="C152" t="s">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="D152" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B153" t="s">
-        <v>383</v>
+        <v>188</v>
       </c>
       <c r="C153" t="s">
-        <v>382</v>
+        <v>186</v>
       </c>
       <c r="D153" t="s">
-        <v>381</v>
+        <v>187</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B154" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="C154" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D154" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B155" t="s">
-        <v>106</v>
+        <v>184</v>
       </c>
       <c r="C155" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D155" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>82</v>
+        <v>214</v>
       </c>
       <c r="B156" t="s">
-        <v>86</v>
+        <v>171</v>
       </c>
       <c r="C156" t="s">
-        <v>61</v>
+        <v>183</v>
       </c>
       <c r="D156" t="s">
-        <v>84</v>
+        <v>189</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>82</v>
+        <v>214</v>
       </c>
       <c r="B157" t="s">
-        <v>69</v>
+        <v>383</v>
       </c>
       <c r="C157" t="s">
-        <v>61</v>
+        <v>382</v>
       </c>
       <c r="D157" t="s">
-        <v>84</v>
+        <v>381</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>347</v>
+        <v>213</v>
       </c>
       <c r="B158" t="s">
-        <v>346</v>
+        <v>188</v>
       </c>
       <c r="C158" t="s">
-        <v>344</v>
+        <v>183</v>
       </c>
       <c r="D158" t="s">
-        <v>346</v>
+        <v>187</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B159" t="s">
-        <v>338</v>
+        <v>106</v>
       </c>
       <c r="C159" t="s">
-        <v>336</v>
+        <v>186</v>
       </c>
       <c r="D159" t="s">
-        <v>339</v>
+        <v>166</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>190</v>
+        <v>82</v>
       </c>
       <c r="B160" t="s">
-        <v>191</v>
+        <v>86</v>
       </c>
       <c r="C160" t="s">
-        <v>192</v>
+        <v>61</v>
       </c>
       <c r="D160" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>190</v>
+        <v>82</v>
       </c>
       <c r="B161" t="s">
-        <v>272</v>
+        <v>69</v>
       </c>
       <c r="C161" t="s">
-        <v>297</v>
+        <v>61</v>
       </c>
       <c r="D161" t="s">
-        <v>273</v>
+        <v>84</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>190</v>
+        <v>347</v>
       </c>
       <c r="B162" t="s">
-        <v>157</v>
+        <v>346</v>
       </c>
       <c r="C162" t="s">
-        <v>158</v>
+        <v>344</v>
       </c>
       <c r="D162" t="s">
-        <v>159</v>
+        <v>346</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -3928,125 +3937,125 @@
         <v>190</v>
       </c>
       <c r="B163" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C163" t="s">
         <v>336</v>
       </c>
       <c r="D163" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B164" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C164" t="s">
-        <v>254</v>
+        <v>192</v>
       </c>
       <c r="D164" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B165" t="s">
-        <v>195</v>
+        <v>272</v>
       </c>
       <c r="C165" t="s">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="D165" t="s">
-        <v>204</v>
+        <v>273</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B166" t="s">
-        <v>199</v>
+        <v>157</v>
       </c>
       <c r="C166" t="s">
-        <v>254</v>
+        <v>158</v>
       </c>
       <c r="D166" t="s">
-        <v>201</v>
+        <v>159</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B167" t="s">
-        <v>199</v>
+        <v>335</v>
       </c>
       <c r="C167" t="s">
-        <v>254</v>
+        <v>336</v>
       </c>
       <c r="D167" t="s">
-        <v>205</v>
+        <v>337</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B168" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C168" t="s">
-        <v>194</v>
+        <v>254</v>
       </c>
       <c r="D168" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B169" t="s">
-        <v>292</v>
+        <v>195</v>
       </c>
       <c r="C169" t="s">
-        <v>301</v>
+        <v>254</v>
       </c>
       <c r="D169" t="s">
-        <v>293</v>
+        <v>204</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B170" t="s">
-        <v>54</v>
+        <v>199</v>
       </c>
       <c r="C170" t="s">
-        <v>52</v>
+        <v>254</v>
       </c>
       <c r="D170" t="s">
-        <v>55</v>
+        <v>201</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B171" t="s">
-        <v>51</v>
+        <v>199</v>
       </c>
       <c r="C171" t="s">
-        <v>52</v>
+        <v>254</v>
       </c>
       <c r="D171" t="s">
-        <v>53</v>
+        <v>205</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4054,13 +4063,13 @@
         <v>47</v>
       </c>
       <c r="B172" t="s">
-        <v>275</v>
+        <v>193</v>
       </c>
       <c r="C172" t="s">
-        <v>297</v>
+        <v>194</v>
       </c>
       <c r="D172" t="s">
-        <v>274</v>
+        <v>198</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4068,13 +4077,13 @@
         <v>47</v>
       </c>
       <c r="B173" t="s">
-        <v>188</v>
+        <v>292</v>
       </c>
       <c r="C173" t="s">
-        <v>267</v>
+        <v>301</v>
       </c>
       <c r="D173" t="s">
-        <v>187</v>
+        <v>293</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4082,13 +4091,13 @@
         <v>47</v>
       </c>
       <c r="B174" t="s">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="C174" t="s">
-        <v>257</v>
+        <v>52</v>
       </c>
       <c r="D174" t="s">
-        <v>125</v>
+        <v>55</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4096,111 +4105,111 @@
         <v>47</v>
       </c>
       <c r="B175" t="s">
-        <v>127</v>
+        <v>51</v>
       </c>
       <c r="C175" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="D175" t="s">
-        <v>129</v>
+        <v>53</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="2" t="s">
+      <c r="A176" t="s">
         <v>47</v>
       </c>
-      <c r="B176" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="D176" s="2" t="s">
-        <v>384</v>
+      <c r="B176" t="s">
+        <v>275</v>
+      </c>
+      <c r="C176" t="s">
+        <v>297</v>
+      </c>
+      <c r="D176" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="2" t="s">
+      <c r="A177" t="s">
         <v>47</v>
       </c>
-      <c r="B177" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D177" s="2" t="s">
-        <v>390</v>
+      <c r="B177" t="s">
+        <v>188</v>
+      </c>
+      <c r="C177" t="s">
+        <v>267</v>
+      </c>
+      <c r="D177" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>212</v>
+        <v>47</v>
       </c>
       <c r="B178" t="s">
-        <v>171</v>
+        <v>125</v>
       </c>
       <c r="C178" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="D178" t="s">
-        <v>172</v>
+        <v>125</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B179" t="s">
-        <v>309</v>
+        <v>127</v>
       </c>
       <c r="C179" t="s">
-        <v>310</v>
+        <v>128</v>
       </c>
       <c r="D179" t="s">
-        <v>308</v>
+        <v>129</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>50</v>
-      </c>
-      <c r="B180" t="s">
-        <v>57</v>
-      </c>
-      <c r="C180" t="s">
-        <v>52</v>
-      </c>
-      <c r="D180" t="s">
-        <v>55</v>
+      <c r="A180" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>50</v>
-      </c>
-      <c r="B181" t="s">
-        <v>59</v>
-      </c>
-      <c r="C181" t="s">
-        <v>52</v>
-      </c>
-      <c r="D181" t="s">
-        <v>55</v>
+      <c r="A181" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>50</v>
+        <v>212</v>
       </c>
       <c r="B182" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C182" t="s">
         <v>266</v>
       </c>
       <c r="D182" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4208,13 +4217,13 @@
         <v>50</v>
       </c>
       <c r="B183" t="s">
-        <v>169</v>
+        <v>309</v>
       </c>
       <c r="C183" t="s">
-        <v>266</v>
+        <v>310</v>
       </c>
       <c r="D183" t="s">
-        <v>170</v>
+        <v>308</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4222,69 +4231,69 @@
         <v>50</v>
       </c>
       <c r="B184" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="C184" t="s">
-        <v>266</v>
+        <v>52</v>
       </c>
       <c r="D184" t="s">
-        <v>174</v>
+        <v>55</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B185" t="s">
-        <v>116</v>
+        <v>59</v>
       </c>
       <c r="C185" t="s">
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="D185" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B186" t="s">
-        <v>118</v>
+        <v>175</v>
       </c>
       <c r="C186" t="s">
-        <v>117</v>
+        <v>266</v>
       </c>
       <c r="D186" t="s">
-        <v>118</v>
+        <v>176</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B187" t="s">
-        <v>119</v>
+        <v>169</v>
       </c>
       <c r="C187" t="s">
-        <v>117</v>
+        <v>266</v>
       </c>
       <c r="D187" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B188" t="s">
-        <v>120</v>
+        <v>173</v>
       </c>
       <c r="C188" t="s">
-        <v>117</v>
+        <v>266</v>
       </c>
       <c r="D188" t="s">
-        <v>121</v>
+        <v>174</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4292,83 +4301,125 @@
         <v>110</v>
       </c>
       <c r="B189" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C189" t="s">
         <v>117</v>
       </c>
       <c r="D189" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>207</v>
+        <v>110</v>
       </c>
       <c r="B190" t="s">
-        <v>195</v>
+        <v>118</v>
       </c>
       <c r="C190" t="s">
-        <v>254</v>
+        <v>117</v>
       </c>
       <c r="D190" t="s">
-        <v>196</v>
+        <v>118</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>207</v>
+        <v>110</v>
       </c>
       <c r="B191" t="s">
-        <v>195</v>
+        <v>119</v>
       </c>
       <c r="C191" t="s">
-        <v>254</v>
+        <v>117</v>
       </c>
       <c r="D191" t="s">
-        <v>202</v>
+        <v>119</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>207</v>
+        <v>110</v>
       </c>
       <c r="B192" t="s">
-        <v>199</v>
+        <v>120</v>
       </c>
       <c r="C192" t="s">
-        <v>254</v>
+        <v>117</v>
       </c>
       <c r="D192" t="s">
-        <v>200</v>
+        <v>121</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>110</v>
+      </c>
+      <c r="B193" t="s">
+        <v>122</v>
+      </c>
+      <c r="C193" t="s">
+        <v>117</v>
+      </c>
+      <c r="D193" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>207</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B194" t="s">
+        <v>195</v>
+      </c>
+      <c r="C194" t="s">
+        <v>254</v>
+      </c>
+      <c r="D194" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>207</v>
+      </c>
+      <c r="B195" t="s">
+        <v>195</v>
+      </c>
+      <c r="C195" t="s">
+        <v>254</v>
+      </c>
+      <c r="D195" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>207</v>
+      </c>
+      <c r="B196" t="s">
         <v>199</v>
       </c>
-      <c r="C193" t="s">
+      <c r="C196" t="s">
         <v>254</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D196" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>207</v>
+      </c>
+      <c r="B197" t="s">
+        <v>199</v>
+      </c>
+      <c r="C197" t="s">
+        <v>254</v>
+      </c>
+      <c r="D197" t="s">
         <v>203</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C194" t="s">
-        <v>297</v>
-      </c>
-      <c r="D194" s="2" t="s">
-        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[excel] (Samples) Mapping snippets for structs that must be set together (#315)
* Mapping snippets for structs that must be set together

* Update snippet-extractor-output/snippets.yaml

Co-Authored-By: Elizabeth Samuel <elizs@microsoft.com>
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21814"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86714E1-80FA-4F75-91D3-3D1E120A7029}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1B50C3-5FAB-4A63-8138-9AD50D51D3E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="406">
   <si>
     <t>Class</t>
   </si>
@@ -1229,6 +1229,15 @@
   </si>
   <si>
     <t>colorAllFormulaRanges</t>
+  </si>
+  <si>
+    <t>prompt</t>
+  </si>
+  <si>
+    <t>zoom</t>
+  </si>
+  <si>
+    <t>setZoom</t>
   </si>
 </sst>
 </file>
@@ -1308,10 +1317,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D194" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D194" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D193">
-    <sortCondition ref="A1:A193"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D197" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D197" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D197">
+    <sortCondition ref="A1:A197"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1640,11 +1649,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D194"/>
+  <dimension ref="A1:D197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D194" sqref="D194"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B182" sqref="B182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2584,21 +2593,21 @@
         <v>222</v>
       </c>
       <c r="B67" t="s">
-        <v>221</v>
+        <v>403</v>
       </c>
       <c r="C67" t="s">
         <v>218</v>
       </c>
       <c r="D67" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="B68" t="s">
-        <v>220</v>
+        <v>69</v>
       </c>
       <c r="C68" t="s">
         <v>218</v>
@@ -2609,86 +2618,86 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="B69" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C69" t="s">
         <v>218</v>
       </c>
       <c r="D69" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>253</v>
       </c>
       <c r="B70" t="s">
-        <v>65</v>
+        <v>220</v>
       </c>
       <c r="C70" t="s">
-        <v>61</v>
+        <v>218</v>
       </c>
       <c r="D70" t="s">
-        <v>77</v>
+        <v>216</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>74</v>
+        <v>253</v>
       </c>
       <c r="B71" t="s">
-        <v>79</v>
+        <v>219</v>
       </c>
       <c r="C71" t="s">
-        <v>61</v>
+        <v>218</v>
       </c>
       <c r="D71" t="s">
-        <v>77</v>
+        <v>215</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>306</v>
+        <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C72" t="s">
-        <v>302</v>
+        <v>61</v>
       </c>
       <c r="D72" t="s">
-        <v>305</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>354</v>
+        <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>355</v>
+        <v>79</v>
       </c>
       <c r="C73" t="s">
-        <v>349</v>
+        <v>61</v>
       </c>
       <c r="D73" t="s">
-        <v>352</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
       <c r="B74" t="s">
-        <v>356</v>
+        <v>86</v>
       </c>
       <c r="C74" t="s">
-        <v>349</v>
+        <v>302</v>
       </c>
       <c r="D74" t="s">
-        <v>352</v>
+        <v>305</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2696,13 +2705,13 @@
         <v>354</v>
       </c>
       <c r="B75" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C75" t="s">
         <v>349</v>
       </c>
       <c r="D75" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2710,97 +2719,97 @@
         <v>354</v>
       </c>
       <c r="B76" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C76" t="s">
         <v>349</v>
       </c>
       <c r="D76" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>10</v>
+        <v>354</v>
       </c>
       <c r="B77" t="s">
-        <v>11</v>
+        <v>357</v>
       </c>
       <c r="C77" t="s">
-        <v>12</v>
+        <v>349</v>
       </c>
       <c r="D77" t="s">
-        <v>13</v>
+        <v>353</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>10</v>
+        <v>354</v>
       </c>
       <c r="B78" t="s">
-        <v>14</v>
+        <v>358</v>
       </c>
       <c r="C78" t="s">
-        <v>15</v>
+        <v>349</v>
       </c>
       <c r="D78" t="s">
-        <v>16</v>
+        <v>353</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B79" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C79" t="s">
         <v>12</v>
       </c>
       <c r="D79" t="s">
-        <v>265</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>320</v>
+        <v>10</v>
       </c>
       <c r="B80" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C80" t="s">
-        <v>321</v>
+        <v>15</v>
       </c>
       <c r="D80" t="s">
-        <v>322</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>325</v>
+        <v>8</v>
       </c>
       <c r="B81" t="s">
-        <v>323</v>
+        <v>9</v>
       </c>
       <c r="C81" t="s">
-        <v>321</v>
+        <v>12</v>
       </c>
       <c r="D81" t="s">
-        <v>326</v>
+        <v>265</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B82" t="s">
-        <v>324</v>
+        <v>9</v>
       </c>
       <c r="C82" t="s">
         <v>321</v>
       </c>
       <c r="D82" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2808,13 +2817,13 @@
         <v>325</v>
       </c>
       <c r="B83" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="C83" t="s">
         <v>321</v>
       </c>
       <c r="D83" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2822,13 +2831,13 @@
         <v>325</v>
       </c>
       <c r="B84" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C84" t="s">
         <v>321</v>
       </c>
       <c r="D84" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2836,69 +2845,69 @@
         <v>325</v>
       </c>
       <c r="B85" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="C85" t="s">
         <v>321</v>
       </c>
       <c r="D85" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>239</v>
+        <v>325</v>
       </c>
       <c r="B86" t="s">
-        <v>240</v>
+        <v>329</v>
       </c>
       <c r="C86" t="s">
-        <v>243</v>
+        <v>321</v>
       </c>
       <c r="D86" t="s">
-        <v>241</v>
+        <v>329</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>226</v>
+        <v>325</v>
       </c>
       <c r="B87" t="s">
-        <v>229</v>
+        <v>327</v>
       </c>
       <c r="C87" t="s">
-        <v>224</v>
+        <v>321</v>
       </c>
       <c r="D87" t="s">
-        <v>228</v>
+        <v>328</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>226</v>
-      </c>
-      <c r="B88" t="s">
-        <v>230</v>
+      <c r="A88" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>404</v>
       </c>
       <c r="C88" t="s">
-        <v>224</v>
-      </c>
-      <c r="D88" t="s">
-        <v>231</v>
+        <v>321</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="B89" t="s">
-        <v>11</v>
+        <v>240</v>
       </c>
       <c r="C89" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="D89" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2906,13 +2915,13 @@
         <v>226</v>
       </c>
       <c r="B90" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C90" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="D90" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2920,97 +2929,97 @@
         <v>226</v>
       </c>
       <c r="B91" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C91" t="s">
         <v>224</v>
       </c>
       <c r="D91" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B92" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C92" t="s">
         <v>224</v>
       </c>
       <c r="D92" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>64</v>
+        <v>226</v>
       </c>
       <c r="B93" t="s">
-        <v>69</v>
+        <v>237</v>
       </c>
       <c r="C93" t="s">
-        <v>61</v>
+        <v>243</v>
       </c>
       <c r="D93" t="s">
-        <v>68</v>
+        <v>238</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>64</v>
+        <v>226</v>
       </c>
       <c r="B94" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="C94" t="s">
-        <v>61</v>
+        <v>224</v>
       </c>
       <c r="D94" t="s">
-        <v>95</v>
+        <v>236</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>24</v>
+        <v>223</v>
       </c>
       <c r="B95" t="s">
-        <v>286</v>
+        <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>299</v>
+        <v>224</v>
       </c>
       <c r="D95" t="s">
-        <v>287</v>
+        <v>225</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B96" t="s">
-        <v>288</v>
+        <v>69</v>
       </c>
       <c r="C96" t="s">
-        <v>300</v>
+        <v>61</v>
       </c>
       <c r="D96" t="s">
-        <v>289</v>
+        <v>68</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B97" t="s">
-        <v>290</v>
+        <v>69</v>
       </c>
       <c r="C97" t="s">
-        <v>300</v>
+        <v>61</v>
       </c>
       <c r="D97" t="s">
-        <v>291</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3018,13 +3027,13 @@
         <v>24</v>
       </c>
       <c r="B98" t="s">
-        <v>27</v>
+        <v>286</v>
       </c>
       <c r="C98" t="s">
-        <v>255</v>
+        <v>299</v>
       </c>
       <c r="D98" t="s">
-        <v>28</v>
+        <v>287</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3032,13 +3041,13 @@
         <v>24</v>
       </c>
       <c r="B99" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="C99" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D99" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -3046,13 +3055,13 @@
         <v>24</v>
       </c>
       <c r="B100" t="s">
-        <v>29</v>
+        <v>290</v>
       </c>
       <c r="C100" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="D100" t="s">
-        <v>28</v>
+        <v>291</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3060,13 +3069,13 @@
         <v>24</v>
       </c>
       <c r="B101" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C101" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="D101" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -3074,13 +3083,13 @@
         <v>24</v>
       </c>
       <c r="B102" t="s">
-        <v>103</v>
+        <v>276</v>
       </c>
       <c r="C102" t="s">
-        <v>104</v>
+        <v>297</v>
       </c>
       <c r="D102" t="s">
-        <v>105</v>
+        <v>277</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3088,13 +3097,13 @@
         <v>24</v>
       </c>
       <c r="B103" t="s">
-        <v>333</v>
+        <v>29</v>
       </c>
       <c r="C103" t="s">
-        <v>332</v>
+        <v>255</v>
       </c>
       <c r="D103" t="s">
-        <v>331</v>
+        <v>28</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -3102,13 +3111,13 @@
         <v>24</v>
       </c>
       <c r="B104" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C104" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="D104" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3116,13 +3125,13 @@
         <v>24</v>
       </c>
       <c r="B105" t="s">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="C105" t="s">
-        <v>258</v>
+        <v>104</v>
       </c>
       <c r="D105" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -3130,223 +3139,223 @@
         <v>24</v>
       </c>
       <c r="B106" t="s">
-        <v>79</v>
+        <v>333</v>
       </c>
       <c r="C106" t="s">
-        <v>256</v>
+        <v>332</v>
       </c>
       <c r="D106" t="s">
-        <v>160</v>
+        <v>331</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>108</v>
+        <v>24</v>
       </c>
       <c r="B107" t="s">
-        <v>113</v>
+        <v>31</v>
       </c>
       <c r="C107" t="s">
-        <v>114</v>
+        <v>258</v>
       </c>
       <c r="D107" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B108" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="C108" t="s">
-        <v>104</v>
+        <v>258</v>
       </c>
       <c r="D108" t="s">
-        <v>105</v>
+        <v>33</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B109" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="C109" t="s">
-        <v>104</v>
+        <v>256</v>
       </c>
       <c r="D109" t="s">
-        <v>112</v>
+        <v>160</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>100</v>
-      </c>
-      <c r="B110" t="s">
-        <v>107</v>
+      <c r="A110" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="C110" t="s">
-        <v>104</v>
-      </c>
-      <c r="D110" t="s">
-        <v>105</v>
+        <v>297</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B111" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C111" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="D111" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>342</v>
+        <v>100</v>
       </c>
       <c r="B112" t="s">
-        <v>334</v>
+        <v>106</v>
       </c>
       <c r="C112" t="s">
-        <v>332</v>
+        <v>104</v>
       </c>
       <c r="D112" t="s">
-        <v>331</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>249</v>
+        <v>100</v>
       </c>
       <c r="B113" t="s">
-        <v>250</v>
+        <v>111</v>
       </c>
       <c r="C113" t="s">
-        <v>251</v>
+        <v>104</v>
       </c>
       <c r="D113" t="s">
-        <v>252</v>
+        <v>112</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="B114" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="C114" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="D114" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="B115" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="C115" t="s">
-        <v>266</v>
+        <v>104</v>
       </c>
       <c r="D115" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>17</v>
+        <v>342</v>
       </c>
       <c r="B116" t="s">
-        <v>23</v>
+        <v>334</v>
       </c>
       <c r="C116" t="s">
-        <v>21</v>
+        <v>332</v>
       </c>
       <c r="D116" t="s">
-        <v>22</v>
+        <v>331</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>17</v>
+        <v>249</v>
       </c>
       <c r="B117" t="s">
-        <v>18</v>
+        <v>250</v>
       </c>
       <c r="C117" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="D117" t="s">
-        <v>19</v>
+        <v>252</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>278</v>
+        <v>20</v>
       </c>
       <c r="B118" t="s">
         <v>11</v>
       </c>
       <c r="C118" t="s">
-        <v>298</v>
+        <v>21</v>
       </c>
       <c r="D118" t="s">
-        <v>285</v>
+        <v>22</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="B119" t="s">
-        <v>284</v>
+        <v>9</v>
       </c>
       <c r="C119" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
       <c r="D119" t="s">
-        <v>283</v>
+        <v>19</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="B120" t="s">
-        <v>366</v>
+        <v>23</v>
       </c>
       <c r="C120" t="s">
-        <v>302</v>
+        <v>21</v>
       </c>
       <c r="D120" t="s">
-        <v>307</v>
+        <v>22</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="B121" t="s">
-        <v>363</v>
+        <v>18</v>
       </c>
       <c r="C121" t="s">
-        <v>361</v>
+        <v>266</v>
       </c>
       <c r="D121" t="s">
-        <v>362</v>
+        <v>19</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3354,13 +3363,13 @@
         <v>278</v>
       </c>
       <c r="B122" t="s">
-        <v>311</v>
+        <v>11</v>
       </c>
       <c r="C122" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="D122" t="s">
-        <v>314</v>
+        <v>285</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3368,13 +3377,13 @@
         <v>278</v>
       </c>
       <c r="B123" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="C123" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D123" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3382,13 +3391,13 @@
         <v>278</v>
       </c>
       <c r="B124" t="s">
-        <v>312</v>
+        <v>366</v>
       </c>
       <c r="C124" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D124" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3396,13 +3405,13 @@
         <v>278</v>
       </c>
       <c r="B125" t="s">
-        <v>134</v>
+        <v>363</v>
       </c>
       <c r="C125" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="D125" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3410,13 +3419,13 @@
         <v>278</v>
       </c>
       <c r="B126" t="s">
-        <v>279</v>
+        <v>311</v>
       </c>
       <c r="C126" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="D126" t="s">
-        <v>280</v>
+        <v>314</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3424,13 +3433,13 @@
         <v>278</v>
       </c>
       <c r="B127" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="C127" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D127" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3438,13 +3447,13 @@
         <v>278</v>
       </c>
       <c r="B128" t="s">
-        <v>380</v>
+        <v>312</v>
       </c>
       <c r="C128" t="s">
         <v>313</v>
       </c>
       <c r="D128" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3452,69 +3461,69 @@
         <v>278</v>
       </c>
       <c r="B129" t="s">
-        <v>318</v>
+        <v>134</v>
       </c>
       <c r="C129" t="s">
-        <v>313</v>
+        <v>349</v>
       </c>
       <c r="D129" t="s">
-        <v>317</v>
+        <v>351</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B130" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C130" t="s">
         <v>298</v>
       </c>
       <c r="D130" t="s">
-        <v>340</v>
+        <v>280</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B131" t="s">
-        <v>364</v>
+        <v>319</v>
       </c>
       <c r="C131" t="s">
-        <v>361</v>
+        <v>313</v>
       </c>
       <c r="D131" t="s">
-        <v>365</v>
+        <v>316</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B132" t="s">
-        <v>294</v>
+        <v>380</v>
       </c>
       <c r="C132" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="D132" t="s">
-        <v>295</v>
+        <v>316</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B133" t="s">
-        <v>348</v>
+        <v>318</v>
       </c>
       <c r="C133" t="s">
-        <v>349</v>
+        <v>313</v>
       </c>
       <c r="D133" t="s">
-        <v>350</v>
+        <v>317</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3522,405 +3531,405 @@
         <v>281</v>
       </c>
       <c r="B134" t="s">
-        <v>343</v>
+        <v>282</v>
       </c>
       <c r="C134" t="s">
-        <v>344</v>
+        <v>298</v>
       </c>
       <c r="D134" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>359</v>
+        <v>281</v>
       </c>
       <c r="B135" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="C135" t="s">
         <v>361</v>
       </c>
       <c r="D135" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>281</v>
+      </c>
+      <c r="B136" t="s">
+        <v>294</v>
+      </c>
+      <c r="C136" t="s">
+        <v>302</v>
+      </c>
+      <c r="D136" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>281</v>
+      </c>
+      <c r="B137" t="s">
+        <v>348</v>
+      </c>
+      <c r="C137" t="s">
+        <v>349</v>
+      </c>
+      <c r="D137" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>281</v>
+      </c>
+      <c r="B138" t="s">
+        <v>343</v>
+      </c>
+      <c r="C138" t="s">
+        <v>344</v>
+      </c>
+      <c r="D138" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>359</v>
+      </c>
+      <c r="B139" t="s">
+        <v>360</v>
+      </c>
+      <c r="C139" t="s">
+        <v>361</v>
+      </c>
+      <c r="D139" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>246</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B140" t="s">
         <v>247</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C140" t="s">
         <v>244</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D140" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>391</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>37</v>
+        <v>397</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>391</v>
       </c>
       <c r="D142" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D146" s="2" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>152</v>
-      </c>
-      <c r="B143" t="s">
-        <v>11</v>
-      </c>
-      <c r="C143" t="s">
-        <v>256</v>
-      </c>
-      <c r="D143" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>152</v>
-      </c>
-      <c r="B144" t="s">
-        <v>149</v>
-      </c>
-      <c r="C144" t="s">
-        <v>256</v>
-      </c>
-      <c r="D144" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>152</v>
-      </c>
-      <c r="B145" t="s">
-        <v>164</v>
-      </c>
-      <c r="C145" t="s">
-        <v>256</v>
-      </c>
-      <c r="D145" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>152</v>
-      </c>
-      <c r="B146" t="s">
-        <v>209</v>
-      </c>
-      <c r="C146" t="s">
-        <v>256</v>
-      </c>
-      <c r="D146" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B147" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C147" t="s">
         <v>256</v>
       </c>
       <c r="D147" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B148" t="s">
-        <v>37</v>
+        <v>149</v>
       </c>
       <c r="C148" t="s">
         <v>256</v>
       </c>
       <c r="D148" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>211</v>
+        <v>152</v>
       </c>
       <c r="B149" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="C149" t="s">
-        <v>186</v>
+        <v>256</v>
       </c>
       <c r="D149" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>211</v>
+        <v>152</v>
       </c>
       <c r="B150" t="s">
-        <v>167</v>
+        <v>209</v>
       </c>
       <c r="C150" t="s">
-        <v>186</v>
+        <v>256</v>
       </c>
       <c r="D150" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>214</v>
+        <v>156</v>
       </c>
       <c r="B151" t="s">
-        <v>184</v>
+        <v>9</v>
       </c>
       <c r="C151" t="s">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="D151" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>214</v>
+        <v>156</v>
       </c>
       <c r="B152" t="s">
-        <v>171</v>
+        <v>37</v>
       </c>
       <c r="C152" t="s">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="D152" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B153" t="s">
-        <v>383</v>
+        <v>188</v>
       </c>
       <c r="C153" t="s">
-        <v>382</v>
+        <v>186</v>
       </c>
       <c r="D153" t="s">
-        <v>381</v>
+        <v>187</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B154" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="C154" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D154" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B155" t="s">
-        <v>106</v>
+        <v>184</v>
       </c>
       <c r="C155" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D155" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>82</v>
+        <v>214</v>
       </c>
       <c r="B156" t="s">
-        <v>86</v>
+        <v>171</v>
       </c>
       <c r="C156" t="s">
-        <v>61</v>
+        <v>183</v>
       </c>
       <c r="D156" t="s">
-        <v>84</v>
+        <v>189</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>82</v>
+        <v>214</v>
       </c>
       <c r="B157" t="s">
-        <v>69</v>
+        <v>383</v>
       </c>
       <c r="C157" t="s">
-        <v>61</v>
+        <v>382</v>
       </c>
       <c r="D157" t="s">
-        <v>84</v>
+        <v>381</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>347</v>
+        <v>213</v>
       </c>
       <c r="B158" t="s">
-        <v>346</v>
+        <v>188</v>
       </c>
       <c r="C158" t="s">
-        <v>344</v>
+        <v>183</v>
       </c>
       <c r="D158" t="s">
-        <v>346</v>
+        <v>187</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B159" t="s">
-        <v>338</v>
+        <v>106</v>
       </c>
       <c r="C159" t="s">
-        <v>336</v>
+        <v>186</v>
       </c>
       <c r="D159" t="s">
-        <v>339</v>
+        <v>166</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>190</v>
+        <v>82</v>
       </c>
       <c r="B160" t="s">
-        <v>191</v>
+        <v>86</v>
       </c>
       <c r="C160" t="s">
-        <v>192</v>
+        <v>61</v>
       </c>
       <c r="D160" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>190</v>
+        <v>82</v>
       </c>
       <c r="B161" t="s">
-        <v>272</v>
+        <v>69</v>
       </c>
       <c r="C161" t="s">
-        <v>297</v>
+        <v>61</v>
       </c>
       <c r="D161" t="s">
-        <v>273</v>
+        <v>84</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>190</v>
+        <v>347</v>
       </c>
       <c r="B162" t="s">
-        <v>157</v>
+        <v>346</v>
       </c>
       <c r="C162" t="s">
-        <v>158</v>
+        <v>344</v>
       </c>
       <c r="D162" t="s">
-        <v>159</v>
+        <v>346</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -3928,125 +3937,125 @@
         <v>190</v>
       </c>
       <c r="B163" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C163" t="s">
         <v>336</v>
       </c>
       <c r="D163" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B164" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C164" t="s">
-        <v>254</v>
+        <v>192</v>
       </c>
       <c r="D164" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B165" t="s">
-        <v>195</v>
+        <v>272</v>
       </c>
       <c r="C165" t="s">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="D165" t="s">
-        <v>204</v>
+        <v>273</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B166" t="s">
-        <v>199</v>
+        <v>157</v>
       </c>
       <c r="C166" t="s">
-        <v>254</v>
+        <v>158</v>
       </c>
       <c r="D166" t="s">
-        <v>201</v>
+        <v>159</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B167" t="s">
-        <v>199</v>
+        <v>335</v>
       </c>
       <c r="C167" t="s">
-        <v>254</v>
+        <v>336</v>
       </c>
       <c r="D167" t="s">
-        <v>205</v>
+        <v>337</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B168" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C168" t="s">
-        <v>194</v>
+        <v>254</v>
       </c>
       <c r="D168" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B169" t="s">
-        <v>292</v>
+        <v>195</v>
       </c>
       <c r="C169" t="s">
-        <v>301</v>
+        <v>254</v>
       </c>
       <c r="D169" t="s">
-        <v>293</v>
+        <v>204</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B170" t="s">
-        <v>54</v>
+        <v>199</v>
       </c>
       <c r="C170" t="s">
-        <v>52</v>
+        <v>254</v>
       </c>
       <c r="D170" t="s">
-        <v>55</v>
+        <v>201</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B171" t="s">
-        <v>51</v>
+        <v>199</v>
       </c>
       <c r="C171" t="s">
-        <v>52</v>
+        <v>254</v>
       </c>
       <c r="D171" t="s">
-        <v>53</v>
+        <v>205</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4054,13 +4063,13 @@
         <v>47</v>
       </c>
       <c r="B172" t="s">
-        <v>275</v>
+        <v>193</v>
       </c>
       <c r="C172" t="s">
-        <v>297</v>
+        <v>194</v>
       </c>
       <c r="D172" t="s">
-        <v>274</v>
+        <v>198</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4068,13 +4077,13 @@
         <v>47</v>
       </c>
       <c r="B173" t="s">
-        <v>188</v>
+        <v>292</v>
       </c>
       <c r="C173" t="s">
-        <v>267</v>
+        <v>301</v>
       </c>
       <c r="D173" t="s">
-        <v>187</v>
+        <v>293</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4082,13 +4091,13 @@
         <v>47</v>
       </c>
       <c r="B174" t="s">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="C174" t="s">
-        <v>257</v>
+        <v>52</v>
       </c>
       <c r="D174" t="s">
-        <v>125</v>
+        <v>55</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4096,111 +4105,111 @@
         <v>47</v>
       </c>
       <c r="B175" t="s">
-        <v>127</v>
+        <v>51</v>
       </c>
       <c r="C175" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="D175" t="s">
-        <v>129</v>
+        <v>53</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="2" t="s">
+      <c r="A176" t="s">
         <v>47</v>
       </c>
-      <c r="B176" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="D176" s="2" t="s">
-        <v>384</v>
+      <c r="B176" t="s">
+        <v>275</v>
+      </c>
+      <c r="C176" t="s">
+        <v>297</v>
+      </c>
+      <c r="D176" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="2" t="s">
+      <c r="A177" t="s">
         <v>47</v>
       </c>
-      <c r="B177" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D177" s="2" t="s">
-        <v>390</v>
+      <c r="B177" t="s">
+        <v>188</v>
+      </c>
+      <c r="C177" t="s">
+        <v>267</v>
+      </c>
+      <c r="D177" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>212</v>
+        <v>47</v>
       </c>
       <c r="B178" t="s">
-        <v>171</v>
+        <v>125</v>
       </c>
       <c r="C178" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="D178" t="s">
-        <v>172</v>
+        <v>125</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B179" t="s">
-        <v>309</v>
+        <v>127</v>
       </c>
       <c r="C179" t="s">
-        <v>310</v>
+        <v>128</v>
       </c>
       <c r="D179" t="s">
-        <v>308</v>
+        <v>129</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>50</v>
-      </c>
-      <c r="B180" t="s">
-        <v>57</v>
-      </c>
-      <c r="C180" t="s">
-        <v>52</v>
-      </c>
-      <c r="D180" t="s">
-        <v>55</v>
+      <c r="A180" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>50</v>
-      </c>
-      <c r="B181" t="s">
-        <v>59</v>
-      </c>
-      <c r="C181" t="s">
-        <v>52</v>
-      </c>
-      <c r="D181" t="s">
-        <v>55</v>
+      <c r="A181" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>50</v>
+        <v>212</v>
       </c>
       <c r="B182" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C182" t="s">
         <v>266</v>
       </c>
       <c r="D182" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4208,13 +4217,13 @@
         <v>50</v>
       </c>
       <c r="B183" t="s">
-        <v>169</v>
+        <v>309</v>
       </c>
       <c r="C183" t="s">
-        <v>266</v>
+        <v>310</v>
       </c>
       <c r="D183" t="s">
-        <v>170</v>
+        <v>308</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4222,69 +4231,69 @@
         <v>50</v>
       </c>
       <c r="B184" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="C184" t="s">
-        <v>266</v>
+        <v>52</v>
       </c>
       <c r="D184" t="s">
-        <v>174</v>
+        <v>55</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B185" t="s">
-        <v>116</v>
+        <v>59</v>
       </c>
       <c r="C185" t="s">
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="D185" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B186" t="s">
-        <v>118</v>
+        <v>175</v>
       </c>
       <c r="C186" t="s">
-        <v>117</v>
+        <v>266</v>
       </c>
       <c r="D186" t="s">
-        <v>118</v>
+        <v>176</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B187" t="s">
-        <v>119</v>
+        <v>169</v>
       </c>
       <c r="C187" t="s">
-        <v>117</v>
+        <v>266</v>
       </c>
       <c r="D187" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B188" t="s">
-        <v>120</v>
+        <v>173</v>
       </c>
       <c r="C188" t="s">
-        <v>117</v>
+        <v>266</v>
       </c>
       <c r="D188" t="s">
-        <v>121</v>
+        <v>174</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4292,83 +4301,125 @@
         <v>110</v>
       </c>
       <c r="B189" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C189" t="s">
         <v>117</v>
       </c>
       <c r="D189" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>207</v>
+        <v>110</v>
       </c>
       <c r="B190" t="s">
-        <v>195</v>
+        <v>118</v>
       </c>
       <c r="C190" t="s">
-        <v>254</v>
+        <v>117</v>
       </c>
       <c r="D190" t="s">
-        <v>196</v>
+        <v>118</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>207</v>
+        <v>110</v>
       </c>
       <c r="B191" t="s">
-        <v>195</v>
+        <v>119</v>
       </c>
       <c r="C191" t="s">
-        <v>254</v>
+        <v>117</v>
       </c>
       <c r="D191" t="s">
-        <v>202</v>
+        <v>119</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>207</v>
+        <v>110</v>
       </c>
       <c r="B192" t="s">
-        <v>199</v>
+        <v>120</v>
       </c>
       <c r="C192" t="s">
-        <v>254</v>
+        <v>117</v>
       </c>
       <c r="D192" t="s">
-        <v>200</v>
+        <v>121</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>110</v>
+      </c>
+      <c r="B193" t="s">
+        <v>122</v>
+      </c>
+      <c r="C193" t="s">
+        <v>117</v>
+      </c>
+      <c r="D193" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>207</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B194" t="s">
+        <v>195</v>
+      </c>
+      <c r="C194" t="s">
+        <v>254</v>
+      </c>
+      <c r="D194" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>207</v>
+      </c>
+      <c r="B195" t="s">
+        <v>195</v>
+      </c>
+      <c r="C195" t="s">
+        <v>254</v>
+      </c>
+      <c r="D195" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>207</v>
+      </c>
+      <c r="B196" t="s">
         <v>199</v>
       </c>
-      <c r="C193" t="s">
+      <c r="C196" t="s">
         <v>254</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D196" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>207</v>
+      </c>
+      <c r="B197" t="s">
+        <v>199</v>
+      </c>
+      <c r="C197" t="s">
+        <v>254</v>
+      </c>
+      <c r="D197" t="s">
         <v>203</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C194" t="s">
-        <v>297</v>
-      </c>
-      <c r="D194" s="2" t="s">
-        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding cell properties sample
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21814"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1B50C3-5FAB-4A63-8138-9AD50D51D3E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A104111A-54B1-431D-B3AB-660F7EA4F90D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="416">
   <si>
     <t>Class</t>
   </si>
@@ -1238,6 +1238,36 @@
   </si>
   <si>
     <t>setZoom</t>
+  </si>
+  <si>
+    <t>setCellProperties</t>
+  </si>
+  <si>
+    <t>excel-range-cell-properties</t>
+  </si>
+  <si>
+    <t>getCellProperties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CellPropertiesLoadOptions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CellPropertiesFillLoadOptions </t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CellPropertiesFontLoadOptions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SettableCellProperties </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CellPropertiesFill </t>
+  </si>
+  <si>
+    <t>CellPropertiesFont</t>
   </si>
 </sst>
 </file>
@@ -1317,10 +1347,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D197" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D197" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D197">
-    <sortCondition ref="A1:A197"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D205" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D205" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D205">
+    <sortCondition ref="A1:A205"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1629,7 +1659,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="6">
+  <wetp:taskpane dockstate="right" visibility="0" width="755" row="6">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1649,11 +1679,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D197"/>
+  <dimension ref="A1:D205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B182" sqref="B182"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B206" sqref="B206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,171 +1751,171 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" t="s">
-        <v>90</v>
+      <c r="A5" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" t="s">
-        <v>90</v>
+      <c r="A6" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C7" t="s">
-        <v>144</v>
-      </c>
-      <c r="D7" t="s">
-        <v>145</v>
+      <c r="A7" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" t="s">
-        <v>144</v>
-      </c>
-      <c r="D8" t="s">
-        <v>148</v>
+      <c r="A8" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" t="s">
-        <v>153</v>
-      </c>
-      <c r="C9" t="s">
-        <v>154</v>
-      </c>
-      <c r="D9" t="s">
-        <v>155</v>
+      <c r="A9" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>208</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>185</v>
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D12" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="C13" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="D13" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="B14" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="C14" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="D14" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B15" t="s">
-        <v>180</v>
-      </c>
-      <c r="C15" t="s">
-        <v>178</v>
-      </c>
-      <c r="D15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>136</v>
-      </c>
-      <c r="B16" t="s">
-        <v>177</v>
-      </c>
-      <c r="C16" t="s">
-        <v>178</v>
-      </c>
-      <c r="D16" t="s">
-        <v>179</v>
+      <c r="B16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1893,307 +1923,307 @@
         <v>136</v>
       </c>
       <c r="B17" t="s">
-        <v>142</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
         <v>139</v>
       </c>
       <c r="D17" t="s">
-        <v>264</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>259</v>
+        <v>136</v>
       </c>
       <c r="B18" t="s">
-        <v>260</v>
+        <v>182</v>
       </c>
       <c r="C18" t="s">
-        <v>261</v>
+        <v>178</v>
       </c>
       <c r="D18" t="s">
-        <v>262</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>259</v>
+        <v>136</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>181</v>
       </c>
       <c r="C19" t="s">
-        <v>261</v>
+        <v>178</v>
       </c>
       <c r="D19" t="s">
-        <v>263</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="C20" t="s">
-        <v>131</v>
+        <v>178</v>
       </c>
       <c r="D20" t="s">
-        <v>133</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>177</v>
       </c>
       <c r="C21" t="s">
-        <v>131</v>
+        <v>178</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B22" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C22" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>259</v>
       </c>
       <c r="B23" t="s">
-        <v>134</v>
+        <v>260</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>261</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>259</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>261</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>373</v>
+        <v>126</v>
       </c>
       <c r="B25" t="s">
-        <v>376</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>367</v>
+        <v>131</v>
       </c>
       <c r="D25" t="s">
-        <v>375</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>373</v>
+        <v>124</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>367</v>
+        <v>131</v>
       </c>
       <c r="D26" t="s">
-        <v>378</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>373</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
-        <v>374</v>
+        <v>134</v>
       </c>
       <c r="C27" t="s">
-        <v>367</v>
+        <v>131</v>
       </c>
       <c r="D27" t="s">
-        <v>372</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>368</v>
+        <v>130</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="C28" t="s">
-        <v>367</v>
+        <v>131</v>
       </c>
       <c r="D28" t="s">
-        <v>369</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>377</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>376</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
-        <v>367</v>
+        <v>61</v>
       </c>
       <c r="D29" t="s">
-        <v>375</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>376</v>
       </c>
       <c r="C30" t="s">
         <v>367</v>
       </c>
       <c r="D30" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
         <v>367</v>
       </c>
       <c r="D31" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>373</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>374</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>367</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>372</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>368</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>367</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>369</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>377</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>376</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>367</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>375</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>377</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>367</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>379</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>370</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>367</v>
       </c>
       <c r="D36" t="s">
-        <v>95</v>
+        <v>371</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="C37" t="s">
         <v>61</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
       </c>
       <c r="D38" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2201,13 +2231,13 @@
         <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="C39" t="s">
         <v>61</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2215,13 +2245,13 @@
         <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C40" t="s">
         <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2229,13 +2259,13 @@
         <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="C41" t="s">
         <v>61</v>
       </c>
       <c r="D41" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2243,853 +2273,853 @@
         <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C42" t="s">
         <v>61</v>
       </c>
       <c r="D42" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="C43" t="s">
         <v>61</v>
       </c>
       <c r="D43" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
         <v>61</v>
       </c>
       <c r="D44" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="C45" t="s">
         <v>61</v>
       </c>
       <c r="D45" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
         <v>61</v>
       </c>
       <c r="D46" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="C47" t="s">
         <v>61</v>
       </c>
       <c r="D47" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
         <v>61</v>
       </c>
       <c r="D48" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="C49" t="s">
         <v>61</v>
       </c>
       <c r="D49" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="C50" t="s">
         <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="C51" t="s">
         <v>61</v>
       </c>
       <c r="D51" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="C52" t="s">
         <v>61</v>
       </c>
       <c r="D52" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C53" t="s">
         <v>61</v>
       </c>
       <c r="D53" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="B54" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="C54" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D54" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="C55" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D55" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D56" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="B57" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="C57" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D57" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="C58" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D58" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B59" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="C59" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D59" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B60" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C60" t="s">
         <v>35</v>
       </c>
       <c r="D60" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B61" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C61" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D61" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B62" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C62" t="s">
         <v>35</v>
       </c>
       <c r="D62" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B63" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D63" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B64" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="C64" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D64" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>234</v>
+        <v>30</v>
       </c>
       <c r="B65" t="s">
-        <v>233</v>
+        <v>37</v>
       </c>
       <c r="C65" t="s">
-        <v>224</v>
+        <v>35</v>
       </c>
       <c r="D65" t="s">
-        <v>232</v>
+        <v>38</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>234</v>
+        <v>43</v>
       </c>
       <c r="B66" t="s">
-        <v>245</v>
+        <v>48</v>
       </c>
       <c r="C66" t="s">
-        <v>244</v>
+        <v>45</v>
       </c>
       <c r="D66" t="s">
-        <v>242</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>222</v>
+        <v>43</v>
       </c>
       <c r="B67" t="s">
-        <v>403</v>
+        <v>23</v>
       </c>
       <c r="C67" t="s">
-        <v>218</v>
+        <v>35</v>
       </c>
       <c r="D67" t="s">
-        <v>215</v>
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>222</v>
+        <v>43</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="C68" t="s">
-        <v>218</v>
+        <v>45</v>
       </c>
       <c r="D68" t="s">
-        <v>216</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>222</v>
+        <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>221</v>
+        <v>75</v>
       </c>
       <c r="C69" t="s">
-        <v>218</v>
+        <v>61</v>
       </c>
       <c r="D69" t="s">
-        <v>217</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="B70" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="C70" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D70" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="B71" t="s">
-        <v>219</v>
+        <v>245</v>
       </c>
       <c r="C71" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="D71" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>222</v>
       </c>
       <c r="B72" t="s">
-        <v>65</v>
+        <v>403</v>
       </c>
       <c r="C72" t="s">
-        <v>61</v>
+        <v>218</v>
       </c>
       <c r="D72" t="s">
-        <v>77</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>222</v>
       </c>
       <c r="B73" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C73" t="s">
-        <v>61</v>
+        <v>218</v>
       </c>
       <c r="D73" t="s">
-        <v>77</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>306</v>
+        <v>222</v>
       </c>
       <c r="B74" t="s">
-        <v>86</v>
+        <v>221</v>
       </c>
       <c r="C74" t="s">
-        <v>302</v>
+        <v>218</v>
       </c>
       <c r="D74" t="s">
-        <v>305</v>
+        <v>217</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>354</v>
+        <v>253</v>
       </c>
       <c r="B75" t="s">
-        <v>355</v>
+        <v>220</v>
       </c>
       <c r="C75" t="s">
-        <v>349</v>
+        <v>218</v>
       </c>
       <c r="D75" t="s">
-        <v>352</v>
+        <v>216</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>354</v>
+        <v>253</v>
       </c>
       <c r="B76" t="s">
-        <v>356</v>
+        <v>219</v>
       </c>
       <c r="C76" t="s">
-        <v>349</v>
+        <v>218</v>
       </c>
       <c r="D76" t="s">
-        <v>352</v>
+        <v>215</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>354</v>
+        <v>74</v>
       </c>
       <c r="B77" t="s">
-        <v>357</v>
+        <v>65</v>
       </c>
       <c r="C77" t="s">
-        <v>349</v>
+        <v>61</v>
       </c>
       <c r="D77" t="s">
-        <v>353</v>
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>354</v>
+        <v>74</v>
       </c>
       <c r="B78" t="s">
-        <v>358</v>
+        <v>79</v>
       </c>
       <c r="C78" t="s">
-        <v>349</v>
+        <v>61</v>
       </c>
       <c r="D78" t="s">
-        <v>353</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>10</v>
+        <v>306</v>
       </c>
       <c r="B79" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C79" t="s">
-        <v>12</v>
+        <v>302</v>
       </c>
       <c r="D79" t="s">
-        <v>13</v>
+        <v>305</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>10</v>
+        <v>354</v>
       </c>
       <c r="B80" t="s">
-        <v>14</v>
+        <v>355</v>
       </c>
       <c r="C80" t="s">
-        <v>15</v>
+        <v>349</v>
       </c>
       <c r="D80" t="s">
-        <v>16</v>
+        <v>352</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>8</v>
+        <v>354</v>
       </c>
       <c r="B81" t="s">
-        <v>9</v>
+        <v>356</v>
       </c>
       <c r="C81" t="s">
-        <v>12</v>
+        <v>349</v>
       </c>
       <c r="D81" t="s">
-        <v>265</v>
+        <v>352</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>320</v>
+        <v>354</v>
       </c>
       <c r="B82" t="s">
-        <v>9</v>
+        <v>357</v>
       </c>
       <c r="C82" t="s">
-        <v>321</v>
+        <v>349</v>
       </c>
       <c r="D82" t="s">
-        <v>322</v>
+        <v>353</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>325</v>
+        <v>354</v>
       </c>
       <c r="B83" t="s">
-        <v>323</v>
+        <v>358</v>
       </c>
       <c r="C83" t="s">
-        <v>321</v>
+        <v>349</v>
       </c>
       <c r="D83" t="s">
-        <v>326</v>
+        <v>353</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>325</v>
+        <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>324</v>
+        <v>11</v>
       </c>
       <c r="C84" t="s">
-        <v>321</v>
+        <v>12</v>
       </c>
       <c r="D84" t="s">
-        <v>326</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>325</v>
+        <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>330</v>
+        <v>14</v>
       </c>
       <c r="C85" t="s">
-        <v>321</v>
+        <v>15</v>
       </c>
       <c r="D85" t="s">
-        <v>341</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>325</v>
+        <v>8</v>
       </c>
       <c r="B86" t="s">
-        <v>329</v>
+        <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>321</v>
+        <v>12</v>
       </c>
       <c r="D86" t="s">
-        <v>329</v>
+        <v>265</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B87" t="s">
-        <v>327</v>
+        <v>9</v>
       </c>
       <c r="C87" t="s">
         <v>321</v>
       </c>
       <c r="D87" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
+      <c r="A88" t="s">
         <v>325</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>404</v>
+      <c r="B88" t="s">
+        <v>323</v>
       </c>
       <c r="C88" t="s">
         <v>321</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>405</v>
+      <c r="D88" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>239</v>
+        <v>325</v>
       </c>
       <c r="B89" t="s">
-        <v>240</v>
+        <v>324</v>
       </c>
       <c r="C89" t="s">
-        <v>243</v>
+        <v>321</v>
       </c>
       <c r="D89" t="s">
-        <v>241</v>
+        <v>326</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>226</v>
+        <v>325</v>
       </c>
       <c r="B90" t="s">
-        <v>229</v>
+        <v>330</v>
       </c>
       <c r="C90" t="s">
-        <v>224</v>
+        <v>321</v>
       </c>
       <c r="D90" t="s">
-        <v>228</v>
+        <v>341</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>226</v>
+        <v>325</v>
       </c>
       <c r="B91" t="s">
-        <v>230</v>
+        <v>329</v>
       </c>
       <c r="C91" t="s">
-        <v>224</v>
+        <v>321</v>
       </c>
       <c r="D91" t="s">
-        <v>231</v>
+        <v>329</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>226</v>
+        <v>325</v>
       </c>
       <c r="B92" t="s">
-        <v>11</v>
+        <v>327</v>
       </c>
       <c r="C92" t="s">
-        <v>224</v>
+        <v>321</v>
       </c>
       <c r="D92" t="s">
-        <v>227</v>
+        <v>328</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>226</v>
-      </c>
-      <c r="B93" t="s">
-        <v>237</v>
+      <c r="A93" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>404</v>
       </c>
       <c r="C93" t="s">
-        <v>243</v>
-      </c>
-      <c r="D93" t="s">
-        <v>238</v>
+        <v>321</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="B94" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="C94" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="D94" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B95" t="s">
-        <v>9</v>
+        <v>229</v>
       </c>
       <c r="C95" t="s">
         <v>224</v>
       </c>
       <c r="D95" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>64</v>
+        <v>226</v>
       </c>
       <c r="B96" t="s">
-        <v>69</v>
+        <v>230</v>
       </c>
       <c r="C96" t="s">
-        <v>61</v>
+        <v>224</v>
       </c>
       <c r="D96" t="s">
-        <v>68</v>
+        <v>231</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>64</v>
+        <v>226</v>
       </c>
       <c r="B97" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="C97" t="s">
-        <v>61</v>
+        <v>224</v>
       </c>
       <c r="D97" t="s">
-        <v>95</v>
+        <v>227</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>24</v>
+        <v>226</v>
       </c>
       <c r="B98" t="s">
-        <v>286</v>
+        <v>237</v>
       </c>
       <c r="C98" t="s">
-        <v>299</v>
+        <v>243</v>
       </c>
       <c r="D98" t="s">
-        <v>287</v>
+        <v>238</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>24</v>
+        <v>226</v>
       </c>
       <c r="B99" t="s">
-        <v>288</v>
+        <v>235</v>
       </c>
       <c r="C99" t="s">
-        <v>300</v>
+        <v>224</v>
       </c>
       <c r="D99" t="s">
-        <v>289</v>
+        <v>236</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>24</v>
+        <v>223</v>
       </c>
       <c r="B100" t="s">
-        <v>290</v>
+        <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>300</v>
+        <v>224</v>
       </c>
       <c r="D100" t="s">
-        <v>291</v>
+        <v>225</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B101" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="C101" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D101" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B102" t="s">
-        <v>276</v>
+        <v>69</v>
       </c>
       <c r="C102" t="s">
-        <v>297</v>
+        <v>61</v>
       </c>
       <c r="D102" t="s">
-        <v>277</v>
+        <v>95</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3097,13 +3127,13 @@
         <v>24</v>
       </c>
       <c r="B103" t="s">
-        <v>29</v>
+        <v>286</v>
       </c>
       <c r="C103" t="s">
-        <v>255</v>
+        <v>299</v>
       </c>
       <c r="D103" t="s">
-        <v>28</v>
+        <v>287</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -3111,13 +3141,13 @@
         <v>24</v>
       </c>
       <c r="B104" t="s">
-        <v>25</v>
+        <v>288</v>
       </c>
       <c r="C104" t="s">
-        <v>268</v>
+        <v>300</v>
       </c>
       <c r="D104" t="s">
-        <v>26</v>
+        <v>289</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3125,13 +3155,13 @@
         <v>24</v>
       </c>
       <c r="B105" t="s">
-        <v>103</v>
+        <v>290</v>
       </c>
       <c r="C105" t="s">
-        <v>104</v>
+        <v>300</v>
       </c>
       <c r="D105" t="s">
-        <v>105</v>
+        <v>291</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -3139,13 +3169,13 @@
         <v>24</v>
       </c>
       <c r="B106" t="s">
-        <v>333</v>
+        <v>27</v>
       </c>
       <c r="C106" t="s">
-        <v>332</v>
+        <v>255</v>
       </c>
       <c r="D106" t="s">
-        <v>331</v>
+        <v>28</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -3153,13 +3183,13 @@
         <v>24</v>
       </c>
       <c r="B107" t="s">
-        <v>31</v>
+        <v>276</v>
       </c>
       <c r="C107" t="s">
-        <v>258</v>
+        <v>297</v>
       </c>
       <c r="D107" t="s">
-        <v>32</v>
+        <v>277</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -3167,13 +3197,13 @@
         <v>24</v>
       </c>
       <c r="B108" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C108" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D108" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3181,293 +3211,293 @@
         <v>24</v>
       </c>
       <c r="B109" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="C109" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="D109" t="s">
-        <v>160</v>
+        <v>26</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>86</v>
+      <c r="A110" t="s">
+        <v>24</v>
+      </c>
+      <c r="B110" t="s">
+        <v>103</v>
       </c>
       <c r="C110" t="s">
-        <v>297</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>402</v>
+        <v>104</v>
+      </c>
+      <c r="D110" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>108</v>
+        <v>24</v>
       </c>
       <c r="B111" t="s">
-        <v>113</v>
+        <v>333</v>
       </c>
       <c r="C111" t="s">
-        <v>114</v>
+        <v>332</v>
       </c>
       <c r="D111" t="s">
-        <v>115</v>
+        <v>331</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B112" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="C112" t="s">
-        <v>104</v>
+        <v>258</v>
       </c>
       <c r="D112" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B113" t="s">
-        <v>111</v>
+        <v>31</v>
       </c>
       <c r="C113" t="s">
-        <v>104</v>
+        <v>258</v>
       </c>
       <c r="D113" t="s">
-        <v>112</v>
+        <v>33</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B114" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="C114" t="s">
-        <v>104</v>
+        <v>256</v>
       </c>
       <c r="D114" t="s">
-        <v>105</v>
+        <v>160</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>100</v>
-      </c>
-      <c r="B115" t="s">
-        <v>109</v>
-      </c>
-      <c r="C115" t="s">
-        <v>104</v>
-      </c>
-      <c r="D115" t="s">
-        <v>105</v>
+      <c r="A115" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>342</v>
-      </c>
-      <c r="B116" t="s">
-        <v>334</v>
-      </c>
-      <c r="C116" t="s">
-        <v>332</v>
-      </c>
-      <c r="D116" t="s">
-        <v>331</v>
+      <c r="A116" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>249</v>
-      </c>
-      <c r="B117" t="s">
-        <v>250</v>
+      <c r="A117" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="C117" t="s">
-        <v>251</v>
-      </c>
-      <c r="D117" t="s">
-        <v>252</v>
+        <v>297</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="B118" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
       <c r="C118" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="D118" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="B119" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="C119" t="s">
-        <v>266</v>
+        <v>104</v>
       </c>
       <c r="D119" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="B120" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="C120" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="D120" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="B121" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="C121" t="s">
-        <v>266</v>
+        <v>104</v>
       </c>
       <c r="D121" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>278</v>
+        <v>100</v>
       </c>
       <c r="B122" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="C122" t="s">
-        <v>298</v>
+        <v>104</v>
       </c>
       <c r="D122" t="s">
-        <v>285</v>
+        <v>105</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>278</v>
+        <v>342</v>
       </c>
       <c r="B123" t="s">
-        <v>284</v>
+        <v>334</v>
       </c>
       <c r="C123" t="s">
-        <v>298</v>
+        <v>332</v>
       </c>
       <c r="D123" t="s">
-        <v>283</v>
+        <v>331</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
       <c r="B124" t="s">
-        <v>366</v>
+        <v>250</v>
       </c>
       <c r="C124" t="s">
-        <v>302</v>
+        <v>251</v>
       </c>
       <c r="D124" t="s">
-        <v>307</v>
+        <v>252</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>278</v>
-      </c>
-      <c r="B125" t="s">
-        <v>363</v>
-      </c>
-      <c r="C125" t="s">
-        <v>361</v>
-      </c>
-      <c r="D125" t="s">
-        <v>362</v>
+      <c r="A125" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>278</v>
+        <v>20</v>
       </c>
       <c r="B126" t="s">
-        <v>311</v>
+        <v>11</v>
       </c>
       <c r="C126" t="s">
-        <v>313</v>
+        <v>21</v>
       </c>
       <c r="D126" t="s">
-        <v>314</v>
+        <v>22</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="B127" t="s">
-        <v>304</v>
+        <v>9</v>
       </c>
       <c r="C127" t="s">
-        <v>302</v>
+        <v>266</v>
       </c>
       <c r="D127" t="s">
-        <v>303</v>
+        <v>19</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="B128" t="s">
-        <v>312</v>
+        <v>23</v>
       </c>
       <c r="C128" t="s">
-        <v>313</v>
+        <v>21</v>
       </c>
       <c r="D128" t="s">
-        <v>315</v>
+        <v>22</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="B129" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
       <c r="C129" t="s">
-        <v>349</v>
+        <v>266</v>
       </c>
       <c r="D129" t="s">
-        <v>351</v>
+        <v>19</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3475,13 +3505,13 @@
         <v>278</v>
       </c>
       <c r="B130" t="s">
-        <v>279</v>
+        <v>11</v>
       </c>
       <c r="C130" t="s">
         <v>298</v>
       </c>
       <c r="D130" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3489,13 +3519,13 @@
         <v>278</v>
       </c>
       <c r="B131" t="s">
-        <v>319</v>
+        <v>284</v>
       </c>
       <c r="C131" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="D131" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3503,13 +3533,13 @@
         <v>278</v>
       </c>
       <c r="B132" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="C132" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D132" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3517,556 +3547,556 @@
         <v>278</v>
       </c>
       <c r="B133" t="s">
-        <v>318</v>
+        <v>363</v>
       </c>
       <c r="C133" t="s">
-        <v>313</v>
+        <v>361</v>
       </c>
       <c r="D133" t="s">
-        <v>317</v>
+        <v>362</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B134" t="s">
-        <v>282</v>
+        <v>311</v>
       </c>
       <c r="C134" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="D134" t="s">
-        <v>340</v>
+        <v>314</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B135" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="C135" t="s">
-        <v>361</v>
+        <v>302</v>
       </c>
       <c r="D135" t="s">
-        <v>365</v>
+        <v>303</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B136" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="C136" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="D136" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B137" t="s">
-        <v>348</v>
+        <v>134</v>
       </c>
       <c r="C137" t="s">
         <v>349</v>
       </c>
       <c r="D137" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B138" t="s">
-        <v>343</v>
+        <v>279</v>
       </c>
       <c r="C138" t="s">
-        <v>344</v>
+        <v>298</v>
       </c>
       <c r="D138" t="s">
-        <v>345</v>
+        <v>280</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>359</v>
+        <v>278</v>
       </c>
       <c r="B139" t="s">
-        <v>360</v>
+        <v>319</v>
       </c>
       <c r="C139" t="s">
-        <v>361</v>
+        <v>313</v>
       </c>
       <c r="D139" t="s">
-        <v>362</v>
+        <v>316</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>246</v>
+        <v>278</v>
       </c>
       <c r="B140" t="s">
-        <v>247</v>
+        <v>380</v>
       </c>
       <c r="C140" t="s">
-        <v>244</v>
+        <v>313</v>
       </c>
       <c r="D140" t="s">
-        <v>248</v>
+        <v>316</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>394</v>
+      <c r="A141" t="s">
+        <v>278</v>
+      </c>
+      <c r="B141" t="s">
+        <v>318</v>
+      </c>
+      <c r="C141" t="s">
+        <v>313</v>
+      </c>
+      <c r="D141" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D142" s="2" t="s">
-        <v>396</v>
+      <c r="A142" t="s">
+        <v>281</v>
+      </c>
+      <c r="B142" t="s">
+        <v>282</v>
+      </c>
+      <c r="C142" t="s">
+        <v>298</v>
+      </c>
+      <c r="D142" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D143" s="2" t="s">
-        <v>399</v>
+      <c r="A143" t="s">
+        <v>281</v>
+      </c>
+      <c r="B143" t="s">
+        <v>364</v>
+      </c>
+      <c r="C143" t="s">
+        <v>361</v>
+      </c>
+      <c r="D143" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D144" s="2" t="s">
-        <v>400</v>
+      <c r="A144" t="s">
+        <v>281</v>
+      </c>
+      <c r="B144" t="s">
+        <v>294</v>
+      </c>
+      <c r="C144" t="s">
+        <v>302</v>
+      </c>
+      <c r="D144" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D145" s="2" t="s">
-        <v>390</v>
+      <c r="A145" t="s">
+        <v>281</v>
+      </c>
+      <c r="B145" t="s">
+        <v>348</v>
+      </c>
+      <c r="C145" t="s">
+        <v>349</v>
+      </c>
+      <c r="D145" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>393</v>
+      <c r="A146" t="s">
+        <v>281</v>
+      </c>
+      <c r="B146" t="s">
+        <v>343</v>
+      </c>
+      <c r="C146" t="s">
+        <v>344</v>
+      </c>
+      <c r="D146" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>152</v>
+        <v>359</v>
       </c>
       <c r="B147" t="s">
-        <v>11</v>
+        <v>360</v>
       </c>
       <c r="C147" t="s">
-        <v>256</v>
+        <v>361</v>
       </c>
       <c r="D147" t="s">
-        <v>163</v>
+        <v>362</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>152</v>
+        <v>246</v>
       </c>
       <c r="B148" t="s">
-        <v>149</v>
+        <v>247</v>
       </c>
       <c r="C148" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="D148" t="s">
-        <v>162</v>
+        <v>248</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>152</v>
-      </c>
-      <c r="B149" t="s">
-        <v>164</v>
-      </c>
-      <c r="C149" t="s">
-        <v>256</v>
-      </c>
-      <c r="D149" t="s">
-        <v>160</v>
+      <c r="A149" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>152</v>
-      </c>
-      <c r="B150" t="s">
-        <v>209</v>
-      </c>
-      <c r="C150" t="s">
-        <v>256</v>
-      </c>
-      <c r="D150" t="s">
-        <v>165</v>
+      <c r="A150" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>156</v>
-      </c>
-      <c r="B151" t="s">
+      <c r="A151" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C151" t="s">
-        <v>256</v>
-      </c>
-      <c r="D151" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>156</v>
-      </c>
-      <c r="B152" t="s">
+      <c r="C153" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B154" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C152" t="s">
-        <v>256</v>
-      </c>
-      <c r="D152" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>211</v>
-      </c>
-      <c r="B153" t="s">
-        <v>188</v>
-      </c>
-      <c r="C153" t="s">
-        <v>186</v>
-      </c>
-      <c r="D153" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>211</v>
-      </c>
-      <c r="B154" t="s">
-        <v>167</v>
-      </c>
-      <c r="C154" t="s">
-        <v>186</v>
-      </c>
-      <c r="D154" t="s">
-        <v>168</v>
+      <c r="C154" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="B155" t="s">
-        <v>184</v>
+        <v>11</v>
       </c>
       <c r="C155" t="s">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="D155" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="B156" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C156" t="s">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="D156" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="B157" t="s">
-        <v>383</v>
+        <v>164</v>
       </c>
       <c r="C157" t="s">
-        <v>382</v>
+        <v>256</v>
       </c>
       <c r="D157" t="s">
-        <v>381</v>
+        <v>160</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>213</v>
+        <v>152</v>
       </c>
       <c r="B158" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="C158" t="s">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="D158" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>210</v>
+        <v>156</v>
       </c>
       <c r="B159" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="C159" t="s">
-        <v>186</v>
+        <v>256</v>
       </c>
       <c r="D159" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="B160" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="C160" t="s">
-        <v>61</v>
+        <v>256</v>
       </c>
       <c r="D160" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>82</v>
+        <v>211</v>
       </c>
       <c r="B161" t="s">
-        <v>69</v>
+        <v>188</v>
       </c>
       <c r="C161" t="s">
-        <v>61</v>
+        <v>186</v>
       </c>
       <c r="D161" t="s">
-        <v>84</v>
+        <v>187</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>347</v>
+        <v>211</v>
       </c>
       <c r="B162" t="s">
-        <v>346</v>
+        <v>167</v>
       </c>
       <c r="C162" t="s">
-        <v>344</v>
+        <v>186</v>
       </c>
       <c r="D162" t="s">
-        <v>346</v>
+        <v>168</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="B163" t="s">
-        <v>338</v>
+        <v>184</v>
       </c>
       <c r="C163" t="s">
-        <v>336</v>
+        <v>183</v>
       </c>
       <c r="D163" t="s">
-        <v>339</v>
+        <v>189</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="B164" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="C164" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D164" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="B165" t="s">
-        <v>272</v>
+        <v>383</v>
       </c>
       <c r="C165" t="s">
-        <v>297</v>
+        <v>382</v>
       </c>
       <c r="D165" t="s">
-        <v>273</v>
+        <v>381</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="B166" t="s">
-        <v>157</v>
+        <v>188</v>
       </c>
       <c r="C166" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="D166" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B167" t="s">
-        <v>335</v>
+        <v>106</v>
       </c>
       <c r="C167" t="s">
-        <v>336</v>
+        <v>186</v>
       </c>
       <c r="D167" t="s">
-        <v>337</v>
+        <v>166</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>206</v>
+        <v>82</v>
       </c>
       <c r="B168" t="s">
-        <v>195</v>
+        <v>86</v>
       </c>
       <c r="C168" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D168" t="s">
-        <v>197</v>
+        <v>84</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>206</v>
+        <v>82</v>
       </c>
       <c r="B169" t="s">
-        <v>195</v>
+        <v>69</v>
       </c>
       <c r="C169" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D169" t="s">
-        <v>204</v>
+        <v>84</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>206</v>
+        <v>347</v>
       </c>
       <c r="B170" t="s">
-        <v>199</v>
+        <v>346</v>
       </c>
       <c r="C170" t="s">
-        <v>254</v>
+        <v>344</v>
       </c>
       <c r="D170" t="s">
-        <v>201</v>
+        <v>346</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B171" t="s">
-        <v>199</v>
+        <v>338</v>
       </c>
       <c r="C171" t="s">
-        <v>254</v>
+        <v>336</v>
       </c>
       <c r="D171" t="s">
-        <v>205</v>
+        <v>339</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="B172" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C172" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D172" t="s">
         <v>198</v>
@@ -4074,351 +4104,463 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="B173" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="C173" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D173" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="B174" t="s">
-        <v>54</v>
+        <v>157</v>
       </c>
       <c r="C174" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="D174" t="s">
-        <v>55</v>
+        <v>159</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="B175" t="s">
-        <v>51</v>
+        <v>335</v>
       </c>
       <c r="C175" t="s">
-        <v>52</v>
+        <v>336</v>
       </c>
       <c r="D175" t="s">
-        <v>53</v>
+        <v>337</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B176" t="s">
-        <v>275</v>
+        <v>195</v>
       </c>
       <c r="C176" t="s">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="D176" t="s">
-        <v>274</v>
+        <v>197</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B177" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C177" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="D177" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B178" t="s">
-        <v>125</v>
+        <v>199</v>
       </c>
       <c r="C178" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D178" t="s">
-        <v>125</v>
+        <v>201</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
+        <v>206</v>
+      </c>
+      <c r="B179" t="s">
+        <v>199</v>
+      </c>
+      <c r="C179" t="s">
+        <v>254</v>
+      </c>
+      <c r="D179" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>47</v>
       </c>
-      <c r="B179" t="s">
-        <v>127</v>
-      </c>
-      <c r="C179" t="s">
-        <v>128</v>
-      </c>
-      <c r="D179" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="2" t="s">
+      <c r="B180" t="s">
+        <v>193</v>
+      </c>
+      <c r="C180" t="s">
+        <v>194</v>
+      </c>
+      <c r="D180" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>47</v>
       </c>
-      <c r="B180" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="C180" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="D180" s="2" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="C181" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D181" s="2" t="s">
-        <v>390</v>
+      <c r="B181" t="s">
+        <v>292</v>
+      </c>
+      <c r="C181" t="s">
+        <v>301</v>
+      </c>
+      <c r="D181" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>212</v>
+        <v>47</v>
       </c>
       <c r="B182" t="s">
-        <v>171</v>
+        <v>54</v>
       </c>
       <c r="C182" t="s">
-        <v>266</v>
+        <v>52</v>
       </c>
       <c r="D182" t="s">
-        <v>172</v>
+        <v>55</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B183" t="s">
-        <v>309</v>
+        <v>51</v>
       </c>
       <c r="C183" t="s">
-        <v>310</v>
+        <v>52</v>
       </c>
       <c r="D183" t="s">
-        <v>308</v>
+        <v>53</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B184" t="s">
-        <v>57</v>
+        <v>275</v>
       </c>
       <c r="C184" t="s">
-        <v>52</v>
+        <v>297</v>
       </c>
       <c r="D184" t="s">
-        <v>55</v>
+        <v>274</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B185" t="s">
-        <v>59</v>
+        <v>188</v>
       </c>
       <c r="C185" t="s">
-        <v>52</v>
+        <v>267</v>
       </c>
       <c r="D185" t="s">
-        <v>55</v>
+        <v>187</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B186" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="C186" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="D186" t="s">
-        <v>176</v>
+        <v>125</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B187" t="s">
-        <v>169</v>
+        <v>127</v>
       </c>
       <c r="C187" t="s">
-        <v>266</v>
+        <v>128</v>
       </c>
       <c r="D187" t="s">
-        <v>170</v>
+        <v>129</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>50</v>
-      </c>
-      <c r="B188" t="s">
-        <v>173</v>
-      </c>
-      <c r="C188" t="s">
-        <v>266</v>
-      </c>
-      <c r="D188" t="s">
-        <v>174</v>
+      <c r="A188" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>110</v>
-      </c>
-      <c r="B189" t="s">
-        <v>116</v>
-      </c>
-      <c r="C189" t="s">
-        <v>117</v>
-      </c>
-      <c r="D189" t="s">
-        <v>116</v>
+      <c r="A189" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>110</v>
+        <v>212</v>
       </c>
       <c r="B190" t="s">
-        <v>118</v>
+        <v>171</v>
       </c>
       <c r="C190" t="s">
-        <v>117</v>
+        <v>266</v>
       </c>
       <c r="D190" t="s">
-        <v>118</v>
+        <v>172</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B191" t="s">
-        <v>119</v>
+        <v>309</v>
       </c>
       <c r="C191" t="s">
-        <v>117</v>
+        <v>310</v>
       </c>
       <c r="D191" t="s">
-        <v>119</v>
+        <v>308</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B192" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="C192" t="s">
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="D192" t="s">
-        <v>121</v>
+        <v>55</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B193" t="s">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="C193" t="s">
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="D193" t="s">
-        <v>123</v>
+        <v>55</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>207</v>
+        <v>50</v>
       </c>
       <c r="B194" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="C194" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="D194" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>207</v>
+        <v>50</v>
       </c>
       <c r="B195" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="C195" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="D195" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>207</v>
+        <v>50</v>
       </c>
       <c r="B196" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="C196" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="D196" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
+        <v>110</v>
+      </c>
+      <c r="B197" t="s">
+        <v>116</v>
+      </c>
+      <c r="C197" t="s">
+        <v>117</v>
+      </c>
+      <c r="D197" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>110</v>
+      </c>
+      <c r="B198" t="s">
+        <v>118</v>
+      </c>
+      <c r="C198" t="s">
+        <v>117</v>
+      </c>
+      <c r="D198" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>110</v>
+      </c>
+      <c r="B199" t="s">
+        <v>119</v>
+      </c>
+      <c r="C199" t="s">
+        <v>117</v>
+      </c>
+      <c r="D199" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>110</v>
+      </c>
+      <c r="B200" t="s">
+        <v>120</v>
+      </c>
+      <c r="C200" t="s">
+        <v>117</v>
+      </c>
+      <c r="D200" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>110</v>
+      </c>
+      <c r="B201" t="s">
+        <v>122</v>
+      </c>
+      <c r="C201" t="s">
+        <v>117</v>
+      </c>
+      <c r="D201" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>207</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B202" t="s">
+        <v>195</v>
+      </c>
+      <c r="C202" t="s">
+        <v>254</v>
+      </c>
+      <c r="D202" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>207</v>
+      </c>
+      <c r="B203" t="s">
+        <v>195</v>
+      </c>
+      <c r="C203" t="s">
+        <v>254</v>
+      </c>
+      <c r="D203" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>207</v>
+      </c>
+      <c r="B204" t="s">
         <v>199</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C204" t="s">
         <v>254</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D204" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>207</v>
+      </c>
+      <c r="B205" t="s">
+        <v>199</v>
+      </c>
+      <c r="C205" t="s">
+        <v>254</v>
+      </c>
+      <c r="D205" t="s">
         <v>203</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[excel] (Range) Cell properties samples (#319)
* Mapping snippets for structs that must be set together

* Adding cell properties sample

* Updating yarn lock
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21814"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1B50C3-5FAB-4A63-8138-9AD50D51D3E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0A8BB1-C249-4398-B565-E104C8E1E110}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="416">
   <si>
     <t>Class</t>
   </si>
@@ -1238,6 +1238,36 @@
   </si>
   <si>
     <t>setZoom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CellPropertiesFill </t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>excel-range-cell-properties</t>
+  </si>
+  <si>
+    <t>setCellProperties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CellPropertiesFillLoadOptions </t>
+  </si>
+  <si>
+    <t>getCellProperties</t>
+  </si>
+  <si>
+    <t>CellPropertiesFont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CellPropertiesFontLoadOptions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CellPropertiesLoadOptions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SettableCellProperties </t>
   </si>
 </sst>
 </file>
@@ -1317,10 +1347,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D197" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D197" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D197">
-    <sortCondition ref="A1:A197"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D205" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D205" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D205">
+    <sortCondition ref="A1:A205"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
@@ -1649,11 +1679,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D197"/>
+  <dimension ref="A1:D205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B182" sqref="B182"/>
+      <selection pane="bottomLeft" activeCell="B208" sqref="B208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,171 +1751,171 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" t="s">
-        <v>90</v>
+      <c r="A5" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" t="s">
-        <v>90</v>
+      <c r="A6" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C7" t="s">
-        <v>144</v>
-      </c>
-      <c r="D7" t="s">
-        <v>145</v>
+      <c r="A7" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" t="s">
-        <v>144</v>
-      </c>
-      <c r="D8" t="s">
-        <v>148</v>
+      <c r="A8" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" t="s">
-        <v>153</v>
-      </c>
-      <c r="C9" t="s">
-        <v>154</v>
-      </c>
-      <c r="D9" t="s">
-        <v>155</v>
+      <c r="A9" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>208</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>185</v>
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D12" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="C13" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="D13" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="B14" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="C14" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="D14" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B15" t="s">
-        <v>180</v>
-      </c>
-      <c r="C15" t="s">
-        <v>178</v>
-      </c>
-      <c r="D15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>136</v>
-      </c>
-      <c r="B16" t="s">
-        <v>177</v>
-      </c>
-      <c r="C16" t="s">
-        <v>178</v>
-      </c>
-      <c r="D16" t="s">
-        <v>179</v>
+      <c r="B16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1893,307 +1923,307 @@
         <v>136</v>
       </c>
       <c r="B17" t="s">
-        <v>142</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
         <v>139</v>
       </c>
       <c r="D17" t="s">
-        <v>264</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>259</v>
+        <v>136</v>
       </c>
       <c r="B18" t="s">
-        <v>260</v>
+        <v>182</v>
       </c>
       <c r="C18" t="s">
-        <v>261</v>
+        <v>178</v>
       </c>
       <c r="D18" t="s">
-        <v>262</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>259</v>
+        <v>136</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>181</v>
       </c>
       <c r="C19" t="s">
-        <v>261</v>
+        <v>178</v>
       </c>
       <c r="D19" t="s">
-        <v>263</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="C20" t="s">
-        <v>131</v>
+        <v>178</v>
       </c>
       <c r="D20" t="s">
-        <v>133</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>177</v>
       </c>
       <c r="C21" t="s">
-        <v>131</v>
+        <v>178</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B22" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C22" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>259</v>
       </c>
       <c r="B23" t="s">
-        <v>134</v>
+        <v>260</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>261</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>259</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>261</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>373</v>
+        <v>126</v>
       </c>
       <c r="B25" t="s">
-        <v>376</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>367</v>
+        <v>131</v>
       </c>
       <c r="D25" t="s">
-        <v>375</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>373</v>
+        <v>124</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>367</v>
+        <v>131</v>
       </c>
       <c r="D26" t="s">
-        <v>378</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>373</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
-        <v>374</v>
+        <v>134</v>
       </c>
       <c r="C27" t="s">
-        <v>367</v>
+        <v>131</v>
       </c>
       <c r="D27" t="s">
-        <v>372</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>368</v>
+        <v>130</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="C28" t="s">
-        <v>367</v>
+        <v>131</v>
       </c>
       <c r="D28" t="s">
-        <v>369</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>377</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>376</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
-        <v>367</v>
+        <v>61</v>
       </c>
       <c r="D29" t="s">
-        <v>375</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>376</v>
       </c>
       <c r="C30" t="s">
         <v>367</v>
       </c>
       <c r="D30" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
         <v>367</v>
       </c>
       <c r="D31" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>373</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>374</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>367</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>372</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>368</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>367</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>369</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>377</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>376</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>367</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>375</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>377</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>367</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>379</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>370</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>367</v>
       </c>
       <c r="D36" t="s">
-        <v>95</v>
+        <v>371</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="C37" t="s">
         <v>61</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
       </c>
       <c r="D38" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2201,13 +2231,13 @@
         <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="C39" t="s">
         <v>61</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2215,13 +2245,13 @@
         <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C40" t="s">
         <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2229,13 +2259,13 @@
         <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="C41" t="s">
         <v>61</v>
       </c>
       <c r="D41" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2243,853 +2273,853 @@
         <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C42" t="s">
         <v>61</v>
       </c>
       <c r="D42" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="C43" t="s">
         <v>61</v>
       </c>
       <c r="D43" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
         <v>61</v>
       </c>
       <c r="D44" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="C45" t="s">
         <v>61</v>
       </c>
       <c r="D45" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
         <v>61</v>
       </c>
       <c r="D46" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="C47" t="s">
         <v>61</v>
       </c>
       <c r="D47" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
         <v>61</v>
       </c>
       <c r="D48" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="C49" t="s">
         <v>61</v>
       </c>
       <c r="D49" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="C50" t="s">
         <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="C51" t="s">
         <v>61</v>
       </c>
       <c r="D51" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="C52" t="s">
         <v>61</v>
       </c>
       <c r="D52" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C53" t="s">
         <v>61</v>
       </c>
       <c r="D53" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="B54" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="C54" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D54" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="C55" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D55" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D56" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="B57" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="C57" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D57" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="C58" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D58" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B59" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="C59" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D59" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B60" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C60" t="s">
         <v>35</v>
       </c>
       <c r="D60" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B61" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C61" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D61" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B62" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C62" t="s">
         <v>35</v>
       </c>
       <c r="D62" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B63" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D63" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B64" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="C64" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D64" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>234</v>
+        <v>30</v>
       </c>
       <c r="B65" t="s">
-        <v>233</v>
+        <v>37</v>
       </c>
       <c r="C65" t="s">
-        <v>224</v>
+        <v>35</v>
       </c>
       <c r="D65" t="s">
-        <v>232</v>
+        <v>38</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>234</v>
+        <v>43</v>
       </c>
       <c r="B66" t="s">
-        <v>245</v>
+        <v>48</v>
       </c>
       <c r="C66" t="s">
-        <v>244</v>
+        <v>45</v>
       </c>
       <c r="D66" t="s">
-        <v>242</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>222</v>
+        <v>43</v>
       </c>
       <c r="B67" t="s">
-        <v>403</v>
+        <v>23</v>
       </c>
       <c r="C67" t="s">
-        <v>218</v>
+        <v>35</v>
       </c>
       <c r="D67" t="s">
-        <v>215</v>
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>222</v>
+        <v>43</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="C68" t="s">
-        <v>218</v>
+        <v>45</v>
       </c>
       <c r="D68" t="s">
-        <v>216</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>222</v>
+        <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>221</v>
+        <v>75</v>
       </c>
       <c r="C69" t="s">
-        <v>218</v>
+        <v>61</v>
       </c>
       <c r="D69" t="s">
-        <v>217</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="B70" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="C70" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D70" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="B71" t="s">
-        <v>219</v>
+        <v>245</v>
       </c>
       <c r="C71" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="D71" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>222</v>
       </c>
       <c r="B72" t="s">
-        <v>65</v>
+        <v>403</v>
       </c>
       <c r="C72" t="s">
-        <v>61</v>
+        <v>218</v>
       </c>
       <c r="D72" t="s">
-        <v>77</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>222</v>
       </c>
       <c r="B73" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C73" t="s">
-        <v>61</v>
+        <v>218</v>
       </c>
       <c r="D73" t="s">
-        <v>77</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>306</v>
+        <v>222</v>
       </c>
       <c r="B74" t="s">
-        <v>86</v>
+        <v>221</v>
       </c>
       <c r="C74" t="s">
-        <v>302</v>
+        <v>218</v>
       </c>
       <c r="D74" t="s">
-        <v>305</v>
+        <v>217</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>354</v>
+        <v>253</v>
       </c>
       <c r="B75" t="s">
-        <v>355</v>
+        <v>220</v>
       </c>
       <c r="C75" t="s">
-        <v>349</v>
+        <v>218</v>
       </c>
       <c r="D75" t="s">
-        <v>352</v>
+        <v>216</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>354</v>
+        <v>253</v>
       </c>
       <c r="B76" t="s">
-        <v>356</v>
+        <v>219</v>
       </c>
       <c r="C76" t="s">
-        <v>349</v>
+        <v>218</v>
       </c>
       <c r="D76" t="s">
-        <v>352</v>
+        <v>215</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>354</v>
+        <v>74</v>
       </c>
       <c r="B77" t="s">
-        <v>357</v>
+        <v>65</v>
       </c>
       <c r="C77" t="s">
-        <v>349</v>
+        <v>61</v>
       </c>
       <c r="D77" t="s">
-        <v>353</v>
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>354</v>
+        <v>74</v>
       </c>
       <c r="B78" t="s">
-        <v>358</v>
+        <v>79</v>
       </c>
       <c r="C78" t="s">
-        <v>349</v>
+        <v>61</v>
       </c>
       <c r="D78" t="s">
-        <v>353</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>10</v>
+        <v>306</v>
       </c>
       <c r="B79" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C79" t="s">
-        <v>12</v>
+        <v>302</v>
       </c>
       <c r="D79" t="s">
-        <v>13</v>
+        <v>305</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>10</v>
+        <v>354</v>
       </c>
       <c r="B80" t="s">
-        <v>14</v>
+        <v>355</v>
       </c>
       <c r="C80" t="s">
-        <v>15</v>
+        <v>349</v>
       </c>
       <c r="D80" t="s">
-        <v>16</v>
+        <v>352</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>8</v>
+        <v>354</v>
       </c>
       <c r="B81" t="s">
-        <v>9</v>
+        <v>356</v>
       </c>
       <c r="C81" t="s">
-        <v>12</v>
+        <v>349</v>
       </c>
       <c r="D81" t="s">
-        <v>265</v>
+        <v>352</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>320</v>
+        <v>354</v>
       </c>
       <c r="B82" t="s">
-        <v>9</v>
+        <v>357</v>
       </c>
       <c r="C82" t="s">
-        <v>321</v>
+        <v>349</v>
       </c>
       <c r="D82" t="s">
-        <v>322</v>
+        <v>353</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>325</v>
+        <v>354</v>
       </c>
       <c r="B83" t="s">
-        <v>323</v>
+        <v>358</v>
       </c>
       <c r="C83" t="s">
-        <v>321</v>
+        <v>349</v>
       </c>
       <c r="D83" t="s">
-        <v>326</v>
+        <v>353</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>325</v>
+        <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>324</v>
+        <v>11</v>
       </c>
       <c r="C84" t="s">
-        <v>321</v>
+        <v>12</v>
       </c>
       <c r="D84" t="s">
-        <v>326</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>325</v>
+        <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>330</v>
+        <v>14</v>
       </c>
       <c r="C85" t="s">
-        <v>321</v>
+        <v>15</v>
       </c>
       <c r="D85" t="s">
-        <v>341</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>325</v>
+        <v>8</v>
       </c>
       <c r="B86" t="s">
-        <v>329</v>
+        <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>321</v>
+        <v>12</v>
       </c>
       <c r="D86" t="s">
-        <v>329</v>
+        <v>265</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B87" t="s">
-        <v>327</v>
+        <v>9</v>
       </c>
       <c r="C87" t="s">
         <v>321</v>
       </c>
       <c r="D87" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
+      <c r="A88" t="s">
         <v>325</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>404</v>
+      <c r="B88" t="s">
+        <v>323</v>
       </c>
       <c r="C88" t="s">
         <v>321</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>405</v>
+      <c r="D88" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>239</v>
+        <v>325</v>
       </c>
       <c r="B89" t="s">
-        <v>240</v>
+        <v>324</v>
       </c>
       <c r="C89" t="s">
-        <v>243</v>
+        <v>321</v>
       </c>
       <c r="D89" t="s">
-        <v>241</v>
+        <v>326</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>226</v>
+        <v>325</v>
       </c>
       <c r="B90" t="s">
-        <v>229</v>
+        <v>330</v>
       </c>
       <c r="C90" t="s">
-        <v>224</v>
+        <v>321</v>
       </c>
       <c r="D90" t="s">
-        <v>228</v>
+        <v>341</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>226</v>
+        <v>325</v>
       </c>
       <c r="B91" t="s">
-        <v>230</v>
+        <v>329</v>
       </c>
       <c r="C91" t="s">
-        <v>224</v>
+        <v>321</v>
       </c>
       <c r="D91" t="s">
-        <v>231</v>
+        <v>329</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>226</v>
+        <v>325</v>
       </c>
       <c r="B92" t="s">
-        <v>11</v>
+        <v>327</v>
       </c>
       <c r="C92" t="s">
-        <v>224</v>
+        <v>321</v>
       </c>
       <c r="D92" t="s">
-        <v>227</v>
+        <v>328</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>226</v>
-      </c>
-      <c r="B93" t="s">
-        <v>237</v>
+      <c r="A93" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>404</v>
       </c>
       <c r="C93" t="s">
-        <v>243</v>
-      </c>
-      <c r="D93" t="s">
-        <v>238</v>
+        <v>321</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="B94" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="C94" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="D94" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B95" t="s">
-        <v>9</v>
+        <v>229</v>
       </c>
       <c r="C95" t="s">
         <v>224</v>
       </c>
       <c r="D95" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>64</v>
+        <v>226</v>
       </c>
       <c r="B96" t="s">
-        <v>69</v>
+        <v>230</v>
       </c>
       <c r="C96" t="s">
-        <v>61</v>
+        <v>224</v>
       </c>
       <c r="D96" t="s">
-        <v>68</v>
+        <v>231</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>64</v>
+        <v>226</v>
       </c>
       <c r="B97" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="C97" t="s">
-        <v>61</v>
+        <v>224</v>
       </c>
       <c r="D97" t="s">
-        <v>95</v>
+        <v>227</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>24</v>
+        <v>226</v>
       </c>
       <c r="B98" t="s">
-        <v>286</v>
+        <v>237</v>
       </c>
       <c r="C98" t="s">
-        <v>299</v>
+        <v>243</v>
       </c>
       <c r="D98" t="s">
-        <v>287</v>
+        <v>238</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>24</v>
+        <v>226</v>
       </c>
       <c r="B99" t="s">
-        <v>288</v>
+        <v>235</v>
       </c>
       <c r="C99" t="s">
-        <v>300</v>
+        <v>224</v>
       </c>
       <c r="D99" t="s">
-        <v>289</v>
+        <v>236</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>24</v>
+        <v>223</v>
       </c>
       <c r="B100" t="s">
-        <v>290</v>
+        <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>300</v>
+        <v>224</v>
       </c>
       <c r="D100" t="s">
-        <v>291</v>
+        <v>225</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B101" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="C101" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D101" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B102" t="s">
-        <v>276</v>
+        <v>69</v>
       </c>
       <c r="C102" t="s">
-        <v>297</v>
+        <v>61</v>
       </c>
       <c r="D102" t="s">
-        <v>277</v>
+        <v>95</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3097,13 +3127,13 @@
         <v>24</v>
       </c>
       <c r="B103" t="s">
-        <v>29</v>
+        <v>286</v>
       </c>
       <c r="C103" t="s">
-        <v>255</v>
+        <v>299</v>
       </c>
       <c r="D103" t="s">
-        <v>28</v>
+        <v>287</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -3111,13 +3141,13 @@
         <v>24</v>
       </c>
       <c r="B104" t="s">
-        <v>25</v>
+        <v>288</v>
       </c>
       <c r="C104" t="s">
-        <v>268</v>
+        <v>300</v>
       </c>
       <c r="D104" t="s">
-        <v>26</v>
+        <v>289</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3125,13 +3155,13 @@
         <v>24</v>
       </c>
       <c r="B105" t="s">
-        <v>103</v>
+        <v>290</v>
       </c>
       <c r="C105" t="s">
-        <v>104</v>
+        <v>300</v>
       </c>
       <c r="D105" t="s">
-        <v>105</v>
+        <v>291</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -3139,13 +3169,13 @@
         <v>24</v>
       </c>
       <c r="B106" t="s">
-        <v>333</v>
+        <v>27</v>
       </c>
       <c r="C106" t="s">
-        <v>332</v>
+        <v>255</v>
       </c>
       <c r="D106" t="s">
-        <v>331</v>
+        <v>28</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -3153,13 +3183,13 @@
         <v>24</v>
       </c>
       <c r="B107" t="s">
-        <v>31</v>
+        <v>276</v>
       </c>
       <c r="C107" t="s">
-        <v>258</v>
+        <v>297</v>
       </c>
       <c r="D107" t="s">
-        <v>32</v>
+        <v>277</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -3167,13 +3197,13 @@
         <v>24</v>
       </c>
       <c r="B108" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C108" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D108" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3181,293 +3211,293 @@
         <v>24</v>
       </c>
       <c r="B109" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="C109" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="D109" t="s">
-        <v>160</v>
+        <v>26</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>86</v>
+      <c r="A110" t="s">
+        <v>24</v>
+      </c>
+      <c r="B110" t="s">
+        <v>103</v>
       </c>
       <c r="C110" t="s">
-        <v>297</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>402</v>
+        <v>104</v>
+      </c>
+      <c r="D110" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>108</v>
+        <v>24</v>
       </c>
       <c r="B111" t="s">
-        <v>113</v>
+        <v>333</v>
       </c>
       <c r="C111" t="s">
-        <v>114</v>
+        <v>332</v>
       </c>
       <c r="D111" t="s">
-        <v>115</v>
+        <v>331</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B112" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="C112" t="s">
-        <v>104</v>
+        <v>258</v>
       </c>
       <c r="D112" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B113" t="s">
-        <v>111</v>
+        <v>31</v>
       </c>
       <c r="C113" t="s">
-        <v>104</v>
+        <v>258</v>
       </c>
       <c r="D113" t="s">
-        <v>112</v>
+        <v>33</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B114" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="C114" t="s">
-        <v>104</v>
+        <v>256</v>
       </c>
       <c r="D114" t="s">
-        <v>105</v>
+        <v>160</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>100</v>
-      </c>
-      <c r="B115" t="s">
-        <v>109</v>
-      </c>
-      <c r="C115" t="s">
-        <v>104</v>
-      </c>
-      <c r="D115" t="s">
-        <v>105</v>
+      <c r="A115" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>342</v>
-      </c>
-      <c r="B116" t="s">
-        <v>334</v>
-      </c>
-      <c r="C116" t="s">
-        <v>332</v>
-      </c>
-      <c r="D116" t="s">
-        <v>331</v>
+      <c r="A116" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>249</v>
-      </c>
-      <c r="B117" t="s">
-        <v>250</v>
+      <c r="A117" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="C117" t="s">
-        <v>251</v>
-      </c>
-      <c r="D117" t="s">
-        <v>252</v>
+        <v>297</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="B118" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
       <c r="C118" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="D118" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="B119" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="C119" t="s">
-        <v>266</v>
+        <v>104</v>
       </c>
       <c r="D119" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="B120" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="C120" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="D120" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="B121" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="C121" t="s">
-        <v>266</v>
+        <v>104</v>
       </c>
       <c r="D121" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>278</v>
+        <v>100</v>
       </c>
       <c r="B122" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="C122" t="s">
-        <v>298</v>
+        <v>104</v>
       </c>
       <c r="D122" t="s">
-        <v>285</v>
+        <v>105</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>278</v>
+        <v>342</v>
       </c>
       <c r="B123" t="s">
-        <v>284</v>
+        <v>334</v>
       </c>
       <c r="C123" t="s">
-        <v>298</v>
+        <v>332</v>
       </c>
       <c r="D123" t="s">
-        <v>283</v>
+        <v>331</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
       <c r="B124" t="s">
-        <v>366</v>
+        <v>250</v>
       </c>
       <c r="C124" t="s">
-        <v>302</v>
+        <v>251</v>
       </c>
       <c r="D124" t="s">
-        <v>307</v>
+        <v>252</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>278</v>
-      </c>
-      <c r="B125" t="s">
-        <v>363</v>
-      </c>
-      <c r="C125" t="s">
-        <v>361</v>
-      </c>
-      <c r="D125" t="s">
-        <v>362</v>
+      <c r="A125" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>278</v>
+        <v>20</v>
       </c>
       <c r="B126" t="s">
-        <v>311</v>
+        <v>11</v>
       </c>
       <c r="C126" t="s">
-        <v>313</v>
+        <v>21</v>
       </c>
       <c r="D126" t="s">
-        <v>314</v>
+        <v>22</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="B127" t="s">
-        <v>304</v>
+        <v>9</v>
       </c>
       <c r="C127" t="s">
-        <v>302</v>
+        <v>266</v>
       </c>
       <c r="D127" t="s">
-        <v>303</v>
+        <v>19</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="B128" t="s">
-        <v>312</v>
+        <v>23</v>
       </c>
       <c r="C128" t="s">
-        <v>313</v>
+        <v>21</v>
       </c>
       <c r="D128" t="s">
-        <v>315</v>
+        <v>22</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="B129" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
       <c r="C129" t="s">
-        <v>349</v>
+        <v>266</v>
       </c>
       <c r="D129" t="s">
-        <v>351</v>
+        <v>19</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3475,13 +3505,13 @@
         <v>278</v>
       </c>
       <c r="B130" t="s">
-        <v>279</v>
+        <v>11</v>
       </c>
       <c r="C130" t="s">
         <v>298</v>
       </c>
       <c r="D130" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3489,13 +3519,13 @@
         <v>278</v>
       </c>
       <c r="B131" t="s">
-        <v>319</v>
+        <v>284</v>
       </c>
       <c r="C131" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="D131" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3503,13 +3533,13 @@
         <v>278</v>
       </c>
       <c r="B132" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="C132" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D132" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3517,556 +3547,556 @@
         <v>278</v>
       </c>
       <c r="B133" t="s">
-        <v>318</v>
+        <v>363</v>
       </c>
       <c r="C133" t="s">
-        <v>313</v>
+        <v>361</v>
       </c>
       <c r="D133" t="s">
-        <v>317</v>
+        <v>362</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B134" t="s">
-        <v>282</v>
+        <v>311</v>
       </c>
       <c r="C134" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="D134" t="s">
-        <v>340</v>
+        <v>314</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B135" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="C135" t="s">
-        <v>361</v>
+        <v>302</v>
       </c>
       <c r="D135" t="s">
-        <v>365</v>
+        <v>303</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B136" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="C136" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="D136" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B137" t="s">
-        <v>348</v>
+        <v>134</v>
       </c>
       <c r="C137" t="s">
         <v>349</v>
       </c>
       <c r="D137" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B138" t="s">
-        <v>343</v>
+        <v>279</v>
       </c>
       <c r="C138" t="s">
-        <v>344</v>
+        <v>298</v>
       </c>
       <c r="D138" t="s">
-        <v>345</v>
+        <v>280</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>359</v>
+        <v>278</v>
       </c>
       <c r="B139" t="s">
-        <v>360</v>
+        <v>319</v>
       </c>
       <c r="C139" t="s">
-        <v>361</v>
+        <v>313</v>
       </c>
       <c r="D139" t="s">
-        <v>362</v>
+        <v>316</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>246</v>
+        <v>278</v>
       </c>
       <c r="B140" t="s">
-        <v>247</v>
+        <v>380</v>
       </c>
       <c r="C140" t="s">
-        <v>244</v>
+        <v>313</v>
       </c>
       <c r="D140" t="s">
-        <v>248</v>
+        <v>316</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>394</v>
+      <c r="A141" t="s">
+        <v>278</v>
+      </c>
+      <c r="B141" t="s">
+        <v>318</v>
+      </c>
+      <c r="C141" t="s">
+        <v>313</v>
+      </c>
+      <c r="D141" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D142" s="2" t="s">
-        <v>396</v>
+      <c r="A142" t="s">
+        <v>281</v>
+      </c>
+      <c r="B142" t="s">
+        <v>282</v>
+      </c>
+      <c r="C142" t="s">
+        <v>298</v>
+      </c>
+      <c r="D142" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D143" s="2" t="s">
-        <v>399</v>
+      <c r="A143" t="s">
+        <v>281</v>
+      </c>
+      <c r="B143" t="s">
+        <v>364</v>
+      </c>
+      <c r="C143" t="s">
+        <v>361</v>
+      </c>
+      <c r="D143" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D144" s="2" t="s">
-        <v>400</v>
+      <c r="A144" t="s">
+        <v>281</v>
+      </c>
+      <c r="B144" t="s">
+        <v>294</v>
+      </c>
+      <c r="C144" t="s">
+        <v>302</v>
+      </c>
+      <c r="D144" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D145" s="2" t="s">
-        <v>390</v>
+      <c r="A145" t="s">
+        <v>281</v>
+      </c>
+      <c r="B145" t="s">
+        <v>348</v>
+      </c>
+      <c r="C145" t="s">
+        <v>349</v>
+      </c>
+      <c r="D145" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>393</v>
+      <c r="A146" t="s">
+        <v>281</v>
+      </c>
+      <c r="B146" t="s">
+        <v>343</v>
+      </c>
+      <c r="C146" t="s">
+        <v>344</v>
+      </c>
+      <c r="D146" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>152</v>
+        <v>359</v>
       </c>
       <c r="B147" t="s">
-        <v>11</v>
+        <v>360</v>
       </c>
       <c r="C147" t="s">
-        <v>256</v>
+        <v>361</v>
       </c>
       <c r="D147" t="s">
-        <v>163</v>
+        <v>362</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>152</v>
+        <v>246</v>
       </c>
       <c r="B148" t="s">
-        <v>149</v>
+        <v>247</v>
       </c>
       <c r="C148" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="D148" t="s">
-        <v>162</v>
+        <v>248</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>152</v>
-      </c>
-      <c r="B149" t="s">
-        <v>164</v>
-      </c>
-      <c r="C149" t="s">
-        <v>256</v>
-      </c>
-      <c r="D149" t="s">
-        <v>160</v>
+      <c r="A149" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>152</v>
-      </c>
-      <c r="B150" t="s">
-        <v>209</v>
-      </c>
-      <c r="C150" t="s">
-        <v>256</v>
-      </c>
-      <c r="D150" t="s">
-        <v>165</v>
+      <c r="A150" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>156</v>
-      </c>
-      <c r="B151" t="s">
+      <c r="A151" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C151" t="s">
-        <v>256</v>
-      </c>
-      <c r="D151" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>156</v>
-      </c>
-      <c r="B152" t="s">
+      <c r="C153" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B154" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C152" t="s">
-        <v>256</v>
-      </c>
-      <c r="D152" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>211</v>
-      </c>
-      <c r="B153" t="s">
-        <v>188</v>
-      </c>
-      <c r="C153" t="s">
-        <v>186</v>
-      </c>
-      <c r="D153" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>211</v>
-      </c>
-      <c r="B154" t="s">
-        <v>167</v>
-      </c>
-      <c r="C154" t="s">
-        <v>186</v>
-      </c>
-      <c r="D154" t="s">
-        <v>168</v>
+      <c r="C154" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="B155" t="s">
-        <v>184</v>
+        <v>11</v>
       </c>
       <c r="C155" t="s">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="D155" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="B156" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C156" t="s">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="D156" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="B157" t="s">
-        <v>383</v>
+        <v>164</v>
       </c>
       <c r="C157" t="s">
-        <v>382</v>
+        <v>256</v>
       </c>
       <c r="D157" t="s">
-        <v>381</v>
+        <v>160</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>213</v>
+        <v>152</v>
       </c>
       <c r="B158" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="C158" t="s">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="D158" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>210</v>
+        <v>156</v>
       </c>
       <c r="B159" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="C159" t="s">
-        <v>186</v>
+        <v>256</v>
       </c>
       <c r="D159" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="B160" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="C160" t="s">
-        <v>61</v>
+        <v>256</v>
       </c>
       <c r="D160" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>82</v>
+        <v>211</v>
       </c>
       <c r="B161" t="s">
-        <v>69</v>
+        <v>188</v>
       </c>
       <c r="C161" t="s">
-        <v>61</v>
+        <v>186</v>
       </c>
       <c r="D161" t="s">
-        <v>84</v>
+        <v>187</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>347</v>
+        <v>211</v>
       </c>
       <c r="B162" t="s">
-        <v>346</v>
+        <v>167</v>
       </c>
       <c r="C162" t="s">
-        <v>344</v>
+        <v>186</v>
       </c>
       <c r="D162" t="s">
-        <v>346</v>
+        <v>168</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="B163" t="s">
-        <v>338</v>
+        <v>184</v>
       </c>
       <c r="C163" t="s">
-        <v>336</v>
+        <v>183</v>
       </c>
       <c r="D163" t="s">
-        <v>339</v>
+        <v>189</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="B164" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="C164" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D164" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="B165" t="s">
-        <v>272</v>
+        <v>383</v>
       </c>
       <c r="C165" t="s">
-        <v>297</v>
+        <v>382</v>
       </c>
       <c r="D165" t="s">
-        <v>273</v>
+        <v>381</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="B166" t="s">
-        <v>157</v>
+        <v>188</v>
       </c>
       <c r="C166" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="D166" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B167" t="s">
-        <v>335</v>
+        <v>106</v>
       </c>
       <c r="C167" t="s">
-        <v>336</v>
+        <v>186</v>
       </c>
       <c r="D167" t="s">
-        <v>337</v>
+        <v>166</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>206</v>
+        <v>82</v>
       </c>
       <c r="B168" t="s">
-        <v>195</v>
+        <v>86</v>
       </c>
       <c r="C168" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D168" t="s">
-        <v>197</v>
+        <v>84</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>206</v>
+        <v>82</v>
       </c>
       <c r="B169" t="s">
-        <v>195</v>
+        <v>69</v>
       </c>
       <c r="C169" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="D169" t="s">
-        <v>204</v>
+        <v>84</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>206</v>
+        <v>347</v>
       </c>
       <c r="B170" t="s">
-        <v>199</v>
+        <v>346</v>
       </c>
       <c r="C170" t="s">
-        <v>254</v>
+        <v>344</v>
       </c>
       <c r="D170" t="s">
-        <v>201</v>
+        <v>346</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B171" t="s">
-        <v>199</v>
+        <v>338</v>
       </c>
       <c r="C171" t="s">
-        <v>254</v>
+        <v>336</v>
       </c>
       <c r="D171" t="s">
-        <v>205</v>
+        <v>339</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="B172" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C172" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D172" t="s">
         <v>198</v>
@@ -4074,351 +4104,463 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="B173" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="C173" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D173" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="B174" t="s">
-        <v>54</v>
+        <v>157</v>
       </c>
       <c r="C174" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="D174" t="s">
-        <v>55</v>
+        <v>159</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="B175" t="s">
-        <v>51</v>
+        <v>335</v>
       </c>
       <c r="C175" t="s">
-        <v>52</v>
+        <v>336</v>
       </c>
       <c r="D175" t="s">
-        <v>53</v>
+        <v>337</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B176" t="s">
-        <v>275</v>
+        <v>195</v>
       </c>
       <c r="C176" t="s">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="D176" t="s">
-        <v>274</v>
+        <v>197</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B177" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C177" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="D177" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B178" t="s">
-        <v>125</v>
+        <v>199</v>
       </c>
       <c r="C178" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D178" t="s">
-        <v>125</v>
+        <v>201</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
+        <v>206</v>
+      </c>
+      <c r="B179" t="s">
+        <v>199</v>
+      </c>
+      <c r="C179" t="s">
+        <v>254</v>
+      </c>
+      <c r="D179" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>47</v>
       </c>
-      <c r="B179" t="s">
-        <v>127</v>
-      </c>
-      <c r="C179" t="s">
-        <v>128</v>
-      </c>
-      <c r="D179" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="2" t="s">
+      <c r="B180" t="s">
+        <v>193</v>
+      </c>
+      <c r="C180" t="s">
+        <v>194</v>
+      </c>
+      <c r="D180" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>47</v>
       </c>
-      <c r="B180" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="C180" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="D180" s="2" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="C181" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D181" s="2" t="s">
-        <v>390</v>
+      <c r="B181" t="s">
+        <v>292</v>
+      </c>
+      <c r="C181" t="s">
+        <v>301</v>
+      </c>
+      <c r="D181" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>212</v>
+        <v>47</v>
       </c>
       <c r="B182" t="s">
-        <v>171</v>
+        <v>54</v>
       </c>
       <c r="C182" t="s">
-        <v>266</v>
+        <v>52</v>
       </c>
       <c r="D182" t="s">
-        <v>172</v>
+        <v>55</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B183" t="s">
-        <v>309</v>
+        <v>51</v>
       </c>
       <c r="C183" t="s">
-        <v>310</v>
+        <v>52</v>
       </c>
       <c r="D183" t="s">
-        <v>308</v>
+        <v>53</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B184" t="s">
-        <v>57</v>
+        <v>275</v>
       </c>
       <c r="C184" t="s">
-        <v>52</v>
+        <v>297</v>
       </c>
       <c r="D184" t="s">
-        <v>55</v>
+        <v>274</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B185" t="s">
-        <v>59</v>
+        <v>188</v>
       </c>
       <c r="C185" t="s">
-        <v>52</v>
+        <v>267</v>
       </c>
       <c r="D185" t="s">
-        <v>55</v>
+        <v>187</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B186" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="C186" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="D186" t="s">
-        <v>176</v>
+        <v>125</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B187" t="s">
-        <v>169</v>
+        <v>127</v>
       </c>
       <c r="C187" t="s">
-        <v>266</v>
+        <v>128</v>
       </c>
       <c r="D187" t="s">
-        <v>170</v>
+        <v>129</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>50</v>
-      </c>
-      <c r="B188" t="s">
-        <v>173</v>
-      </c>
-      <c r="C188" t="s">
-        <v>266</v>
-      </c>
-      <c r="D188" t="s">
-        <v>174</v>
+      <c r="A188" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>110</v>
-      </c>
-      <c r="B189" t="s">
-        <v>116</v>
-      </c>
-      <c r="C189" t="s">
-        <v>117</v>
-      </c>
-      <c r="D189" t="s">
-        <v>116</v>
+      <c r="A189" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>110</v>
+        <v>212</v>
       </c>
       <c r="B190" t="s">
-        <v>118</v>
+        <v>171</v>
       </c>
       <c r="C190" t="s">
-        <v>117</v>
+        <v>266</v>
       </c>
       <c r="D190" t="s">
-        <v>118</v>
+        <v>172</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B191" t="s">
-        <v>119</v>
+        <v>309</v>
       </c>
       <c r="C191" t="s">
-        <v>117</v>
+        <v>310</v>
       </c>
       <c r="D191" t="s">
-        <v>119</v>
+        <v>308</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B192" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="C192" t="s">
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="D192" t="s">
-        <v>121</v>
+        <v>55</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B193" t="s">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="C193" t="s">
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="D193" t="s">
-        <v>123</v>
+        <v>55</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>207</v>
+        <v>50</v>
       </c>
       <c r="B194" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="C194" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="D194" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>207</v>
+        <v>50</v>
       </c>
       <c r="B195" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="C195" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="D195" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>207</v>
+        <v>50</v>
       </c>
       <c r="B196" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="C196" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="D196" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
+        <v>110</v>
+      </c>
+      <c r="B197" t="s">
+        <v>116</v>
+      </c>
+      <c r="C197" t="s">
+        <v>117</v>
+      </c>
+      <c r="D197" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>110</v>
+      </c>
+      <c r="B198" t="s">
+        <v>118</v>
+      </c>
+      <c r="C198" t="s">
+        <v>117</v>
+      </c>
+      <c r="D198" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>110</v>
+      </c>
+      <c r="B199" t="s">
+        <v>119</v>
+      </c>
+      <c r="C199" t="s">
+        <v>117</v>
+      </c>
+      <c r="D199" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>110</v>
+      </c>
+      <c r="B200" t="s">
+        <v>120</v>
+      </c>
+      <c r="C200" t="s">
+        <v>117</v>
+      </c>
+      <c r="D200" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>110</v>
+      </c>
+      <c r="B201" t="s">
+        <v>122</v>
+      </c>
+      <c r="C201" t="s">
+        <v>117</v>
+      </c>
+      <c r="D201" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>207</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B202" t="s">
+        <v>195</v>
+      </c>
+      <c r="C202" t="s">
+        <v>254</v>
+      </c>
+      <c r="D202" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>207</v>
+      </c>
+      <c r="B203" t="s">
+        <v>195</v>
+      </c>
+      <c r="C203" t="s">
+        <v>254</v>
+      </c>
+      <c r="D203" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>207</v>
+      </c>
+      <c r="B204" t="s">
         <v>199</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C204" t="s">
         <v>254</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D204" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>207</v>
+      </c>
+      <c r="B205" t="s">
+        <v>199</v>
+      </c>
+      <c r="C205" t="s">
+        <v>254</v>
+      </c>
+      <c r="D205" t="s">
         <v>203</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove spaces from mapping file
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0A8BB1-C249-4398-B565-E104C8E1E110}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5647262E-8AEC-4E66-8191-17A9E4427C2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -1240,9 +1240,6 @@
     <t>setZoom</t>
   </si>
   <si>
-    <t xml:space="preserve">CellPropertiesFill </t>
-  </si>
-  <si>
     <t>color</t>
   </si>
   <si>
@@ -1252,22 +1249,25 @@
     <t>setCellProperties</t>
   </si>
   <si>
-    <t xml:space="preserve">CellPropertiesFillLoadOptions </t>
-  </si>
-  <si>
     <t>getCellProperties</t>
   </si>
   <si>
     <t>CellPropertiesFont</t>
   </si>
   <si>
-    <t xml:space="preserve">CellPropertiesFontLoadOptions </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CellPropertiesLoadOptions </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SettableCellProperties </t>
+    <t>CellPropertiesFill</t>
+  </si>
+  <si>
+    <t>CellPropertiesFillLoadOptions</t>
+  </si>
+  <si>
+    <t>CellPropertiesFontLoadOptions</t>
+  </si>
+  <si>
+    <t>CellPropertiesLoadOptions</t>
+  </si>
+  <si>
+    <t>SettableCellProperties</t>
   </si>
 </sst>
 </file>
@@ -1682,19 +1682,19 @@
   <dimension ref="A1:D205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B208" sqref="B208"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>269</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>386</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1750,63 +1750,63 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>413</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>408</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>414</v>
       </c>
@@ -1814,13 +1814,13 @@
         <v>106</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>146</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>208</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>136</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>136</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>136</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>136</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>136</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>136</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>259</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>259</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>126</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>124</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>373</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>373</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>373</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>368</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>377</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>377</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>370</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>91</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>96</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>78</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>78</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>78</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>85</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>93</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>34</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>30</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>30</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>30</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>43</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>234</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>234</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>222</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>222</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>222</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>253</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>253</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>306</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>354</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>354</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>354</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>354</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>320</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>325</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>325</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>325</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>325</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>325</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93" s="2" t="s">
         <v>325</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>239</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>226</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>226</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>226</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>226</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>226</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>223</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>64</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>64</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>24</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>24</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>24</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>24</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>24</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>24</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>24</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>24</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>24</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>24</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>24</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>24</v>
       </c>
@@ -3290,35 +3290,35 @@
         <v>160</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A115" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C115" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D115" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D115" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A116" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A117" s="2" t="s">
         <v>401</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>108</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>100</v>
       </c>
@@ -3360,7 +3360,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>100</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>100</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>100</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>342</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>249</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A125" s="2" t="s">
         <v>415</v>
       </c>
@@ -3438,13 +3438,13 @@
         <v>79</v>
       </c>
       <c r="C125" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D125" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D125" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>20</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>17</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>17</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>17</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>278</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>278</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>278</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>278</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>278</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>278</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>278</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>278</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>278</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>278</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>278</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>278</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>281</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>281</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>281</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>281</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>281</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>359</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>246</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A149" s="2" t="s">
         <v>395</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A150" s="2" t="s">
         <v>395</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A151" s="2" t="s">
         <v>395</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A152" s="2" t="s">
         <v>395</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A153" s="2" t="s">
         <v>389</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A154" s="2" t="s">
         <v>389</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>152</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>152</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>152</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>152</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>156</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>156</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>211</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>211</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>214</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>214</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>214</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>213</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>210</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>82</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>82</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>347</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>190</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>190</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>190</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>190</v>
       </c>
@@ -4130,7 +4130,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>190</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>206</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>206</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
         <v>206</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
         <v>206</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
         <v>47</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
         <v>47</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
         <v>47</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
         <v>47</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
         <v>47</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
         <v>47</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
         <v>47</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
         <v>47</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A188" s="2" t="s">
         <v>47</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A189" s="2" t="s">
         <v>47</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
         <v>212</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
         <v>50</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
         <v>50</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>50</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>50</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>50</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>50</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>110</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>110</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>110</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>110</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>110</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>207</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>207</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>207</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>207</v>
       </c>

</xml_diff>

<commit_message>
Remove spaces from mapping file (#321)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0A8BB1-C249-4398-B565-E104C8E1E110}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5647262E-8AEC-4E66-8191-17A9E4427C2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -1240,9 +1240,6 @@
     <t>setZoom</t>
   </si>
   <si>
-    <t xml:space="preserve">CellPropertiesFill </t>
-  </si>
-  <si>
     <t>color</t>
   </si>
   <si>
@@ -1252,22 +1249,25 @@
     <t>setCellProperties</t>
   </si>
   <si>
-    <t xml:space="preserve">CellPropertiesFillLoadOptions </t>
-  </si>
-  <si>
     <t>getCellProperties</t>
   </si>
   <si>
     <t>CellPropertiesFont</t>
   </si>
   <si>
-    <t xml:space="preserve">CellPropertiesFontLoadOptions </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CellPropertiesLoadOptions </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SettableCellProperties </t>
+    <t>CellPropertiesFill</t>
+  </si>
+  <si>
+    <t>CellPropertiesFillLoadOptions</t>
+  </si>
+  <si>
+    <t>CellPropertiesFontLoadOptions</t>
+  </si>
+  <si>
+    <t>CellPropertiesLoadOptions</t>
+  </si>
+  <si>
+    <t>SettableCellProperties</t>
   </si>
 </sst>
 </file>
@@ -1682,19 +1682,19 @@
   <dimension ref="A1:D205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B208" sqref="B208"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>269</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>386</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1750,63 +1750,63 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>413</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>408</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>414</v>
       </c>
@@ -1814,13 +1814,13 @@
         <v>106</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>146</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>208</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>136</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>136</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>136</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>136</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>136</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>136</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>259</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>259</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>126</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>124</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>373</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>373</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>373</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>368</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>377</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>377</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>370</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>91</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>96</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>78</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>78</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>78</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>85</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>93</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>34</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>30</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>30</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>30</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>43</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>234</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>234</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>222</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>222</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>222</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>253</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>253</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>306</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>354</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>354</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>354</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>354</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>320</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>325</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>325</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>325</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>325</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>325</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93" s="2" t="s">
         <v>325</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>239</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>226</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>226</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>226</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>226</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>226</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>223</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>64</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>64</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>24</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>24</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>24</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>24</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>24</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>24</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>24</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>24</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>24</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>24</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>24</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>24</v>
       </c>
@@ -3290,35 +3290,35 @@
         <v>160</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A115" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C115" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D115" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D115" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A116" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A117" s="2" t="s">
         <v>401</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>108</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>100</v>
       </c>
@@ -3360,7 +3360,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>100</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>100</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>100</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>342</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>249</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A125" s="2" t="s">
         <v>415</v>
       </c>
@@ -3438,13 +3438,13 @@
         <v>79</v>
       </c>
       <c r="C125" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D125" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D125" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>20</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>17</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>17</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>17</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>278</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>278</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>278</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>278</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>278</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>278</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>278</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>278</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>278</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>278</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>278</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>278</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>281</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>281</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>281</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>281</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>281</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>359</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>246</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A149" s="2" t="s">
         <v>395</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A150" s="2" t="s">
         <v>395</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A151" s="2" t="s">
         <v>395</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A152" s="2" t="s">
         <v>395</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A153" s="2" t="s">
         <v>389</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A154" s="2" t="s">
         <v>389</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>152</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>152</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>152</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>152</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>156</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>156</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>211</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>211</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>214</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>214</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>214</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>213</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>210</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>82</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>82</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>347</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>190</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>190</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>190</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>190</v>
       </c>
@@ -4130,7 +4130,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>190</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>206</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>206</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
         <v>206</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
         <v>206</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
         <v>47</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
         <v>47</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
         <v>47</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
         <v>47</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
         <v>47</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
         <v>47</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
         <v>47</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
         <v>47</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A188" s="2" t="s">
         <v>47</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A189" s="2" t="s">
         <v>47</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
         <v>212</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
         <v>50</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
         <v>50</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>50</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>50</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>50</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>50</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>110</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>110</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>110</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>110</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>110</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>207</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>207</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>207</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>207</v>
       </c>

</xml_diff>

<commit_message>
Adding single click event sample
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21814"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5647262E-8AEC-4E66-8191-17A9E4427C2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69351F3B-09BC-4515-B316-6D10752E825E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="421">
   <si>
     <t>Class</t>
   </si>
@@ -1268,6 +1268,21 @@
   </si>
   <si>
     <t>SettableCellProperties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WorksheetSingleClickedEventArgs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">address </t>
+  </si>
+  <si>
+    <t>excel-event-worksheet-single-click</t>
+  </si>
+  <si>
+    <t>registerClickHandler</t>
+  </si>
+  <si>
+    <t>onSingleClicked</t>
   </si>
 </sst>
 </file>
@@ -1347,8 +1362,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D205" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D205" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D207" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D207" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D205">
     <sortCondition ref="A1:A205"/>
   </sortState>
@@ -1679,22 +1694,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D205"/>
+  <dimension ref="A1:D207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A125" sqref="A125"/>
+      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D207" sqref="D207"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1708,7 +1723,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>269</v>
       </c>
@@ -1722,7 +1737,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>386</v>
       </c>
@@ -1736,7 +1751,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1750,7 +1765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>411</v>
       </c>
@@ -1764,7 +1779,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>412</v>
       </c>
@@ -1778,7 +1793,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>410</v>
       </c>
@@ -1792,7 +1807,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>413</v>
       </c>
@@ -1806,7 +1821,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>414</v>
       </c>
@@ -1820,7 +1835,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -1834,7 +1849,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -1848,7 +1863,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -1862,7 +1877,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -1876,7 +1891,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>146</v>
       </c>
@@ -1890,7 +1905,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>208</v>
       </c>
@@ -1904,7 +1919,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>136</v>
       </c>
@@ -1918,7 +1933,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -1932,7 +1947,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>136</v>
       </c>
@@ -1946,7 +1961,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>136</v>
       </c>
@@ -1960,7 +1975,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>136</v>
       </c>
@@ -1974,7 +1989,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>136</v>
       </c>
@@ -1988,7 +2003,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>136</v>
       </c>
@@ -2002,7 +2017,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>259</v>
       </c>
@@ -2016,7 +2031,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>259</v>
       </c>
@@ -2030,7 +2045,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>126</v>
       </c>
@@ -2044,7 +2059,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>124</v>
       </c>
@@ -2058,7 +2073,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -2072,7 +2087,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -2086,7 +2101,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -2100,7 +2115,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>373</v>
       </c>
@@ -2114,7 +2129,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>373</v>
       </c>
@@ -2128,7 +2143,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>373</v>
       </c>
@@ -2142,7 +2157,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>368</v>
       </c>
@@ -2156,7 +2171,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>377</v>
       </c>
@@ -2170,7 +2185,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>377</v>
       </c>
@@ -2184,7 +2199,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>370</v>
       </c>
@@ -2198,7 +2213,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>91</v>
       </c>
@@ -2212,7 +2227,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -2226,7 +2241,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -2240,7 +2255,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -2254,7 +2269,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -2268,7 +2283,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2282,7 +2297,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -2296,7 +2311,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2310,7 +2325,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -2324,7 +2339,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -2338,7 +2353,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -2352,7 +2367,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -2366,7 +2381,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -2380,7 +2395,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2394,7 +2409,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>96</v>
       </c>
@@ -2408,7 +2423,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>78</v>
       </c>
@@ -2422,7 +2437,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -2436,7 +2451,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>78</v>
       </c>
@@ -2450,7 +2465,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>78</v>
       </c>
@@ -2464,7 +2479,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -2478,7 +2493,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>85</v>
       </c>
@@ -2492,7 +2507,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>93</v>
       </c>
@@ -2506,7 +2521,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -2520,7 +2535,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -2534,7 +2549,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>34</v>
       </c>
@@ -2548,7 +2563,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -2562,7 +2577,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>30</v>
       </c>
@@ -2576,7 +2591,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>30</v>
       </c>
@@ -2590,7 +2605,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>30</v>
       </c>
@@ -2604,7 +2619,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -2618,7 +2633,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -2632,7 +2647,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>43</v>
       </c>
@@ -2646,7 +2661,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -2660,7 +2675,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>234</v>
       </c>
@@ -2674,7 +2689,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>234</v>
       </c>
@@ -2688,7 +2703,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>222</v>
       </c>
@@ -2702,7 +2717,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>222</v>
       </c>
@@ -2716,7 +2731,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>222</v>
       </c>
@@ -2730,7 +2745,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>253</v>
       </c>
@@ -2744,7 +2759,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>253</v>
       </c>
@@ -2758,7 +2773,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -2772,7 +2787,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -2786,7 +2801,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>306</v>
       </c>
@@ -2800,7 +2815,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>354</v>
       </c>
@@ -2814,7 +2829,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>354</v>
       </c>
@@ -2828,7 +2843,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>354</v>
       </c>
@@ -2842,7 +2857,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>354</v>
       </c>
@@ -2856,7 +2871,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -2870,7 +2885,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -2884,7 +2899,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -2898,7 +2913,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>320</v>
       </c>
@@ -2912,7 +2927,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>325</v>
       </c>
@@ -2926,7 +2941,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>325</v>
       </c>
@@ -2940,7 +2955,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>325</v>
       </c>
@@ -2954,7 +2969,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>325</v>
       </c>
@@ -2968,7 +2983,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>325</v>
       </c>
@@ -2982,7 +2997,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>325</v>
       </c>
@@ -2996,7 +3011,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>239</v>
       </c>
@@ -3010,7 +3025,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>226</v>
       </c>
@@ -3024,7 +3039,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>226</v>
       </c>
@@ -3038,7 +3053,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>226</v>
       </c>
@@ -3052,7 +3067,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>226</v>
       </c>
@@ -3066,7 +3081,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>226</v>
       </c>
@@ -3080,7 +3095,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>223</v>
       </c>
@@ -3094,7 +3109,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>64</v>
       </c>
@@ -3108,7 +3123,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>64</v>
       </c>
@@ -3122,7 +3137,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>24</v>
       </c>
@@ -3136,7 +3151,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>24</v>
       </c>
@@ -3150,7 +3165,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>24</v>
       </c>
@@ -3164,7 +3179,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>24</v>
       </c>
@@ -3178,7 +3193,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>24</v>
       </c>
@@ -3192,7 +3207,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>24</v>
       </c>
@@ -3206,7 +3221,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>24</v>
       </c>
@@ -3220,7 +3235,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>24</v>
       </c>
@@ -3234,7 +3249,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>24</v>
       </c>
@@ -3248,7 +3263,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>24</v>
       </c>
@@ -3262,7 +3277,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>24</v>
       </c>
@@ -3276,7 +3291,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>24</v>
       </c>
@@ -3290,7 +3305,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>24</v>
       </c>
@@ -3304,7 +3319,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>24</v>
       </c>
@@ -3318,7 +3333,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>401</v>
       </c>
@@ -3332,7 +3347,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>108</v>
       </c>
@@ -3346,7 +3361,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>100</v>
       </c>
@@ -3360,7 +3375,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>100</v>
       </c>
@@ -3374,7 +3389,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>100</v>
       </c>
@@ -3388,7 +3403,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>100</v>
       </c>
@@ -3402,7 +3417,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>342</v>
       </c>
@@ -3416,7 +3431,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>249</v>
       </c>
@@ -3430,7 +3445,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>415</v>
       </c>
@@ -3444,7 +3459,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>20</v>
       </c>
@@ -3458,7 +3473,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>17</v>
       </c>
@@ -3472,7 +3487,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>17</v>
       </c>
@@ -3486,7 +3501,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>17</v>
       </c>
@@ -3500,7 +3515,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>278</v>
       </c>
@@ -3514,7 +3529,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>278</v>
       </c>
@@ -3528,7 +3543,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>278</v>
       </c>
@@ -3542,7 +3557,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>278</v>
       </c>
@@ -3556,7 +3571,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>278</v>
       </c>
@@ -3570,7 +3585,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>278</v>
       </c>
@@ -3584,7 +3599,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>278</v>
       </c>
@@ -3598,7 +3613,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>278</v>
       </c>
@@ -3612,7 +3627,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>278</v>
       </c>
@@ -3626,7 +3641,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>278</v>
       </c>
@@ -3640,7 +3655,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>278</v>
       </c>
@@ -3654,7 +3669,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>278</v>
       </c>
@@ -3668,7 +3683,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>281</v>
       </c>
@@ -3682,7 +3697,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>281</v>
       </c>
@@ -3696,7 +3711,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>281</v>
       </c>
@@ -3710,7 +3725,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>281</v>
       </c>
@@ -3724,7 +3739,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>281</v>
       </c>
@@ -3738,7 +3753,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>359</v>
       </c>
@@ -3752,7 +3767,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>246</v>
       </c>
@@ -3766,7 +3781,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>395</v>
       </c>
@@ -3780,7 +3795,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>395</v>
       </c>
@@ -3794,7 +3809,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>395</v>
       </c>
@@ -3808,7 +3823,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>395</v>
       </c>
@@ -3822,7 +3837,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>389</v>
       </c>
@@ -3836,7 +3851,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>389</v>
       </c>
@@ -3850,7 +3865,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>152</v>
       </c>
@@ -3864,7 +3879,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>152</v>
       </c>
@@ -3878,7 +3893,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>152</v>
       </c>
@@ -3892,7 +3907,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>152</v>
       </c>
@@ -3906,7 +3921,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>156</v>
       </c>
@@ -3920,7 +3935,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>156</v>
       </c>
@@ -3934,7 +3949,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>211</v>
       </c>
@@ -3948,7 +3963,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>211</v>
       </c>
@@ -3962,7 +3977,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>214</v>
       </c>
@@ -3976,7 +3991,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>214</v>
       </c>
@@ -3990,7 +4005,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>214</v>
       </c>
@@ -4004,7 +4019,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>213</v>
       </c>
@@ -4018,7 +4033,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>210</v>
       </c>
@@ -4032,7 +4047,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>82</v>
       </c>
@@ -4046,7 +4061,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>82</v>
       </c>
@@ -4060,7 +4075,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>347</v>
       </c>
@@ -4074,7 +4089,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>190</v>
       </c>
@@ -4088,7 +4103,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>190</v>
       </c>
@@ -4102,7 +4117,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>190</v>
       </c>
@@ -4116,7 +4131,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>190</v>
       </c>
@@ -4130,7 +4145,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>190</v>
       </c>
@@ -4144,7 +4159,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>206</v>
       </c>
@@ -4158,7 +4173,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>206</v>
       </c>
@@ -4172,7 +4187,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>206</v>
       </c>
@@ -4186,7 +4201,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>206</v>
       </c>
@@ -4200,7 +4215,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>47</v>
       </c>
@@ -4214,7 +4229,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>47</v>
       </c>
@@ -4228,7 +4243,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>47</v>
       </c>
@@ -4242,7 +4257,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>47</v>
       </c>
@@ -4256,7 +4271,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>47</v>
       </c>
@@ -4270,7 +4285,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>47</v>
       </c>
@@ -4284,7 +4299,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>47</v>
       </c>
@@ -4298,7 +4313,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>47</v>
       </c>
@@ -4312,7 +4327,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>47</v>
       </c>
@@ -4326,7 +4341,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>47</v>
       </c>
@@ -4340,7 +4355,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>212</v>
       </c>
@@ -4354,7 +4369,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>50</v>
       </c>
@@ -4368,7 +4383,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>50</v>
       </c>
@@ -4382,7 +4397,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>50</v>
       </c>
@@ -4396,7 +4411,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>50</v>
       </c>
@@ -4410,7 +4425,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>50</v>
       </c>
@@ -4424,7 +4439,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>50</v>
       </c>
@@ -4438,7 +4453,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>110</v>
       </c>
@@ -4452,7 +4467,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>110</v>
       </c>
@@ -4466,7 +4481,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>110</v>
       </c>
@@ -4480,7 +4495,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>110</v>
       </c>
@@ -4494,7 +4509,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>110</v>
       </c>
@@ -4508,7 +4523,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>207</v>
       </c>
@@ -4522,7 +4537,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>207</v>
       </c>
@@ -4536,7 +4551,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>207</v>
       </c>
@@ -4550,7 +4565,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>207</v>
       </c>
@@ -4562,6 +4577,34 @@
       </c>
       <c r="D205" t="s">
         <v>203</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding single click event sample (#327)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21814"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5647262E-8AEC-4E66-8191-17A9E4427C2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69351F3B-09BC-4515-B316-6D10752E825E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="421">
   <si>
     <t>Class</t>
   </si>
@@ -1268,6 +1268,21 @@
   </si>
   <si>
     <t>SettableCellProperties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WorksheetSingleClickedEventArgs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">address </t>
+  </si>
+  <si>
+    <t>excel-event-worksheet-single-click</t>
+  </si>
+  <si>
+    <t>registerClickHandler</t>
+  </si>
+  <si>
+    <t>onSingleClicked</t>
   </si>
 </sst>
 </file>
@@ -1347,8 +1362,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D205" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D205" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D207" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D207" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D205">
     <sortCondition ref="A1:A205"/>
   </sortState>
@@ -1679,22 +1694,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D205"/>
+  <dimension ref="A1:D207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A125" sqref="A125"/>
+      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D207" sqref="D207"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1708,7 +1723,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>269</v>
       </c>
@@ -1722,7 +1737,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>386</v>
       </c>
@@ -1736,7 +1751,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1750,7 +1765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>411</v>
       </c>
@@ -1764,7 +1779,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>412</v>
       </c>
@@ -1778,7 +1793,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>410</v>
       </c>
@@ -1792,7 +1807,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>413</v>
       </c>
@@ -1806,7 +1821,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>414</v>
       </c>
@@ -1820,7 +1835,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -1834,7 +1849,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -1848,7 +1863,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -1862,7 +1877,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -1876,7 +1891,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>146</v>
       </c>
@@ -1890,7 +1905,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>208</v>
       </c>
@@ -1904,7 +1919,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>136</v>
       </c>
@@ -1918,7 +1933,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -1932,7 +1947,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>136</v>
       </c>
@@ -1946,7 +1961,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>136</v>
       </c>
@@ -1960,7 +1975,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>136</v>
       </c>
@@ -1974,7 +1989,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>136</v>
       </c>
@@ -1988,7 +2003,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>136</v>
       </c>
@@ -2002,7 +2017,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>259</v>
       </c>
@@ -2016,7 +2031,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>259</v>
       </c>
@@ -2030,7 +2045,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>126</v>
       </c>
@@ -2044,7 +2059,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>124</v>
       </c>
@@ -2058,7 +2073,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -2072,7 +2087,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -2086,7 +2101,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -2100,7 +2115,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>373</v>
       </c>
@@ -2114,7 +2129,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>373</v>
       </c>
@@ -2128,7 +2143,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>373</v>
       </c>
@@ -2142,7 +2157,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>368</v>
       </c>
@@ -2156,7 +2171,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>377</v>
       </c>
@@ -2170,7 +2185,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>377</v>
       </c>
@@ -2184,7 +2199,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>370</v>
       </c>
@@ -2198,7 +2213,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>91</v>
       </c>
@@ -2212,7 +2227,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -2226,7 +2241,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -2240,7 +2255,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -2254,7 +2269,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -2268,7 +2283,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2282,7 +2297,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -2296,7 +2311,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2310,7 +2325,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -2324,7 +2339,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -2338,7 +2353,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -2352,7 +2367,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -2366,7 +2381,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -2380,7 +2395,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2394,7 +2409,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>96</v>
       </c>
@@ -2408,7 +2423,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>78</v>
       </c>
@@ -2422,7 +2437,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -2436,7 +2451,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>78</v>
       </c>
@@ -2450,7 +2465,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>78</v>
       </c>
@@ -2464,7 +2479,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -2478,7 +2493,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>85</v>
       </c>
@@ -2492,7 +2507,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>93</v>
       </c>
@@ -2506,7 +2521,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -2520,7 +2535,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -2534,7 +2549,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>34</v>
       </c>
@@ -2548,7 +2563,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -2562,7 +2577,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>30</v>
       </c>
@@ -2576,7 +2591,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>30</v>
       </c>
@@ -2590,7 +2605,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>30</v>
       </c>
@@ -2604,7 +2619,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -2618,7 +2633,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -2632,7 +2647,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>43</v>
       </c>
@@ -2646,7 +2661,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -2660,7 +2675,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>234</v>
       </c>
@@ -2674,7 +2689,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>234</v>
       </c>
@@ -2688,7 +2703,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>222</v>
       </c>
@@ -2702,7 +2717,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>222</v>
       </c>
@@ -2716,7 +2731,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>222</v>
       </c>
@@ -2730,7 +2745,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>253</v>
       </c>
@@ -2744,7 +2759,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>253</v>
       </c>
@@ -2758,7 +2773,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -2772,7 +2787,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -2786,7 +2801,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>306</v>
       </c>
@@ -2800,7 +2815,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>354</v>
       </c>
@@ -2814,7 +2829,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>354</v>
       </c>
@@ -2828,7 +2843,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>354</v>
       </c>
@@ -2842,7 +2857,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>354</v>
       </c>
@@ -2856,7 +2871,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -2870,7 +2885,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -2884,7 +2899,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -2898,7 +2913,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>320</v>
       </c>
@@ -2912,7 +2927,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>325</v>
       </c>
@@ -2926,7 +2941,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>325</v>
       </c>
@@ -2940,7 +2955,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>325</v>
       </c>
@@ -2954,7 +2969,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>325</v>
       </c>
@@ -2968,7 +2983,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>325</v>
       </c>
@@ -2982,7 +2997,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>325</v>
       </c>
@@ -2996,7 +3011,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>239</v>
       </c>
@@ -3010,7 +3025,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>226</v>
       </c>
@@ -3024,7 +3039,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>226</v>
       </c>
@@ -3038,7 +3053,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>226</v>
       </c>
@@ -3052,7 +3067,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>226</v>
       </c>
@@ -3066,7 +3081,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>226</v>
       </c>
@@ -3080,7 +3095,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>223</v>
       </c>
@@ -3094,7 +3109,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>64</v>
       </c>
@@ -3108,7 +3123,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>64</v>
       </c>
@@ -3122,7 +3137,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>24</v>
       </c>
@@ -3136,7 +3151,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>24</v>
       </c>
@@ -3150,7 +3165,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>24</v>
       </c>
@@ -3164,7 +3179,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>24</v>
       </c>
@@ -3178,7 +3193,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>24</v>
       </c>
@@ -3192,7 +3207,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>24</v>
       </c>
@@ -3206,7 +3221,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>24</v>
       </c>
@@ -3220,7 +3235,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>24</v>
       </c>
@@ -3234,7 +3249,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>24</v>
       </c>
@@ -3248,7 +3263,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>24</v>
       </c>
@@ -3262,7 +3277,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>24</v>
       </c>
@@ -3276,7 +3291,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>24</v>
       </c>
@@ -3290,7 +3305,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>24</v>
       </c>
@@ -3304,7 +3319,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>24</v>
       </c>
@@ -3318,7 +3333,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>401</v>
       </c>
@@ -3332,7 +3347,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>108</v>
       </c>
@@ -3346,7 +3361,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>100</v>
       </c>
@@ -3360,7 +3375,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>100</v>
       </c>
@@ -3374,7 +3389,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>100</v>
       </c>
@@ -3388,7 +3403,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>100</v>
       </c>
@@ -3402,7 +3417,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>342</v>
       </c>
@@ -3416,7 +3431,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>249</v>
       </c>
@@ -3430,7 +3445,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>415</v>
       </c>
@@ -3444,7 +3459,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>20</v>
       </c>
@@ -3458,7 +3473,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>17</v>
       </c>
@@ -3472,7 +3487,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>17</v>
       </c>
@@ -3486,7 +3501,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>17</v>
       </c>
@@ -3500,7 +3515,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>278</v>
       </c>
@@ -3514,7 +3529,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>278</v>
       </c>
@@ -3528,7 +3543,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>278</v>
       </c>
@@ -3542,7 +3557,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>278</v>
       </c>
@@ -3556,7 +3571,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>278</v>
       </c>
@@ -3570,7 +3585,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>278</v>
       </c>
@@ -3584,7 +3599,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>278</v>
       </c>
@@ -3598,7 +3613,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>278</v>
       </c>
@@ -3612,7 +3627,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>278</v>
       </c>
@@ -3626,7 +3641,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>278</v>
       </c>
@@ -3640,7 +3655,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>278</v>
       </c>
@@ -3654,7 +3669,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>278</v>
       </c>
@@ -3668,7 +3683,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>281</v>
       </c>
@@ -3682,7 +3697,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>281</v>
       </c>
@@ -3696,7 +3711,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>281</v>
       </c>
@@ -3710,7 +3725,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>281</v>
       </c>
@@ -3724,7 +3739,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>281</v>
       </c>
@@ -3738,7 +3753,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>359</v>
       </c>
@@ -3752,7 +3767,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>246</v>
       </c>
@@ -3766,7 +3781,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>395</v>
       </c>
@@ -3780,7 +3795,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>395</v>
       </c>
@@ -3794,7 +3809,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>395</v>
       </c>
@@ -3808,7 +3823,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>395</v>
       </c>
@@ -3822,7 +3837,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>389</v>
       </c>
@@ -3836,7 +3851,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>389</v>
       </c>
@@ -3850,7 +3865,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>152</v>
       </c>
@@ -3864,7 +3879,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>152</v>
       </c>
@@ -3878,7 +3893,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>152</v>
       </c>
@@ -3892,7 +3907,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>152</v>
       </c>
@@ -3906,7 +3921,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>156</v>
       </c>
@@ -3920,7 +3935,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>156</v>
       </c>
@@ -3934,7 +3949,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>211</v>
       </c>
@@ -3948,7 +3963,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>211</v>
       </c>
@@ -3962,7 +3977,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>214</v>
       </c>
@@ -3976,7 +3991,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>214</v>
       </c>
@@ -3990,7 +4005,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>214</v>
       </c>
@@ -4004,7 +4019,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>213</v>
       </c>
@@ -4018,7 +4033,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>210</v>
       </c>
@@ -4032,7 +4047,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>82</v>
       </c>
@@ -4046,7 +4061,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>82</v>
       </c>
@@ -4060,7 +4075,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>347</v>
       </c>
@@ -4074,7 +4089,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>190</v>
       </c>
@@ -4088,7 +4103,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>190</v>
       </c>
@@ -4102,7 +4117,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>190</v>
       </c>
@@ -4116,7 +4131,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>190</v>
       </c>
@@ -4130,7 +4145,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>190</v>
       </c>
@@ -4144,7 +4159,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>206</v>
       </c>
@@ -4158,7 +4173,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>206</v>
       </c>
@@ -4172,7 +4187,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>206</v>
       </c>
@@ -4186,7 +4201,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>206</v>
       </c>
@@ -4200,7 +4215,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>47</v>
       </c>
@@ -4214,7 +4229,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>47</v>
       </c>
@@ -4228,7 +4243,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>47</v>
       </c>
@@ -4242,7 +4257,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>47</v>
       </c>
@@ -4256,7 +4271,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>47</v>
       </c>
@@ -4270,7 +4285,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>47</v>
       </c>
@@ -4284,7 +4299,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>47</v>
       </c>
@@ -4298,7 +4313,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>47</v>
       </c>
@@ -4312,7 +4327,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>47</v>
       </c>
@@ -4326,7 +4341,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>47</v>
       </c>
@@ -4340,7 +4355,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>212</v>
       </c>
@@ -4354,7 +4369,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>50</v>
       </c>
@@ -4368,7 +4383,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>50</v>
       </c>
@@ -4382,7 +4397,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>50</v>
       </c>
@@ -4396,7 +4411,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>50</v>
       </c>
@@ -4410,7 +4425,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>50</v>
       </c>
@@ -4424,7 +4439,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>50</v>
       </c>
@@ -4438,7 +4453,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>110</v>
       </c>
@@ -4452,7 +4467,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>110</v>
       </c>
@@ -4466,7 +4481,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>110</v>
       </c>
@@ -4480,7 +4495,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>110</v>
       </c>
@@ -4494,7 +4509,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>110</v>
       </c>
@@ -4508,7 +4523,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>207</v>
       </c>
@@ -4522,7 +4537,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>207</v>
       </c>
@@ -4536,7 +4551,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>207</v>
       </c>
@@ -4550,7 +4565,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>207</v>
       </c>
@@ -4562,6 +4577,34 @@
       </c>
       <c r="D205" t="s">
         <v>203</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trimming white space from snippet generator
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21916"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D102768-7975-406F-90DD-6E8A85FC9F19}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249ECC4A-8945-4B7C-B60A-5307AC6BE13F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -565,721 +565,721 @@
     <t>markerSize</t>
   </si>
   <si>
+    <t>markerBackgroundColor</t>
+  </si>
+  <si>
+    <t>excel-events-tablecollection-changed</t>
+  </si>
+  <si>
+    <t>tableId</t>
+  </si>
+  <si>
+    <t>// setXAxisValues</t>
+  </si>
+  <si>
+    <t>excel-events-table-changed</t>
+  </si>
+  <si>
+    <t>registerOnChangedHandler</t>
+  </si>
+  <si>
+    <t>onChanged</t>
+  </si>
+  <si>
+    <t>onChange</t>
+  </si>
+  <si>
+    <t>Workbook</t>
+  </si>
+  <si>
+    <t>getActiveCell</t>
+  </si>
+  <si>
+    <t>excel-workbook-get-active-cell</t>
+  </si>
+  <si>
+    <t>copy</t>
+  </si>
+  <si>
+    <t>excel-worksheet-copy</t>
+  </si>
+  <si>
+    <t>protect</t>
+  </si>
+  <si>
+    <t>protectDataInWorksheet</t>
+  </si>
+  <si>
+    <t>protectWorkbookStructure</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>unprotect</t>
+  </si>
+  <si>
+    <t>unprotectDataInWorksheet</t>
+  </si>
+  <si>
+    <t>unprotectWorkbookStructure</t>
+  </si>
+  <si>
+    <t>passwordProtectDataInWorksheet</t>
+  </si>
+  <si>
+    <t>passwordUnprotectDataInWorksheet</t>
+  </si>
+  <si>
+    <t>passwordProtectWorkbookStructure</t>
+  </si>
+  <si>
+    <t>passwordUnprotectWorkbookStructure</t>
+  </si>
+  <si>
+    <t>WorkbookProtection</t>
+  </si>
+  <si>
+    <t>WorksheetProtection</t>
+  </si>
+  <si>
+    <t>ChartLegendFormat</t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t>TableSelectionChangedEventArgs</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>WorksheetAddedEventArgs</t>
+  </si>
+  <si>
+    <t>TableCollection</t>
+  </si>
+  <si>
+    <t>TableChangedEventArgs</t>
+  </si>
+  <si>
+    <t>addPositiveNumberRequirement</t>
+  </si>
+  <si>
+    <t>requireApprovedName</t>
+  </si>
+  <si>
+    <t>warnAboutCommentRedundancy</t>
+  </si>
+  <si>
+    <t>excel-data-validation</t>
+  </si>
+  <si>
+    <t>wholeNumber</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>errorAlert</t>
+  </si>
+  <si>
+    <t>DataValidation</t>
+  </si>
+  <si>
+    <t>PivotTableCollection</t>
+  </si>
+  <si>
+    <t>excel-pivottable-create-and-modify</t>
+  </si>
+  <si>
+    <t>createWithNames</t>
+  </si>
+  <si>
+    <t>PivotTable</t>
+  </si>
+  <si>
+    <t>deletePivot</t>
+  </si>
+  <si>
+    <t>toggleColumn</t>
+  </si>
+  <si>
+    <t>columnHierarchies</t>
+  </si>
+  <si>
+    <t>dataHierarchies</t>
+  </si>
+  <si>
+    <t>addValues</t>
+  </si>
+  <si>
+    <t>changeHierarchyNames</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>DataPivotHierarchy</t>
+  </si>
+  <si>
+    <t>layout</t>
+  </si>
+  <si>
+    <t>changeLayout</t>
+  </si>
+  <si>
+    <t>filterHierarchies</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>PivotLayout</t>
+  </si>
+  <si>
+    <t>getDataBodyRange</t>
+  </si>
+  <si>
+    <t>getCrateTotal</t>
+  </si>
+  <si>
+    <t>showPercentages</t>
+  </si>
+  <si>
+    <t>excel-pivottable-filters-and-summaries</t>
+  </si>
+  <si>
+    <t>excel-pivottable-calculations</t>
+  </si>
+  <si>
+    <t>showAs</t>
+  </si>
+  <si>
+    <t>ShowAsRule</t>
+  </si>
+  <si>
+    <t>baseItem</t>
+  </si>
+  <si>
+    <t>showDifferenceFrom</t>
+  </si>
+  <si>
+    <t>Runtime</t>
+  </si>
+  <si>
+    <t>enableEvents</t>
+  </si>
+  <si>
+    <t>excel-events-disable-events</t>
+  </si>
+  <si>
+    <t>toggleEvents</t>
+  </si>
+  <si>
+    <t>DataValidationRule</t>
+  </si>
+  <si>
+    <t>excel-workbook-data-protection</t>
+  </si>
+  <si>
+    <t>excel-range-range-relationships</t>
+  </si>
+  <si>
+    <t>excel-table-style</t>
+  </si>
+  <si>
+    <t>excel-worksheet-gridlines</t>
+  </si>
+  <si>
+    <t>excel-scenarios-multiple-property-set</t>
+  </si>
+  <si>
+    <t>ChartTitle</t>
+  </si>
+  <si>
+    <t>getSubstring</t>
+  </si>
+  <si>
+    <t>excel-chart-title-format</t>
+  </si>
+  <si>
+    <t>changeTitleSubstring</t>
+  </si>
+  <si>
+    <t>changeTitleOrientation</t>
+  </si>
+  <si>
+    <t>addSeries</t>
+  </si>
+  <si>
+    <t>addNameToHeader</t>
+  </si>
+  <si>
+    <t>excel-events-workbook-and-worksheet-collection</t>
+  </si>
+  <si>
+    <t>excel-events-worksheet</t>
+  </si>
+  <si>
+    <t>excel-range-used-range</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>suspendScreenUpdatingUntilNextSync</t>
+  </si>
+  <si>
+    <t>refreshData</t>
+  </si>
+  <si>
+    <t>getSelectedRanges</t>
+  </si>
+  <si>
+    <t>colorSelectedRanges</t>
+  </si>
+  <si>
+    <t>colorSpecifiedRanges</t>
+  </si>
+  <si>
+    <t>getRanges</t>
+  </si>
+  <si>
+    <t>getSpecialCells</t>
+  </si>
+  <si>
+    <t>colorAllLogicalAndTextRanges</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>rotation</t>
+  </si>
+  <si>
+    <t>createTriangle</t>
+  </si>
+  <si>
+    <t>ShapeCollection</t>
+  </si>
+  <si>
+    <t>addGeometricShape</t>
+  </si>
+  <si>
+    <t>createSmileyFace</t>
+  </si>
+  <si>
+    <t>fill</t>
+  </si>
+  <si>
+    <t>removeAll</t>
+  </si>
+  <si>
+    <t>copyFrom</t>
+  </si>
+  <si>
+    <t>copyFormula</t>
+  </si>
+  <si>
+    <t>find</t>
+  </si>
+  <si>
+    <t>findText</t>
+  </si>
+  <si>
+    <t>findOrNullObject</t>
+  </si>
+  <si>
+    <t>findTextWithNullCheck</t>
+  </si>
+  <si>
+    <t>findAllOrNullObject</t>
+  </si>
+  <si>
+    <t>findCompleted</t>
+  </si>
+  <si>
+    <t>addImage</t>
+  </si>
+  <si>
+    <t>readImageFromFile</t>
+  </si>
+  <si>
+    <t>excel-performance-optimization</t>
+  </si>
+  <si>
+    <t>excel-range-areas</t>
+  </si>
+  <si>
+    <t>excel-shape-create-and-delete</t>
+  </si>
+  <si>
+    <t>excel-range-copyfrom</t>
+  </si>
+  <si>
+    <t>excel-range-find</t>
+  </si>
+  <si>
+    <t>excel-worksheet-find-all</t>
+  </si>
+  <si>
+    <t>excel-shape-images</t>
+  </si>
+  <si>
+    <t>flipImage</t>
+  </si>
+  <si>
+    <t>incrementRotation</t>
+  </si>
+  <si>
+    <t>getImageFormat</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>writeOutImageString</t>
+  </si>
+  <si>
+    <t>insertSheets</t>
+  </si>
+  <si>
+    <t>addFromBase64</t>
+  </si>
+  <si>
+    <t>excel-workbook-insert-external-worksheets</t>
+  </si>
+  <si>
+    <t>incrementLeft</t>
+  </si>
+  <si>
+    <t>incrementTop</t>
+  </si>
+  <si>
+    <t>excel-shape-move-and-order</t>
+  </si>
+  <si>
+    <t>moveLeft</t>
+  </si>
+  <si>
+    <t>moveDown</t>
+  </si>
+  <si>
+    <t>scaleUp</t>
+  </si>
+  <si>
+    <t>moveZOrderDown</t>
+  </si>
+  <si>
+    <t>setZOrder</t>
+  </si>
+  <si>
+    <t>scaleHeight</t>
+  </si>
+  <si>
+    <t>PageBreakCollection</t>
+  </si>
+  <si>
+    <t>excel-worksheet-page-layout</t>
+  </si>
+  <si>
+    <t>setPageBreaks</t>
+  </si>
+  <si>
+    <t>centerHorizontally</t>
+  </si>
+  <si>
+    <t>centerVertically</t>
+  </si>
+  <si>
+    <t>PageLayout</t>
+  </si>
+  <si>
+    <t>center</t>
+  </si>
+  <si>
+    <t>setPrintTitleRows</t>
+  </si>
+  <si>
+    <t>setPrintTitleRow</t>
+  </si>
+  <si>
+    <t>setPrintArea</t>
+  </si>
+  <si>
+    <t>orientation</t>
+  </si>
+  <si>
+    <t>deleteName</t>
+  </si>
+  <si>
+    <t>excel-range-remove-duplicates</t>
+  </si>
+  <si>
+    <t>removeDuplicates</t>
+  </si>
+  <si>
+    <t>uniqueRemaining</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>excel-workbook-save-and-close</t>
+  </si>
+  <si>
+    <t>saveWithoutPrompt</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>closeWithSave</t>
+  </si>
+  <si>
+    <t>createHexagon</t>
+  </si>
+  <si>
+    <t>changeOrientation</t>
+  </si>
+  <si>
+    <t>RemoveDuplicatesResult</t>
+  </si>
+  <si>
+    <t>addTextBox</t>
+  </si>
+  <si>
+    <t>excel-shape-textboxes</t>
+  </si>
+  <si>
+    <t>createTextbox</t>
+  </si>
+  <si>
+    <t>deleteText</t>
+  </si>
+  <si>
+    <t>TextFrame</t>
+  </si>
+  <si>
+    <t>addLine</t>
+  </si>
+  <si>
+    <t>excel-shape-lines</t>
+  </si>
+  <si>
+    <t>addStraightLine</t>
+  </si>
+  <si>
+    <t>arrowLine</t>
+  </si>
+  <si>
+    <t>connectStraightLine</t>
+  </si>
+  <si>
+    <t>disconnectStraightLine</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>connectBeginShape</t>
+  </si>
+  <si>
+    <t>connectEndShape</t>
+  </si>
+  <si>
+    <t>disconnectBeginShape</t>
+  </si>
+  <si>
+    <t>disconnectEndShape</t>
+  </si>
+  <si>
+    <t>ShapeGroup</t>
+  </si>
+  <si>
+    <t>ungroup</t>
+  </si>
+  <si>
+    <t>excel-shape-groups</t>
+  </si>
+  <si>
+    <t>ungroupShapes</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>addGroup</t>
+  </si>
+  <si>
+    <t>groupShapes</t>
+  </si>
+  <si>
+    <t>getAsImage</t>
+  </si>
+  <si>
+    <t>excel-comment</t>
+  </si>
+  <si>
+    <t>CommentCollection</t>
+  </si>
+  <si>
+    <t>addCommentToCell</t>
+  </si>
+  <si>
+    <t>CommentReplyCollection</t>
+  </si>
+  <si>
+    <t>addCommentReply</t>
+  </si>
+  <si>
+    <t>getCommentMetadata</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>load_2</t>
+  </si>
+  <si>
+    <t>editComment</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>CommentReply</t>
+  </si>
+  <si>
+    <t>deleteComment</t>
+  </si>
+  <si>
+    <t>deleteCommentReply</t>
+  </si>
+  <si>
+    <t>lockAspectRatio</t>
+  </si>
+  <si>
+    <t>onTableChanged</t>
+  </si>
+  <si>
+    <t>excel-data-change-event-details</t>
+  </si>
+  <si>
+    <t>details</t>
+  </si>
+  <si>
+    <t>addAutoFilter</t>
+  </si>
+  <si>
+    <t>excel-worksheet-auto-filter</t>
+  </si>
+  <si>
+    <t>AutoFilter</t>
+  </si>
+  <si>
+    <t>apply</t>
+  </si>
+  <si>
+    <t>autoFilter</t>
+  </si>
+  <si>
+    <t>SlicerCollection</t>
+  </si>
+  <si>
+    <t>addSlicer</t>
+  </si>
+  <si>
+    <t>excel-pivottable-slicer</t>
+  </si>
+  <si>
+    <t>slicers</t>
+  </si>
+  <si>
+    <t>formatSlicer</t>
+  </si>
+  <si>
+    <t>applyStyle</t>
+  </si>
+  <si>
+    <t>Slicer</t>
+  </si>
+  <si>
+    <t>addFilters</t>
+  </si>
+  <si>
+    <t>selectItems</t>
+  </si>
+  <si>
+    <t>clearFilters</t>
+  </si>
+  <si>
+    <t>removeFilters</t>
+  </si>
+  <si>
+    <t>removeSlicer</t>
+  </si>
+  <si>
+    <t>RangeAreas</t>
+  </si>
+  <si>
+    <t>colorAllFormulaRanges</t>
+  </si>
+  <si>
+    <t>prompt</t>
+  </si>
+  <si>
+    <t>zoom</t>
+  </si>
+  <si>
+    <t>setZoom</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>excel-range-cell-properties</t>
+  </si>
+  <si>
+    <t>setCellProperties</t>
+  </si>
+  <si>
+    <t>getCellProperties</t>
+  </si>
+  <si>
+    <t>CellPropertiesFont</t>
+  </si>
+  <si>
+    <t>CellPropertiesFill</t>
+  </si>
+  <si>
+    <t>CellPropertiesFillLoadOptions</t>
+  </si>
+  <si>
+    <t>CellPropertiesFontLoadOptions</t>
+  </si>
+  <si>
+    <t>CellPropertiesLoadOptions</t>
+  </si>
+  <si>
+    <t>SettableCellProperties</t>
+  </si>
+  <si>
+    <t>excel-event-worksheet-single-click</t>
+  </si>
+  <si>
+    <t>registerClickHandler</t>
+  </si>
+  <si>
+    <t>onSingleClicked</t>
+  </si>
+  <si>
+    <t>WorksheetSingleClickedEventArgs</t>
+  </si>
+  <si>
     <t>markerForegroundColor</t>
-  </si>
-  <si>
-    <t>markerBackgroundColor</t>
-  </si>
-  <si>
-    <t>excel-events-tablecollection-changed</t>
-  </si>
-  <si>
-    <t>tableId</t>
-  </si>
-  <si>
-    <t>// setXAxisValues</t>
-  </si>
-  <si>
-    <t>excel-events-table-changed</t>
-  </si>
-  <si>
-    <t>registerOnChangedHandler</t>
-  </si>
-  <si>
-    <t>onChanged</t>
-  </si>
-  <si>
-    <t>onChange</t>
-  </si>
-  <si>
-    <t>Workbook</t>
-  </si>
-  <si>
-    <t>getActiveCell</t>
-  </si>
-  <si>
-    <t>excel-workbook-get-active-cell</t>
-  </si>
-  <si>
-    <t>copy</t>
-  </si>
-  <si>
-    <t>excel-worksheet-copy</t>
-  </si>
-  <si>
-    <t>protect</t>
-  </si>
-  <si>
-    <t>protectDataInWorksheet</t>
-  </si>
-  <si>
-    <t>protectWorkbookStructure</t>
-  </si>
-  <si>
-    <t>run</t>
-  </si>
-  <si>
-    <t>unprotect</t>
-  </si>
-  <si>
-    <t>unprotectDataInWorksheet</t>
-  </si>
-  <si>
-    <t>unprotectWorkbookStructure</t>
-  </si>
-  <si>
-    <t>passwordProtectDataInWorksheet</t>
-  </si>
-  <si>
-    <t>passwordUnprotectDataInWorksheet</t>
-  </si>
-  <si>
-    <t>passwordProtectWorkbookStructure</t>
-  </si>
-  <si>
-    <t>passwordUnprotectWorkbookStructure</t>
-  </si>
-  <si>
-    <t>WorkbookProtection</t>
-  </si>
-  <si>
-    <t>WorksheetProtection</t>
-  </si>
-  <si>
-    <t>ChartLegendFormat</t>
-  </si>
-  <si>
-    <t>load</t>
-  </si>
-  <si>
-    <t>TableSelectionChangedEventArgs</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>WorksheetAddedEventArgs</t>
-  </si>
-  <si>
-    <t>TableCollection</t>
-  </si>
-  <si>
-    <t>TableChangedEventArgs</t>
-  </si>
-  <si>
-    <t>addPositiveNumberRequirement</t>
-  </si>
-  <si>
-    <t>requireApprovedName</t>
-  </si>
-  <si>
-    <t>warnAboutCommentRedundancy</t>
-  </si>
-  <si>
-    <t>excel-data-validation</t>
-  </si>
-  <si>
-    <t>wholeNumber</t>
-  </si>
-  <si>
-    <t>list</t>
-  </si>
-  <si>
-    <t>errorAlert</t>
-  </si>
-  <si>
-    <t>DataValidation</t>
-  </si>
-  <si>
-    <t>PivotTableCollection</t>
-  </si>
-  <si>
-    <t>excel-pivottable-create-and-modify</t>
-  </si>
-  <si>
-    <t>createWithNames</t>
-  </si>
-  <si>
-    <t>PivotTable</t>
-  </si>
-  <si>
-    <t>deletePivot</t>
-  </si>
-  <si>
-    <t>toggleColumn</t>
-  </si>
-  <si>
-    <t>columnHierarchies</t>
-  </si>
-  <si>
-    <t>dataHierarchies</t>
-  </si>
-  <si>
-    <t>addValues</t>
-  </si>
-  <si>
-    <t>changeHierarchyNames</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>DataPivotHierarchy</t>
-  </si>
-  <si>
-    <t>layout</t>
-  </si>
-  <si>
-    <t>changeLayout</t>
-  </si>
-  <si>
-    <t>filterHierarchies</t>
-  </si>
-  <si>
-    <t>filter</t>
-  </si>
-  <si>
-    <t>PivotLayout</t>
-  </si>
-  <si>
-    <t>getDataBodyRange</t>
-  </si>
-  <si>
-    <t>getCrateTotal</t>
-  </si>
-  <si>
-    <t>showPercentages</t>
-  </si>
-  <si>
-    <t>excel-pivottable-filters-and-summaries</t>
-  </si>
-  <si>
-    <t>excel-pivottable-calculations</t>
-  </si>
-  <si>
-    <t>showAs</t>
-  </si>
-  <si>
-    <t>ShowAsRule</t>
-  </si>
-  <si>
-    <t>baseItem</t>
-  </si>
-  <si>
-    <t>showDifferenceFrom</t>
-  </si>
-  <si>
-    <t>Runtime</t>
-  </si>
-  <si>
-    <t>enableEvents</t>
-  </si>
-  <si>
-    <t>excel-events-disable-events</t>
-  </si>
-  <si>
-    <t>toggleEvents</t>
-  </si>
-  <si>
-    <t>DataValidationRule</t>
-  </si>
-  <si>
-    <t>excel-workbook-data-protection</t>
-  </si>
-  <si>
-    <t>excel-range-range-relationships</t>
-  </si>
-  <si>
-    <t>excel-table-style</t>
-  </si>
-  <si>
-    <t>excel-worksheet-gridlines</t>
-  </si>
-  <si>
-    <t>excel-scenarios-multiple-property-set</t>
-  </si>
-  <si>
-    <t>ChartTitle</t>
-  </si>
-  <si>
-    <t>getSubstring</t>
-  </si>
-  <si>
-    <t>excel-chart-title-format</t>
-  </si>
-  <si>
-    <t>changeTitleSubstring</t>
-  </si>
-  <si>
-    <t>changeTitleOrientation</t>
-  </si>
-  <si>
-    <t>addSeries</t>
-  </si>
-  <si>
-    <t>addNameToHeader</t>
-  </si>
-  <si>
-    <t>excel-events-workbook-and-worksheet-collection</t>
-  </si>
-  <si>
-    <t>excel-events-worksheet</t>
-  </si>
-  <si>
-    <t>excel-range-used-range</t>
-  </si>
-  <si>
-    <t>Application</t>
-  </si>
-  <si>
-    <t>suspendScreenUpdatingUntilNextSync</t>
-  </si>
-  <si>
-    <t>refreshData</t>
-  </si>
-  <si>
-    <t>getSelectedRanges</t>
-  </si>
-  <si>
-    <t>colorSelectedRanges</t>
-  </si>
-  <si>
-    <t>colorSpecifiedRanges</t>
-  </si>
-  <si>
-    <t>getRanges</t>
-  </si>
-  <si>
-    <t>getSpecialCells</t>
-  </si>
-  <si>
-    <t>colorAllLogicalAndTextRanges</t>
-  </si>
-  <si>
-    <t>Shape</t>
-  </si>
-  <si>
-    <t>rotation</t>
-  </si>
-  <si>
-    <t>createTriangle</t>
-  </si>
-  <si>
-    <t>ShapeCollection</t>
-  </si>
-  <si>
-    <t>addGeometricShape</t>
-  </si>
-  <si>
-    <t>createSmileyFace</t>
-  </si>
-  <si>
-    <t>fill</t>
-  </si>
-  <si>
-    <t>removeAll</t>
-  </si>
-  <si>
-    <t>copyFrom</t>
-  </si>
-  <si>
-    <t>copyFormula</t>
-  </si>
-  <si>
-    <t>find</t>
-  </si>
-  <si>
-    <t>findText</t>
-  </si>
-  <si>
-    <t>findOrNullObject</t>
-  </si>
-  <si>
-    <t>findTextWithNullCheck</t>
-  </si>
-  <si>
-    <t>findAllOrNullObject</t>
-  </si>
-  <si>
-    <t>findCompleted</t>
-  </si>
-  <si>
-    <t>addImage</t>
-  </si>
-  <si>
-    <t>readImageFromFile</t>
-  </si>
-  <si>
-    <t>excel-performance-optimization</t>
-  </si>
-  <si>
-    <t>excel-range-areas</t>
-  </si>
-  <si>
-    <t>excel-shape-create-and-delete</t>
-  </si>
-  <si>
-    <t>excel-range-copyfrom</t>
-  </si>
-  <si>
-    <t>excel-range-find</t>
-  </si>
-  <si>
-    <t>excel-worksheet-find-all</t>
-  </si>
-  <si>
-    <t>excel-shape-images</t>
-  </si>
-  <si>
-    <t>flipImage</t>
-  </si>
-  <si>
-    <t>incrementRotation</t>
-  </si>
-  <si>
-    <t>getImageFormat</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>writeOutImageString</t>
-  </si>
-  <si>
-    <t>insertSheets</t>
-  </si>
-  <si>
-    <t>addFromBase64</t>
-  </si>
-  <si>
-    <t>excel-workbook-insert-external-worksheets</t>
-  </si>
-  <si>
-    <t>incrementLeft</t>
-  </si>
-  <si>
-    <t>incrementTop</t>
-  </si>
-  <si>
-    <t>excel-shape-move-and-order</t>
-  </si>
-  <si>
-    <t>moveLeft</t>
-  </si>
-  <si>
-    <t>moveDown</t>
-  </si>
-  <si>
-    <t>scaleUp</t>
-  </si>
-  <si>
-    <t>moveZOrderDown</t>
-  </si>
-  <si>
-    <t>setZOrder</t>
-  </si>
-  <si>
-    <t>scaleHeight</t>
-  </si>
-  <si>
-    <t>PageBreakCollection</t>
-  </si>
-  <si>
-    <t>excel-worksheet-page-layout</t>
-  </si>
-  <si>
-    <t>setPageBreaks</t>
-  </si>
-  <si>
-    <t>centerHorizontally</t>
-  </si>
-  <si>
-    <t>centerVertically</t>
-  </si>
-  <si>
-    <t>PageLayout</t>
-  </si>
-  <si>
-    <t>center</t>
-  </si>
-  <si>
-    <t>setPrintTitleRows</t>
-  </si>
-  <si>
-    <t>setPrintTitleRow</t>
-  </si>
-  <si>
-    <t>setPrintArea</t>
-  </si>
-  <si>
-    <t>orientation</t>
-  </si>
-  <si>
-    <t>deleteName</t>
-  </si>
-  <si>
-    <t>excel-range-remove-duplicates</t>
-  </si>
-  <si>
-    <t>removeDuplicates</t>
-  </si>
-  <si>
-    <t>uniqueRemaining</t>
-  </si>
-  <si>
-    <t>save</t>
-  </si>
-  <si>
-    <t>excel-workbook-save-and-close</t>
-  </si>
-  <si>
-    <t>saveWithoutPrompt</t>
-  </si>
-  <si>
-    <t>close</t>
-  </si>
-  <si>
-    <t>closeWithSave</t>
-  </si>
-  <si>
-    <t>createHexagon</t>
-  </si>
-  <si>
-    <t>changeOrientation</t>
-  </si>
-  <si>
-    <t>RemoveDuplicatesResult</t>
-  </si>
-  <si>
-    <t>addTextBox</t>
-  </si>
-  <si>
-    <t>excel-shape-textboxes</t>
-  </si>
-  <si>
-    <t>createTextbox</t>
-  </si>
-  <si>
-    <t>deleteText</t>
-  </si>
-  <si>
-    <t>TextFrame</t>
-  </si>
-  <si>
-    <t>addLine</t>
-  </si>
-  <si>
-    <t>excel-shape-lines</t>
-  </si>
-  <si>
-    <t>addStraightLine</t>
-  </si>
-  <si>
-    <t>arrowLine</t>
-  </si>
-  <si>
-    <t>connectStraightLine</t>
-  </si>
-  <si>
-    <t>disconnectStraightLine</t>
-  </si>
-  <si>
-    <t>Line</t>
-  </si>
-  <si>
-    <t>connectBeginShape</t>
-  </si>
-  <si>
-    <t>connectEndShape</t>
-  </si>
-  <si>
-    <t>disconnectBeginShape</t>
-  </si>
-  <si>
-    <t>disconnectEndShape</t>
-  </si>
-  <si>
-    <t>ShapeGroup</t>
-  </si>
-  <si>
-    <t>ungroup</t>
-  </si>
-  <si>
-    <t>excel-shape-groups</t>
-  </si>
-  <si>
-    <t>ungroupShapes</t>
-  </si>
-  <si>
-    <t>group</t>
-  </si>
-  <si>
-    <t>addGroup</t>
-  </si>
-  <si>
-    <t>groupShapes</t>
-  </si>
-  <si>
-    <t>getAsImage</t>
-  </si>
-  <si>
-    <t>excel-comment</t>
-  </si>
-  <si>
-    <t>CommentCollection</t>
-  </si>
-  <si>
-    <t>addCommentToCell</t>
-  </si>
-  <si>
-    <t>CommentReplyCollection</t>
-  </si>
-  <si>
-    <t>addCommentReply</t>
-  </si>
-  <si>
-    <t>getCommentMetadata</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>load_2</t>
-  </si>
-  <si>
-    <t>editComment</t>
-  </si>
-  <si>
-    <t>content</t>
-  </si>
-  <si>
-    <t>CommentReply</t>
-  </si>
-  <si>
-    <t>deleteComment</t>
-  </si>
-  <si>
-    <t>deleteCommentReply</t>
-  </si>
-  <si>
-    <t>lockAspectRatio</t>
-  </si>
-  <si>
-    <t>onTableChanged</t>
-  </si>
-  <si>
-    <t>excel-data-change-event-details</t>
-  </si>
-  <si>
-    <t>details</t>
-  </si>
-  <si>
-    <t>addAutoFilter</t>
-  </si>
-  <si>
-    <t>excel-worksheet-auto-filter</t>
-  </si>
-  <si>
-    <t>AutoFilter</t>
-  </si>
-  <si>
-    <t>apply</t>
-  </si>
-  <si>
-    <t>autoFilter</t>
-  </si>
-  <si>
-    <t>SlicerCollection</t>
-  </si>
-  <si>
-    <t>addSlicer</t>
-  </si>
-  <si>
-    <t>excel-pivottable-slicer</t>
-  </si>
-  <si>
-    <t>slicers</t>
-  </si>
-  <si>
-    <t>formatSlicer</t>
-  </si>
-  <si>
-    <t>applyStyle</t>
-  </si>
-  <si>
-    <t>Slicer</t>
-  </si>
-  <si>
-    <t>addFilters</t>
-  </si>
-  <si>
-    <t>selectItems</t>
-  </si>
-  <si>
-    <t>clearFilters</t>
-  </si>
-  <si>
-    <t>removeFilters</t>
-  </si>
-  <si>
-    <t>removeSlicer</t>
-  </si>
-  <si>
-    <t>RangeAreas</t>
-  </si>
-  <si>
-    <t>colorAllFormulaRanges</t>
-  </si>
-  <si>
-    <t>prompt</t>
-  </si>
-  <si>
-    <t>zoom</t>
-  </si>
-  <si>
-    <t>setZoom</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>excel-range-cell-properties</t>
-  </si>
-  <si>
-    <t>setCellProperties</t>
-  </si>
-  <si>
-    <t>getCellProperties</t>
-  </si>
-  <si>
-    <t>CellPropertiesFont</t>
-  </si>
-  <si>
-    <t>CellPropertiesFill</t>
-  </si>
-  <si>
-    <t>CellPropertiesFillLoadOptions</t>
-  </si>
-  <si>
-    <t>CellPropertiesFontLoadOptions</t>
-  </si>
-  <si>
-    <t>CellPropertiesLoadOptions</t>
-  </si>
-  <si>
-    <t>SettableCellProperties</t>
-  </si>
-  <si>
-    <t>excel-event-worksheet-single-click</t>
-  </si>
-  <si>
-    <t>registerClickHandler</t>
-  </si>
-  <si>
-    <t>onSingleClicked</t>
-  </si>
-  <si>
-    <t>WorksheetSingleClickedEventArgs</t>
   </si>
 </sst>
 </file>
@@ -1694,8 +1694,8 @@
   <dimension ref="A1:D207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K206" sqref="K206"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,30 +1722,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" t="s">
         <v>269</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D2" t="s">
         <v>270</v>
-      </c>
-      <c r="C2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D2" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>387</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1764,72 +1764,72 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>106</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1904,7 +1904,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B15" t="s">
         <v>149</v>
@@ -1927,7 +1927,7 @@
         <v>139</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1949,7 +1949,7 @@
         <v>136</v>
       </c>
       <c r="B18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C18" t="s">
         <v>178</v>
@@ -1963,7 +1963,7 @@
         <v>136</v>
       </c>
       <c r="B19" t="s">
-        <v>181</v>
+        <v>419</v>
       </c>
       <c r="C19" t="s">
         <v>178</v>
@@ -2011,35 +2011,35 @@
         <v>139</v>
       </c>
       <c r="D22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>258</v>
+      </c>
+      <c r="B23" t="s">
         <v>259</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>260</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>261</v>
-      </c>
-      <c r="D23" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B24" t="s">
         <v>113</v>
       </c>
       <c r="C24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D24" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2114,100 +2114,100 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B30" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C30" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D30" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D31" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>372</v>
+      </c>
+      <c r="B32" t="s">
         <v>373</v>
       </c>
-      <c r="B32" t="s">
-        <v>374</v>
-      </c>
       <c r="C32" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D32" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D33" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B34" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C34" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D34" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D35" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D36" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2674,100 +2674,100 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B70" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C70" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D70" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B71" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C71" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D71" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B72" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C72" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D72" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B73" t="s">
         <v>69</v>
       </c>
       <c r="C73" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D73" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B74" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C74" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D74" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B75" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C75" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D75" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B76" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C76" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D76" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2800,72 +2800,72 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B79" t="s">
         <v>86</v>
       </c>
       <c r="C79" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D79" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>353</v>
+      </c>
+      <c r="B80" t="s">
         <v>354</v>
       </c>
-      <c r="B80" t="s">
-        <v>355</v>
-      </c>
       <c r="C80" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D80" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B81" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C81" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D81" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B82" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C82" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D82" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B83" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C83" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D83" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2907,203 +2907,203 @@
         <v>12</v>
       </c>
       <c r="D86" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B87" t="s">
         <v>9</v>
       </c>
       <c r="C87" t="s">
+        <v>320</v>
+      </c>
+      <c r="D87" t="s">
         <v>321</v>
-      </c>
-      <c r="D87" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>324</v>
+      </c>
+      <c r="B88" t="s">
+        <v>322</v>
+      </c>
+      <c r="C88" t="s">
+        <v>320</v>
+      </c>
+      <c r="D88" t="s">
         <v>325</v>
-      </c>
-      <c r="B88" t="s">
-        <v>323</v>
-      </c>
-      <c r="C88" t="s">
-        <v>321</v>
-      </c>
-      <c r="D88" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>324</v>
+      </c>
+      <c r="B89" t="s">
+        <v>323</v>
+      </c>
+      <c r="C89" t="s">
+        <v>320</v>
+      </c>
+      <c r="D89" t="s">
         <v>325</v>
-      </c>
-      <c r="B89" t="s">
-        <v>324</v>
-      </c>
-      <c r="C89" t="s">
-        <v>321</v>
-      </c>
-      <c r="D89" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B90" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C90" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D90" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B91" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C91" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D91" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B92" t="s">
+        <v>326</v>
+      </c>
+      <c r="C92" t="s">
+        <v>320</v>
+      </c>
+      <c r="D92" t="s">
         <v>327</v>
-      </c>
-      <c r="C92" t="s">
-        <v>321</v>
-      </c>
-      <c r="D92" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C93" t="s">
+        <v>320</v>
+      </c>
+      <c r="D93" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="C93" t="s">
-        <v>321</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>238</v>
+      </c>
+      <c r="B94" t="s">
         <v>239</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
+        <v>242</v>
+      </c>
+      <c r="D94" t="s">
         <v>240</v>
-      </c>
-      <c r="C94" t="s">
-        <v>243</v>
-      </c>
-      <c r="D94" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B95" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C95" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D95" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B96" t="s">
+        <v>229</v>
+      </c>
+      <c r="C96" t="s">
+        <v>223</v>
+      </c>
+      <c r="D96" t="s">
         <v>230</v>
-      </c>
-      <c r="C96" t="s">
-        <v>224</v>
-      </c>
-      <c r="D96" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B97" t="s">
         <v>11</v>
       </c>
       <c r="C97" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D97" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B98" t="s">
+        <v>236</v>
+      </c>
+      <c r="C98" t="s">
+        <v>242</v>
+      </c>
+      <c r="D98" t="s">
         <v>237</v>
-      </c>
-      <c r="C98" t="s">
-        <v>243</v>
-      </c>
-      <c r="D98" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B99" t="s">
+        <v>234</v>
+      </c>
+      <c r="C99" t="s">
+        <v>223</v>
+      </c>
+      <c r="D99" t="s">
         <v>235</v>
-      </c>
-      <c r="C99" t="s">
-        <v>224</v>
-      </c>
-      <c r="D99" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B100" t="s">
         <v>9</v>
       </c>
       <c r="C100" t="s">
+        <v>223</v>
+      </c>
+      <c r="D100" t="s">
         <v>224</v>
-      </c>
-      <c r="D100" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3139,13 +3139,13 @@
         <v>24</v>
       </c>
       <c r="B103" t="s">
+        <v>285</v>
+      </c>
+      <c r="C103" t="s">
+        <v>298</v>
+      </c>
+      <c r="D103" t="s">
         <v>286</v>
-      </c>
-      <c r="C103" t="s">
-        <v>299</v>
-      </c>
-      <c r="D103" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -3153,13 +3153,13 @@
         <v>24</v>
       </c>
       <c r="B104" t="s">
+        <v>287</v>
+      </c>
+      <c r="C104" t="s">
+        <v>299</v>
+      </c>
+      <c r="D104" t="s">
         <v>288</v>
-      </c>
-      <c r="C104" t="s">
-        <v>300</v>
-      </c>
-      <c r="D104" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3167,13 +3167,13 @@
         <v>24</v>
       </c>
       <c r="B105" t="s">
+        <v>289</v>
+      </c>
+      <c r="C105" t="s">
+        <v>299</v>
+      </c>
+      <c r="D105" t="s">
         <v>290</v>
-      </c>
-      <c r="C105" t="s">
-        <v>300</v>
-      </c>
-      <c r="D105" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -3184,7 +3184,7 @@
         <v>27</v>
       </c>
       <c r="C106" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D106" t="s">
         <v>28</v>
@@ -3195,13 +3195,13 @@
         <v>24</v>
       </c>
       <c r="B107" t="s">
+        <v>275</v>
+      </c>
+      <c r="C107" t="s">
+        <v>296</v>
+      </c>
+      <c r="D107" t="s">
         <v>276</v>
-      </c>
-      <c r="C107" t="s">
-        <v>297</v>
-      </c>
-      <c r="D107" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -3212,7 +3212,7 @@
         <v>29</v>
       </c>
       <c r="C108" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D108" t="s">
         <v>28</v>
@@ -3226,7 +3226,7 @@
         <v>25</v>
       </c>
       <c r="C109" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D109" t="s">
         <v>26</v>
@@ -3251,13 +3251,13 @@
         <v>24</v>
       </c>
       <c r="B111" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C111" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D111" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -3268,7 +3268,7 @@
         <v>31</v>
       </c>
       <c r="C112" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D112" t="s">
         <v>32</v>
@@ -3282,7 +3282,7 @@
         <v>31</v>
       </c>
       <c r="C113" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D113" t="s">
         <v>33</v>
@@ -3296,7 +3296,7 @@
         <v>79</v>
       </c>
       <c r="C114" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D114" t="s">
         <v>160</v>
@@ -3307,13 +3307,13 @@
         <v>24</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C115" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D115" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3321,27 +3321,27 @@
         <v>24</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C117" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3416,44 +3416,44 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B123" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C123" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D123" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>248</v>
+      </c>
+      <c r="B124" t="s">
         <v>249</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" t="s">
         <v>250</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D124" t="s">
         <v>251</v>
-      </c>
-      <c r="D124" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C125" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D125" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3478,7 +3478,7 @@
         <v>9</v>
       </c>
       <c r="C127" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D127" t="s">
         <v>19</v>
@@ -3506,7 +3506,7 @@
         <v>18</v>
       </c>
       <c r="C129" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D129" t="s">
         <v>19</v>
@@ -3514,352 +3514,352 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B130" t="s">
         <v>11</v>
       </c>
       <c r="C130" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D130" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B131" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C131" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D131" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B132" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C132" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D132" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B133" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C133" t="s">
+        <v>360</v>
+      </c>
+      <c r="D133" t="s">
         <v>361</v>
-      </c>
-      <c r="D133" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B134" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C134" t="s">
+        <v>312</v>
+      </c>
+      <c r="D134" t="s">
         <v>313</v>
-      </c>
-      <c r="D134" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B135" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C135" t="s">
+        <v>301</v>
+      </c>
+      <c r="D135" t="s">
         <v>302</v>
-      </c>
-      <c r="D135" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B136" t="s">
+        <v>311</v>
+      </c>
+      <c r="C136" t="s">
         <v>312</v>
       </c>
-      <c r="C136" t="s">
-        <v>313</v>
-      </c>
       <c r="D136" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B137" t="s">
         <v>134</v>
       </c>
       <c r="C137" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D137" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>277</v>
+      </c>
+      <c r="B138" t="s">
         <v>278</v>
       </c>
-      <c r="B138" t="s">
+      <c r="C138" t="s">
+        <v>297</v>
+      </c>
+      <c r="D138" t="s">
         <v>279</v>
-      </c>
-      <c r="C138" t="s">
-        <v>298</v>
-      </c>
-      <c r="D138" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B139" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C139" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D139" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B140" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C140" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D140" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B141" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C141" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D141" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>280</v>
+      </c>
+      <c r="B142" t="s">
         <v>281</v>
       </c>
-      <c r="B142" t="s">
-        <v>282</v>
-      </c>
       <c r="C142" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D142" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B143" t="s">
+        <v>363</v>
+      </c>
+      <c r="C143" t="s">
+        <v>360</v>
+      </c>
+      <c r="D143" t="s">
         <v>364</v>
-      </c>
-      <c r="C143" t="s">
-        <v>361</v>
-      </c>
-      <c r="D143" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B144" t="s">
+        <v>293</v>
+      </c>
+      <c r="C144" t="s">
+        <v>301</v>
+      </c>
+      <c r="D144" t="s">
         <v>294</v>
-      </c>
-      <c r="C144" t="s">
-        <v>302</v>
-      </c>
-      <c r="D144" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B145" t="s">
+        <v>347</v>
+      </c>
+      <c r="C145" t="s">
         <v>348</v>
       </c>
-      <c r="C145" t="s">
+      <c r="D145" t="s">
         <v>349</v>
-      </c>
-      <c r="D145" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B146" t="s">
+        <v>342</v>
+      </c>
+      <c r="C146" t="s">
         <v>343</v>
       </c>
-      <c r="C146" t="s">
+      <c r="D146" t="s">
         <v>344</v>
-      </c>
-      <c r="D146" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>358</v>
+      </c>
+      <c r="B147" t="s">
         <v>359</v>
       </c>
-      <c r="B147" t="s">
+      <c r="C147" t="s">
         <v>360</v>
       </c>
-      <c r="C147" t="s">
+      <c r="D147" t="s">
         <v>361</v>
-      </c>
-      <c r="D147" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>245</v>
+      </c>
+      <c r="B148" t="s">
         <v>246</v>
       </c>
-      <c r="B148" t="s">
+      <c r="C148" t="s">
+        <v>243</v>
+      </c>
+      <c r="D148" t="s">
         <v>247</v>
-      </c>
-      <c r="C148" t="s">
-        <v>244</v>
-      </c>
-      <c r="D148" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D150" s="2" t="s">
         <v>395</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D150" s="2" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B151" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D151" s="2" t="s">
         <v>398</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D151" s="2" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -3870,7 +3870,7 @@
         <v>11</v>
       </c>
       <c r="C155" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D155" t="s">
         <v>163</v>
@@ -3884,7 +3884,7 @@
         <v>149</v>
       </c>
       <c r="C156" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D156" t="s">
         <v>162</v>
@@ -3898,7 +3898,7 @@
         <v>164</v>
       </c>
       <c r="C157" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D157" t="s">
         <v>160</v>
@@ -3909,10 +3909,10 @@
         <v>152</v>
       </c>
       <c r="B158" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C158" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D158" t="s">
         <v>165</v>
@@ -3926,7 +3926,7 @@
         <v>9</v>
       </c>
       <c r="C159" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3940,7 +3940,7 @@
         <v>37</v>
       </c>
       <c r="C160" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D160" t="s">
         <v>161</v>
@@ -3948,27 +3948,27 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B161" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C161" t="s">
+        <v>185</v>
+      </c>
+      <c r="D161" t="s">
         <v>186</v>
-      </c>
-      <c r="D161" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B162" t="s">
         <v>167</v>
       </c>
       <c r="C162" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D162" t="s">
         <v>168</v>
@@ -3976,69 +3976,69 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B163" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C163" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D163" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B164" t="s">
         <v>171</v>
       </c>
       <c r="C164" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D164" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B165" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C165" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D165" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B166" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C166" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D166" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B167" t="s">
         <v>106</v>
       </c>
       <c r="C167" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D167" t="s">
         <v>166</v>
@@ -4074,63 +4074,63 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B170" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C170" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D170" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B171" t="s">
+        <v>337</v>
+      </c>
+      <c r="C171" t="s">
+        <v>335</v>
+      </c>
+      <c r="D171" t="s">
         <v>338</v>
-      </c>
-      <c r="C171" t="s">
-        <v>336</v>
-      </c>
-      <c r="D171" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
+        <v>189</v>
+      </c>
+      <c r="B172" t="s">
         <v>190</v>
       </c>
-      <c r="B172" t="s">
+      <c r="C172" t="s">
         <v>191</v>
       </c>
-      <c r="C172" t="s">
-        <v>192</v>
-      </c>
       <c r="D172" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B173" t="s">
+        <v>271</v>
+      </c>
+      <c r="C173" t="s">
+        <v>296</v>
+      </c>
+      <c r="D173" t="s">
         <v>272</v>
-      </c>
-      <c r="C173" t="s">
-        <v>297</v>
-      </c>
-      <c r="D173" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B174" t="s">
         <v>157</v>
@@ -4144,72 +4144,72 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B175" t="s">
+        <v>334</v>
+      </c>
+      <c r="C175" t="s">
         <v>335</v>
       </c>
-      <c r="C175" t="s">
+      <c r="D175" t="s">
         <v>336</v>
-      </c>
-      <c r="D175" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B176" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C176" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D176" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B177" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C177" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D177" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B178" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C178" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D178" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B179" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C179" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D179" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4217,13 +4217,13 @@
         <v>47</v>
       </c>
       <c r="B180" t="s">
+        <v>192</v>
+      </c>
+      <c r="C180" t="s">
         <v>193</v>
       </c>
-      <c r="C180" t="s">
-        <v>194</v>
-      </c>
       <c r="D180" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4231,13 +4231,13 @@
         <v>47</v>
       </c>
       <c r="B181" t="s">
+        <v>291</v>
+      </c>
+      <c r="C181" t="s">
+        <v>300</v>
+      </c>
+      <c r="D181" t="s">
         <v>292</v>
-      </c>
-      <c r="C181" t="s">
-        <v>301</v>
-      </c>
-      <c r="D181" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4273,13 +4273,13 @@
         <v>47</v>
       </c>
       <c r="B184" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C184" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D184" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4287,13 +4287,13 @@
         <v>47</v>
       </c>
       <c r="B185" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C185" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D185" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4304,7 +4304,7 @@
         <v>125</v>
       </c>
       <c r="C186" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D186" t="s">
         <v>125</v>
@@ -4329,13 +4329,13 @@
         <v>47</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4343,24 +4343,24 @@
         <v>47</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B190" t="s">
         <v>171</v>
       </c>
       <c r="C190" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D190" t="s">
         <v>172</v>
@@ -4371,13 +4371,13 @@
         <v>50</v>
       </c>
       <c r="B191" t="s">
+        <v>308</v>
+      </c>
+      <c r="C191" t="s">
         <v>309</v>
       </c>
-      <c r="C191" t="s">
-        <v>310</v>
-      </c>
       <c r="D191" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4416,7 +4416,7 @@
         <v>175</v>
       </c>
       <c r="C194" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D194" t="s">
         <v>176</v>
@@ -4430,7 +4430,7 @@
         <v>169</v>
       </c>
       <c r="C195" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D195" t="s">
         <v>170</v>
@@ -4444,7 +4444,7 @@
         <v>173</v>
       </c>
       <c r="C196" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D196" t="s">
         <v>174</v>
@@ -4522,72 +4522,72 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B202" t="s">
+        <v>194</v>
+      </c>
+      <c r="C202" t="s">
+        <v>253</v>
+      </c>
+      <c r="D202" t="s">
         <v>195</v>
-      </c>
-      <c r="C202" t="s">
-        <v>254</v>
-      </c>
-      <c r="D202" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B203" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C203" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D203" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B204" t="s">
+        <v>198</v>
+      </c>
+      <c r="C204" t="s">
+        <v>253</v>
+      </c>
+      <c r="D204" t="s">
         <v>199</v>
-      </c>
-      <c r="C204" t="s">
-        <v>254</v>
-      </c>
-      <c r="D204" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B205" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C205" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D205" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>106</v>
       </c>
       <c r="C206" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D206" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="D206" s="2" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -4595,13 +4595,13 @@
         <v>47</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C207" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D207" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="D207" s="2" t="s">
-        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merging to prod (#330)
* Adding single click event sample (#327)

* Fixing space (#328)

* Updating yarn lock (#326)

* Fix Yarn (#329)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21814"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5647262E-8AEC-4E66-8191-17A9E4427C2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D102768-7975-406F-90DD-6E8A85FC9F19}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="420">
   <si>
     <t>Class</t>
   </si>
@@ -1268,6 +1268,18 @@
   </si>
   <si>
     <t>SettableCellProperties</t>
+  </si>
+  <si>
+    <t>excel-event-worksheet-single-click</t>
+  </si>
+  <si>
+    <t>registerClickHandler</t>
+  </si>
+  <si>
+    <t>onSingleClicked</t>
+  </si>
+  <si>
+    <t>WorksheetSingleClickedEventArgs</t>
   </si>
 </sst>
 </file>
@@ -1347,8 +1359,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D205" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D205" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D207" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D207" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D205">
     <sortCondition ref="A1:A205"/>
   </sortState>
@@ -1679,22 +1691,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D205"/>
+  <dimension ref="A1:D207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A125" sqref="A125"/>
+      <pane ySplit="1" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K206" sqref="K206"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1708,7 +1720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>269</v>
       </c>
@@ -1722,7 +1734,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>386</v>
       </c>
@@ -1736,7 +1748,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1750,7 +1762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>411</v>
       </c>
@@ -1764,7 +1776,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>412</v>
       </c>
@@ -1778,7 +1790,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>410</v>
       </c>
@@ -1792,7 +1804,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>413</v>
       </c>
@@ -1806,7 +1818,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>414</v>
       </c>
@@ -1820,7 +1832,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -1834,7 +1846,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -1848,7 +1860,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -1862,7 +1874,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -1876,7 +1888,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>146</v>
       </c>
@@ -1890,7 +1902,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>208</v>
       </c>
@@ -1904,7 +1916,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>136</v>
       </c>
@@ -1918,7 +1930,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -1932,7 +1944,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>136</v>
       </c>
@@ -1946,7 +1958,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>136</v>
       </c>
@@ -1960,7 +1972,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>136</v>
       </c>
@@ -1974,7 +1986,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>136</v>
       </c>
@@ -1988,7 +2000,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>136</v>
       </c>
@@ -2002,7 +2014,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>259</v>
       </c>
@@ -2016,7 +2028,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>259</v>
       </c>
@@ -2030,7 +2042,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>126</v>
       </c>
@@ -2044,7 +2056,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>124</v>
       </c>
@@ -2058,7 +2070,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -2072,7 +2084,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -2086,7 +2098,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -2100,7 +2112,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>373</v>
       </c>
@@ -2114,7 +2126,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>373</v>
       </c>
@@ -2128,7 +2140,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>373</v>
       </c>
@@ -2142,7 +2154,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>368</v>
       </c>
@@ -2156,7 +2168,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>377</v>
       </c>
@@ -2170,7 +2182,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>377</v>
       </c>
@@ -2184,7 +2196,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>370</v>
       </c>
@@ -2198,7 +2210,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>91</v>
       </c>
@@ -2212,7 +2224,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -2226,7 +2238,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -2240,7 +2252,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -2254,7 +2266,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -2268,7 +2280,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2282,7 +2294,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -2296,7 +2308,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2310,7 +2322,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -2324,7 +2336,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -2338,7 +2350,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -2352,7 +2364,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -2366,7 +2378,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -2380,7 +2392,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2394,7 +2406,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>96</v>
       </c>
@@ -2408,7 +2420,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>78</v>
       </c>
@@ -2422,7 +2434,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -2436,7 +2448,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>78</v>
       </c>
@@ -2450,7 +2462,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>78</v>
       </c>
@@ -2464,7 +2476,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -2478,7 +2490,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>85</v>
       </c>
@@ -2492,7 +2504,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>93</v>
       </c>
@@ -2506,7 +2518,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -2520,7 +2532,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -2534,7 +2546,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>34</v>
       </c>
@@ -2548,7 +2560,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -2562,7 +2574,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>30</v>
       </c>
@@ -2576,7 +2588,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>30</v>
       </c>
@@ -2590,7 +2602,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>30</v>
       </c>
@@ -2604,7 +2616,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -2618,7 +2630,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -2632,7 +2644,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>43</v>
       </c>
@@ -2646,7 +2658,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -2660,7 +2672,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>234</v>
       </c>
@@ -2674,7 +2686,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>234</v>
       </c>
@@ -2688,7 +2700,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>222</v>
       </c>
@@ -2702,7 +2714,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>222</v>
       </c>
@@ -2716,7 +2728,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>222</v>
       </c>
@@ -2730,7 +2742,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>253</v>
       </c>
@@ -2744,7 +2756,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>253</v>
       </c>
@@ -2758,7 +2770,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -2772,7 +2784,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -2786,7 +2798,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>306</v>
       </c>
@@ -2800,7 +2812,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>354</v>
       </c>
@@ -2814,7 +2826,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>354</v>
       </c>
@@ -2828,7 +2840,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>354</v>
       </c>
@@ -2842,7 +2854,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>354</v>
       </c>
@@ -2856,7 +2868,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -2870,7 +2882,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -2884,7 +2896,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -2898,7 +2910,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>320</v>
       </c>
@@ -2912,7 +2924,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>325</v>
       </c>
@@ -2926,7 +2938,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>325</v>
       </c>
@@ -2940,7 +2952,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>325</v>
       </c>
@@ -2954,7 +2966,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>325</v>
       </c>
@@ -2968,7 +2980,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>325</v>
       </c>
@@ -2982,7 +2994,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>325</v>
       </c>
@@ -2996,7 +3008,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>239</v>
       </c>
@@ -3010,7 +3022,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>226</v>
       </c>
@@ -3024,7 +3036,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>226</v>
       </c>
@@ -3038,7 +3050,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>226</v>
       </c>
@@ -3052,7 +3064,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>226</v>
       </c>
@@ -3066,7 +3078,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>226</v>
       </c>
@@ -3080,7 +3092,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>223</v>
       </c>
@@ -3094,7 +3106,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>64</v>
       </c>
@@ -3108,7 +3120,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>64</v>
       </c>
@@ -3122,7 +3134,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>24</v>
       </c>
@@ -3136,7 +3148,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>24</v>
       </c>
@@ -3150,7 +3162,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>24</v>
       </c>
@@ -3164,7 +3176,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>24</v>
       </c>
@@ -3178,7 +3190,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>24</v>
       </c>
@@ -3192,7 +3204,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>24</v>
       </c>
@@ -3206,7 +3218,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>24</v>
       </c>
@@ -3220,7 +3232,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>24</v>
       </c>
@@ -3234,7 +3246,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>24</v>
       </c>
@@ -3248,7 +3260,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>24</v>
       </c>
@@ -3262,7 +3274,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>24</v>
       </c>
@@ -3276,7 +3288,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>24</v>
       </c>
@@ -3290,7 +3302,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>24</v>
       </c>
@@ -3304,7 +3316,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>24</v>
       </c>
@@ -3318,7 +3330,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>401</v>
       </c>
@@ -3332,7 +3344,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>108</v>
       </c>
@@ -3346,7 +3358,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>100</v>
       </c>
@@ -3360,7 +3372,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>100</v>
       </c>
@@ -3374,7 +3386,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>100</v>
       </c>
@@ -3388,7 +3400,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>100</v>
       </c>
@@ -3402,7 +3414,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>342</v>
       </c>
@@ -3416,7 +3428,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>249</v>
       </c>
@@ -3430,7 +3442,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>415</v>
       </c>
@@ -3444,7 +3456,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>20</v>
       </c>
@@ -3458,7 +3470,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>17</v>
       </c>
@@ -3472,7 +3484,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>17</v>
       </c>
@@ -3486,7 +3498,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>17</v>
       </c>
@@ -3500,7 +3512,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>278</v>
       </c>
@@ -3514,7 +3526,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>278</v>
       </c>
@@ -3528,7 +3540,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>278</v>
       </c>
@@ -3542,7 +3554,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>278</v>
       </c>
@@ -3556,7 +3568,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>278</v>
       </c>
@@ -3570,7 +3582,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>278</v>
       </c>
@@ -3584,7 +3596,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>278</v>
       </c>
@@ -3598,7 +3610,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>278</v>
       </c>
@@ -3612,7 +3624,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>278</v>
       </c>
@@ -3626,7 +3638,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>278</v>
       </c>
@@ -3640,7 +3652,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>278</v>
       </c>
@@ -3654,7 +3666,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>278</v>
       </c>
@@ -3668,7 +3680,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>281</v>
       </c>
@@ -3682,7 +3694,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>281</v>
       </c>
@@ -3696,7 +3708,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>281</v>
       </c>
@@ -3710,7 +3722,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>281</v>
       </c>
@@ -3724,7 +3736,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>281</v>
       </c>
@@ -3738,7 +3750,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>359</v>
       </c>
@@ -3752,7 +3764,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>246</v>
       </c>
@@ -3766,7 +3778,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>395</v>
       </c>
@@ -3780,7 +3792,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>395</v>
       </c>
@@ -3794,7 +3806,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>395</v>
       </c>
@@ -3808,7 +3820,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>395</v>
       </c>
@@ -3822,7 +3834,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>389</v>
       </c>
@@ -3836,7 +3848,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>389</v>
       </c>
@@ -3850,7 +3862,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>152</v>
       </c>
@@ -3864,7 +3876,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>152</v>
       </c>
@@ -3878,7 +3890,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>152</v>
       </c>
@@ -3892,7 +3904,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>152</v>
       </c>
@@ -3906,7 +3918,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>156</v>
       </c>
@@ -3920,7 +3932,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>156</v>
       </c>
@@ -3934,7 +3946,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>211</v>
       </c>
@@ -3948,7 +3960,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>211</v>
       </c>
@@ -3962,7 +3974,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>214</v>
       </c>
@@ -3976,7 +3988,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>214</v>
       </c>
@@ -3990,7 +4002,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>214</v>
       </c>
@@ -4004,7 +4016,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>213</v>
       </c>
@@ -4018,7 +4030,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>210</v>
       </c>
@@ -4032,7 +4044,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>82</v>
       </c>
@@ -4046,7 +4058,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>82</v>
       </c>
@@ -4060,7 +4072,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>347</v>
       </c>
@@ -4074,7 +4086,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>190</v>
       </c>
@@ -4088,7 +4100,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>190</v>
       </c>
@@ -4102,7 +4114,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>190</v>
       </c>
@@ -4116,7 +4128,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>190</v>
       </c>
@@ -4130,7 +4142,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>190</v>
       </c>
@@ -4144,7 +4156,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>206</v>
       </c>
@@ -4158,7 +4170,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>206</v>
       </c>
@@ -4172,7 +4184,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>206</v>
       </c>
@@ -4186,7 +4198,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>206</v>
       </c>
@@ -4200,7 +4212,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>47</v>
       </c>
@@ -4214,7 +4226,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>47</v>
       </c>
@@ -4228,7 +4240,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>47</v>
       </c>
@@ -4242,7 +4254,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>47</v>
       </c>
@@ -4256,7 +4268,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>47</v>
       </c>
@@ -4270,7 +4282,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>47</v>
       </c>
@@ -4284,7 +4296,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>47</v>
       </c>
@@ -4298,7 +4310,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>47</v>
       </c>
@@ -4312,7 +4324,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>47</v>
       </c>
@@ -4326,7 +4338,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>47</v>
       </c>
@@ -4340,7 +4352,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>212</v>
       </c>
@@ -4354,7 +4366,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>50</v>
       </c>
@@ -4368,7 +4380,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>50</v>
       </c>
@@ -4382,7 +4394,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>50</v>
       </c>
@@ -4396,7 +4408,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>50</v>
       </c>
@@ -4410,7 +4422,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>50</v>
       </c>
@@ -4424,7 +4436,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>50</v>
       </c>
@@ -4438,7 +4450,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>110</v>
       </c>
@@ -4452,7 +4464,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>110</v>
       </c>
@@ -4466,7 +4478,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>110</v>
       </c>
@@ -4480,7 +4492,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>110</v>
       </c>
@@ -4494,7 +4506,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>110</v>
       </c>
@@ -4508,7 +4520,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>207</v>
       </c>
@@ -4522,7 +4534,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>207</v>
       </c>
@@ -4536,7 +4548,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>207</v>
       </c>
@@ -4550,7 +4562,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>207</v>
       </c>
@@ -4562,6 +4574,34 @@
       </c>
       <c r="D205" t="s">
         <v>203</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[admin] (Snippet Generator) Trimming white space from class and method names (#331)
* Fix Yarn

* Trimming white space from snippet generator
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21916"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D102768-7975-406F-90DD-6E8A85FC9F19}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249ECC4A-8945-4B7C-B60A-5307AC6BE13F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -565,721 +565,721 @@
     <t>markerSize</t>
   </si>
   <si>
+    <t>markerBackgroundColor</t>
+  </si>
+  <si>
+    <t>excel-events-tablecollection-changed</t>
+  </si>
+  <si>
+    <t>tableId</t>
+  </si>
+  <si>
+    <t>// setXAxisValues</t>
+  </si>
+  <si>
+    <t>excel-events-table-changed</t>
+  </si>
+  <si>
+    <t>registerOnChangedHandler</t>
+  </si>
+  <si>
+    <t>onChanged</t>
+  </si>
+  <si>
+    <t>onChange</t>
+  </si>
+  <si>
+    <t>Workbook</t>
+  </si>
+  <si>
+    <t>getActiveCell</t>
+  </si>
+  <si>
+    <t>excel-workbook-get-active-cell</t>
+  </si>
+  <si>
+    <t>copy</t>
+  </si>
+  <si>
+    <t>excel-worksheet-copy</t>
+  </si>
+  <si>
+    <t>protect</t>
+  </si>
+  <si>
+    <t>protectDataInWorksheet</t>
+  </si>
+  <si>
+    <t>protectWorkbookStructure</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>unprotect</t>
+  </si>
+  <si>
+    <t>unprotectDataInWorksheet</t>
+  </si>
+  <si>
+    <t>unprotectWorkbookStructure</t>
+  </si>
+  <si>
+    <t>passwordProtectDataInWorksheet</t>
+  </si>
+  <si>
+    <t>passwordUnprotectDataInWorksheet</t>
+  </si>
+  <si>
+    <t>passwordProtectWorkbookStructure</t>
+  </si>
+  <si>
+    <t>passwordUnprotectWorkbookStructure</t>
+  </si>
+  <si>
+    <t>WorkbookProtection</t>
+  </si>
+  <si>
+    <t>WorksheetProtection</t>
+  </si>
+  <si>
+    <t>ChartLegendFormat</t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t>TableSelectionChangedEventArgs</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>WorksheetAddedEventArgs</t>
+  </si>
+  <si>
+    <t>TableCollection</t>
+  </si>
+  <si>
+    <t>TableChangedEventArgs</t>
+  </si>
+  <si>
+    <t>addPositiveNumberRequirement</t>
+  </si>
+  <si>
+    <t>requireApprovedName</t>
+  </si>
+  <si>
+    <t>warnAboutCommentRedundancy</t>
+  </si>
+  <si>
+    <t>excel-data-validation</t>
+  </si>
+  <si>
+    <t>wholeNumber</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>errorAlert</t>
+  </si>
+  <si>
+    <t>DataValidation</t>
+  </si>
+  <si>
+    <t>PivotTableCollection</t>
+  </si>
+  <si>
+    <t>excel-pivottable-create-and-modify</t>
+  </si>
+  <si>
+    <t>createWithNames</t>
+  </si>
+  <si>
+    <t>PivotTable</t>
+  </si>
+  <si>
+    <t>deletePivot</t>
+  </si>
+  <si>
+    <t>toggleColumn</t>
+  </si>
+  <si>
+    <t>columnHierarchies</t>
+  </si>
+  <si>
+    <t>dataHierarchies</t>
+  </si>
+  <si>
+    <t>addValues</t>
+  </si>
+  <si>
+    <t>changeHierarchyNames</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>DataPivotHierarchy</t>
+  </si>
+  <si>
+    <t>layout</t>
+  </si>
+  <si>
+    <t>changeLayout</t>
+  </si>
+  <si>
+    <t>filterHierarchies</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>PivotLayout</t>
+  </si>
+  <si>
+    <t>getDataBodyRange</t>
+  </si>
+  <si>
+    <t>getCrateTotal</t>
+  </si>
+  <si>
+    <t>showPercentages</t>
+  </si>
+  <si>
+    <t>excel-pivottable-filters-and-summaries</t>
+  </si>
+  <si>
+    <t>excel-pivottable-calculations</t>
+  </si>
+  <si>
+    <t>showAs</t>
+  </si>
+  <si>
+    <t>ShowAsRule</t>
+  </si>
+  <si>
+    <t>baseItem</t>
+  </si>
+  <si>
+    <t>showDifferenceFrom</t>
+  </si>
+  <si>
+    <t>Runtime</t>
+  </si>
+  <si>
+    <t>enableEvents</t>
+  </si>
+  <si>
+    <t>excel-events-disable-events</t>
+  </si>
+  <si>
+    <t>toggleEvents</t>
+  </si>
+  <si>
+    <t>DataValidationRule</t>
+  </si>
+  <si>
+    <t>excel-workbook-data-protection</t>
+  </si>
+  <si>
+    <t>excel-range-range-relationships</t>
+  </si>
+  <si>
+    <t>excel-table-style</t>
+  </si>
+  <si>
+    <t>excel-worksheet-gridlines</t>
+  </si>
+  <si>
+    <t>excel-scenarios-multiple-property-set</t>
+  </si>
+  <si>
+    <t>ChartTitle</t>
+  </si>
+  <si>
+    <t>getSubstring</t>
+  </si>
+  <si>
+    <t>excel-chart-title-format</t>
+  </si>
+  <si>
+    <t>changeTitleSubstring</t>
+  </si>
+  <si>
+    <t>changeTitleOrientation</t>
+  </si>
+  <si>
+    <t>addSeries</t>
+  </si>
+  <si>
+    <t>addNameToHeader</t>
+  </si>
+  <si>
+    <t>excel-events-workbook-and-worksheet-collection</t>
+  </si>
+  <si>
+    <t>excel-events-worksheet</t>
+  </si>
+  <si>
+    <t>excel-range-used-range</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>suspendScreenUpdatingUntilNextSync</t>
+  </si>
+  <si>
+    <t>refreshData</t>
+  </si>
+  <si>
+    <t>getSelectedRanges</t>
+  </si>
+  <si>
+    <t>colorSelectedRanges</t>
+  </si>
+  <si>
+    <t>colorSpecifiedRanges</t>
+  </si>
+  <si>
+    <t>getRanges</t>
+  </si>
+  <si>
+    <t>getSpecialCells</t>
+  </si>
+  <si>
+    <t>colorAllLogicalAndTextRanges</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>rotation</t>
+  </si>
+  <si>
+    <t>createTriangle</t>
+  </si>
+  <si>
+    <t>ShapeCollection</t>
+  </si>
+  <si>
+    <t>addGeometricShape</t>
+  </si>
+  <si>
+    <t>createSmileyFace</t>
+  </si>
+  <si>
+    <t>fill</t>
+  </si>
+  <si>
+    <t>removeAll</t>
+  </si>
+  <si>
+    <t>copyFrom</t>
+  </si>
+  <si>
+    <t>copyFormula</t>
+  </si>
+  <si>
+    <t>find</t>
+  </si>
+  <si>
+    <t>findText</t>
+  </si>
+  <si>
+    <t>findOrNullObject</t>
+  </si>
+  <si>
+    <t>findTextWithNullCheck</t>
+  </si>
+  <si>
+    <t>findAllOrNullObject</t>
+  </si>
+  <si>
+    <t>findCompleted</t>
+  </si>
+  <si>
+    <t>addImage</t>
+  </si>
+  <si>
+    <t>readImageFromFile</t>
+  </si>
+  <si>
+    <t>excel-performance-optimization</t>
+  </si>
+  <si>
+    <t>excel-range-areas</t>
+  </si>
+  <si>
+    <t>excel-shape-create-and-delete</t>
+  </si>
+  <si>
+    <t>excel-range-copyfrom</t>
+  </si>
+  <si>
+    <t>excel-range-find</t>
+  </si>
+  <si>
+    <t>excel-worksheet-find-all</t>
+  </si>
+  <si>
+    <t>excel-shape-images</t>
+  </si>
+  <si>
+    <t>flipImage</t>
+  </si>
+  <si>
+    <t>incrementRotation</t>
+  </si>
+  <si>
+    <t>getImageFormat</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>writeOutImageString</t>
+  </si>
+  <si>
+    <t>insertSheets</t>
+  </si>
+  <si>
+    <t>addFromBase64</t>
+  </si>
+  <si>
+    <t>excel-workbook-insert-external-worksheets</t>
+  </si>
+  <si>
+    <t>incrementLeft</t>
+  </si>
+  <si>
+    <t>incrementTop</t>
+  </si>
+  <si>
+    <t>excel-shape-move-and-order</t>
+  </si>
+  <si>
+    <t>moveLeft</t>
+  </si>
+  <si>
+    <t>moveDown</t>
+  </si>
+  <si>
+    <t>scaleUp</t>
+  </si>
+  <si>
+    <t>moveZOrderDown</t>
+  </si>
+  <si>
+    <t>setZOrder</t>
+  </si>
+  <si>
+    <t>scaleHeight</t>
+  </si>
+  <si>
+    <t>PageBreakCollection</t>
+  </si>
+  <si>
+    <t>excel-worksheet-page-layout</t>
+  </si>
+  <si>
+    <t>setPageBreaks</t>
+  </si>
+  <si>
+    <t>centerHorizontally</t>
+  </si>
+  <si>
+    <t>centerVertically</t>
+  </si>
+  <si>
+    <t>PageLayout</t>
+  </si>
+  <si>
+    <t>center</t>
+  </si>
+  <si>
+    <t>setPrintTitleRows</t>
+  </si>
+  <si>
+    <t>setPrintTitleRow</t>
+  </si>
+  <si>
+    <t>setPrintArea</t>
+  </si>
+  <si>
+    <t>orientation</t>
+  </si>
+  <si>
+    <t>deleteName</t>
+  </si>
+  <si>
+    <t>excel-range-remove-duplicates</t>
+  </si>
+  <si>
+    <t>removeDuplicates</t>
+  </si>
+  <si>
+    <t>uniqueRemaining</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>excel-workbook-save-and-close</t>
+  </si>
+  <si>
+    <t>saveWithoutPrompt</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>closeWithSave</t>
+  </si>
+  <si>
+    <t>createHexagon</t>
+  </si>
+  <si>
+    <t>changeOrientation</t>
+  </si>
+  <si>
+    <t>RemoveDuplicatesResult</t>
+  </si>
+  <si>
+    <t>addTextBox</t>
+  </si>
+  <si>
+    <t>excel-shape-textboxes</t>
+  </si>
+  <si>
+    <t>createTextbox</t>
+  </si>
+  <si>
+    <t>deleteText</t>
+  </si>
+  <si>
+    <t>TextFrame</t>
+  </si>
+  <si>
+    <t>addLine</t>
+  </si>
+  <si>
+    <t>excel-shape-lines</t>
+  </si>
+  <si>
+    <t>addStraightLine</t>
+  </si>
+  <si>
+    <t>arrowLine</t>
+  </si>
+  <si>
+    <t>connectStraightLine</t>
+  </si>
+  <si>
+    <t>disconnectStraightLine</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>connectBeginShape</t>
+  </si>
+  <si>
+    <t>connectEndShape</t>
+  </si>
+  <si>
+    <t>disconnectBeginShape</t>
+  </si>
+  <si>
+    <t>disconnectEndShape</t>
+  </si>
+  <si>
+    <t>ShapeGroup</t>
+  </si>
+  <si>
+    <t>ungroup</t>
+  </si>
+  <si>
+    <t>excel-shape-groups</t>
+  </si>
+  <si>
+    <t>ungroupShapes</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>addGroup</t>
+  </si>
+  <si>
+    <t>groupShapes</t>
+  </si>
+  <si>
+    <t>getAsImage</t>
+  </si>
+  <si>
+    <t>excel-comment</t>
+  </si>
+  <si>
+    <t>CommentCollection</t>
+  </si>
+  <si>
+    <t>addCommentToCell</t>
+  </si>
+  <si>
+    <t>CommentReplyCollection</t>
+  </si>
+  <si>
+    <t>addCommentReply</t>
+  </si>
+  <si>
+    <t>getCommentMetadata</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>load_2</t>
+  </si>
+  <si>
+    <t>editComment</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>CommentReply</t>
+  </si>
+  <si>
+    <t>deleteComment</t>
+  </si>
+  <si>
+    <t>deleteCommentReply</t>
+  </si>
+  <si>
+    <t>lockAspectRatio</t>
+  </si>
+  <si>
+    <t>onTableChanged</t>
+  </si>
+  <si>
+    <t>excel-data-change-event-details</t>
+  </si>
+  <si>
+    <t>details</t>
+  </si>
+  <si>
+    <t>addAutoFilter</t>
+  </si>
+  <si>
+    <t>excel-worksheet-auto-filter</t>
+  </si>
+  <si>
+    <t>AutoFilter</t>
+  </si>
+  <si>
+    <t>apply</t>
+  </si>
+  <si>
+    <t>autoFilter</t>
+  </si>
+  <si>
+    <t>SlicerCollection</t>
+  </si>
+  <si>
+    <t>addSlicer</t>
+  </si>
+  <si>
+    <t>excel-pivottable-slicer</t>
+  </si>
+  <si>
+    <t>slicers</t>
+  </si>
+  <si>
+    <t>formatSlicer</t>
+  </si>
+  <si>
+    <t>applyStyle</t>
+  </si>
+  <si>
+    <t>Slicer</t>
+  </si>
+  <si>
+    <t>addFilters</t>
+  </si>
+  <si>
+    <t>selectItems</t>
+  </si>
+  <si>
+    <t>clearFilters</t>
+  </si>
+  <si>
+    <t>removeFilters</t>
+  </si>
+  <si>
+    <t>removeSlicer</t>
+  </si>
+  <si>
+    <t>RangeAreas</t>
+  </si>
+  <si>
+    <t>colorAllFormulaRanges</t>
+  </si>
+  <si>
+    <t>prompt</t>
+  </si>
+  <si>
+    <t>zoom</t>
+  </si>
+  <si>
+    <t>setZoom</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>excel-range-cell-properties</t>
+  </si>
+  <si>
+    <t>setCellProperties</t>
+  </si>
+  <si>
+    <t>getCellProperties</t>
+  </si>
+  <si>
+    <t>CellPropertiesFont</t>
+  </si>
+  <si>
+    <t>CellPropertiesFill</t>
+  </si>
+  <si>
+    <t>CellPropertiesFillLoadOptions</t>
+  </si>
+  <si>
+    <t>CellPropertiesFontLoadOptions</t>
+  </si>
+  <si>
+    <t>CellPropertiesLoadOptions</t>
+  </si>
+  <si>
+    <t>SettableCellProperties</t>
+  </si>
+  <si>
+    <t>excel-event-worksheet-single-click</t>
+  </si>
+  <si>
+    <t>registerClickHandler</t>
+  </si>
+  <si>
+    <t>onSingleClicked</t>
+  </si>
+  <si>
+    <t>WorksheetSingleClickedEventArgs</t>
+  </si>
+  <si>
     <t>markerForegroundColor</t>
-  </si>
-  <si>
-    <t>markerBackgroundColor</t>
-  </si>
-  <si>
-    <t>excel-events-tablecollection-changed</t>
-  </si>
-  <si>
-    <t>tableId</t>
-  </si>
-  <si>
-    <t>// setXAxisValues</t>
-  </si>
-  <si>
-    <t>excel-events-table-changed</t>
-  </si>
-  <si>
-    <t>registerOnChangedHandler</t>
-  </si>
-  <si>
-    <t>onChanged</t>
-  </si>
-  <si>
-    <t>onChange</t>
-  </si>
-  <si>
-    <t>Workbook</t>
-  </si>
-  <si>
-    <t>getActiveCell</t>
-  </si>
-  <si>
-    <t>excel-workbook-get-active-cell</t>
-  </si>
-  <si>
-    <t>copy</t>
-  </si>
-  <si>
-    <t>excel-worksheet-copy</t>
-  </si>
-  <si>
-    <t>protect</t>
-  </si>
-  <si>
-    <t>protectDataInWorksheet</t>
-  </si>
-  <si>
-    <t>protectWorkbookStructure</t>
-  </si>
-  <si>
-    <t>run</t>
-  </si>
-  <si>
-    <t>unprotect</t>
-  </si>
-  <si>
-    <t>unprotectDataInWorksheet</t>
-  </si>
-  <si>
-    <t>unprotectWorkbookStructure</t>
-  </si>
-  <si>
-    <t>passwordProtectDataInWorksheet</t>
-  </si>
-  <si>
-    <t>passwordUnprotectDataInWorksheet</t>
-  </si>
-  <si>
-    <t>passwordProtectWorkbookStructure</t>
-  </si>
-  <si>
-    <t>passwordUnprotectWorkbookStructure</t>
-  </si>
-  <si>
-    <t>WorkbookProtection</t>
-  </si>
-  <si>
-    <t>WorksheetProtection</t>
-  </si>
-  <si>
-    <t>ChartLegendFormat</t>
-  </si>
-  <si>
-    <t>load</t>
-  </si>
-  <si>
-    <t>TableSelectionChangedEventArgs</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>WorksheetAddedEventArgs</t>
-  </si>
-  <si>
-    <t>TableCollection</t>
-  </si>
-  <si>
-    <t>TableChangedEventArgs</t>
-  </si>
-  <si>
-    <t>addPositiveNumberRequirement</t>
-  </si>
-  <si>
-    <t>requireApprovedName</t>
-  </si>
-  <si>
-    <t>warnAboutCommentRedundancy</t>
-  </si>
-  <si>
-    <t>excel-data-validation</t>
-  </si>
-  <si>
-    <t>wholeNumber</t>
-  </si>
-  <si>
-    <t>list</t>
-  </si>
-  <si>
-    <t>errorAlert</t>
-  </si>
-  <si>
-    <t>DataValidation</t>
-  </si>
-  <si>
-    <t>PivotTableCollection</t>
-  </si>
-  <si>
-    <t>excel-pivottable-create-and-modify</t>
-  </si>
-  <si>
-    <t>createWithNames</t>
-  </si>
-  <si>
-    <t>PivotTable</t>
-  </si>
-  <si>
-    <t>deletePivot</t>
-  </si>
-  <si>
-    <t>toggleColumn</t>
-  </si>
-  <si>
-    <t>columnHierarchies</t>
-  </si>
-  <si>
-    <t>dataHierarchies</t>
-  </si>
-  <si>
-    <t>addValues</t>
-  </si>
-  <si>
-    <t>changeHierarchyNames</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>DataPivotHierarchy</t>
-  </si>
-  <si>
-    <t>layout</t>
-  </si>
-  <si>
-    <t>changeLayout</t>
-  </si>
-  <si>
-    <t>filterHierarchies</t>
-  </si>
-  <si>
-    <t>filter</t>
-  </si>
-  <si>
-    <t>PivotLayout</t>
-  </si>
-  <si>
-    <t>getDataBodyRange</t>
-  </si>
-  <si>
-    <t>getCrateTotal</t>
-  </si>
-  <si>
-    <t>showPercentages</t>
-  </si>
-  <si>
-    <t>excel-pivottable-filters-and-summaries</t>
-  </si>
-  <si>
-    <t>excel-pivottable-calculations</t>
-  </si>
-  <si>
-    <t>showAs</t>
-  </si>
-  <si>
-    <t>ShowAsRule</t>
-  </si>
-  <si>
-    <t>baseItem</t>
-  </si>
-  <si>
-    <t>showDifferenceFrom</t>
-  </si>
-  <si>
-    <t>Runtime</t>
-  </si>
-  <si>
-    <t>enableEvents</t>
-  </si>
-  <si>
-    <t>excel-events-disable-events</t>
-  </si>
-  <si>
-    <t>toggleEvents</t>
-  </si>
-  <si>
-    <t>DataValidationRule</t>
-  </si>
-  <si>
-    <t>excel-workbook-data-protection</t>
-  </si>
-  <si>
-    <t>excel-range-range-relationships</t>
-  </si>
-  <si>
-    <t>excel-table-style</t>
-  </si>
-  <si>
-    <t>excel-worksheet-gridlines</t>
-  </si>
-  <si>
-    <t>excel-scenarios-multiple-property-set</t>
-  </si>
-  <si>
-    <t>ChartTitle</t>
-  </si>
-  <si>
-    <t>getSubstring</t>
-  </si>
-  <si>
-    <t>excel-chart-title-format</t>
-  </si>
-  <si>
-    <t>changeTitleSubstring</t>
-  </si>
-  <si>
-    <t>changeTitleOrientation</t>
-  </si>
-  <si>
-    <t>addSeries</t>
-  </si>
-  <si>
-    <t>addNameToHeader</t>
-  </si>
-  <si>
-    <t>excel-events-workbook-and-worksheet-collection</t>
-  </si>
-  <si>
-    <t>excel-events-worksheet</t>
-  </si>
-  <si>
-    <t>excel-range-used-range</t>
-  </si>
-  <si>
-    <t>Application</t>
-  </si>
-  <si>
-    <t>suspendScreenUpdatingUntilNextSync</t>
-  </si>
-  <si>
-    <t>refreshData</t>
-  </si>
-  <si>
-    <t>getSelectedRanges</t>
-  </si>
-  <si>
-    <t>colorSelectedRanges</t>
-  </si>
-  <si>
-    <t>colorSpecifiedRanges</t>
-  </si>
-  <si>
-    <t>getRanges</t>
-  </si>
-  <si>
-    <t>getSpecialCells</t>
-  </si>
-  <si>
-    <t>colorAllLogicalAndTextRanges</t>
-  </si>
-  <si>
-    <t>Shape</t>
-  </si>
-  <si>
-    <t>rotation</t>
-  </si>
-  <si>
-    <t>createTriangle</t>
-  </si>
-  <si>
-    <t>ShapeCollection</t>
-  </si>
-  <si>
-    <t>addGeometricShape</t>
-  </si>
-  <si>
-    <t>createSmileyFace</t>
-  </si>
-  <si>
-    <t>fill</t>
-  </si>
-  <si>
-    <t>removeAll</t>
-  </si>
-  <si>
-    <t>copyFrom</t>
-  </si>
-  <si>
-    <t>copyFormula</t>
-  </si>
-  <si>
-    <t>find</t>
-  </si>
-  <si>
-    <t>findText</t>
-  </si>
-  <si>
-    <t>findOrNullObject</t>
-  </si>
-  <si>
-    <t>findTextWithNullCheck</t>
-  </si>
-  <si>
-    <t>findAllOrNullObject</t>
-  </si>
-  <si>
-    <t>findCompleted</t>
-  </si>
-  <si>
-    <t>addImage</t>
-  </si>
-  <si>
-    <t>readImageFromFile</t>
-  </si>
-  <si>
-    <t>excel-performance-optimization</t>
-  </si>
-  <si>
-    <t>excel-range-areas</t>
-  </si>
-  <si>
-    <t>excel-shape-create-and-delete</t>
-  </si>
-  <si>
-    <t>excel-range-copyfrom</t>
-  </si>
-  <si>
-    <t>excel-range-find</t>
-  </si>
-  <si>
-    <t>excel-worksheet-find-all</t>
-  </si>
-  <si>
-    <t>excel-shape-images</t>
-  </si>
-  <si>
-    <t>flipImage</t>
-  </si>
-  <si>
-    <t>incrementRotation</t>
-  </si>
-  <si>
-    <t>getImageFormat</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>writeOutImageString</t>
-  </si>
-  <si>
-    <t>insertSheets</t>
-  </si>
-  <si>
-    <t>addFromBase64</t>
-  </si>
-  <si>
-    <t>excel-workbook-insert-external-worksheets</t>
-  </si>
-  <si>
-    <t>incrementLeft</t>
-  </si>
-  <si>
-    <t>incrementTop</t>
-  </si>
-  <si>
-    <t>excel-shape-move-and-order</t>
-  </si>
-  <si>
-    <t>moveLeft</t>
-  </si>
-  <si>
-    <t>moveDown</t>
-  </si>
-  <si>
-    <t>scaleUp</t>
-  </si>
-  <si>
-    <t>moveZOrderDown</t>
-  </si>
-  <si>
-    <t>setZOrder</t>
-  </si>
-  <si>
-    <t>scaleHeight</t>
-  </si>
-  <si>
-    <t>PageBreakCollection</t>
-  </si>
-  <si>
-    <t>excel-worksheet-page-layout</t>
-  </si>
-  <si>
-    <t>setPageBreaks</t>
-  </si>
-  <si>
-    <t>centerHorizontally</t>
-  </si>
-  <si>
-    <t>centerVertically</t>
-  </si>
-  <si>
-    <t>PageLayout</t>
-  </si>
-  <si>
-    <t>center</t>
-  </si>
-  <si>
-    <t>setPrintTitleRows</t>
-  </si>
-  <si>
-    <t>setPrintTitleRow</t>
-  </si>
-  <si>
-    <t>setPrintArea</t>
-  </si>
-  <si>
-    <t>orientation</t>
-  </si>
-  <si>
-    <t>deleteName</t>
-  </si>
-  <si>
-    <t>excel-range-remove-duplicates</t>
-  </si>
-  <si>
-    <t>removeDuplicates</t>
-  </si>
-  <si>
-    <t>uniqueRemaining</t>
-  </si>
-  <si>
-    <t>save</t>
-  </si>
-  <si>
-    <t>excel-workbook-save-and-close</t>
-  </si>
-  <si>
-    <t>saveWithoutPrompt</t>
-  </si>
-  <si>
-    <t>close</t>
-  </si>
-  <si>
-    <t>closeWithSave</t>
-  </si>
-  <si>
-    <t>createHexagon</t>
-  </si>
-  <si>
-    <t>changeOrientation</t>
-  </si>
-  <si>
-    <t>RemoveDuplicatesResult</t>
-  </si>
-  <si>
-    <t>addTextBox</t>
-  </si>
-  <si>
-    <t>excel-shape-textboxes</t>
-  </si>
-  <si>
-    <t>createTextbox</t>
-  </si>
-  <si>
-    <t>deleteText</t>
-  </si>
-  <si>
-    <t>TextFrame</t>
-  </si>
-  <si>
-    <t>addLine</t>
-  </si>
-  <si>
-    <t>excel-shape-lines</t>
-  </si>
-  <si>
-    <t>addStraightLine</t>
-  </si>
-  <si>
-    <t>arrowLine</t>
-  </si>
-  <si>
-    <t>connectStraightLine</t>
-  </si>
-  <si>
-    <t>disconnectStraightLine</t>
-  </si>
-  <si>
-    <t>Line</t>
-  </si>
-  <si>
-    <t>connectBeginShape</t>
-  </si>
-  <si>
-    <t>connectEndShape</t>
-  </si>
-  <si>
-    <t>disconnectBeginShape</t>
-  </si>
-  <si>
-    <t>disconnectEndShape</t>
-  </si>
-  <si>
-    <t>ShapeGroup</t>
-  </si>
-  <si>
-    <t>ungroup</t>
-  </si>
-  <si>
-    <t>excel-shape-groups</t>
-  </si>
-  <si>
-    <t>ungroupShapes</t>
-  </si>
-  <si>
-    <t>group</t>
-  </si>
-  <si>
-    <t>addGroup</t>
-  </si>
-  <si>
-    <t>groupShapes</t>
-  </si>
-  <si>
-    <t>getAsImage</t>
-  </si>
-  <si>
-    <t>excel-comment</t>
-  </si>
-  <si>
-    <t>CommentCollection</t>
-  </si>
-  <si>
-    <t>addCommentToCell</t>
-  </si>
-  <si>
-    <t>CommentReplyCollection</t>
-  </si>
-  <si>
-    <t>addCommentReply</t>
-  </si>
-  <si>
-    <t>getCommentMetadata</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>load_2</t>
-  </si>
-  <si>
-    <t>editComment</t>
-  </si>
-  <si>
-    <t>content</t>
-  </si>
-  <si>
-    <t>CommentReply</t>
-  </si>
-  <si>
-    <t>deleteComment</t>
-  </si>
-  <si>
-    <t>deleteCommentReply</t>
-  </si>
-  <si>
-    <t>lockAspectRatio</t>
-  </si>
-  <si>
-    <t>onTableChanged</t>
-  </si>
-  <si>
-    <t>excel-data-change-event-details</t>
-  </si>
-  <si>
-    <t>details</t>
-  </si>
-  <si>
-    <t>addAutoFilter</t>
-  </si>
-  <si>
-    <t>excel-worksheet-auto-filter</t>
-  </si>
-  <si>
-    <t>AutoFilter</t>
-  </si>
-  <si>
-    <t>apply</t>
-  </si>
-  <si>
-    <t>autoFilter</t>
-  </si>
-  <si>
-    <t>SlicerCollection</t>
-  </si>
-  <si>
-    <t>addSlicer</t>
-  </si>
-  <si>
-    <t>excel-pivottable-slicer</t>
-  </si>
-  <si>
-    <t>slicers</t>
-  </si>
-  <si>
-    <t>formatSlicer</t>
-  </si>
-  <si>
-    <t>applyStyle</t>
-  </si>
-  <si>
-    <t>Slicer</t>
-  </si>
-  <si>
-    <t>addFilters</t>
-  </si>
-  <si>
-    <t>selectItems</t>
-  </si>
-  <si>
-    <t>clearFilters</t>
-  </si>
-  <si>
-    <t>removeFilters</t>
-  </si>
-  <si>
-    <t>removeSlicer</t>
-  </si>
-  <si>
-    <t>RangeAreas</t>
-  </si>
-  <si>
-    <t>colorAllFormulaRanges</t>
-  </si>
-  <si>
-    <t>prompt</t>
-  </si>
-  <si>
-    <t>zoom</t>
-  </si>
-  <si>
-    <t>setZoom</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>excel-range-cell-properties</t>
-  </si>
-  <si>
-    <t>setCellProperties</t>
-  </si>
-  <si>
-    <t>getCellProperties</t>
-  </si>
-  <si>
-    <t>CellPropertiesFont</t>
-  </si>
-  <si>
-    <t>CellPropertiesFill</t>
-  </si>
-  <si>
-    <t>CellPropertiesFillLoadOptions</t>
-  </si>
-  <si>
-    <t>CellPropertiesFontLoadOptions</t>
-  </si>
-  <si>
-    <t>CellPropertiesLoadOptions</t>
-  </si>
-  <si>
-    <t>SettableCellProperties</t>
-  </si>
-  <si>
-    <t>excel-event-worksheet-single-click</t>
-  </si>
-  <si>
-    <t>registerClickHandler</t>
-  </si>
-  <si>
-    <t>onSingleClicked</t>
-  </si>
-  <si>
-    <t>WorksheetSingleClickedEventArgs</t>
   </si>
 </sst>
 </file>
@@ -1694,8 +1694,8 @@
   <dimension ref="A1:D207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K206" sqref="K206"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,30 +1722,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" t="s">
         <v>269</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D2" t="s">
         <v>270</v>
-      </c>
-      <c r="C2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D2" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>387</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1764,72 +1764,72 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>106</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1904,7 +1904,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B15" t="s">
         <v>149</v>
@@ -1927,7 +1927,7 @@
         <v>139</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1949,7 +1949,7 @@
         <v>136</v>
       </c>
       <c r="B18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C18" t="s">
         <v>178</v>
@@ -1963,7 +1963,7 @@
         <v>136</v>
       </c>
       <c r="B19" t="s">
-        <v>181</v>
+        <v>419</v>
       </c>
       <c r="C19" t="s">
         <v>178</v>
@@ -2011,35 +2011,35 @@
         <v>139</v>
       </c>
       <c r="D22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>258</v>
+      </c>
+      <c r="B23" t="s">
         <v>259</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>260</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>261</v>
-      </c>
-      <c r="D23" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B24" t="s">
         <v>113</v>
       </c>
       <c r="C24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D24" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2114,100 +2114,100 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B30" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C30" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D30" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D31" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>372</v>
+      </c>
+      <c r="B32" t="s">
         <v>373</v>
       </c>
-      <c r="B32" t="s">
-        <v>374</v>
-      </c>
       <c r="C32" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D32" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D33" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B34" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C34" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D34" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D35" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D36" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2674,100 +2674,100 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B70" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C70" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D70" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B71" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C71" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D71" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B72" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C72" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D72" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B73" t="s">
         <v>69</v>
       </c>
       <c r="C73" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D73" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B74" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C74" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D74" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B75" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C75" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D75" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B76" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C76" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D76" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2800,72 +2800,72 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B79" t="s">
         <v>86</v>
       </c>
       <c r="C79" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D79" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>353</v>
+      </c>
+      <c r="B80" t="s">
         <v>354</v>
       </c>
-      <c r="B80" t="s">
-        <v>355</v>
-      </c>
       <c r="C80" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D80" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B81" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C81" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D81" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B82" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C82" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D82" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B83" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C83" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D83" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2907,203 +2907,203 @@
         <v>12</v>
       </c>
       <c r="D86" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B87" t="s">
         <v>9</v>
       </c>
       <c r="C87" t="s">
+        <v>320</v>
+      </c>
+      <c r="D87" t="s">
         <v>321</v>
-      </c>
-      <c r="D87" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>324</v>
+      </c>
+      <c r="B88" t="s">
+        <v>322</v>
+      </c>
+      <c r="C88" t="s">
+        <v>320</v>
+      </c>
+      <c r="D88" t="s">
         <v>325</v>
-      </c>
-      <c r="B88" t="s">
-        <v>323</v>
-      </c>
-      <c r="C88" t="s">
-        <v>321</v>
-      </c>
-      <c r="D88" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>324</v>
+      </c>
+      <c r="B89" t="s">
+        <v>323</v>
+      </c>
+      <c r="C89" t="s">
+        <v>320</v>
+      </c>
+      <c r="D89" t="s">
         <v>325</v>
-      </c>
-      <c r="B89" t="s">
-        <v>324</v>
-      </c>
-      <c r="C89" t="s">
-        <v>321</v>
-      </c>
-      <c r="D89" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B90" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C90" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D90" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B91" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C91" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D91" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B92" t="s">
+        <v>326</v>
+      </c>
+      <c r="C92" t="s">
+        <v>320</v>
+      </c>
+      <c r="D92" t="s">
         <v>327</v>
-      </c>
-      <c r="C92" t="s">
-        <v>321</v>
-      </c>
-      <c r="D92" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C93" t="s">
+        <v>320</v>
+      </c>
+      <c r="D93" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="C93" t="s">
-        <v>321</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>238</v>
+      </c>
+      <c r="B94" t="s">
         <v>239</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
+        <v>242</v>
+      </c>
+      <c r="D94" t="s">
         <v>240</v>
-      </c>
-      <c r="C94" t="s">
-        <v>243</v>
-      </c>
-      <c r="D94" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B95" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C95" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D95" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B96" t="s">
+        <v>229</v>
+      </c>
+      <c r="C96" t="s">
+        <v>223</v>
+      </c>
+      <c r="D96" t="s">
         <v>230</v>
-      </c>
-      <c r="C96" t="s">
-        <v>224</v>
-      </c>
-      <c r="D96" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B97" t="s">
         <v>11</v>
       </c>
       <c r="C97" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D97" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B98" t="s">
+        <v>236</v>
+      </c>
+      <c r="C98" t="s">
+        <v>242</v>
+      </c>
+      <c r="D98" t="s">
         <v>237</v>
-      </c>
-      <c r="C98" t="s">
-        <v>243</v>
-      </c>
-      <c r="D98" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B99" t="s">
+        <v>234</v>
+      </c>
+      <c r="C99" t="s">
+        <v>223</v>
+      </c>
+      <c r="D99" t="s">
         <v>235</v>
-      </c>
-      <c r="C99" t="s">
-        <v>224</v>
-      </c>
-      <c r="D99" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B100" t="s">
         <v>9</v>
       </c>
       <c r="C100" t="s">
+        <v>223</v>
+      </c>
+      <c r="D100" t="s">
         <v>224</v>
-      </c>
-      <c r="D100" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3139,13 +3139,13 @@
         <v>24</v>
       </c>
       <c r="B103" t="s">
+        <v>285</v>
+      </c>
+      <c r="C103" t="s">
+        <v>298</v>
+      </c>
+      <c r="D103" t="s">
         <v>286</v>
-      </c>
-      <c r="C103" t="s">
-        <v>299</v>
-      </c>
-      <c r="D103" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -3153,13 +3153,13 @@
         <v>24</v>
       </c>
       <c r="B104" t="s">
+        <v>287</v>
+      </c>
+      <c r="C104" t="s">
+        <v>299</v>
+      </c>
+      <c r="D104" t="s">
         <v>288</v>
-      </c>
-      <c r="C104" t="s">
-        <v>300</v>
-      </c>
-      <c r="D104" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3167,13 +3167,13 @@
         <v>24</v>
       </c>
       <c r="B105" t="s">
+        <v>289</v>
+      </c>
+      <c r="C105" t="s">
+        <v>299</v>
+      </c>
+      <c r="D105" t="s">
         <v>290</v>
-      </c>
-      <c r="C105" t="s">
-        <v>300</v>
-      </c>
-      <c r="D105" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -3184,7 +3184,7 @@
         <v>27</v>
       </c>
       <c r="C106" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D106" t="s">
         <v>28</v>
@@ -3195,13 +3195,13 @@
         <v>24</v>
       </c>
       <c r="B107" t="s">
+        <v>275</v>
+      </c>
+      <c r="C107" t="s">
+        <v>296</v>
+      </c>
+      <c r="D107" t="s">
         <v>276</v>
-      </c>
-      <c r="C107" t="s">
-        <v>297</v>
-      </c>
-      <c r="D107" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -3212,7 +3212,7 @@
         <v>29</v>
       </c>
       <c r="C108" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D108" t="s">
         <v>28</v>
@@ -3226,7 +3226,7 @@
         <v>25</v>
       </c>
       <c r="C109" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D109" t="s">
         <v>26</v>
@@ -3251,13 +3251,13 @@
         <v>24</v>
       </c>
       <c r="B111" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C111" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D111" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -3268,7 +3268,7 @@
         <v>31</v>
       </c>
       <c r="C112" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D112" t="s">
         <v>32</v>
@@ -3282,7 +3282,7 @@
         <v>31</v>
       </c>
       <c r="C113" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D113" t="s">
         <v>33</v>
@@ -3296,7 +3296,7 @@
         <v>79</v>
       </c>
       <c r="C114" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D114" t="s">
         <v>160</v>
@@ -3307,13 +3307,13 @@
         <v>24</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C115" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D115" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3321,27 +3321,27 @@
         <v>24</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C117" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3416,44 +3416,44 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B123" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C123" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D123" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>248</v>
+      </c>
+      <c r="B124" t="s">
         <v>249</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" t="s">
         <v>250</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D124" t="s">
         <v>251</v>
-      </c>
-      <c r="D124" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C125" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D125" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3478,7 +3478,7 @@
         <v>9</v>
       </c>
       <c r="C127" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D127" t="s">
         <v>19</v>
@@ -3506,7 +3506,7 @@
         <v>18</v>
       </c>
       <c r="C129" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D129" t="s">
         <v>19</v>
@@ -3514,352 +3514,352 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B130" t="s">
         <v>11</v>
       </c>
       <c r="C130" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D130" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B131" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C131" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D131" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B132" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C132" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D132" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B133" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C133" t="s">
+        <v>360</v>
+      </c>
+      <c r="D133" t="s">
         <v>361</v>
-      </c>
-      <c r="D133" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B134" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C134" t="s">
+        <v>312</v>
+      </c>
+      <c r="D134" t="s">
         <v>313</v>
-      </c>
-      <c r="D134" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B135" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C135" t="s">
+        <v>301</v>
+      </c>
+      <c r="D135" t="s">
         <v>302</v>
-      </c>
-      <c r="D135" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B136" t="s">
+        <v>311</v>
+      </c>
+      <c r="C136" t="s">
         <v>312</v>
       </c>
-      <c r="C136" t="s">
-        <v>313</v>
-      </c>
       <c r="D136" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B137" t="s">
         <v>134</v>
       </c>
       <c r="C137" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D137" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>277</v>
+      </c>
+      <c r="B138" t="s">
         <v>278</v>
       </c>
-      <c r="B138" t="s">
+      <c r="C138" t="s">
+        <v>297</v>
+      </c>
+      <c r="D138" t="s">
         <v>279</v>
-      </c>
-      <c r="C138" t="s">
-        <v>298</v>
-      </c>
-      <c r="D138" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B139" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C139" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D139" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B140" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C140" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D140" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B141" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C141" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D141" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>280</v>
+      </c>
+      <c r="B142" t="s">
         <v>281</v>
       </c>
-      <c r="B142" t="s">
-        <v>282</v>
-      </c>
       <c r="C142" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D142" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B143" t="s">
+        <v>363</v>
+      </c>
+      <c r="C143" t="s">
+        <v>360</v>
+      </c>
+      <c r="D143" t="s">
         <v>364</v>
-      </c>
-      <c r="C143" t="s">
-        <v>361</v>
-      </c>
-      <c r="D143" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B144" t="s">
+        <v>293</v>
+      </c>
+      <c r="C144" t="s">
+        <v>301</v>
+      </c>
+      <c r="D144" t="s">
         <v>294</v>
-      </c>
-      <c r="C144" t="s">
-        <v>302</v>
-      </c>
-      <c r="D144" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B145" t="s">
+        <v>347</v>
+      </c>
+      <c r="C145" t="s">
         <v>348</v>
       </c>
-      <c r="C145" t="s">
+      <c r="D145" t="s">
         <v>349</v>
-      </c>
-      <c r="D145" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B146" t="s">
+        <v>342</v>
+      </c>
+      <c r="C146" t="s">
         <v>343</v>
       </c>
-      <c r="C146" t="s">
+      <c r="D146" t="s">
         <v>344</v>
-      </c>
-      <c r="D146" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>358</v>
+      </c>
+      <c r="B147" t="s">
         <v>359</v>
       </c>
-      <c r="B147" t="s">
+      <c r="C147" t="s">
         <v>360</v>
       </c>
-      <c r="C147" t="s">
+      <c r="D147" t="s">
         <v>361</v>
-      </c>
-      <c r="D147" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>245</v>
+      </c>
+      <c r="B148" t="s">
         <v>246</v>
       </c>
-      <c r="B148" t="s">
+      <c r="C148" t="s">
+        <v>243</v>
+      </c>
+      <c r="D148" t="s">
         <v>247</v>
-      </c>
-      <c r="C148" t="s">
-        <v>244</v>
-      </c>
-      <c r="D148" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D150" s="2" t="s">
         <v>395</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D150" s="2" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B151" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D151" s="2" t="s">
         <v>398</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D151" s="2" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -3870,7 +3870,7 @@
         <v>11</v>
       </c>
       <c r="C155" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D155" t="s">
         <v>163</v>
@@ -3884,7 +3884,7 @@
         <v>149</v>
       </c>
       <c r="C156" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D156" t="s">
         <v>162</v>
@@ -3898,7 +3898,7 @@
         <v>164</v>
       </c>
       <c r="C157" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D157" t="s">
         <v>160</v>
@@ -3909,10 +3909,10 @@
         <v>152</v>
       </c>
       <c r="B158" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C158" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D158" t="s">
         <v>165</v>
@@ -3926,7 +3926,7 @@
         <v>9</v>
       </c>
       <c r="C159" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3940,7 +3940,7 @@
         <v>37</v>
       </c>
       <c r="C160" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D160" t="s">
         <v>161</v>
@@ -3948,27 +3948,27 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B161" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C161" t="s">
+        <v>185</v>
+      </c>
+      <c r="D161" t="s">
         <v>186</v>
-      </c>
-      <c r="D161" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B162" t="s">
         <v>167</v>
       </c>
       <c r="C162" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D162" t="s">
         <v>168</v>
@@ -3976,69 +3976,69 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B163" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C163" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D163" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B164" t="s">
         <v>171</v>
       </c>
       <c r="C164" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D164" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B165" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C165" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D165" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B166" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C166" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D166" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B167" t="s">
         <v>106</v>
       </c>
       <c r="C167" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D167" t="s">
         <v>166</v>
@@ -4074,63 +4074,63 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B170" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C170" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D170" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B171" t="s">
+        <v>337</v>
+      </c>
+      <c r="C171" t="s">
+        <v>335</v>
+      </c>
+      <c r="D171" t="s">
         <v>338</v>
-      </c>
-      <c r="C171" t="s">
-        <v>336</v>
-      </c>
-      <c r="D171" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
+        <v>189</v>
+      </c>
+      <c r="B172" t="s">
         <v>190</v>
       </c>
-      <c r="B172" t="s">
+      <c r="C172" t="s">
         <v>191</v>
       </c>
-      <c r="C172" t="s">
-        <v>192</v>
-      </c>
       <c r="D172" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B173" t="s">
+        <v>271</v>
+      </c>
+      <c r="C173" t="s">
+        <v>296</v>
+      </c>
+      <c r="D173" t="s">
         <v>272</v>
-      </c>
-      <c r="C173" t="s">
-        <v>297</v>
-      </c>
-      <c r="D173" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B174" t="s">
         <v>157</v>
@@ -4144,72 +4144,72 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B175" t="s">
+        <v>334</v>
+      </c>
+      <c r="C175" t="s">
         <v>335</v>
       </c>
-      <c r="C175" t="s">
+      <c r="D175" t="s">
         <v>336</v>
-      </c>
-      <c r="D175" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B176" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C176" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D176" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B177" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C177" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D177" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B178" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C178" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D178" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B179" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C179" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D179" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4217,13 +4217,13 @@
         <v>47</v>
       </c>
       <c r="B180" t="s">
+        <v>192</v>
+      </c>
+      <c r="C180" t="s">
         <v>193</v>
       </c>
-      <c r="C180" t="s">
-        <v>194</v>
-      </c>
       <c r="D180" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4231,13 +4231,13 @@
         <v>47</v>
       </c>
       <c r="B181" t="s">
+        <v>291</v>
+      </c>
+      <c r="C181" t="s">
+        <v>300</v>
+      </c>
+      <c r="D181" t="s">
         <v>292</v>
-      </c>
-      <c r="C181" t="s">
-        <v>301</v>
-      </c>
-      <c r="D181" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4273,13 +4273,13 @@
         <v>47</v>
       </c>
       <c r="B184" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C184" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D184" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4287,13 +4287,13 @@
         <v>47</v>
       </c>
       <c r="B185" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C185" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D185" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4304,7 +4304,7 @@
         <v>125</v>
       </c>
       <c r="C186" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D186" t="s">
         <v>125</v>
@@ -4329,13 +4329,13 @@
         <v>47</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4343,24 +4343,24 @@
         <v>47</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B190" t="s">
         <v>171</v>
       </c>
       <c r="C190" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D190" t="s">
         <v>172</v>
@@ -4371,13 +4371,13 @@
         <v>50</v>
       </c>
       <c r="B191" t="s">
+        <v>308</v>
+      </c>
+      <c r="C191" t="s">
         <v>309</v>
       </c>
-      <c r="C191" t="s">
-        <v>310</v>
-      </c>
       <c r="D191" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4416,7 +4416,7 @@
         <v>175</v>
       </c>
       <c r="C194" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D194" t="s">
         <v>176</v>
@@ -4430,7 +4430,7 @@
         <v>169</v>
       </c>
       <c r="C195" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D195" t="s">
         <v>170</v>
@@ -4444,7 +4444,7 @@
         <v>173</v>
       </c>
       <c r="C196" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D196" t="s">
         <v>174</v>
@@ -4522,72 +4522,72 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B202" t="s">
+        <v>194</v>
+      </c>
+      <c r="C202" t="s">
+        <v>253</v>
+      </c>
+      <c r="D202" t="s">
         <v>195</v>
-      </c>
-      <c r="C202" t="s">
-        <v>254</v>
-      </c>
-      <c r="D202" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B203" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C203" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D203" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B204" t="s">
+        <v>198</v>
+      </c>
+      <c r="C204" t="s">
+        <v>253</v>
+      </c>
+      <c r="D204" t="s">
         <v>199</v>
-      </c>
-      <c r="C204" t="s">
-        <v>254</v>
-      </c>
-      <c r="D204" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B205" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C205" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D205" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>106</v>
       </c>
       <c r="C206" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D206" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="D206" s="2" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -4595,13 +4595,13 @@
         <v>47</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C207" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D207" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="D207" s="2" t="s">
-        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[excel] (Sort, Events) Samples for onRowSorted and onColumnSorted (#347)
* Initial work

* Partial work

* Running yarn start
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22103"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249ECC4A-8945-4B7C-B60A-5307AC6BE13F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC3567A-C89A-42A7-A00A-552D2F60B82B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-38595" yWindow="-195" windowWidth="38790" windowHeight="21390" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="427">
   <si>
     <t>Class</t>
   </si>
@@ -1280,6 +1280,27 @@
   </si>
   <si>
     <t>markerForegroundColor</t>
+  </si>
+  <si>
+    <t>sort</t>
+  </si>
+  <si>
+    <t>excel-event-column-and-row-sort</t>
+  </si>
+  <si>
+    <t>sortTopToBottom</t>
+  </si>
+  <si>
+    <t>registerRowSortHandler</t>
+  </si>
+  <si>
+    <t>onRowSorted</t>
+  </si>
+  <si>
+    <t>onColumnSorted</t>
+  </si>
+  <si>
+    <t>registerColumnSortHandler</t>
   </si>
 </sst>
 </file>
@@ -1359,8 +1380,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D207" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D207" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:D210" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D210" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D205">
     <sortCondition ref="A1:A205"/>
   </sortState>
@@ -1691,11 +1712,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:D207"/>
+  <dimension ref="A1:D210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <pane ySplit="1" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D210" sqref="D210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4604,6 +4625,48 @@
         <v>416</v>
       </c>
     </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D208" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D209" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D210" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixing snippet maps (#349)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/excel.xlsx
+++ b/snippet-extractor-metadata/excel.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22107"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65C8D5C-A705-4BE2-A0C8-6658DE479AA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FA66FB-554D-463C-A66E-D66D46D8A4DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-450" yWindow="1140" windowWidth="38370" windowHeight="20970" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1385,15 +1386,15 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E210" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:E210" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E205">
-    <sortCondition ref="A1:A205"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E210">
+    <sortCondition ref="A1:A210"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Member Name" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{11AB9856-754B-44BE-89BC-C88E508065F2}" name="Member ID (methods only)" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{93F3F1A3-FAC6-45AF-9419-DAE9A30621C6}" name="SnippetIdIntheYAMLFile" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{C72A9590-19FF-45ED-9604-345729551F30}" name="MethodNameInTheSnippet" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{11AB9856-754B-44BE-89BC-C88E508065F2}" name="Member ID (methods only)" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{93F3F1A3-FAC6-45AF-9419-DAE9A30621C6}" name="SnippetIdIntheYAMLFile" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{C72A9590-19FF-45ED-9604-345729551F30}" name="MethodNameInTheSnippet" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1719,8 +1720,8 @@
   <dimension ref="A1:E210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C210" sqref="C210"/>
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C188" sqref="C188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,9 +1791,6 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
@@ -1924,9 +1922,6 @@
       <c r="B13" t="s">
         <v>146</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
       <c r="D13" t="s">
         <v>143</v>
       </c>
@@ -2378,6 +2373,9 @@
       <c r="B43" t="s">
         <v>98</v>
       </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
       <c r="D43" t="s">
         <v>60</v>
       </c>
@@ -3518,45 +3516,46 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C117" s="2"/>
-      <c r="D117" t="s">
+      <c r="C118" s="2"/>
+      <c r="D118" t="s">
         <v>295</v>
       </c>
-      <c r="E117" s="2" t="s">
+      <c r="E118" s="2" t="s">
         <v>399</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>107</v>
-      </c>
-      <c r="B118" t="s">
-        <v>112</v>
-      </c>
-      <c r="D118" t="s">
-        <v>113</v>
-      </c>
-      <c r="E118" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B119" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D119" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E119" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3564,13 +3563,13 @@
         <v>99</v>
       </c>
       <c r="B120" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D120" t="s">
         <v>103</v>
       </c>
       <c r="E120" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3578,13 +3577,13 @@
         <v>99</v>
       </c>
       <c r="B121" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D121" t="s">
         <v>103</v>
       </c>
       <c r="E121" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3592,7 +3591,7 @@
         <v>99</v>
       </c>
       <c r="B122" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D122" t="s">
         <v>103</v>
@@ -3603,82 +3602,76 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>340</v>
+        <v>99</v>
       </c>
       <c r="B123" t="s">
-        <v>332</v>
+        <v>108</v>
       </c>
       <c r="D123" t="s">
-        <v>330</v>
+        <v>103</v>
       </c>
       <c r="E123" t="s">
-        <v>329</v>
+        <v>104</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>340</v>
+      </c>
+      <c r="B124" t="s">
+        <v>332</v>
+      </c>
+      <c r="D124" t="s">
+        <v>330</v>
+      </c>
+      <c r="E124" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>247</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B125" t="s">
         <v>248</v>
       </c>
-      <c r="C124">
-        <v>1</v>
-      </c>
-      <c r="D124" t="s">
+      <c r="D125" t="s">
         <v>249</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E125" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B126" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C125" s="2"/>
-      <c r="D125" s="2" t="s">
+      <c r="C126" s="2"/>
+      <c r="D126" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="E125" s="2" t="s">
+      <c r="E126" s="2" t="s">
         <v>405</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>19</v>
-      </c>
-      <c r="B126" t="s">
-        <v>10</v>
-      </c>
-      <c r="C126">
-        <v>1</v>
-      </c>
-      <c r="D126" t="s">
-        <v>20</v>
-      </c>
-      <c r="E126" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B127" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>264</v>
+        <v>20</v>
       </c>
       <c r="E127" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3686,16 +3679,16 @@
         <v>16</v>
       </c>
       <c r="B128" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>20</v>
+        <v>264</v>
       </c>
       <c r="E128" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -3703,30 +3696,30 @@
         <v>16</v>
       </c>
       <c r="B129" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>264</v>
+        <v>20</v>
       </c>
       <c r="E129" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>276</v>
+        <v>16</v>
       </c>
       <c r="B130" t="s">
-        <v>10</v>
-      </c>
-      <c r="C130">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D130" t="s">
-        <v>296</v>
+        <v>264</v>
       </c>
       <c r="E130" t="s">
-        <v>283</v>
+        <v>18</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3734,13 +3727,16 @@
         <v>276</v>
       </c>
       <c r="B131" t="s">
-        <v>282</v>
+        <v>10</v>
+      </c>
+      <c r="C131">
+        <v>1</v>
       </c>
       <c r="D131" t="s">
         <v>296</v>
       </c>
       <c r="E131" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -3748,16 +3744,13 @@
         <v>276</v>
       </c>
       <c r="B132" t="s">
-        <v>364</v>
-      </c>
-      <c r="C132">
-        <v>1</v>
+        <v>282</v>
       </c>
       <c r="D132" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E132" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -3765,16 +3758,16 @@
         <v>276</v>
       </c>
       <c r="B133" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>359</v>
+        <v>300</v>
       </c>
       <c r="E133" t="s">
-        <v>360</v>
+        <v>305</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3782,16 +3775,16 @@
         <v>276</v>
       </c>
       <c r="B134" t="s">
-        <v>309</v>
+        <v>361</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134" t="s">
-        <v>311</v>
+        <v>359</v>
       </c>
       <c r="E134" t="s">
-        <v>312</v>
+        <v>360</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3799,16 +3792,16 @@
         <v>276</v>
       </c>
       <c r="B135" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="E135" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3816,16 +3809,16 @@
         <v>276</v>
       </c>
       <c r="B136" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C136">
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="E136" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3833,13 +3826,16 @@
         <v>276</v>
       </c>
       <c r="B137" t="s">
-        <v>133</v>
+        <v>310</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>347</v>
+        <v>311</v>
       </c>
       <c r="E137" t="s">
-        <v>349</v>
+        <v>313</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3847,13 +3843,13 @@
         <v>276</v>
       </c>
       <c r="B138" t="s">
-        <v>277</v>
+        <v>133</v>
       </c>
       <c r="D138" t="s">
-        <v>296</v>
+        <v>347</v>
       </c>
       <c r="E138" t="s">
-        <v>278</v>
+        <v>349</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3861,16 +3857,13 @@
         <v>276</v>
       </c>
       <c r="B139" t="s">
-        <v>317</v>
-      </c>
-      <c r="C139">
-        <v>1</v>
+        <v>277</v>
       </c>
       <c r="D139" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="E139" t="s">
-        <v>314</v>
+        <v>278</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -3878,7 +3871,10 @@
         <v>276</v>
       </c>
       <c r="B140" t="s">
-        <v>377</v>
+        <v>317</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
       </c>
       <c r="D140" t="s">
         <v>311</v>
@@ -3892,33 +3888,30 @@
         <v>276</v>
       </c>
       <c r="B141" t="s">
-        <v>316</v>
-      </c>
-      <c r="C141">
-        <v>1</v>
+        <v>377</v>
       </c>
       <c r="D141" t="s">
         <v>311</v>
       </c>
       <c r="E141" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B142" t="s">
-        <v>280</v>
+        <v>316</v>
       </c>
       <c r="C142">
         <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>296</v>
+        <v>311</v>
       </c>
       <c r="E142" t="s">
-        <v>338</v>
+        <v>315</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -3926,16 +3919,16 @@
         <v>279</v>
       </c>
       <c r="B143" t="s">
-        <v>362</v>
+        <v>280</v>
       </c>
       <c r="C143">
         <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>359</v>
+        <v>296</v>
       </c>
       <c r="E143" t="s">
-        <v>363</v>
+        <v>338</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -3943,16 +3936,16 @@
         <v>279</v>
       </c>
       <c r="B144" t="s">
-        <v>292</v>
+        <v>362</v>
       </c>
       <c r="C144">
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>300</v>
+        <v>359</v>
       </c>
       <c r="E144" t="s">
-        <v>293</v>
+        <v>363</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -3960,16 +3953,16 @@
         <v>279</v>
       </c>
       <c r="B145" t="s">
-        <v>346</v>
+        <v>292</v>
       </c>
       <c r="C145">
         <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>347</v>
+        <v>300</v>
       </c>
       <c r="E145" t="s">
-        <v>348</v>
+        <v>293</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -3977,62 +3970,64 @@
         <v>279</v>
       </c>
       <c r="B146" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="E146" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>357</v>
+        <v>279</v>
       </c>
       <c r="B147" t="s">
-        <v>358</v>
+        <v>341</v>
       </c>
       <c r="C147">
         <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>359</v>
+        <v>342</v>
       </c>
       <c r="E147" t="s">
-        <v>360</v>
+        <v>343</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>357</v>
+      </c>
+      <c r="B148" t="s">
+        <v>358</v>
+      </c>
+      <c r="C148">
+        <v>1</v>
+      </c>
+      <c r="D148" t="s">
+        <v>359</v>
+      </c>
+      <c r="E148" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>244</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B149" t="s">
         <v>245</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D149" t="s">
         <v>242</v>
       </c>
-      <c r="E148" t="s">
+      <c r="E149" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C149" s="2"/>
-      <c r="D149" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="E149" s="2" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -4040,16 +4035,14 @@
         <v>392</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="C150" s="2">
-        <v>1</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C150" s="2"/>
       <c r="D150" s="2" t="s">
         <v>388</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4057,7 +4050,7 @@
         <v>392</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C151" s="2">
         <v>1</v>
@@ -4066,7 +4059,7 @@
         <v>388</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4074,7 +4067,7 @@
         <v>392</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>10</v>
+        <v>395</v>
       </c>
       <c r="C152" s="2">
         <v>1</v>
@@ -4083,15 +4076,15 @@
         <v>388</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C153" s="2">
         <v>1</v>
@@ -4100,7 +4093,7 @@
         <v>388</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4108,7 +4101,7 @@
         <v>386</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C154" s="2">
         <v>1</v>
@@ -4117,24 +4110,24 @@
         <v>388</v>
       </c>
       <c r="E154" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C155" s="2">
+        <v>1</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E155" s="2" t="s">
         <v>390</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>151</v>
-      </c>
-      <c r="B155" t="s">
-        <v>10</v>
-      </c>
-      <c r="C155">
-        <v>1</v>
-      </c>
-      <c r="D155" t="s">
-        <v>254</v>
-      </c>
-      <c r="E155" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4142,13 +4135,16 @@
         <v>151</v>
       </c>
       <c r="B156" t="s">
-        <v>148</v>
+        <v>10</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
       </c>
       <c r="D156" t="s">
         <v>254</v>
       </c>
       <c r="E156" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4156,13 +4152,13 @@
         <v>151</v>
       </c>
       <c r="B157" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D157" t="s">
         <v>254</v>
       </c>
       <c r="E157" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -4170,24 +4166,21 @@
         <v>151</v>
       </c>
       <c r="B158" t="s">
-        <v>207</v>
-      </c>
-      <c r="C158">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="D158" t="s">
         <v>254</v>
       </c>
       <c r="E158" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B159" t="s">
-        <v>8</v>
+        <v>207</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -4196,7 +4189,7 @@
         <v>254</v>
       </c>
       <c r="E159" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4204,7 +4197,7 @@
         <v>155</v>
       </c>
       <c r="B160" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C160">
         <v>1</v>
@@ -4218,16 +4211,19 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>209</v>
+        <v>155</v>
       </c>
       <c r="B161" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="C161">
+        <v>1</v>
       </c>
       <c r="D161" t="s">
-        <v>184</v>
+        <v>254</v>
       </c>
       <c r="E161" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4235,27 +4231,27 @@
         <v>209</v>
       </c>
       <c r="B162" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="D162" t="s">
         <v>184</v>
       </c>
       <c r="E162" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B163" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="D163" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E163" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4263,7 +4259,7 @@
         <v>212</v>
       </c>
       <c r="B164" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="D164" t="s">
         <v>181</v>
@@ -4277,55 +4273,55 @@
         <v>212</v>
       </c>
       <c r="B165" t="s">
-        <v>380</v>
+        <v>170</v>
       </c>
       <c r="D165" t="s">
-        <v>379</v>
+        <v>181</v>
       </c>
       <c r="E165" t="s">
-        <v>378</v>
+        <v>187</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B166" t="s">
-        <v>186</v>
+        <v>380</v>
       </c>
       <c r="D166" t="s">
-        <v>181</v>
+        <v>379</v>
       </c>
       <c r="E166" t="s">
-        <v>185</v>
+        <v>378</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B167" t="s">
-        <v>105</v>
+        <v>186</v>
       </c>
       <c r="D167" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E167" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>81</v>
+        <v>208</v>
       </c>
       <c r="B168" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="D168" t="s">
-        <v>60</v>
+        <v>184</v>
       </c>
       <c r="E168" t="s">
-        <v>83</v>
+        <v>165</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -4333,7 +4329,7 @@
         <v>81</v>
       </c>
       <c r="B169" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="D169" t="s">
         <v>60</v>
@@ -4344,36 +4340,33 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>345</v>
+        <v>81</v>
       </c>
       <c r="B170" t="s">
-        <v>344</v>
-      </c>
-      <c r="C170">
-        <v>1</v>
+        <v>68</v>
       </c>
       <c r="D170" t="s">
-        <v>342</v>
+        <v>60</v>
       </c>
       <c r="E170" t="s">
-        <v>344</v>
+        <v>83</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>188</v>
+        <v>345</v>
       </c>
       <c r="B171" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="C171">
         <v>1</v>
       </c>
       <c r="D171" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="E171" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -4381,16 +4374,16 @@
         <v>188</v>
       </c>
       <c r="B172" t="s">
-        <v>189</v>
+        <v>336</v>
       </c>
       <c r="C172">
         <v>1</v>
       </c>
       <c r="D172" t="s">
-        <v>190</v>
+        <v>334</v>
       </c>
       <c r="E172" t="s">
-        <v>196</v>
+        <v>337</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4398,16 +4391,16 @@
         <v>188</v>
       </c>
       <c r="B173" t="s">
-        <v>270</v>
+        <v>189</v>
       </c>
       <c r="C173">
         <v>1</v>
       </c>
       <c r="D173" t="s">
-        <v>295</v>
+        <v>190</v>
       </c>
       <c r="E173" t="s">
-        <v>271</v>
+        <v>196</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4415,13 +4408,16 @@
         <v>188</v>
       </c>
       <c r="B174" t="s">
-        <v>156</v>
+        <v>270</v>
+      </c>
+      <c r="C174">
+        <v>1</v>
       </c>
       <c r="D174" t="s">
-        <v>157</v>
+        <v>295</v>
       </c>
       <c r="E174" t="s">
-        <v>158</v>
+        <v>271</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -4429,33 +4425,30 @@
         <v>188</v>
       </c>
       <c r="B175" t="s">
-        <v>333</v>
-      </c>
-      <c r="C175">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="D175" t="s">
-        <v>334</v>
+        <v>157</v>
       </c>
       <c r="E175" t="s">
-        <v>335</v>
+        <v>158</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="B176" t="s">
-        <v>193</v>
+        <v>333</v>
       </c>
       <c r="C176">
         <v>1</v>
       </c>
       <c r="D176" t="s">
-        <v>252</v>
+        <v>334</v>
       </c>
       <c r="E176" t="s">
-        <v>195</v>
+        <v>335</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -4472,7 +4465,7 @@
         <v>252</v>
       </c>
       <c r="E177" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -4480,7 +4473,7 @@
         <v>204</v>
       </c>
       <c r="B178" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C178">
         <v>1</v>
@@ -4489,7 +4482,7 @@
         <v>252</v>
       </c>
       <c r="E178" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -4506,24 +4499,24 @@
         <v>252</v>
       </c>
       <c r="E179" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>46</v>
+        <v>204</v>
       </c>
       <c r="B180" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C180">
         <v>1</v>
       </c>
       <c r="D180" t="s">
-        <v>192</v>
+        <v>252</v>
       </c>
       <c r="E180" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -4531,16 +4524,16 @@
         <v>46</v>
       </c>
       <c r="B181" t="s">
-        <v>290</v>
+        <v>191</v>
       </c>
       <c r="C181">
         <v>1</v>
       </c>
       <c r="D181" t="s">
-        <v>299</v>
+        <v>192</v>
       </c>
       <c r="E181" t="s">
-        <v>291</v>
+        <v>196</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -4548,16 +4541,16 @@
         <v>46</v>
       </c>
       <c r="B182" t="s">
-        <v>53</v>
+        <v>290</v>
       </c>
       <c r="C182">
         <v>1</v>
       </c>
       <c r="D182" t="s">
-        <v>51</v>
+        <v>299</v>
       </c>
       <c r="E182" t="s">
-        <v>54</v>
+        <v>291</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -4565,7 +4558,7 @@
         <v>46</v>
       </c>
       <c r="B183" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C183">
         <v>1</v>
@@ -4574,7 +4567,7 @@
         <v>51</v>
       </c>
       <c r="E183" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -4582,16 +4575,16 @@
         <v>46</v>
       </c>
       <c r="B184" t="s">
-        <v>273</v>
+        <v>50</v>
       </c>
       <c r="C184">
         <v>1</v>
       </c>
       <c r="D184" t="s">
-        <v>295</v>
+        <v>51</v>
       </c>
       <c r="E184" t="s">
-        <v>272</v>
+        <v>52</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -4599,13 +4592,16 @@
         <v>46</v>
       </c>
       <c r="B185" t="s">
-        <v>186</v>
+        <v>273</v>
+      </c>
+      <c r="C185">
+        <v>1</v>
       </c>
       <c r="D185" t="s">
-        <v>265</v>
+        <v>295</v>
       </c>
       <c r="E185" t="s">
-        <v>185</v>
+        <v>272</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -4613,16 +4609,13 @@
         <v>46</v>
       </c>
       <c r="B186" t="s">
-        <v>124</v>
-      </c>
-      <c r="C186">
-        <v>1</v>
+        <v>186</v>
       </c>
       <c r="D186" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="E186" t="s">
-        <v>124</v>
+        <v>185</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -4630,28 +4623,27 @@
         <v>46</v>
       </c>
       <c r="B187" t="s">
+        <v>124</v>
+      </c>
+      <c r="D187" t="s">
+        <v>255</v>
+      </c>
+      <c r="E187" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>46</v>
+      </c>
+      <c r="B188" t="s">
         <v>126</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D188" t="s">
         <v>127</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E188" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="C188" s="2"/>
-      <c r="D188" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="E188" s="2" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -4659,93 +4651,88 @@
         <v>46</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C189" s="2"/>
       <c r="D189" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C190" s="2"/>
+      <c r="D190" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="E189" s="2" t="s">
+      <c r="E190" s="2" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>210</v>
-      </c>
-      <c r="B190" t="s">
-        <v>170</v>
-      </c>
-      <c r="D190" t="s">
-        <v>264</v>
-      </c>
-      <c r="E190" t="s">
-        <v>171</v>
-      </c>
-    </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>49</v>
-      </c>
-      <c r="B191" t="s">
-        <v>307</v>
-      </c>
-      <c r="C191">
-        <v>1</v>
-      </c>
-      <c r="D191" t="s">
-        <v>308</v>
-      </c>
-      <c r="E191" t="s">
-        <v>306</v>
+      <c r="A191" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C191" s="2"/>
+      <c r="D191" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="E191" s="2" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>49</v>
-      </c>
-      <c r="B192" t="s">
-        <v>56</v>
-      </c>
-      <c r="C192">
-        <v>1</v>
-      </c>
-      <c r="D192" t="s">
-        <v>51</v>
-      </c>
-      <c r="E192" t="s">
-        <v>54</v>
+      <c r="A192" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C192" s="2"/>
+      <c r="D192" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E192" s="2" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>49</v>
-      </c>
-      <c r="B193" t="s">
-        <v>58</v>
-      </c>
-      <c r="C193">
-        <v>1</v>
-      </c>
-      <c r="D193" t="s">
-        <v>51</v>
-      </c>
-      <c r="E193" t="s">
-        <v>54</v>
+      <c r="A193" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C193" s="2"/>
+      <c r="D193" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E193" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>49</v>
+        <v>210</v>
       </c>
       <c r="B194" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D194" t="s">
         <v>264</v>
       </c>
       <c r="E194" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -4753,13 +4740,16 @@
         <v>49</v>
       </c>
       <c r="B195" t="s">
-        <v>168</v>
+        <v>307</v>
+      </c>
+      <c r="C195">
+        <v>1</v>
       </c>
       <c r="D195" t="s">
-        <v>264</v>
+        <v>308</v>
       </c>
       <c r="E195" t="s">
-        <v>169</v>
+        <v>306</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -4767,81 +4757,75 @@
         <v>49</v>
       </c>
       <c r="B196" t="s">
-        <v>172</v>
+        <v>56</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
       </c>
       <c r="D196" t="s">
-        <v>264</v>
+        <v>51</v>
       </c>
       <c r="E196" t="s">
-        <v>173</v>
+        <v>54</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="B197" t="s">
-        <v>115</v>
+        <v>58</v>
       </c>
       <c r="C197">
         <v>1</v>
       </c>
       <c r="D197" t="s">
-        <v>116</v>
+        <v>51</v>
       </c>
       <c r="E197" t="s">
-        <v>115</v>
+        <v>54</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="B198" t="s">
-        <v>117</v>
-      </c>
-      <c r="C198">
-        <v>1</v>
+        <v>174</v>
       </c>
       <c r="D198" t="s">
-        <v>116</v>
+        <v>264</v>
       </c>
       <c r="E198" t="s">
-        <v>117</v>
+        <v>175</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="B199" t="s">
-        <v>118</v>
-      </c>
-      <c r="C199">
-        <v>1</v>
+        <v>168</v>
       </c>
       <c r="D199" t="s">
-        <v>116</v>
+        <v>264</v>
       </c>
       <c r="E199" t="s">
-        <v>118</v>
+        <v>169</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="B200" t="s">
-        <v>119</v>
-      </c>
-      <c r="C200">
-        <v>1</v>
+        <v>172</v>
       </c>
       <c r="D200" t="s">
-        <v>116</v>
+        <v>264</v>
       </c>
       <c r="E200" t="s">
-        <v>120</v>
+        <v>173</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -4849,7 +4833,7 @@
         <v>109</v>
       </c>
       <c r="B201" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C201">
         <v>1</v>
@@ -4858,152 +4842,158 @@
         <v>116</v>
       </c>
       <c r="E201" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>205</v>
+        <v>109</v>
       </c>
       <c r="B202" t="s">
-        <v>193</v>
+        <v>117</v>
       </c>
       <c r="C202">
         <v>1</v>
       </c>
       <c r="D202" t="s">
-        <v>252</v>
+        <v>116</v>
       </c>
       <c r="E202" t="s">
-        <v>194</v>
+        <v>117</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>205</v>
+        <v>109</v>
       </c>
       <c r="B203" t="s">
-        <v>193</v>
+        <v>118</v>
       </c>
       <c r="C203">
         <v>1</v>
       </c>
       <c r="D203" t="s">
-        <v>252</v>
+        <v>116</v>
       </c>
       <c r="E203" t="s">
-        <v>200</v>
+        <v>118</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>205</v>
+        <v>109</v>
       </c>
       <c r="B204" t="s">
-        <v>197</v>
+        <v>119</v>
       </c>
       <c r="C204">
         <v>1</v>
       </c>
       <c r="D204" t="s">
-        <v>252</v>
+        <v>116</v>
       </c>
       <c r="E204" t="s">
-        <v>198</v>
+        <v>120</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
+        <v>109</v>
+      </c>
+      <c r="B205" t="s">
+        <v>121</v>
+      </c>
+      <c r="C205">
+        <v>1</v>
+      </c>
+      <c r="D205" t="s">
+        <v>116</v>
+      </c>
+      <c r="E205" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
         <v>205</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B206" t="s">
+        <v>193</v>
+      </c>
+      <c r="C206">
+        <v>1</v>
+      </c>
+      <c r="D206" t="s">
+        <v>252</v>
+      </c>
+      <c r="E206" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>205</v>
+      </c>
+      <c r="B207" t="s">
+        <v>193</v>
+      </c>
+      <c r="C207">
+        <v>1</v>
+      </c>
+      <c r="D207" t="s">
+        <v>252</v>
+      </c>
+      <c r="E207" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>205</v>
+      </c>
+      <c r="B208" t="s">
         <v>197</v>
       </c>
-      <c r="C205">
-        <v>1</v>
-      </c>
-      <c r="D205" t="s">
+      <c r="C208">
+  